<commit_message>
minor changes to carbon ledger wkbk
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1565FD-B4AE-0244-B667-EB5778BF7F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D919B1-785D-7041-B023-9DDA159EA843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="760" windowWidth="22100" windowHeight="18540" activeTab="1" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
+    <workbookView xWindow="1680" yWindow="500" windowWidth="22400" windowHeight="16720" activeTab="1" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>Removals (tonnes)</t>
   </si>
   <si>
-    <t>Satisficable</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Demanded</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Satisfiable</t>
   </si>
 </sst>
 </file>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E3B73C-8C04-4845-96FD-F75302BA5D7D}">
   <dimension ref="A1:AX31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AN8" sqref="AN8"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,22 +869,22 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
       <c r="U1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V1" s="12"/>
       <c r="W1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="AC1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
@@ -892,7 +892,7 @@
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
       <c r="AI1" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
@@ -900,13 +900,13 @@
       <c r="AM1" s="1"/>
       <c r="AN1"/>
       <c r="AP1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AQ1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AR1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.2">
@@ -923,7 +923,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>24</v>
@@ -950,10 +950,10 @@
         <v>25</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>24</v>
@@ -968,13 +968,13 @@
         <v>25</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U2" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X2" s="6" t="s">
         <v>24</v>
@@ -983,10 +983,10 @@
         <v>25</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC2" s="4" t="s">
         <v>19</v>
@@ -998,10 +998,10 @@
         <v>21</v>
       </c>
       <c r="AF2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG2" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="AH2" s="4" t="s">
         <v>22</v>
@@ -1016,10 +1016,10 @@
         <v>21</v>
       </c>
       <c r="AL2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM2" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="AN2" s="4" t="s">
         <v>22</v>
@@ -1302,27 +1302,27 @@
         <v>0</v>
       </c>
       <c r="AI4" s="4">
-        <f>AC4*$AQ3</f>
-        <v>1</v>
+        <f>AC4*$AQ2</f>
+        <v>0</v>
       </c>
       <c r="AJ4" s="4">
-        <f>AD4*$AQ3</f>
+        <f t="shared" ref="AJ4:AN4" si="4">AD4*$AQ2</f>
         <v>0</v>
       </c>
       <c r="AK4" s="4">
-        <f>AE4*$AQ3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AL4" s="4">
-        <f>AF4*$AQ3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM4" s="4">
-        <f>AG4*$AQ3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN4" s="4">
-        <f>AH4*$AQ3</f>
+        <f>AH4*$AQ2</f>
         <v>0</v>
       </c>
       <c r="AP4">
@@ -1339,7 +1339,7 @@
         <v>4100000</v>
       </c>
       <c r="AX4">
-        <f t="shared" ref="AX4:AX30" si="4">ROUND(AW4/4,0)</f>
+        <f t="shared" ref="AX4:AX30" si="5">ROUND(AW4/4,0)</f>
         <v>1025000</v>
       </c>
     </row>
@@ -1358,7 +1358,7 @@
         <v>142.193365444888</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G30" si="5">G$3*AA5</f>
+        <f t="shared" ref="G5:G30" si="6">G$3*AA5</f>
         <v>97.794292882182489</v>
       </c>
       <c r="H5" s="5">
@@ -1368,11 +1368,11 @@
         <v>50000</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J30" si="6">J$3*Z5</f>
+        <f t="shared" ref="J5:J30" si="7">J$3*Z5</f>
         <v>0.94795576963258665</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" ref="K5:K30" si="7">K$3*AA5</f>
+        <f t="shared" ref="K5:K30" si="8">K$3*AA5</f>
         <v>2.9338287864654746</v>
       </c>
       <c r="L5" s="6">
@@ -1380,7 +1380,7 @@
         <v>9900</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" ref="M5:M30" si="8">MAX(M4-D4,I4)</f>
+        <f t="shared" ref="M5:M30" si="9">MAX(M4-D4,I4)</f>
         <v>249800</v>
       </c>
       <c r="N5" s="7">
@@ -1399,11 +1399,11 @@
         <v>1024800.8689355539</v>
       </c>
       <c r="R5" s="5">
-        <f t="shared" ref="R5:R30" si="9">MAX(L5-H5,0)*F$3</f>
+        <f t="shared" ref="R5:R30" si="10">MAX(L5-H5,0)*F$3</f>
         <v>735000</v>
       </c>
       <c r="S5" s="5">
-        <f t="shared" ref="S5:S30" si="10">MAX(M5-I5, 0)*G$3</f>
+        <f t="shared" ref="S5:S30" si="11">MAX(M5-I5, 0)*G$3</f>
         <v>19980000</v>
       </c>
       <c r="T5" s="5">
@@ -1456,27 +1456,27 @@
         <v>0</v>
       </c>
       <c r="AI5" s="4">
-        <f>AC5*$AQ4</f>
-        <v>6.0000000000000009</v>
+        <f t="shared" ref="AI5:AI30" si="12">AC5*$AQ3</f>
+        <v>1</v>
       </c>
       <c r="AJ5" s="4">
-        <f>AD5*$AQ4</f>
-        <v>6.0000000000000009</v>
+        <f t="shared" ref="AJ5:AJ30" si="13">AD5*$AQ3</f>
+        <v>1</v>
       </c>
       <c r="AK5" s="4">
-        <f>AE5*$AQ4</f>
+        <f t="shared" ref="AK5:AK30" si="14">AE5*$AQ3</f>
         <v>0</v>
       </c>
       <c r="AL5" s="4">
-        <f>AF5*$AQ4</f>
+        <f t="shared" ref="AL5:AL30" si="15">AF5*$AQ3</f>
         <v>0</v>
       </c>
       <c r="AM5" s="4">
-        <f>AG5*$AQ4</f>
+        <f t="shared" ref="AM5:AM30" si="16">AG5*$AQ3</f>
         <v>0</v>
       </c>
       <c r="AN5" s="4">
-        <f>AH5*$AQ4</f>
+        <f>AH5*$AQ3</f>
         <v>0</v>
       </c>
       <c r="AP5">
@@ -1493,7 +1493,7 @@
         <v>4250000</v>
       </c>
       <c r="AX5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1062500</v>
       </c>
     </row>
@@ -1508,11 +1508,11 @@
         <v>0.7</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ref="F5:F30" si="11">F$3*Z6</f>
+        <f t="shared" ref="F5:F30" si="17">F$3*Z6</f>
         <v>137.52987726421449</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>96.389308996039688</v>
       </c>
       <c r="H6" s="5">
@@ -1522,19 +1522,19 @@
         <v>50000</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.9168658484280966</v>
       </c>
       <c r="K6" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.8916792698811906</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" ref="L6:L30" si="12">MAX(L5-C5,H5)</f>
+        <f t="shared" ref="L6:L30" si="18">MAX(L5-C5,H5)</f>
         <v>9860</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>249680</v>
       </c>
       <c r="N6" s="7">
@@ -1553,11 +1553,11 @@
         <v>1061255.2543846935</v>
       </c>
       <c r="R6" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>729000</v>
       </c>
       <c r="S6" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19968000</v>
       </c>
       <c r="T6" s="5">
@@ -1572,23 +1572,23 @@
         <v>0</v>
       </c>
       <c r="W6" s="5">
-        <f t="shared" ref="W4:W30" si="13">(R6+S6)*(1-T6)+U6</f>
+        <f t="shared" ref="W4:W30" si="19">(R6+S6)*(1-T6)+U6</f>
         <v>14500328.89308949</v>
       </c>
       <c r="X6" s="5">
-        <f t="shared" ref="X6:X30" si="14">X5-P5+L6*J5</f>
+        <f t="shared" ref="X6:X30" si="20">X5-P5+L6*J5</f>
         <v>668395.2035040824</v>
       </c>
       <c r="Y6" s="5">
-        <f t="shared" ref="Y6:Y30" si="15">Y5-Q5+M6*K5</f>
+        <f t="shared" ref="Y6:Y30" si="21">Y5-Q5+M6*K5</f>
         <v>19247017.220329206</v>
       </c>
       <c r="Z6" s="4">
-        <f t="shared" ref="Z6:Z30" si="16">X6/R6</f>
+        <f t="shared" ref="Z6:Z30" si="22">X6/R6</f>
         <v>0.9168658484280966</v>
       </c>
       <c r="AA6" s="4">
-        <f t="shared" ref="AA6:AA30" si="17">Y6/S6</f>
+        <f t="shared" ref="AA6:AA30" si="23">Y6/S6</f>
         <v>0.96389308996039691</v>
       </c>
       <c r="AB6" s="5">
@@ -1610,27 +1610,27 @@
         <v>0</v>
       </c>
       <c r="AI6" s="4">
-        <f>AC6*$AQ5</f>
-        <v>26</v>
+        <f t="shared" si="12"/>
+        <v>6.0000000000000009</v>
       </c>
       <c r="AJ6" s="4">
-        <f>AD6*$AQ5</f>
-        <v>26</v>
+        <f t="shared" si="13"/>
+        <v>6.0000000000000009</v>
       </c>
       <c r="AK6" s="4">
-        <f>AE6*$AQ5</f>
-        <v>33.800000000000004</v>
+        <f t="shared" si="14"/>
+        <v>7.8000000000000007</v>
       </c>
       <c r="AL6" s="4">
-        <f>AF6*$AQ5</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AM6" s="4">
-        <f>AG6*$AQ5</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN6" s="4">
-        <f>AH6*$AQ5</f>
+        <f t="shared" ref="AN5:AN30" si="24">AH6*$AQ4</f>
         <v>0</v>
       </c>
       <c r="AP6">
@@ -1647,7 +1647,7 @@
         <v>4400000</v>
       </c>
       <c r="AX6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1100000</v>
       </c>
     </row>
@@ -1662,11 +1662,11 @@
         <v>0.7</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>132.6374862286807</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>94.745487294728719</v>
       </c>
       <c r="H7" s="5">
@@ -1676,19 +1676,19 @@
         <v>50000</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.88424990819120475</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.8423646188418616</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9815</v>
       </c>
       <c r="M7" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>249560</v>
       </c>
       <c r="N7" s="7">
@@ -1707,11 +1707,11 @@
         <v>1066404.5555112255</v>
       </c>
       <c r="R7" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>722250</v>
       </c>
       <c r="S7" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19956000</v>
       </c>
       <c r="T7" s="5">
@@ -1726,23 +1726,23 @@
         <v>0</v>
       </c>
       <c r="W7" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14486911.701748962</v>
       </c>
       <c r="X7" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>638649.49619109766</v>
       </c>
       <c r="Y7" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>18907409.444536064</v>
       </c>
       <c r="Z7" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.88424990819120475</v>
       </c>
       <c r="AA7" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.94745487294728725</v>
       </c>
       <c r="AB7" s="6">
@@ -1764,27 +1764,27 @@
         <v>0</v>
       </c>
       <c r="AI7" s="4">
-        <f>AC7*$AQ6</f>
-        <v>86</v>
+        <f t="shared" si="12"/>
+        <v>26</v>
       </c>
       <c r="AJ7" s="4">
-        <f>AD7*$AQ6</f>
-        <v>86</v>
+        <f t="shared" si="13"/>
+        <v>26</v>
       </c>
       <c r="AK7" s="4">
-        <f>AE7*$AQ6</f>
-        <v>111.8</v>
+        <f t="shared" si="14"/>
+        <v>33.800000000000004</v>
       </c>
       <c r="AL7" s="4">
-        <f>AF7*$AQ6</f>
-        <v>172</v>
+        <f t="shared" si="15"/>
+        <v>52</v>
       </c>
       <c r="AM7" s="4">
-        <f>AG7*$AQ6</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN7" s="4">
-        <f>AH7*$AQ6</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AP7">
@@ -1801,7 +1801,7 @@
         <v>4420000</v>
       </c>
       <c r="AX7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1105000</v>
       </c>
     </row>
@@ -1816,11 +1816,11 @@
         <v>0.7</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>127.60863172019944</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>93.01045086015219</v>
       </c>
       <c r="H8" s="5">
@@ -1830,19 +1830,19 @@
         <v>50000</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.85072421146799626</v>
       </c>
       <c r="K8" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.7903135258045655</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9770</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>249440</v>
       </c>
       <c r="N8" s="7">
@@ -1853,19 +1853,19 @@
         <v>1127100</v>
       </c>
       <c r="P8" s="7">
-        <f t="shared" ref="P8:P30" si="18">$O8*R8/($R8+$S8)</f>
+        <f t="shared" ref="P8:P30" si="25">$O8*R8/($R8+$S8)</f>
         <v>39034.829013286864</v>
       </c>
       <c r="Q8" s="7">
-        <f t="shared" ref="Q8:Q30" si="19">$O8*S8/($R8+$S8)</f>
+        <f t="shared" ref="Q8:Q30" si="26">$O8*S8/($R8+$S8)</f>
         <v>1088065.1709867131</v>
       </c>
       <c r="R8" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>715500</v>
       </c>
       <c r="S8" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19944000</v>
       </c>
       <c r="T8" s="5">
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="W8" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14473035.919560418</v>
       </c>
       <c r="X8" s="5">
@@ -1888,15 +1888,15 @@
         <v>608693.17330535129</v>
       </c>
       <c r="Y8" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>18550004.319548752</v>
       </c>
       <c r="Z8" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.85072421146799626</v>
       </c>
       <c r="AA8" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.93010450860152183</v>
       </c>
       <c r="AB8" s="6">
@@ -1918,27 +1918,27 @@
         <v>200</v>
       </c>
       <c r="AI8" s="4">
-        <f>AC8*$AQ7</f>
-        <v>266</v>
+        <f t="shared" si="12"/>
+        <v>86</v>
       </c>
       <c r="AJ8" s="4">
-        <f>AD8*$AQ7</f>
-        <v>266</v>
+        <f t="shared" si="13"/>
+        <v>86</v>
       </c>
       <c r="AK8" s="4">
-        <f>AE8*$AQ7</f>
-        <v>345.8</v>
+        <f t="shared" si="14"/>
+        <v>111.8</v>
       </c>
       <c r="AL8" s="4">
-        <f>AF8*$AQ7</f>
-        <v>532</v>
+        <f t="shared" si="15"/>
+        <v>172</v>
       </c>
       <c r="AM8" s="4">
-        <f>AG8*$AQ7</f>
-        <v>532</v>
+        <f t="shared" si="16"/>
+        <v>172</v>
       </c>
       <c r="AN8" s="4">
-        <f>AH8*$AQ7</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AP8">
@@ -1955,7 +1955,7 @@
         <v>4508400</v>
       </c>
       <c r="AX8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1127100</v>
       </c>
     </row>
@@ -1970,11 +1970,11 @@
         <v>0.7</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>122.18517777370995</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>91.097833217016017</v>
       </c>
       <c r="H9" s="5">
@@ -1984,19 +1984,19 @@
         <v>50000</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.81456785182473301</v>
       </c>
       <c r="K9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.7329349965104806</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9730</v>
       </c>
       <c r="M9" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>249320</v>
       </c>
       <c r="N9" s="7">
@@ -2007,19 +2007,19 @@
         <v>1149643</v>
       </c>
       <c r="P9" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>39516.10631494804</v>
       </c>
       <c r="Q9" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1110126.8936850519</v>
       </c>
       <c r="R9" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>709500</v>
       </c>
       <c r="S9" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19932000</v>
       </c>
       <c r="T9" s="5">
@@ -2034,23 +2034,23 @@
         <v>0</v>
       </c>
       <c r="W9" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14460978.699212309</v>
       </c>
       <c r="X9" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>577935.89086964808</v>
       </c>
       <c r="Y9" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>18157620.116815634</v>
       </c>
       <c r="Z9" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.81456785182473301</v>
       </c>
       <c r="AA9" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.91097833217016022</v>
       </c>
       <c r="AB9" s="5">
@@ -2075,28 +2075,28 @@
         <v>200</v>
       </c>
       <c r="AI9" s="4">
-        <f>AC9*$AQ8</f>
-        <v>566</v>
+        <f t="shared" si="12"/>
+        <v>266</v>
       </c>
       <c r="AJ9" s="4">
-        <f>AD9*$AQ8</f>
-        <v>566</v>
+        <f t="shared" si="13"/>
+        <v>266</v>
       </c>
       <c r="AK9" s="4">
-        <f>AE9*$AQ8</f>
-        <v>735.80000000000007</v>
+        <f t="shared" si="14"/>
+        <v>345.8</v>
       </c>
       <c r="AL9" s="4">
-        <f>AF9*$AQ8</f>
-        <v>1132</v>
+        <f t="shared" si="15"/>
+        <v>532</v>
       </c>
       <c r="AM9" s="4">
-        <f>AG9*$AQ8</f>
-        <v>1132</v>
+        <f t="shared" si="16"/>
+        <v>532</v>
       </c>
       <c r="AN9" s="4">
-        <f>AH9*$AQ8</f>
-        <v>1132</v>
+        <f t="shared" si="24"/>
+        <v>532</v>
       </c>
       <c r="AP9">
         <v>6</v>
@@ -2112,7 +2112,7 @@
         <v>4598570</v>
       </c>
       <c r="AX9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1149643</v>
       </c>
     </row>
@@ -2127,11 +2127,11 @@
         <v>0.7</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>116.73179516247083</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>88.9986979129568</v>
       </c>
       <c r="H10" s="5">
@@ -2141,19 +2141,19 @@
         <v>50000</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.7782119677498055</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.6699609373887041</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9680</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>249200</v>
       </c>
       <c r="N10" s="7">
@@ -2164,19 +2164,19 @@
         <v>1172635</v>
       </c>
       <c r="P10" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>39918.037532732036</v>
       </c>
       <c r="Q10" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1132716.9624672679</v>
       </c>
       <c r="R10" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>702000</v>
       </c>
       <c r="S10" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19920000</v>
       </c>
       <c r="T10" s="5">
@@ -2191,23 +2191,23 @@
         <v>0</v>
       </c>
       <c r="W10" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14447778.626021512</v>
       </c>
       <c r="X10" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>546304.80136036349</v>
       </c>
       <c r="Y10" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>17728540.624260996</v>
       </c>
       <c r="Z10" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.7782119677498055</v>
       </c>
       <c r="AA10" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.88998697912956803</v>
       </c>
       <c r="AB10" s="6">
@@ -2232,28 +2232,28 @@
         <v>200</v>
       </c>
       <c r="AI10" s="4">
-        <f>AC10*$AQ9</f>
-        <v>1166</v>
+        <f t="shared" si="12"/>
+        <v>566</v>
       </c>
       <c r="AJ10" s="4">
-        <f>AD10*$AQ9</f>
-        <v>1166</v>
+        <f t="shared" si="13"/>
+        <v>566</v>
       </c>
       <c r="AK10" s="4">
-        <f>AE10*$AQ9</f>
-        <v>1515.8</v>
+        <f t="shared" si="14"/>
+        <v>735.80000000000007</v>
       </c>
       <c r="AL10" s="4">
-        <f>AF10*$AQ9</f>
-        <v>2332</v>
+        <f t="shared" si="15"/>
+        <v>1132</v>
       </c>
       <c r="AM10" s="4">
-        <f>AG10*$AQ9</f>
-        <v>2332</v>
+        <f t="shared" si="16"/>
+        <v>1132</v>
       </c>
       <c r="AN10" s="4">
-        <f>AH10*$AQ9</f>
-        <v>2332</v>
+        <f t="shared" si="24"/>
+        <v>1132</v>
       </c>
       <c r="AP10">
         <v>10</v>
@@ -2269,7 +2269,7 @@
         <v>4690540</v>
       </c>
       <c r="AX10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1172635</v>
       </c>
     </row>
@@ -2284,11 +2284,11 @@
         <v>0.7</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>111.22795735008324</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>86.703122021692309</v>
       </c>
       <c r="H11" s="5">
@@ -2298,19 +2298,19 @@
         <v>50000</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.74151971566722163</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.6010936606507693</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9620</v>
       </c>
       <c r="M11" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>249080</v>
       </c>
       <c r="N11" s="7">
@@ -2321,19 +2321,19 @@
         <v>1196088</v>
       </c>
       <c r="P11" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>40235.376146788993</v>
       </c>
       <c r="Q11" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1155852.6238532111</v>
       </c>
       <c r="R11" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>693000</v>
       </c>
       <c r="S11" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19908000</v>
       </c>
       <c r="T11" s="5">
@@ -2348,23 +2348,23 @@
         <v>0</v>
       </c>
       <c r="W11" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14435769.019264327</v>
       </c>
       <c r="X11" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>513873.1629573846</v>
       </c>
       <c r="Y11" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>17260857.532078505</v>
       </c>
       <c r="Z11" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.74151971566722163</v>
       </c>
       <c r="AA11" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.86703122021692303</v>
       </c>
       <c r="AB11" s="6">
@@ -2389,28 +2389,28 @@
         <v>200</v>
       </c>
       <c r="AI11" s="4">
-        <f>AC11*$AQ10</f>
-        <v>2166</v>
+        <f t="shared" si="12"/>
+        <v>1166</v>
       </c>
       <c r="AJ11" s="4">
-        <f>AD11*$AQ10</f>
-        <v>2166</v>
+        <f t="shared" si="13"/>
+        <v>1166</v>
       </c>
       <c r="AK11" s="4">
-        <f>AE11*$AQ10</f>
-        <v>2815.8</v>
+        <f t="shared" si="14"/>
+        <v>1515.8</v>
       </c>
       <c r="AL11" s="4">
-        <f>AF11*$AQ10</f>
-        <v>4332</v>
+        <f t="shared" si="15"/>
+        <v>2332</v>
       </c>
       <c r="AM11" s="4">
-        <f>AG11*$AQ10</f>
-        <v>4332</v>
+        <f t="shared" si="16"/>
+        <v>2332</v>
       </c>
       <c r="AN11" s="4">
-        <f>AH11*$AQ10</f>
-        <v>4332</v>
+        <f t="shared" si="24"/>
+        <v>2332</v>
       </c>
       <c r="AP11">
         <v>12</v>
@@ -2426,7 +2426,7 @@
         <v>4784350</v>
       </c>
       <c r="AX11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1196088</v>
       </c>
     </row>
@@ -2441,11 +2441,11 @@
         <v>0.7</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>106.34890586366096</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>84.200709619928176</v>
       </c>
       <c r="H12" s="5">
@@ -2455,19 +2455,19 @@
         <v>50000</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.70899270575773976</v>
       </c>
       <c r="K12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.5260212885978452</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9520</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248960</v>
       </c>
       <c r="N12" s="7">
@@ -2478,19 +2478,19 @@
         <v>1220010</v>
       </c>
       <c r="P12" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>40204.470691163602</v>
       </c>
       <c r="Q12" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1179805.5293088364</v>
       </c>
       <c r="R12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>678000</v>
       </c>
       <c r="S12" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19896000</v>
       </c>
       <c r="T12" s="5">
@@ -2505,23 +2505,23 @@
         <v>0</v>
       </c>
       <c r="W12" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14416317.283018529</v>
       </c>
       <c r="X12" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>480697.05450374755</v>
       </c>
       <c r="Y12" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>16752573.18598091</v>
       </c>
       <c r="Z12" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.70899270575773976</v>
       </c>
       <c r="AA12" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.84200709619928182</v>
       </c>
       <c r="AB12" s="5">
@@ -2546,28 +2546,28 @@
         <v>200</v>
       </c>
       <c r="AI12" s="4">
-        <f>AC12*$AQ11</f>
-        <v>3365.9999999999995</v>
+        <f t="shared" si="12"/>
+        <v>2166</v>
       </c>
       <c r="AJ12" s="4">
-        <f>AD12*$AQ11</f>
-        <v>3365.9999999999995</v>
+        <f t="shared" si="13"/>
+        <v>2166</v>
       </c>
       <c r="AK12" s="4">
-        <f>AE12*$AQ11</f>
-        <v>4375.7999999999993</v>
+        <f t="shared" si="14"/>
+        <v>2815.8</v>
       </c>
       <c r="AL12" s="4">
-        <f>AF12*$AQ11</f>
-        <v>6731.9999999999991</v>
+        <f t="shared" si="15"/>
+        <v>4332</v>
       </c>
       <c r="AM12" s="4">
-        <f>AG12*$AQ11</f>
-        <v>6731.9999999999991</v>
+        <f t="shared" si="16"/>
+        <v>4332</v>
       </c>
       <c r="AN12" s="4">
-        <f>AH12*$AQ11</f>
-        <v>6731.9999999999991</v>
+        <f t="shared" si="24"/>
+        <v>4332</v>
       </c>
       <c r="AP12">
         <v>13.5</v>
@@ -2583,7 +2583,7 @@
         <v>4880040</v>
       </c>
       <c r="AX12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1220010</v>
       </c>
     </row>
@@ -2598,11 +2598,11 @@
         <v>0.7</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>101.16997626715425</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>81.479293875109448</v>
       </c>
       <c r="H13" s="5">
@@ -2612,19 +2612,19 @@
         <v>50000</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.67446650844769507</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.4443788162532836</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9420</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248840</v>
       </c>
       <c r="N13" s="7">
@@ -2635,19 +2635,19 @@
         <v>1244410</v>
       </c>
       <c r="P13" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>40153.980143086585</v>
       </c>
       <c r="Q13" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1204256.0198569135</v>
       </c>
       <c r="R13" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>663000</v>
       </c>
       <c r="S13" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19884000</v>
       </c>
       <c r="T13" s="5">
@@ -2662,23 +2662,23 @@
         <v>0</v>
       </c>
       <c r="W13" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14396826.159024211</v>
       </c>
       <c r="X13" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>447171.29510082182</v>
       </c>
       <c r="Y13" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>16201342.794126762</v>
       </c>
       <c r="Z13" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.67446650844769507</v>
       </c>
       <c r="AA13" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.81479293875109449</v>
       </c>
       <c r="AB13" s="6">
@@ -2703,28 +2703,28 @@
         <v>200</v>
       </c>
       <c r="AI13" s="4">
-        <f>AC13*$AQ12</f>
-        <v>4716</v>
+        <f t="shared" si="12"/>
+        <v>3365.9999999999995</v>
       </c>
       <c r="AJ13" s="4">
-        <f>AD13*$AQ12</f>
-        <v>4716</v>
+        <f t="shared" si="13"/>
+        <v>3365.9999999999995</v>
       </c>
       <c r="AK13" s="4">
-        <f>AE13*$AQ12</f>
-        <v>6130.7999999999993</v>
+        <f t="shared" si="14"/>
+        <v>4375.7999999999993</v>
       </c>
       <c r="AL13" s="4">
-        <f>AF13*$AQ12</f>
-        <v>9432</v>
+        <f t="shared" si="15"/>
+        <v>6731.9999999999991</v>
       </c>
       <c r="AM13" s="4">
-        <f>AG13*$AQ12</f>
-        <v>9432</v>
+        <f t="shared" si="16"/>
+        <v>6731.9999999999991</v>
       </c>
       <c r="AN13" s="4">
-        <f>AH13*$AQ12</f>
-        <v>9432</v>
+        <f t="shared" si="24"/>
+        <v>6731.9999999999991</v>
       </c>
       <c r="AP13">
         <v>12</v>
@@ -2740,7 +2740,7 @@
         <v>4977640</v>
       </c>
       <c r="AX13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1244410</v>
       </c>
     </row>
@@ -2755,11 +2755,11 @@
         <v>0.7</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>95.672070096404568</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>78.527841553182185</v>
       </c>
       <c r="H14" s="5">
@@ -2769,19 +2769,19 @@
         <v>50000</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.6378138006426971</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.3558352465954657</v>
       </c>
       <c r="L14" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9320</v>
       </c>
       <c r="M14" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248720</v>
       </c>
       <c r="N14" s="7">
@@ -2792,19 +2792,19 @@
         <v>1269298</v>
       </c>
       <c r="P14" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>40083.094736842104</v>
       </c>
       <c r="Q14" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1229214.9052631578</v>
       </c>
       <c r="R14" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>648000</v>
       </c>
       <c r="S14" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19872000</v>
       </c>
       <c r="T14" s="5">
@@ -2819,23 +2819,23 @@
         <v>0</v>
       </c>
       <c r="W14" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14375953.974615866</v>
       </c>
       <c r="X14" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>413303.34281646775</v>
       </c>
       <c r="Y14" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>15605052.673448365</v>
       </c>
       <c r="Z14" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.6378138006426971</v>
       </c>
       <c r="AA14" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.78527841553182187</v>
       </c>
       <c r="AB14" s="6">
@@ -2860,28 +2860,28 @@
         <v>200</v>
       </c>
       <c r="AI14" s="4">
-        <f>AC14*$AQ13</f>
-        <v>5916</v>
+        <f t="shared" si="12"/>
+        <v>4716</v>
       </c>
       <c r="AJ14" s="4">
-        <f>AD14*$AQ13</f>
-        <v>5916</v>
+        <f t="shared" si="13"/>
+        <v>4716</v>
       </c>
       <c r="AK14" s="4">
-        <f>AE14*$AQ13</f>
-        <v>7690.7999999999993</v>
+        <f t="shared" si="14"/>
+        <v>6130.7999999999993</v>
       </c>
       <c r="AL14" s="4">
-        <f>AF14*$AQ13</f>
-        <v>11832</v>
+        <f t="shared" si="15"/>
+        <v>9432</v>
       </c>
       <c r="AM14" s="4">
-        <f>AG14*$AQ13</f>
-        <v>11832</v>
+        <f t="shared" si="16"/>
+        <v>9432</v>
       </c>
       <c r="AN14" s="4">
-        <f>AH14*$AQ13</f>
-        <v>11832</v>
+        <f t="shared" si="24"/>
+        <v>9432</v>
       </c>
       <c r="AP14">
         <v>10</v>
@@ -2897,7 +2897,7 @@
         <v>5077190</v>
       </c>
       <c r="AX14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1269298</v>
       </c>
     </row>
@@ -2912,11 +2912,11 @@
         <v>0.7</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>89.413596131500981</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75.334835903770596</v>
       </c>
       <c r="H15" s="5">
@@ -2926,19 +2926,19 @@
         <v>50000</v>
       </c>
       <c r="J15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.59609064087667318</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.2600450771131175</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9240</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248600</v>
       </c>
       <c r="N15" s="7">
@@ -2949,19 +2949,19 @@
         <v>1294683</v>
       </c>
       <c r="P15" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>40174.589578454332</v>
       </c>
       <c r="Q15" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1254508.4104215456</v>
       </c>
       <c r="R15" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>636000</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19860000</v>
       </c>
       <c r="T15" s="5">
@@ -2976,23 +2976,23 @@
         <v>0</v>
       </c>
       <c r="W15" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14358222.34001282</v>
       </c>
       <c r="X15" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>379113.64759756415</v>
       </c>
       <c r="Y15" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>14961498.41048884</v>
       </c>
       <c r="Z15" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.59609064087667318</v>
       </c>
       <c r="AA15" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.75334835903770592</v>
       </c>
       <c r="AB15" s="5">
@@ -3017,28 +3017,28 @@
         <v>200</v>
       </c>
       <c r="AI15" s="4">
-        <f>AC15*$AQ14</f>
-        <v>6916</v>
+        <f t="shared" si="12"/>
+        <v>5916</v>
       </c>
       <c r="AJ15" s="4">
-        <f>AD15*$AQ14</f>
-        <v>6916</v>
+        <f t="shared" si="13"/>
+        <v>5916</v>
       </c>
       <c r="AK15" s="4">
-        <f>AE15*$AQ14</f>
-        <v>8990.7999999999993</v>
+        <f t="shared" si="14"/>
+        <v>7690.7999999999993</v>
       </c>
       <c r="AL15" s="4">
-        <f>AF15*$AQ14</f>
-        <v>13832</v>
+        <f t="shared" si="15"/>
+        <v>11832</v>
       </c>
       <c r="AM15" s="4">
-        <f>AG15*$AQ14</f>
-        <v>13832</v>
+        <f t="shared" si="16"/>
+        <v>11832</v>
       </c>
       <c r="AN15" s="4">
-        <f>AH15*$AQ14</f>
-        <v>13832</v>
+        <f t="shared" si="24"/>
+        <v>11832</v>
       </c>
       <c r="AP15">
         <v>6</v>
@@ -3054,7 +3054,7 @@
         <v>5178730</v>
       </c>
       <c r="AX15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1294683</v>
       </c>
     </row>
@@ -3069,11 +3069,11 @@
         <v>0.7</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>82.689610742555715</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>71.88918783166244</v>
       </c>
       <c r="H16" s="5">
@@ -3083,19 +3083,19 @@
         <v>50000</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.55126407161703805</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.156675634949873</v>
       </c>
       <c r="L16" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9165</v>
       </c>
       <c r="M16" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248480</v>
       </c>
       <c r="N16" s="7">
@@ -3106,19 +3106,19 @@
         <v>1320575</v>
       </c>
       <c r="P16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>40298.896398871671</v>
       </c>
       <c r="Q16" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1280276.1036011283</v>
       </c>
       <c r="R16" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>624750</v>
       </c>
       <c r="S16" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19848000</v>
       </c>
       <c r="T16" s="5">
@@ -3133,23 +3133,23 @@
         <v>0</v>
       </c>
       <c r="W16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14340436.655429047</v>
       </c>
       <c r="X16" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>344402.22874274454</v>
       </c>
       <c r="Y16" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>14268566.000828361</v>
       </c>
       <c r="Z16" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.55126407161703805</v>
       </c>
       <c r="AA16" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.71889187831662438</v>
       </c>
       <c r="AB16" s="6">
@@ -3174,28 +3174,28 @@
         <v>200</v>
       </c>
       <c r="AI16" s="4">
-        <f>AC16*$AQ15</f>
-        <v>7516</v>
+        <f t="shared" si="12"/>
+        <v>6916</v>
       </c>
       <c r="AJ16" s="4">
-        <f>AD16*$AQ15</f>
-        <v>7516</v>
+        <f t="shared" si="13"/>
+        <v>6916</v>
       </c>
       <c r="AK16" s="4">
-        <f>AE16*$AQ15</f>
-        <v>9770.7999999999993</v>
+        <f t="shared" si="14"/>
+        <v>8990.7999999999993</v>
       </c>
       <c r="AL16" s="4">
-        <f>AF16*$AQ15</f>
-        <v>15032</v>
+        <f t="shared" si="15"/>
+        <v>13832</v>
       </c>
       <c r="AM16" s="4">
-        <f>AG16*$AQ15</f>
-        <v>15032</v>
+        <f t="shared" si="16"/>
+        <v>13832</v>
       </c>
       <c r="AN16" s="4">
-        <f>AH16*$AQ15</f>
-        <v>15032</v>
+        <f t="shared" si="24"/>
+        <v>13832</v>
       </c>
       <c r="AP16">
         <v>3</v>
@@ -3211,7 +3211,7 @@
         <v>5282300</v>
       </c>
       <c r="AX16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1320575</v>
       </c>
     </row>
@@ -3226,11 +3226,11 @@
         <v>0.7</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>75.303920028245059</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>68.17867441985976</v>
       </c>
       <c r="H17" s="5">
@@ -3240,19 +3240,19 @@
         <v>50000</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.50202613352163372</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.0453602325957929</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9105</v>
       </c>
       <c r="M17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248360</v>
       </c>
       <c r="N17" s="7">
@@ -3263,19 +3263,19 @@
         <v>1346988</v>
       </c>
       <c r="P17" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>40554.371190729398</v>
       </c>
       <c r="Q17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1306433.6288092707</v>
       </c>
       <c r="R17" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>615750</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19836000</v>
       </c>
       <c r="T17" s="5">
@@ -3290,23 +3290,23 @@
         <v>0</v>
       </c>
       <c r="W17" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14324060.518412059</v>
       </c>
       <c r="X17" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>309122.59171594598</v>
       </c>
       <c r="Y17" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>13523921.857923383</v>
       </c>
       <c r="Z17" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.50202613352163372</v>
       </c>
       <c r="AA17" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.68178674419859764</v>
       </c>
       <c r="AB17" s="6">
@@ -3331,28 +3331,28 @@
         <v>200</v>
       </c>
       <c r="AI17" s="4">
-        <f>AC17*$AQ16</f>
-        <v>7816</v>
+        <f t="shared" si="12"/>
+        <v>7516</v>
       </c>
       <c r="AJ17" s="4">
-        <f>AD17*$AQ16</f>
-        <v>7816</v>
+        <f t="shared" si="13"/>
+        <v>7516</v>
       </c>
       <c r="AK17" s="4">
-        <f>AE17*$AQ16</f>
-        <v>10160.799999999999</v>
+        <f t="shared" si="14"/>
+        <v>9770.7999999999993</v>
       </c>
       <c r="AL17" s="4">
-        <f>AF17*$AQ16</f>
-        <v>15632</v>
+        <f t="shared" si="15"/>
+        <v>15032</v>
       </c>
       <c r="AM17" s="4">
-        <f>AG17*$AQ16</f>
-        <v>15632</v>
+        <f t="shared" si="16"/>
+        <v>15032</v>
       </c>
       <c r="AN17" s="4">
-        <f>AH17*$AQ16</f>
-        <v>15632</v>
+        <f t="shared" si="24"/>
+        <v>15032</v>
       </c>
       <c r="AP17">
         <v>1.8</v>
@@ -3368,7 +3368,7 @@
         <v>5387950</v>
       </c>
       <c r="AX17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1346988</v>
       </c>
     </row>
@@ -3383,11 +3383,11 @@
         <v>0.7</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>67.187967386369053</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64.191023271053737</v>
       </c>
       <c r="H18" s="5">
@@ -3397,19 +3397,19 @@
         <v>50000</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.44791978257579368</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.9257306981316122</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9065</v>
       </c>
       <c r="M18" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248240</v>
       </c>
       <c r="N18" s="7">
@@ -3420,19 +3420,19 @@
         <v>1373928</v>
       </c>
       <c r="P18" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>40998.475463387775</v>
       </c>
       <c r="Q18" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1332929.5245366122</v>
       </c>
       <c r="R18" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>609750</v>
       </c>
       <c r="S18" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19824000</v>
       </c>
       <c r="T18" s="5">
@@ -3447,23 +3447,23 @@
         <v>0</v>
       </c>
       <c r="W18" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14309957.677498179</v>
       </c>
       <c r="X18" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>273119.0874255902</v>
       </c>
       <c r="Y18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>12725228.453253692</v>
       </c>
       <c r="Z18" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.44791978257579368</v>
       </c>
       <c r="AA18" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.64191023271053738</v>
       </c>
       <c r="AB18" s="5">
@@ -3488,28 +3488,28 @@
         <v>200</v>
       </c>
       <c r="AI18" s="4">
-        <f>AC18*$AQ17</f>
-        <v>7995.9999999999991</v>
+        <f t="shared" si="12"/>
+        <v>7816</v>
       </c>
       <c r="AJ18" s="4">
-        <f>AD18*$AQ17</f>
-        <v>7995.9999999999991</v>
+        <f t="shared" si="13"/>
+        <v>7816</v>
       </c>
       <c r="AK18" s="4">
-        <f>AE18*$AQ17</f>
-        <v>10394.799999999999</v>
+        <f t="shared" si="14"/>
+        <v>10160.799999999999</v>
       </c>
       <c r="AL18" s="4">
-        <f>AF18*$AQ17</f>
-        <v>15991.999999999998</v>
+        <f t="shared" si="15"/>
+        <v>15632</v>
       </c>
       <c r="AM18" s="4">
-        <f>AG18*$AQ17</f>
-        <v>15991.999999999998</v>
+        <f t="shared" si="16"/>
+        <v>15632</v>
       </c>
       <c r="AN18" s="4">
-        <f>AH18*$AQ17</f>
-        <v>15991.999999999998</v>
+        <f t="shared" si="24"/>
+        <v>15632</v>
       </c>
       <c r="AP18">
         <v>1.1000000000000001</v>
@@ -3525,7 +3525,7 @@
         <v>5495710</v>
       </c>
       <c r="AX18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1373928</v>
       </c>
     </row>
@@ -3540,11 +3540,11 @@
         <v>0.7</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>58.386167217700972</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59.913745354015226</v>
       </c>
       <c r="H19" s="5">
@@ -3554,19 +3554,19 @@
         <v>50000</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.38924111478467316</v>
       </c>
       <c r="K19" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.7974123606204566</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9045</v>
       </c>
       <c r="M19" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248120</v>
       </c>
       <c r="N19" s="7">
@@ -3577,19 +3577,19 @@
         <v>1401405</v>
       </c>
       <c r="P19" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>41643.219283746555</v>
       </c>
       <c r="Q19" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1359761.7807162534</v>
       </c>
       <c r="R19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>606750</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19812000</v>
       </c>
       <c r="T19" s="5">
@@ -3604,23 +3604,23 @@
         <v>0</v>
       </c>
       <c r="W19" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14298975.160950786</v>
       </c>
       <c r="X19" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>236172.04639560045</v>
       </c>
       <c r="Y19" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>11870111.229537496</v>
       </c>
       <c r="Z19" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.38924111478467316</v>
       </c>
       <c r="AA19" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.59913745354015224</v>
       </c>
       <c r="AB19" s="6">
@@ -3645,28 +3645,28 @@
         <v>200</v>
       </c>
       <c r="AI19" s="4">
-        <f>AC19*$AQ18</f>
-        <v>8105.9999999999991</v>
+        <f t="shared" si="12"/>
+        <v>7995.9999999999991</v>
       </c>
       <c r="AJ19" s="4">
-        <f>AD19*$AQ18</f>
-        <v>8105.9999999999991</v>
+        <f t="shared" si="13"/>
+        <v>7995.9999999999991</v>
       </c>
       <c r="AK19" s="4">
-        <f>AE19*$AQ18</f>
-        <v>10537.8</v>
+        <f t="shared" si="14"/>
+        <v>10394.799999999999</v>
       </c>
       <c r="AL19" s="4">
-        <f>AF19*$AQ18</f>
-        <v>16211.999999999998</v>
+        <f t="shared" si="15"/>
+        <v>15991.999999999998</v>
       </c>
       <c r="AM19" s="4">
-        <f>AG19*$AQ18</f>
-        <v>16211.999999999998</v>
+        <f t="shared" si="16"/>
+        <v>15991.999999999998</v>
       </c>
       <c r="AN19" s="4">
-        <f>AH19*$AQ18</f>
-        <v>16211.999999999998</v>
+        <f t="shared" si="24"/>
+        <v>15991.999999999998</v>
       </c>
       <c r="AP19">
         <v>0.5</v>
@@ -3682,7 +3682,7 @@
         <v>5605620</v>
       </c>
       <c r="AX19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1401405</v>
       </c>
     </row>
@@ -3697,11 +3697,11 @@
         <v>0.7</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>49.202913831747971</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55.333877344722815</v>
       </c>
       <c r="H20" s="5">
@@ -3711,19 +3711,19 @@
         <v>50000</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.32801942554498648</v>
       </c>
       <c r="K20" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.6600163203416844</v>
       </c>
       <c r="L20" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9025</v>
       </c>
       <c r="M20" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>248000</v>
       </c>
       <c r="N20" s="7">
@@ -3734,19 +3734,19 @@
         <v>1429433</v>
       </c>
       <c r="P20" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>42297.135269251972</v>
       </c>
       <c r="Q20" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1387135.8647307481</v>
       </c>
       <c r="R20" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>603750</v>
       </c>
       <c r="S20" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19800000</v>
       </c>
       <c r="T20" s="5">
@@ -3761,23 +3761,23 @@
         <v>0</v>
       </c>
       <c r="W20" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14287961.886490602</v>
       </c>
       <c r="X20" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>198041.72817278557</v>
       </c>
       <c r="Y20" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>10956107.714255117</v>
       </c>
       <c r="Z20" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.32801942554498648</v>
       </c>
       <c r="AA20" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.55333877344722815</v>
       </c>
       <c r="AB20" s="6">
@@ -3802,28 +3802,28 @@
         <v>200</v>
       </c>
       <c r="AI20" s="4">
-        <f>AC20*$AQ19</f>
-        <v>8155.9999999999991</v>
+        <f t="shared" si="12"/>
+        <v>8105.9999999999991</v>
       </c>
       <c r="AJ20" s="4">
-        <f>AD20*$AQ19</f>
-        <v>8155.9999999999991</v>
+        <f t="shared" si="13"/>
+        <v>8105.9999999999991</v>
       </c>
       <c r="AK20" s="4">
-        <f>AE20*$AQ19</f>
-        <v>10602.8</v>
+        <f t="shared" si="14"/>
+        <v>10537.8</v>
       </c>
       <c r="AL20" s="4">
-        <f>AF20*$AQ19</f>
-        <v>16311.999999999998</v>
+        <f t="shared" si="15"/>
+        <v>16211.999999999998</v>
       </c>
       <c r="AM20" s="4">
-        <f>AG20*$AQ19</f>
-        <v>16311.999999999998</v>
+        <f t="shared" si="16"/>
+        <v>16211.999999999998</v>
       </c>
       <c r="AN20" s="4">
-        <f>AH20*$AQ19</f>
-        <v>16311.999999999998</v>
+        <f t="shared" si="24"/>
+        <v>16211.999999999998</v>
       </c>
       <c r="AP20">
         <v>0.3</v>
@@ -3839,7 +3839,7 @@
         <v>5717730</v>
       </c>
       <c r="AX20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1429433</v>
       </c>
     </row>
@@ -3854,11 +3854,11 @@
         <v>0.7</v>
       </c>
       <c r="F21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>39.625070619367335</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50.436914771632637</v>
       </c>
       <c r="H21" s="5">
@@ -3868,19 +3868,19 @@
         <v>50000</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.26416713746244891</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.513107443148979</v>
       </c>
       <c r="L21" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9005</v>
       </c>
       <c r="M21" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>247880</v>
       </c>
       <c r="N21" s="7">
@@ -3891,19 +3891,19 @@
         <v>0</v>
       </c>
       <c r="P21" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q21" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R21" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>600750</v>
       </c>
       <c r="S21" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19788000</v>
       </c>
       <c r="T21" s="5">
@@ -3918,23 +3918,23 @@
         <v>0</v>
       </c>
       <c r="W21" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14276916.451829487</v>
       </c>
       <c r="X21" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>158698.4078305662</v>
       </c>
       <c r="Y21" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>9980456.6950106658</v>
       </c>
       <c r="Z21" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.26416713746244891</v>
       </c>
       <c r="AA21" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.50436914771632635</v>
       </c>
       <c r="AB21" s="5">
@@ -3959,28 +3959,28 @@
         <v>200</v>
       </c>
       <c r="AI21" s="4">
-        <f>AC21*$AQ20</f>
-        <v>8185.9999999999982</v>
+        <f t="shared" si="12"/>
+        <v>8155.9999999999991</v>
       </c>
       <c r="AJ21" s="4">
-        <f>AD21*$AQ20</f>
-        <v>8185.9999999999982</v>
+        <f t="shared" si="13"/>
+        <v>8155.9999999999991</v>
       </c>
       <c r="AK21" s="4">
-        <f>AE21*$AQ20</f>
-        <v>10641.799999999997</v>
+        <f t="shared" si="14"/>
+        <v>10602.8</v>
       </c>
       <c r="AL21" s="4">
-        <f>AF21*$AQ20</f>
-        <v>16371.999999999996</v>
+        <f t="shared" si="15"/>
+        <v>16311.999999999998</v>
       </c>
       <c r="AM21" s="4">
-        <f>AG21*$AQ20</f>
-        <v>16371.999999999996</v>
+        <f t="shared" si="16"/>
+        <v>16311.999999999998</v>
       </c>
       <c r="AN21" s="4">
-        <f>AH21*$AQ20</f>
-        <v>16371.999999999996</v>
+        <f t="shared" si="24"/>
+        <v>16311.999999999998</v>
       </c>
       <c r="AP21">
         <v>0.2</v>
@@ -3996,7 +3996,7 @@
         <v>5832080</v>
       </c>
       <c r="AX21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1458020</v>
       </c>
     </row>
@@ -4011,11 +4011,11 @@
         <v>0.7</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>40.419560742952648</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>52.363188688942444</v>
       </c>
       <c r="H22" s="5">
@@ -4025,19 +4025,19 @@
         <v>50000</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.26946373828635101</v>
       </c>
       <c r="K22" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5708956606682731</v>
       </c>
       <c r="L22" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8985</v>
       </c>
       <c r="M22" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>247760</v>
       </c>
       <c r="N22" s="7">
@@ -4048,19 +4048,19 @@
         <v>0</v>
       </c>
       <c r="P22" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q22" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R22" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>597750</v>
       </c>
       <c r="S22" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19776000</v>
       </c>
       <c r="T22" s="5">
@@ -4075,23 +4075,23 @@
         <v>0</v>
       </c>
       <c r="W22" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14266589.381700272</v>
       </c>
       <c r="X22" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>161071.94956066631</v>
       </c>
       <c r="Y22" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>10355344.195125258</v>
       </c>
       <c r="Z22" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.26946373828635101</v>
       </c>
       <c r="AA22" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.52363188688942441</v>
       </c>
       <c r="AB22" s="6">
@@ -4116,28 +4116,28 @@
         <v>200</v>
       </c>
       <c r="AI22" s="4">
-        <f>AC22*$AQ21</f>
-        <v>8205.9999999999982</v>
+        <f t="shared" si="12"/>
+        <v>8185.9999999999982</v>
       </c>
       <c r="AJ22" s="4">
-        <f>AD22*$AQ21</f>
-        <v>8205.9999999999982</v>
+        <f t="shared" si="13"/>
+        <v>8185.9999999999982</v>
       </c>
       <c r="AK22" s="4">
-        <f>AE22*$AQ21</f>
-        <v>10667.8</v>
+        <f t="shared" si="14"/>
+        <v>10641.799999999997</v>
       </c>
       <c r="AL22" s="4">
-        <f>AF22*$AQ21</f>
-        <v>16411.999999999996</v>
+        <f t="shared" si="15"/>
+        <v>16371.999999999996</v>
       </c>
       <c r="AM22" s="4">
-        <f>AG22*$AQ21</f>
-        <v>16411.999999999996</v>
+        <f t="shared" si="16"/>
+        <v>16371.999999999996</v>
       </c>
       <c r="AN22" s="4">
-        <f>AH22*$AQ21</f>
-        <v>16411.999999999996</v>
+        <f t="shared" si="24"/>
+        <v>16371.999999999996</v>
       </c>
       <c r="AP22">
         <v>0.18</v>
@@ -4153,7 +4153,7 @@
         <v>5948720</v>
       </c>
       <c r="AX22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1487180</v>
       </c>
     </row>
@@ -4168,11 +4168,11 @@
         <v>0.7</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>41.23270919909293</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54.36329081427418</v>
       </c>
       <c r="H23" s="5">
@@ -4182,19 +4182,19 @@
         <v>50000</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.27488472799395286</v>
       </c>
       <c r="K23" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.6308987244282254</v>
       </c>
       <c r="L23" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8965</v>
       </c>
       <c r="M23" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>247640</v>
       </c>
       <c r="N23" s="7">
@@ -4205,19 +4205,19 @@
         <v>0</v>
       </c>
       <c r="P23" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q23" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R23" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>594750</v>
       </c>
       <c r="S23" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19764000</v>
       </c>
       <c r="T23" s="5">
@@ -4232,23 +4232,23 @@
         <v>0</v>
       </c>
       <c r="W23" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14256268.774357187</v>
       </c>
       <c r="X23" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>163487.69197440345</v>
       </c>
       <c r="Y23" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>10744360.796533149</v>
       </c>
       <c r="Z23" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.27488472799395286</v>
       </c>
       <c r="AA23" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.54363290814274179</v>
       </c>
       <c r="AB23" s="6">
@@ -4273,28 +4273,28 @@
         <v>200</v>
       </c>
       <c r="AI23" s="4">
-        <f>AC23*$AQ22</f>
-        <v>8224</v>
+        <f t="shared" si="12"/>
+        <v>8205.9999999999982</v>
       </c>
       <c r="AJ23" s="4">
-        <f>AD23*$AQ22</f>
-        <v>8224</v>
+        <f t="shared" si="13"/>
+        <v>8205.9999999999982</v>
       </c>
       <c r="AK23" s="4">
-        <f>AE23*$AQ22</f>
-        <v>10691.199999999999</v>
+        <f t="shared" si="14"/>
+        <v>10667.8</v>
       </c>
       <c r="AL23" s="4">
-        <f>AF23*$AQ22</f>
-        <v>16448</v>
+        <f t="shared" si="15"/>
+        <v>16411.999999999996</v>
       </c>
       <c r="AM23" s="4">
-        <f>AG23*$AQ22</f>
-        <v>16448</v>
+        <f t="shared" si="16"/>
+        <v>16411.999999999996</v>
       </c>
       <c r="AN23" s="4">
-        <f>AH23*$AQ22</f>
-        <v>16448</v>
+        <f t="shared" si="24"/>
+        <v>16411.999999999996</v>
       </c>
       <c r="AP23">
         <v>0.17</v>
@@ -4310,7 +4310,7 @@
         <v>6067690</v>
       </c>
       <c r="AX23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1516923</v>
       </c>
     </row>
@@ -4325,11 +4325,11 @@
         <v>0.7</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>42.065028102993502</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56.440061000423356</v>
       </c>
       <c r="H24" s="5">
@@ -4339,19 +4339,19 @@
         <v>50000</v>
       </c>
       <c r="J24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.28043352068662336</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.6932018300127007</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8945</v>
       </c>
       <c r="M24" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>247520</v>
       </c>
       <c r="N24" s="7">
@@ -4362,19 +4362,19 @@
         <v>0</v>
       </c>
       <c r="P24" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q24" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R24" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>591750</v>
       </c>
       <c r="S24" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19752000</v>
       </c>
       <c r="T24" s="5">
@@ -4386,26 +4386,26 @@
       </c>
       <c r="V24" s="14">
         <f t="shared" si="3"/>
-        <v>8241</v>
+        <v>8224</v>
       </c>
       <c r="W24" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14245954.875517478</v>
       </c>
       <c r="X24" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>165946.53586630936</v>
       </c>
       <c r="Y24" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>11148040.848803623</v>
       </c>
       <c r="Z24" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.28043352068662336</v>
       </c>
       <c r="AA24" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.56440061000423358</v>
       </c>
       <c r="AB24" s="5">
@@ -4430,28 +4430,28 @@
         <v>200</v>
       </c>
       <c r="AI24" s="4">
-        <f>AC24*$AQ23</f>
-        <v>8241</v>
+        <f t="shared" si="12"/>
+        <v>8224</v>
       </c>
       <c r="AJ24" s="4">
-        <f>AD24*$AQ23</f>
-        <v>8241</v>
+        <f t="shared" si="13"/>
+        <v>8224</v>
       </c>
       <c r="AK24" s="4">
-        <f>AE24*$AQ23</f>
-        <v>10713.3</v>
+        <f t="shared" si="14"/>
+        <v>10691.199999999999</v>
       </c>
       <c r="AL24" s="4">
-        <f>AF24*$AQ23</f>
-        <v>16482</v>
+        <f t="shared" si="15"/>
+        <v>16448</v>
       </c>
       <c r="AM24" s="4">
-        <f>AG24*$AQ23</f>
-        <v>16482</v>
+        <f t="shared" si="16"/>
+        <v>16448</v>
       </c>
       <c r="AN24" s="4">
-        <f>AH24*$AQ23</f>
-        <v>16482</v>
+        <f t="shared" si="24"/>
+        <v>16448</v>
       </c>
       <c r="AP24">
         <v>0.16</v>
@@ -4467,7 +4467,7 @@
         <v>6189040</v>
       </c>
       <c r="AX24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1547260</v>
       </c>
     </row>
@@ -4482,11 +4482,11 @@
         <v>0.7</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>42.9170458696656</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>58.596448741381792</v>
       </c>
       <c r="H25" s="5">
@@ -4496,19 +4496,19 @@
         <v>50000</v>
       </c>
       <c r="J25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.28611363913110399</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.7578934622414537</v>
       </c>
       <c r="L25" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8925</v>
       </c>
       <c r="M25" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>247400</v>
       </c>
       <c r="N25" s="7">
@@ -4519,19 +4519,19 @@
         <v>0</v>
       </c>
       <c r="P25" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q25" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R25" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>588750</v>
       </c>
       <c r="S25" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19740000</v>
       </c>
       <c r="T25" s="5">
@@ -4543,26 +4543,26 @@
       </c>
       <c r="V25" s="14">
         <f t="shared" si="3"/>
-        <v>16514</v>
+        <v>16482</v>
       </c>
       <c r="W25" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14235647.940336451</v>
       </c>
       <c r="X25" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>168449.40503843749</v>
       </c>
       <c r="Y25" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>11566938.981548766</v>
       </c>
       <c r="Z25" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.28611363913110399</v>
       </c>
       <c r="AA25" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.5859644874138179</v>
       </c>
       <c r="AB25" s="6">
@@ -4587,28 +4587,28 @@
         <v>200</v>
       </c>
       <c r="AI25" s="4">
-        <f>AC25*$AQ24</f>
-        <v>8257</v>
+        <f t="shared" si="12"/>
+        <v>8241</v>
       </c>
       <c r="AJ25" s="4">
-        <f>AD25*$AQ24</f>
-        <v>8257</v>
+        <f t="shared" si="13"/>
+        <v>8241</v>
       </c>
       <c r="AK25" s="4">
-        <f>AE25*$AQ24</f>
-        <v>10734.099999999999</v>
+        <f t="shared" si="14"/>
+        <v>10713.3</v>
       </c>
       <c r="AL25" s="4">
-        <f>AF25*$AQ24</f>
-        <v>16514</v>
+        <f t="shared" si="15"/>
+        <v>16482</v>
       </c>
       <c r="AM25" s="4">
-        <f>AG25*$AQ24</f>
-        <v>16514</v>
+        <f t="shared" si="16"/>
+        <v>16482</v>
       </c>
       <c r="AN25" s="4">
-        <f>AH25*$AQ24</f>
-        <v>16514</v>
+        <f t="shared" si="24"/>
+        <v>16482</v>
       </c>
       <c r="AP25">
         <v>0.15</v>
@@ -4624,7 +4624,7 @@
         <v>6312820</v>
       </c>
       <c r="AX25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1578205</v>
       </c>
     </row>
@@ -4639,11 +4639,11 @@
         <v>0.7</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>43.789307809193332</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60.835517421390072</v>
       </c>
       <c r="H26" s="5">
@@ -4653,19 +4653,19 @@
         <v>50000</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.29192871872795556</v>
       </c>
       <c r="K26" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.8250655226417023</v>
       </c>
       <c r="L26" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8905</v>
       </c>
       <c r="M26" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>247280</v>
       </c>
       <c r="N26" s="7">
@@ -4676,19 +4676,19 @@
         <v>0</v>
       </c>
       <c r="P26" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q26" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R26" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>585750</v>
       </c>
       <c r="S26" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19728000</v>
       </c>
       <c r="T26" s="5">
@@ -4700,26 +4700,26 @@
       </c>
       <c r="V26" s="14">
         <f t="shared" si="3"/>
-        <v>27297.599999999999</v>
+        <v>27248.1</v>
       </c>
       <c r="W26" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14225348.233772725</v>
       </c>
       <c r="X26" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>170997.24699489996</v>
       </c>
       <c r="Y26" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>12001630.876891833</v>
       </c>
       <c r="Z26" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.29192871872795556</v>
       </c>
       <c r="AA26" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.60835517421390073</v>
       </c>
       <c r="AB26" s="6">
@@ -4744,28 +4744,28 @@
         <v>200</v>
       </c>
       <c r="AI26" s="4">
-        <f>AC26*$AQ25</f>
-        <v>8272</v>
+        <f t="shared" si="12"/>
+        <v>8257</v>
       </c>
       <c r="AJ26" s="4">
-        <f>AD26*$AQ25</f>
-        <v>8272</v>
+        <f t="shared" si="13"/>
+        <v>8257</v>
       </c>
       <c r="AK26" s="4">
-        <f>AE26*$AQ25</f>
-        <v>10753.6</v>
+        <f t="shared" si="14"/>
+        <v>10734.099999999999</v>
       </c>
       <c r="AL26" s="4">
-        <f>AF26*$AQ25</f>
-        <v>16544</v>
+        <f t="shared" si="15"/>
+        <v>16514</v>
       </c>
       <c r="AM26" s="4">
-        <f>AG26*$AQ25</f>
-        <v>16544</v>
+        <f t="shared" si="16"/>
+        <v>16514</v>
       </c>
       <c r="AN26" s="4">
-        <f>AH26*$AQ25</f>
-        <v>16544</v>
+        <f t="shared" si="24"/>
+        <v>16514</v>
       </c>
       <c r="AP26">
         <v>0.14000000000000001</v>
@@ -4781,7 +4781,7 @@
         <v>6439080</v>
       </c>
       <c r="AX26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1609770</v>
       </c>
     </row>
@@ -4796,11 +4796,11 @@
         <v>0.7</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>44.682376746666108</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63.16044872929578</v>
       </c>
       <c r="H27" s="5">
@@ -4810,19 +4810,19 @@
         <v>50000</v>
       </c>
       <c r="J27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.29788251164444074</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.8948134618788735</v>
       </c>
       <c r="L27" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8885</v>
       </c>
       <c r="M27" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>247160</v>
       </c>
       <c r="N27" s="7">
@@ -4833,19 +4833,19 @@
         <v>0</v>
       </c>
       <c r="P27" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q27" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R27" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>582750</v>
       </c>
       <c r="S27" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19716000</v>
       </c>
       <c r="T27" s="5">
@@ -4857,26 +4857,26 @@
       </c>
       <c r="V27" s="14">
         <f t="shared" si="3"/>
-        <v>43915.8</v>
+        <v>43841.599999999999</v>
       </c>
       <c r="W27" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14214743.254330488</v>
       </c>
       <c r="X27" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>173591.03366079784</v>
       </c>
       <c r="Y27" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>12452714.071467957</v>
       </c>
       <c r="Z27" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.29788251164444074</v>
       </c>
       <c r="AA27" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.63160448729295782</v>
       </c>
       <c r="AB27" s="5">
@@ -4901,28 +4901,28 @@
         <v>200</v>
       </c>
       <c r="AI27" s="4">
-        <f>AC27*$AQ26</f>
-        <v>8286</v>
+        <f t="shared" si="12"/>
+        <v>8272</v>
       </c>
       <c r="AJ27" s="4">
-        <f>AD27*$AQ26</f>
-        <v>8286</v>
+        <f t="shared" si="13"/>
+        <v>8272</v>
       </c>
       <c r="AK27" s="4">
-        <f>AE27*$AQ26</f>
-        <v>10771.8</v>
+        <f t="shared" si="14"/>
+        <v>10753.6</v>
       </c>
       <c r="AL27" s="4">
-        <f>AF27*$AQ26</f>
-        <v>16572</v>
+        <f t="shared" si="15"/>
+        <v>16544</v>
       </c>
       <c r="AM27" s="4">
-        <f>AG27*$AQ26</f>
-        <v>16572</v>
+        <f t="shared" si="16"/>
+        <v>16544</v>
       </c>
       <c r="AN27" s="4">
-        <f>AH27*$AQ26</f>
-        <v>16572</v>
+        <f t="shared" si="24"/>
+        <v>16544</v>
       </c>
       <c r="AP27">
         <v>0.13</v>
@@ -4938,7 +4938,7 @@
         <v>6567860</v>
       </c>
       <c r="AX27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1641965</v>
       </c>
     </row>
@@ -4953,11 +4953,11 @@
         <v>0.7</v>
       </c>
       <c r="F28" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>45.4799331488109</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65.574547244673738</v>
       </c>
       <c r="H28" s="5">
@@ -4967,19 +4967,19 @@
         <v>50000</v>
       </c>
       <c r="J28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.30319955432540602</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.9672364173402124</v>
       </c>
       <c r="L28" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8875</v>
       </c>
       <c r="M28" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>247040</v>
       </c>
       <c r="N28" s="7">
@@ -4990,19 +4990,19 @@
         <v>1674805</v>
       </c>
       <c r="P28" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>47989.569083447335</v>
       </c>
       <c r="Q28" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>1626815.4309165527</v>
       </c>
       <c r="R28" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>581250</v>
       </c>
       <c r="S28" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19704000</v>
       </c>
       <c r="T28" s="5">
@@ -5014,26 +5014,26 @@
       </c>
       <c r="V28" s="14">
         <f t="shared" si="3"/>
-        <v>60582.7</v>
+        <v>60487.8</v>
       </c>
       <c r="W28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14205501.621500595</v>
       </c>
       <c r="X28" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>176234.74095164225</v>
       </c>
       <c r="Y28" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>12920808.789090514</v>
       </c>
       <c r="Z28" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.30319955432540602</v>
       </c>
       <c r="AA28" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.65574547244673742</v>
       </c>
       <c r="AB28" s="6">
@@ -5058,28 +5058,28 @@
         <v>200</v>
       </c>
       <c r="AI28" s="4">
-        <f>AC28*$AQ27</f>
-        <v>8299</v>
+        <f t="shared" si="12"/>
+        <v>8286</v>
       </c>
       <c r="AJ28" s="4">
-        <f>AD28*$AQ27</f>
-        <v>8299</v>
+        <f t="shared" si="13"/>
+        <v>8286</v>
       </c>
       <c r="AK28" s="4">
-        <f>AE28*$AQ27</f>
-        <v>10788.699999999999</v>
+        <f t="shared" si="14"/>
+        <v>10771.8</v>
       </c>
       <c r="AL28" s="4">
-        <f>AF28*$AQ27</f>
-        <v>16598</v>
+        <f t="shared" si="15"/>
+        <v>16572</v>
       </c>
       <c r="AM28" s="4">
-        <f>AG28*$AQ27</f>
-        <v>16598</v>
+        <f t="shared" si="16"/>
+        <v>16572</v>
       </c>
       <c r="AN28" s="4">
-        <f>AH28*$AQ27</f>
-        <v>16598</v>
+        <f t="shared" si="24"/>
+        <v>16572</v>
       </c>
       <c r="AP28">
         <v>0.125</v>
@@ -5095,7 +5095,7 @@
         <v>6699220</v>
       </c>
       <c r="AX28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1674805</v>
       </c>
     </row>
@@ -5110,11 +5110,11 @@
         <v>0.7</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>33.876594027759289</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59.819944009463768</v>
       </c>
       <c r="H29" s="5">
@@ -5124,19 +5124,19 @@
         <v>50000</v>
       </c>
       <c r="J29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.22584396018506192</v>
       </c>
       <c r="K29" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.7945983202839129</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8865</v>
       </c>
       <c r="M29" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>246920</v>
       </c>
       <c r="N29" s="7">
@@ -5147,19 +5147,19 @@
         <v>0</v>
       </c>
       <c r="P29" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q29" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R29" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>579750</v>
       </c>
       <c r="S29" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19692000</v>
       </c>
       <c r="T29" s="5">
@@ -5171,26 +5171,26 @@
       </c>
       <c r="V29" s="14">
         <f t="shared" si="3"/>
-        <v>60673.95</v>
+        <v>60582.7</v>
       </c>
       <c r="W29" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14195368.443375893</v>
       </c>
       <c r="X29" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>130933.03591728964</v>
       </c>
       <c r="Y29" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>11779743.374343606</v>
       </c>
       <c r="Z29" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.22584396018506192</v>
       </c>
       <c r="AA29" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.59819944009463766</v>
       </c>
       <c r="AB29" s="6">
@@ -5215,28 +5215,28 @@
         <v>200</v>
       </c>
       <c r="AI29" s="4">
-        <f>AC29*$AQ28</f>
-        <v>8311.5</v>
+        <f t="shared" si="12"/>
+        <v>8299</v>
       </c>
       <c r="AJ29" s="4">
-        <f>AD29*$AQ28</f>
-        <v>8311.5</v>
+        <f t="shared" si="13"/>
+        <v>8299</v>
       </c>
       <c r="AK29" s="4">
-        <f>AE29*$AQ28</f>
-        <v>10804.949999999999</v>
+        <f t="shared" si="14"/>
+        <v>10788.699999999999</v>
       </c>
       <c r="AL29" s="4">
-        <f>AF29*$AQ28</f>
-        <v>16623</v>
+        <f t="shared" si="15"/>
+        <v>16598</v>
       </c>
       <c r="AM29" s="4">
-        <f>AG29*$AQ28</f>
-        <v>16623</v>
+        <f t="shared" si="16"/>
+        <v>16598</v>
       </c>
       <c r="AN29" s="4">
-        <f>AH29*$AQ28</f>
-        <v>16623</v>
+        <f t="shared" si="24"/>
+        <v>16598</v>
       </c>
       <c r="AP29">
         <v>0.1225</v>
@@ -5252,7 +5252,7 @@
         <v>6833200</v>
       </c>
       <c r="AX29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1708300</v>
       </c>
     </row>
@@ -5267,11 +5267,11 @@
         <v>0.7</v>
       </c>
       <c r="F30" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>34.438863576302921</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62.106962600557289</v>
       </c>
       <c r="H30" s="5">
@@ -5281,19 +5281,19 @@
         <v>50000</v>
       </c>
       <c r="J30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.22959242384201947</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.8632088780167186</v>
       </c>
       <c r="L30" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8860</v>
       </c>
       <c r="M30" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>246800</v>
       </c>
       <c r="N30" s="7">
@@ -5304,19 +5304,19 @@
         <v>0</v>
       </c>
       <c r="P30" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="Q30" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R30" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>579000</v>
       </c>
       <c r="S30" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19680000</v>
       </c>
       <c r="T30" s="5">
@@ -5328,26 +5328,26 @@
       </c>
       <c r="V30" s="14">
         <f t="shared" si="3"/>
-        <v>60763.375</v>
+        <v>60673.95</v>
       </c>
       <c r="W30" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>14186637.520880964</v>
       </c>
       <c r="X30" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>132934.01340452928</v>
       </c>
       <c r="Y30" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>12222650.239789676</v>
       </c>
       <c r="Z30" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0.22959242384201947</v>
       </c>
       <c r="AA30" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0.62106962600557292</v>
       </c>
       <c r="AB30" s="5">
@@ -5372,28 +5372,28 @@
         <v>200</v>
       </c>
       <c r="AI30" s="4">
-        <f>AC30*$AQ29</f>
-        <v>8323.75</v>
+        <f t="shared" si="12"/>
+        <v>8311.5</v>
       </c>
       <c r="AJ30" s="4">
-        <f>AD30*$AQ29</f>
-        <v>8323.75</v>
+        <f t="shared" si="13"/>
+        <v>8311.5</v>
       </c>
       <c r="AK30" s="4">
-        <f>AE30*$AQ29</f>
-        <v>10820.875</v>
+        <f t="shared" si="14"/>
+        <v>10804.949999999999</v>
       </c>
       <c r="AL30" s="4">
-        <f>AF30*$AQ29</f>
-        <v>16647.5</v>
+        <f t="shared" si="15"/>
+        <v>16623</v>
       </c>
       <c r="AM30" s="4">
-        <f>AG30*$AQ29</f>
-        <v>16647.5</v>
+        <f t="shared" si="16"/>
+        <v>16623</v>
       </c>
       <c r="AN30" s="4">
-        <f>AH30*$AQ29</f>
-        <v>16647.5</v>
+        <f t="shared" si="24"/>
+        <v>16623</v>
       </c>
       <c r="AP30">
         <v>0.12239999999999999</v>
@@ -5409,7 +5409,7 @@
         <v>6969860</v>
       </c>
       <c r="AX30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1742465</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor update to workbook
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F24505-A3C9-FA40-9649-D29A953EF31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE5110E-AA8A-0949-A78E-AD3CE8A4FF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="780" windowWidth="33680" windowHeight="19880" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
@@ -5621,7 +5621,7 @@
   <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
intermediat push of carbon ledger workbook
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE5110E-AA8A-0949-A78E-AD3CE8A4FF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BCE304-90C2-984A-9BC2-F6666261E3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="780" windowWidth="33680" windowHeight="19880" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
+    <workbookView xWindow="2280" yWindow="760" windowWidth="33680" windowHeight="19880" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="166">
   <si>
     <t>forest_primary_c_ha</t>
   </si>
@@ -196,9 +196,6 @@
     <t>t = 0</t>
   </si>
   <si>
-    <t>tonne C/ha</t>
-  </si>
-  <si>
     <t>protected area</t>
   </si>
   <si>
@@ -208,39 +205,21 @@
     <t xml:space="preserve">c available from conversion </t>
   </si>
   <si>
-    <t>min frac original stock required (minimum fraction of original stock that must remain on the land to allow it to remain that land use type)</t>
-  </si>
-  <si>
     <t>frac la conversion available for use</t>
   </si>
   <si>
     <t>land use conversion away</t>
   </si>
   <si>
-    <t>average stock per ha available--subtracts out min frac of original value that mus tremain in each type</t>
-  </si>
-  <si>
     <t>Demand</t>
   </si>
   <si>
     <t>calculated variables</t>
   </si>
   <si>
-    <t>demand satisfiable</t>
-  </si>
-  <si>
-    <t>total c available</t>
-  </si>
-  <si>
-    <t>c_available_from_new_forests (based on lag)</t>
-  </si>
-  <si>
     <t>C stock</t>
   </si>
   <si>
-    <t>adjusted sequestration</t>
-  </si>
-  <si>
     <t>Sequestration</t>
   </si>
   <si>
@@ -259,9 +238,6 @@
     <t>current average stock</t>
   </si>
   <si>
-    <t>c available from stock without sequestration</t>
-  </si>
-  <si>
     <t>c available from new sequestration</t>
   </si>
   <si>
@@ -286,15 +262,9 @@
     <t>Aforestation</t>
   </si>
   <si>
-    <t>area_from _t0</t>
-  </si>
-  <si>
     <t>area_from_t1</t>
   </si>
   <si>
-    <t>area_from_T2</t>
-  </si>
-  <si>
     <t>c_stock_t0</t>
   </si>
   <si>
@@ -304,14 +274,275 @@
     <t>c_stock_t2</t>
   </si>
   <si>
-    <t>`</t>
+    <t>Protection</t>
+  </si>
+  <si>
+    <t>Removals</t>
+  </si>
+  <si>
+    <t>original forest</t>
+  </si>
+  <si>
+    <t>average stock per ha available (accounts for min frac)</t>
+  </si>
+  <si>
+    <t>new forest</t>
+  </si>
+  <si>
+    <t>c available from stock beginning of period</t>
+  </si>
+  <si>
+    <t>after X years, new forests enter the full pool, and it's assumed that wood is pulled uniformly (deal with average sequestration factors)</t>
+  </si>
+  <si>
+    <t>t = 3</t>
+  </si>
+  <si>
+    <t>area_from_t2</t>
+  </si>
+  <si>
+    <t>area_from_t3</t>
+  </si>
+  <si>
+    <t>c_stock_t3</t>
+  </si>
+  <si>
+    <t>protection applies in an oldest first set</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>t = 4</t>
+  </si>
+  <si>
+    <t>t = 5</t>
+  </si>
+  <si>
+    <t>T x T</t>
+  </si>
+  <si>
+    <t>NEW FOREST PROTECTION MATRIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Y) area_from _t0</t>
+  </si>
+  <si>
+    <t>zeros</t>
+  </si>
+  <si>
+    <t>adjusted sequestration in original</t>
+  </si>
+  <si>
+    <t>NPP Curve and Young Forest Assumptions</t>
+  </si>
+  <si>
+    <t>sequestration_factor_t0_base</t>
+  </si>
+  <si>
+    <t>sequestration_factor_t1_base</t>
+  </si>
+  <si>
+    <t>sequestration_factor_t2_base</t>
+  </si>
+  <si>
+    <t>sequestration_factor_t3_base</t>
+  </si>
+  <si>
+    <t>unproctected</t>
+  </si>
+  <si>
+    <t>protected</t>
+  </si>
+  <si>
+    <t>orig</t>
+  </si>
+  <si>
+    <t>young</t>
+  </si>
+  <si>
+    <t>avail</t>
+  </si>
+  <si>
+    <t>unavail</t>
+  </si>
+  <si>
+    <t>c stock</t>
+  </si>
+  <si>
+    <t>6 bins</t>
+  </si>
+  <si>
+    <t>descrip</t>
+  </si>
+  <si>
+    <t>from original forests, c stock available</t>
+  </si>
+  <si>
+    <t>from original forests, c stock that is unavailable without affecting land use transition</t>
+  </si>
+  <si>
+    <t>from new forests, c stock available</t>
+  </si>
+  <si>
+    <t>from new forests, c stock unavailable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from original forests, c stock </t>
+  </si>
+  <si>
+    <t xml:space="preserve">from protected forests, c stock </t>
+  </si>
+  <si>
+    <t>last in, last out</t>
+  </si>
+  <si>
+    <t>LILO</t>
+  </si>
+  <si>
+    <t>young_forest_protected</t>
+  </si>
+  <si>
+    <t>c_stock_over_thresh_t0</t>
+  </si>
+  <si>
+    <t>c_stock_over_thresh_t1</t>
+  </si>
+  <si>
+    <t>c_stock_over_thresh_t2</t>
+  </si>
+  <si>
+    <t>c_stock_over_thresh_t3</t>
+  </si>
+  <si>
+    <t>D = P + I - E</t>
+  </si>
+  <si>
+    <t>FRAC_IMPORTS = I/(P + I - E)</t>
+  </si>
+  <si>
+    <t>adjusted sequestration_factor_t0</t>
+  </si>
+  <si>
+    <t>adjusted sequestration_factor_t1</t>
+  </si>
+  <si>
+    <t>adjusted sequestration_factor_t2</t>
+  </si>
+  <si>
+    <t>adjusted sequestration_factor_t3</t>
+  </si>
+  <si>
+    <t>removals_from_nf_planted_at_t0</t>
+  </si>
+  <si>
+    <t>removals_from_nf_planted_at_t1</t>
+  </si>
+  <si>
+    <t>removals_from_nf_planted_at_t2</t>
+  </si>
+  <si>
+    <t>removals_from_nf_planted_at_t3</t>
+  </si>
+  <si>
+    <t>if_untouched_c_stock_t0</t>
+  </si>
+  <si>
+    <t>if_untouched_c_stock_t1</t>
+  </si>
+  <si>
+    <t>if_untouched_c_stock_t2</t>
+  </si>
+  <si>
+    <t>if_untouched_c_stock_t3</t>
+  </si>
+  <si>
+    <t>land use conversion away from new forest</t>
+  </si>
+  <si>
+    <t>forest area (start)</t>
+  </si>
+  <si>
+    <t>c_stock_available_for_harvest_planted_at_t0</t>
+  </si>
+  <si>
+    <t>c_stock_available_for_harvest_planted_at_t1</t>
+  </si>
+  <si>
+    <t>c_stock_available_for_harvest_planted_at_t2</t>
+  </si>
+  <si>
+    <t>c_stock_available_for_harvest_planted_at_t3</t>
+  </si>
+  <si>
+    <t>base tonne C/ha reqd maintained</t>
+  </si>
+  <si>
+    <t>base storage tonne C/ha</t>
+  </si>
+  <si>
+    <t>removals from nf</t>
+  </si>
+  <si>
+    <t>buffer</t>
+  </si>
+  <si>
+    <t>dead storage (minimum fraction of original stock that must remain on the land to allow it to remain that land use type)</t>
+  </si>
+  <si>
+    <t>buffer zone (fraction of stock above dead storage which contributes to slowing removals)</t>
+  </si>
+  <si>
+    <t>some reservoir terms</t>
+  </si>
+  <si>
+    <t>(percentage of forest stock available out of full stock  ) carbon_stock_factor</t>
+  </si>
+  <si>
+    <t>healthy storage available</t>
+  </si>
+  <si>
+    <t>frac_removals_satisficable</t>
+  </si>
+  <si>
+    <t>removals allocation</t>
+  </si>
+  <si>
+    <t>removals from original</t>
+  </si>
+  <si>
+    <t>total starting stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stock in unprotected reservoir dead storage </t>
+  </si>
+  <si>
+    <t>stock to allocate from original pool excluding conversion</t>
+  </si>
+  <si>
+    <t>total starting stock in original</t>
+  </si>
+  <si>
+    <t>total starting stock in new</t>
+  </si>
+  <si>
+    <t>total accessible pool</t>
+  </si>
+  <si>
+    <t>removals  unmet by original</t>
+  </si>
+  <si>
+    <t>drops</t>
+  </si>
+  <si>
+    <t>cumulative_vals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,6 +575,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -391,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -419,24 +656,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -454,9 +673,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -465,6 +681,38 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1011,60 +1259,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="10" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="10" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="12" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="14" t="s">
+      <c r="M1" s="22"/>
+      <c r="N1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="12" t="s">
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="13" t="s">
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="13"/>
+      <c r="V1" s="23"/>
       <c r="W1" s="4" t="s">
         <v>46</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AC1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
       <c r="AI1" s="7" t="s">
         <v>37</v>
       </c>
@@ -1411,7 +1659,7 @@
         <v>1025000</v>
       </c>
       <c r="P4" s="5">
-        <f t="shared" ref="P4:P7" si="1">$O4*R4/($R4+$S4)</f>
+        <f t="shared" ref="P4:P5" si="1">$O4*R4/($R4+$S4)</f>
         <v>36708.669962619075</v>
       </c>
       <c r="Q4" s="5">
@@ -1430,7 +1678,7 @@
         <v>0.3</v>
       </c>
       <c r="U4" s="9">
-        <f t="shared" ref="U3:U30" si="3">(C4*F4 + D4*G4)*E4</f>
+        <f t="shared" ref="U4:U30" si="3">(C4*F4 + D4*G4)*E4</f>
         <v>12046.325970274902</v>
       </c>
       <c r="V4" s="9">
@@ -1561,7 +1809,7 @@
         <v>1062500</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" ref="O4:O30" si="11">INT(Z5&gt;T5)*MIN(N5,W5)</f>
+        <f t="shared" ref="O5:O30" si="11">INT(Z5&gt;T5)*MIN(N5,W5)</f>
         <v>1062500</v>
       </c>
       <c r="P5" s="5">
@@ -1784,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="AI6" s="3">
-        <f t="shared" ref="AI5:AI30" si="25">AC6*$AQ4</f>
+        <f t="shared" ref="AI6:AI30" si="25">AC6*$AQ4</f>
         <v>6.0000000000000009</v>
       </c>
       <c r="AJ6" s="3">
@@ -5601,16 +5849,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="R1:T1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="AC1:AH1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5618,37 +5866,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40F0562-A765-A442-B9DB-CF71D123E451}">
-  <dimension ref="A1:U61"/>
+  <dimension ref="A1:AJ134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.83203125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="56" style="10" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="2.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="5" customWidth="1"/>
     <col min="6" max="7" width="13.33203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="5" customWidth="1"/>
     <col min="9" max="10" width="13.33203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="4.33203125" customWidth="1"/>
-    <col min="19" max="19" width="4.1640625" customWidth="1"/>
-    <col min="21" max="21" width="9.1640625" customWidth="1"/>
-    <col min="22" max="22" width="3.33203125" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" style="5" customWidth="1"/>
+    <col min="15" max="16" width="13.33203125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="23.6640625" style="5" customWidth="1"/>
+    <col min="18" max="19" width="13.33203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="4.33203125" customWidth="1"/>
+    <col min="21" max="23" width="14.6640625" customWidth="1"/>
+    <col min="27" max="27" width="4.1640625" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" customWidth="1"/>
+    <col min="30" max="30" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
-      <c r="B1" s="16"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E1" s="5">
         <v>1</v>
@@ -5659,85 +5914,156 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+    </row>
+    <row r="2" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="16"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="14">
+        <v>64</v>
+      </c>
+      <c r="E2" s="21">
         <v>150</v>
       </c>
-      <c r="F2" s="14"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="5"/>
+      <c r="M2" s="4">
+        <v>249700</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
-      <c r="B3" s="16"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="14">
+        <v>65</v>
+      </c>
+      <c r="E3" s="21">
         <v>30</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="23"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="25"/>
-    </row>
-    <row r="5" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:29" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="26">
+        <v>1</v>
+      </c>
+      <c r="G4" s="26"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="26">
+        <v>2</v>
+      </c>
+      <c r="J4" s="26"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="26">
+        <v>3</v>
+      </c>
+      <c r="M4" s="26"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="26">
+        <v>4</v>
+      </c>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="26">
+        <v>5</v>
+      </c>
+      <c r="S4" s="26"/>
+      <c r="U4" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="AC4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="I5" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="J5" s="15"/>
-      <c r="M5" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="I5" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="L5" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="25"/>
+      <c r="O5" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="P5" s="25"/>
+      <c r="R5" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5" s="25"/>
+      <c r="U5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="N5" t="s">
+      <c r="V5" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="O5" t="s">
+      <c r="W5" s="27" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="AC5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -5758,20 +6084,38 @@
       <c r="J6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <f>SUM(M$6:M6)</f>
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
-        <v>78</v>
+      <c r="L6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="24">
+        <v>0</v>
+      </c>
+      <c r="V6" s="24">
+        <f>SUM(U$6:U6)</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="C7" s="4">
         <v>10000</v>
@@ -5780,957 +6124,2555 @@
         <v>250000</v>
       </c>
       <c r="F7" s="4">
-        <f>C7-C8</f>
+        <f>C7-C9</f>
         <v>9950</v>
       </c>
       <c r="G7" s="4">
-        <f>D7-D8</f>
+        <f>MAX(D7-D9,0)</f>
         <v>249900</v>
       </c>
       <c r="I7" s="4">
-        <f>F7-F8</f>
+        <f>F7-F9</f>
         <v>9888</v>
       </c>
       <c r="J7" s="4">
-        <f>G7-G8</f>
+        <f>MAX(G7-G9,0)</f>
         <v>249790</v>
       </c>
-      <c r="M7">
+      <c r="L7" s="4">
+        <f>I7-I9</f>
+        <v>9830</v>
+      </c>
+      <c r="M7" s="4">
+        <f>MAX(J7-J9,0)</f>
+        <v>249696</v>
+      </c>
+      <c r="O7" s="4">
+        <f>L7-L9</f>
+        <v>9760</v>
+      </c>
+      <c r="P7" s="4">
+        <f>MAX(M7-M9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <f>O7-O9</f>
+        <v>9660</v>
+      </c>
+      <c r="S7" s="4">
+        <f>MAX(P7-P9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="24">
         <v>0.01</v>
       </c>
-      <c r="N7">
-        <f>SUM(M$6:M7)</f>
+      <c r="V7" s="24">
+        <f>SUM(U$6:U7)</f>
         <v>0.01</v>
       </c>
-      <c r="O7">
+      <c r="W7" s="24">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>4000000</v>
+      </c>
+      <c r="AC7">
+        <f>ROUND(AB7/4,0)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C7</f>
+        <v>10000</v>
+      </c>
+      <c r="D8" s="4">
+        <f>D7</f>
+        <v>250000</v>
+      </c>
+      <c r="F8" s="4">
+        <f>F7</f>
+        <v>9950</v>
+      </c>
+      <c r="G8" s="4">
+        <f>D8-D9+D11</f>
+        <v>249985</v>
+      </c>
+      <c r="I8" s="4">
+        <f>I7</f>
+        <v>9888</v>
+      </c>
+      <c r="J8" s="4">
+        <f>G8-G9+G11</f>
+        <v>249955</v>
+      </c>
+      <c r="L8" s="4">
+        <f>L7</f>
+        <v>9830</v>
+      </c>
+      <c r="M8" s="4">
+        <f>J8-J9+J11</f>
+        <v>249953</v>
+      </c>
+      <c r="O8" s="4">
+        <f>O7</f>
+        <v>9760</v>
+      </c>
+      <c r="P8" s="4">
+        <f>M8-M9+M11</f>
+        <v>296</v>
+      </c>
+      <c r="R8" s="4">
+        <f>R7</f>
+        <v>9660</v>
+      </c>
+      <c r="S8" s="4">
+        <f>P8-P9+P11</f>
+        <v>349</v>
+      </c>
+      <c r="U8" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="V8" s="24">
+        <f>SUM(U$6:U8)</f>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="W8" s="24">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="5"/>
+    </row>
+    <row r="9" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="4">
+        <v>50</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100</v>
+      </c>
+      <c r="F9" s="4">
+        <v>62</v>
+      </c>
+      <c r="G9" s="4">
+        <v>110</v>
+      </c>
+      <c r="I9" s="4">
+        <v>58</v>
+      </c>
+      <c r="J9" s="4">
+        <v>94</v>
+      </c>
+      <c r="L9" s="4">
+        <v>70</v>
+      </c>
+      <c r="M9" s="4">
+        <v>249700</v>
+      </c>
+      <c r="O9" s="4">
+        <v>100</v>
+      </c>
+      <c r="P9" s="4">
+        <v>39</v>
+      </c>
+      <c r="R9" s="4">
+        <v>98</v>
+      </c>
+      <c r="S9" s="4">
+        <v>105</v>
+      </c>
+      <c r="U9" s="24">
+        <v>0.12</v>
+      </c>
+      <c r="V9" s="24">
+        <f>SUM(U$6:U9)</f>
+        <v>0.18</v>
+      </c>
+      <c r="W9" s="24">
+        <v>2</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>4100000</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" ref="AC9:AC133" si="0">ROUND(AB9/4,0)</f>
+        <v>1025000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="4">
+        <f>-MIN(D7-D9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <f>-MIN(G7-G9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <f>-MIN(J7-J9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <f>-MIN(M7-M9,0)</f>
+        <v>4</v>
+      </c>
+      <c r="P10" s="4">
+        <f>-MIN(P7-P9,0)</f>
+        <v>39</v>
+      </c>
+      <c r="S10" s="4">
+        <f>-MIN(S7-S9,0)</f>
+        <v>105</v>
+      </c>
+      <c r="U10" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="V10" s="24">
+        <f>SUM(U$6:U10)</f>
+        <v>0.38</v>
+      </c>
+      <c r="W10" s="24">
         <v>20</v>
       </c>
-      <c r="T7" s="5">
-        <v>4000000</v>
-      </c>
-      <c r="U7">
-        <f>ROUND(T7/4,0)</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="4">
-        <v>50</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="F8" s="4">
-        <v>62</v>
-      </c>
-      <c r="G8" s="4">
-        <v>110</v>
-      </c>
-      <c r="I8" s="4">
-        <v>58</v>
-      </c>
-      <c r="J8" s="4">
-        <v>94</v>
-      </c>
-      <c r="M8">
-        <v>0.05</v>
-      </c>
-      <c r="N8">
-        <f>SUM(M$6:M8)</f>
-        <v>6.0000000000000005E-2</v>
-      </c>
-      <c r="O8">
+      <c r="AB10" s="5"/>
+    </row>
+    <row r="11" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="4">
+        <v>85</v>
+      </c>
+      <c r="G11" s="4">
+        <v>80</v>
+      </c>
+      <c r="J11" s="4">
+        <v>92</v>
+      </c>
+      <c r="M11" s="4">
+        <v>43</v>
+      </c>
+      <c r="P11" s="4">
+        <v>92</v>
+      </c>
+      <c r="S11" s="4">
+        <v>43</v>
+      </c>
+      <c r="U11" s="24">
+        <v>0.36</v>
+      </c>
+      <c r="V11" s="24">
+        <f>SUM(U$6:U11)</f>
+        <v>0.74</v>
+      </c>
+      <c r="W11" s="24">
         <v>20</v>
       </c>
-      <c r="T8" s="5">
-        <v>4100000</v>
-      </c>
-      <c r="U8">
-        <f t="shared" ref="U8:U60" si="0">ROUND(T8/4,0)</f>
-        <v>1025000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B9" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="4">
-        <v>85</v>
-      </c>
-      <c r="G9" s="4">
-        <v>80</v>
-      </c>
-      <c r="J9" s="4">
-        <v>92</v>
-      </c>
-      <c r="T9" s="5"/>
-    </row>
-    <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="AB11" s="5"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="U12" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="V12" s="24">
+        <f>SUM(U$6:U12)</f>
+        <v>1.3399999999999999</v>
+      </c>
+      <c r="W12" s="24">
+        <v>20</v>
+      </c>
+      <c r="AB12" s="5"/>
+    </row>
+    <row r="13" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="4">
         <v>0.7</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F13" s="4">
         <v>0.7</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I13" s="4">
         <v>0.7</v>
       </c>
-      <c r="M10">
-        <v>0.2</v>
-      </c>
-      <c r="N10">
-        <f>SUM(M$6:M10)</f>
-        <v>0.26</v>
-      </c>
-      <c r="O10">
+      <c r="L13" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="R13" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="U13" s="24">
+        <v>1.8</v>
+      </c>
+      <c r="V13" s="24">
+        <f>SUM(U$6:U13)</f>
+        <v>3.1399999999999997</v>
+      </c>
+      <c r="W13" s="24">
         <v>20</v>
       </c>
-      <c r="T10" s="5">
+      <c r="AB13" s="5">
         <v>4250000</v>
       </c>
-      <c r="U10">
+      <c r="AC13">
         <f t="shared" si="0"/>
         <v>1062500</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="B11" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="4">
+    <row r="14" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="4">
         <v>0.3</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F14" s="4">
         <v>0.3</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I14" s="4">
         <v>0.3</v>
       </c>
-      <c r="T11" s="5"/>
-    </row>
-    <row r="12" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B12" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="L14" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="R14" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="U14" s="24">
+        <v>3</v>
+      </c>
+      <c r="V14" s="24">
+        <f>SUM(U$6:U14)</f>
+        <v>6.14</v>
+      </c>
+      <c r="W14" s="24">
+        <v>20</v>
+      </c>
+      <c r="AB14" s="5"/>
+    </row>
+    <row r="15" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
+      <c r="B15" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="D12" s="4">
+      <c r="C15" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="U15" s="24">
+        <v>6</v>
+      </c>
+      <c r="V15" s="24">
+        <f>SUM(U$6:U15)</f>
+        <v>12.14</v>
+      </c>
+      <c r="W15" s="24">
+        <v>20</v>
+      </c>
+      <c r="AB15" s="5"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" s="30"/>
+      <c r="U16" s="24">
+        <v>10</v>
+      </c>
+      <c r="V16" s="24">
+        <f>SUM(U$6:U16)</f>
+        <v>22.14</v>
+      </c>
+      <c r="W16" s="24">
+        <v>20</v>
+      </c>
+      <c r="AB16" s="5"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A17" s="30"/>
+      <c r="U17" s="24">
+        <v>12</v>
+      </c>
+      <c r="V17" s="24">
+        <f>SUM(U$6:U17)</f>
+        <v>34.14</v>
+      </c>
+      <c r="W17" s="24">
+        <v>20</v>
+      </c>
+      <c r="AB17" s="5"/>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A18" s="30"/>
+      <c r="U18" s="24">
+        <v>13.5</v>
+      </c>
+      <c r="V18" s="24">
+        <f>SUM(U$6:U18)</f>
+        <v>47.64</v>
+      </c>
+      <c r="W18" s="24">
+        <v>20</v>
+      </c>
+      <c r="AB18" s="5"/>
+    </row>
+    <row r="19" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="4">
+        <v>150</v>
+      </c>
+      <c r="D19" s="4">
         <v>100</v>
       </c>
-      <c r="M12">
-        <v>0.6</v>
-      </c>
-      <c r="N12">
-        <f>SUM(M$6:M12)</f>
-        <v>0.86</v>
-      </c>
-      <c r="O12">
+      <c r="U19" s="24">
+        <v>12</v>
+      </c>
+      <c r="V19" s="24">
+        <f>SUM(U$6:U19)</f>
+        <v>59.64</v>
+      </c>
+      <c r="W19" s="24">
         <v>20</v>
       </c>
-      <c r="T12" s="5">
+      <c r="AB19" s="5">
         <v>4400000</v>
       </c>
-      <c r="U12">
+      <c r="AC19">
         <f t="shared" si="0"/>
         <v>1100000</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="4">
+    <row r="20" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="4">
+        <f>C$19*$C$14</f>
+        <v>45</v>
+      </c>
+      <c r="D20" s="4">
+        <f>D$19*$C$14</f>
+        <v>30</v>
+      </c>
+      <c r="U20" s="24">
+        <v>10</v>
+      </c>
+      <c r="V20" s="24">
+        <f>SUM(U$6:U20)</f>
+        <v>69.64</v>
+      </c>
+      <c r="W20" s="24">
+        <v>20</v>
+      </c>
+      <c r="AB20" s="5"/>
+    </row>
+    <row r="21" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="B21" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="4">
+        <f>C19-C20</f>
+        <v>105</v>
+      </c>
+      <c r="D21" s="4">
+        <f>D19-D20</f>
+        <v>70</v>
+      </c>
+      <c r="U21" s="24">
+        <v>6</v>
+      </c>
+      <c r="V21" s="24">
+        <f>SUM(U$6:U21)</f>
+        <v>75.64</v>
+      </c>
+      <c r="W21" s="24">
+        <v>20</v>
+      </c>
+      <c r="AB21" s="5"/>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="U22" s="24">
+        <v>3</v>
+      </c>
+      <c r="V22" s="24">
+        <f>SUM(U$6:U22)</f>
+        <v>78.64</v>
+      </c>
+      <c r="W22" s="24">
+        <v>20</v>
+      </c>
+      <c r="AB22" s="5"/>
+    </row>
+    <row r="23" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="4">
         <v>5000</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D23" s="4">
         <v>50000</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F23" s="4">
         <v>5000</v>
       </c>
-      <c r="G13" s="4">
-        <v>50000</v>
-      </c>
-      <c r="I13" s="4">
+      <c r="G23" s="4">
+        <v>250000</v>
+      </c>
+      <c r="I23" s="4">
         <v>6000</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J23" s="4">
+        <v>250000</v>
+      </c>
+      <c r="L23" s="4">
+        <v>6000</v>
+      </c>
+      <c r="M23" s="4">
+        <v>249800</v>
+      </c>
+      <c r="O23" s="4">
+        <v>6500</v>
+      </c>
+      <c r="P23" s="4">
         <v>49000</v>
       </c>
-      <c r="M13">
+      <c r="R23" s="4">
+        <v>7200</v>
+      </c>
+      <c r="S23" s="4">
+        <v>49500</v>
+      </c>
+      <c r="U23" s="24">
         <v>1.8</v>
       </c>
-      <c r="N13">
-        <f>SUM(M$6:M13)</f>
-        <v>2.66</v>
-      </c>
-      <c r="O13">
+      <c r="V23" s="24">
+        <f>SUM(U$6:U23)</f>
+        <v>80.44</v>
+      </c>
+      <c r="W23" s="24">
         <v>20</v>
       </c>
-      <c r="T13" s="5">
+      <c r="AB23" s="5">
         <v>4420000</v>
       </c>
-      <c r="U13">
+      <c r="AC23">
         <f t="shared" si="0"/>
         <v>1105000</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="T14" s="5"/>
-    </row>
-    <row r="15" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
-        <v>3</v>
-      </c>
-      <c r="T15" s="5"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T16" s="5"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M17">
-        <v>3</v>
-      </c>
-      <c r="N17">
-        <f>SUM(M$6:M17)</f>
-        <v>5.66</v>
-      </c>
-      <c r="O17">
-        <v>20</v>
-      </c>
-      <c r="T17" s="5">
+      <c r="AG23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="AB24" s="5"/>
+      <c r="AI24" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="B25" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.92</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="AB25" s="5"/>
+      <c r="AG25" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AB26" s="5"/>
+      <c r="AG26" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI26" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AB27" s="5">
         <v>4508400</v>
       </c>
-      <c r="U17">
+      <c r="AC27">
         <f t="shared" si="0"/>
         <v>1127100</v>
       </c>
-    </row>
-    <row r="18" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="M18">
-        <v>6</v>
-      </c>
-      <c r="N18">
-        <f>SUM(M$6:M18)</f>
-        <v>11.66</v>
-      </c>
-      <c r="O18">
-        <v>20</v>
-      </c>
-      <c r="T18" s="5">
+      <c r="AG27" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="AB28" s="5">
         <v>4598570</v>
       </c>
-      <c r="U18">
+      <c r="AC28">
         <f t="shared" si="0"/>
         <v>1149643</v>
       </c>
-    </row>
-    <row r="19" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="M19">
-        <v>10</v>
-      </c>
-      <c r="N19">
-        <f>SUM(M$6:M19)</f>
-        <v>21.66</v>
-      </c>
-      <c r="O19">
-        <v>20</v>
-      </c>
-      <c r="T19" s="5">
+      <c r="AG28" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="4">
+        <v>200000</v>
+      </c>
+      <c r="F29" s="4">
+        <v>205000</v>
+      </c>
+      <c r="I29" s="4">
+        <v>211000</v>
+      </c>
+      <c r="L29" s="4">
+        <v>221000</v>
+      </c>
+      <c r="O29" s="4">
+        <v>211000</v>
+      </c>
+      <c r="R29" s="4">
+        <v>221000</v>
+      </c>
+      <c r="AB29" s="5">
         <v>4690540</v>
       </c>
-      <c r="U19">
+      <c r="AC29">
         <f t="shared" si="0"/>
         <v>1172635</v>
       </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M20">
-        <v>12</v>
-      </c>
-      <c r="N20">
-        <f>SUM(M$6:M20)</f>
-        <v>33.659999999999997</v>
-      </c>
-      <c r="O20">
-        <v>20</v>
-      </c>
-      <c r="T20" s="5">
+      <c r="AG29" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB30" s="5">
         <v>4784350</v>
       </c>
-      <c r="U20">
+      <c r="AC30">
         <f t="shared" si="0"/>
         <v>1196088</v>
       </c>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M21">
-        <v>13.5</v>
-      </c>
-      <c r="N21">
-        <f>SUM(M$6:M21)</f>
-        <v>47.16</v>
-      </c>
-      <c r="O21">
-        <v>20</v>
-      </c>
-      <c r="T21" s="5">
+      <c r="AG30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AB31" s="5">
         <v>4880040</v>
       </c>
-      <c r="U21">
+      <c r="AC31">
         <f t="shared" si="0"/>
         <v>1220010</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M22">
-        <v>12</v>
-      </c>
-      <c r="N22">
-        <f>SUM(M$6:M22)</f>
-        <v>59.16</v>
-      </c>
-      <c r="O22">
-        <v>20</v>
-      </c>
-      <c r="T22" s="5">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AB32" s="5">
         <v>4977640</v>
       </c>
-      <c r="U22">
+      <c r="AC32">
         <f t="shared" si="0"/>
         <v>1244410</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M23">
-        <v>10</v>
-      </c>
-      <c r="N23">
-        <f>SUM(M$6:M23)</f>
-        <v>69.16</v>
-      </c>
-      <c r="O23">
-        <v>20</v>
-      </c>
-      <c r="T23" s="5">
+    <row r="33" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AB33" s="5">
         <v>5077190</v>
       </c>
-      <c r="U23">
+      <c r="AC33">
         <f t="shared" si="0"/>
         <v>1269298</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M24">
-        <v>6</v>
-      </c>
-      <c r="N24">
-        <f>SUM(M$6:M24)</f>
-        <v>75.16</v>
-      </c>
-      <c r="O24">
-        <v>20</v>
-      </c>
-      <c r="T24" s="5">
+    <row r="34" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AB34" s="5">
         <v>5178730</v>
       </c>
-      <c r="U24">
+      <c r="AC34">
         <f t="shared" si="0"/>
         <v>1294683</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M25">
-        <v>3</v>
-      </c>
-      <c r="N25">
-        <f>SUM(M$6:M25)</f>
-        <v>78.16</v>
-      </c>
-      <c r="O25">
-        <v>20</v>
-      </c>
-      <c r="T25" s="5">
+    <row r="35" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AB35" s="5">
         <v>5282300</v>
       </c>
-      <c r="U25">
+      <c r="AC35">
         <f t="shared" si="0"/>
         <v>1320575</v>
       </c>
     </row>
-    <row r="26" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="M26">
-        <v>1.8</v>
-      </c>
-      <c r="N26">
-        <f>SUM(M$6:M26)</f>
-        <v>79.959999999999994</v>
-      </c>
-      <c r="O26">
-        <v>20</v>
-      </c>
-      <c r="T26" s="5">
+    <row r="36" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B36" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="AB36" s="5">
         <v>5387950</v>
       </c>
-      <c r="U26">
+      <c r="AC36">
         <f t="shared" si="0"/>
         <v>1346988</v>
       </c>
     </row>
-    <row r="27" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="4">
-        <f>C15</f>
+    <row r="37" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B37" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="4">
+        <f>C25</f>
+        <v>0.92</v>
+      </c>
+      <c r="D37" s="4">
+        <f>D25</f>
+        <v>0.3</v>
+      </c>
+      <c r="AB37" s="5"/>
+    </row>
+    <row r="38" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B38" s="14"/>
+      <c r="AB38" s="5"/>
+    </row>
+    <row r="39" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AB39" s="5"/>
+    </row>
+    <row r="40" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B40" s="14"/>
+      <c r="AB40" s="5"/>
+    </row>
+    <row r="41" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AB41" s="5"/>
+    </row>
+    <row r="42" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B42" s="14"/>
+      <c r="AB42" s="5"/>
+    </row>
+    <row r="43" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B43" s="14"/>
+      <c r="U43" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB43" s="5"/>
+    </row>
+    <row r="44" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B44" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="F44" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB44" s="5"/>
+    </row>
+    <row r="45" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B45" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5">
+        <f>SUM(G$45:G45)</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0</v>
+      </c>
+      <c r="H45" s="5">
+        <f>SUM(J$45:J45)</f>
+        <v>0</v>
+      </c>
+      <c r="J45" s="4">
+        <v>0</v>
+      </c>
+      <c r="K45" s="5">
+        <f>SUM(M$45:M45)</f>
+        <v>0</v>
+      </c>
+      <c r="M45" s="4">
+        <v>0</v>
+      </c>
+      <c r="N45" s="5">
+        <f>SUM(P$45:P45)</f>
+        <v>0</v>
+      </c>
+      <c r="P45" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="5">
+        <f>SUM(S$45:S45)</f>
+        <v>0</v>
+      </c>
+      <c r="S45" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="5"/>
+    </row>
+    <row r="46" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B46" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="4">
+        <f>D11</f>
+        <v>85</v>
+      </c>
+      <c r="E46" s="5">
+        <f>SUM(D$45:D46)</f>
+        <v>85</v>
+      </c>
+      <c r="F46" s="4">
+        <f>IF(E46&gt;=G$10, IF(E45&lt;G$10, G$10-E45, 0),D46)</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="4">
+        <f>D46-F46</f>
+        <v>85</v>
+      </c>
+      <c r="H46" s="5">
+        <f>SUM(G$45:G46)</f>
+        <v>85</v>
+      </c>
+      <c r="I46" s="4">
+        <f>IF(H46&gt;=J$10, IF(H45&lt;J$10, J$10-H45, 0),G46)</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="4">
+        <f>D11</f>
+        <v>85</v>
+      </c>
+      <c r="K46" s="5">
+        <f>SUM(J$45:J46)</f>
+        <v>85</v>
+      </c>
+      <c r="L46" s="4">
+        <f>IF(K46&gt;=M$10, IF(K45&lt;M$10, M$10-K45, 0),J46)</f>
+        <v>4</v>
+      </c>
+      <c r="M46" s="4">
+        <f>J46-L46</f>
+        <v>81</v>
+      </c>
+      <c r="N46" s="5">
+        <f>SUM(M$45:M46)</f>
+        <v>81</v>
+      </c>
+      <c r="O46" s="4">
+        <f>IF(N46&gt;=P$10, IF(N45&lt;P$10, P$10-N45, 0),M46)</f>
+        <v>39</v>
+      </c>
+      <c r="P46" s="4">
+        <f>M46-O46</f>
+        <v>42</v>
+      </c>
+      <c r="Q46" s="5">
+        <f>SUM(P$45:P46)</f>
+        <v>42</v>
+      </c>
+      <c r="R46" s="4">
+        <f>IF(Q46&gt;=S$10, IF(Q45&lt;S$10, S$10-Q45, 0),P46)</f>
+        <v>42</v>
+      </c>
+      <c r="S46" s="4">
+        <f>P46-R46</f>
+        <v>0</v>
+      </c>
+      <c r="AB46" s="5"/>
+    </row>
+    <row r="47" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B47" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="5">
+        <f>SUM(D$45:D47)</f>
+        <v>85</v>
+      </c>
+      <c r="F47" s="4">
+        <f t="shared" ref="F47:F49" si="1">IF(E47&gt;=G$10, IF(E46&lt;G$10, G$10-E46, 0),D47)</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="4">
+        <f>G11</f>
+        <v>80</v>
+      </c>
+      <c r="H47" s="5">
+        <f>SUM(G$45:G47)</f>
+        <v>165</v>
+      </c>
+      <c r="I47" s="4">
+        <f t="shared" ref="I47:I49" si="2">IF(H47&gt;=J$10, IF(H46&lt;J$10, J$10-H46, 0),G47)</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="4">
+        <f>G47-I47</f>
+        <v>80</v>
+      </c>
+      <c r="K47" s="5">
+        <f>SUM(J$45:J47)</f>
+        <v>165</v>
+      </c>
+      <c r="L47" s="4">
+        <f t="shared" ref="L47:L49" si="3">IF(K47&gt;=M$10, IF(K46&lt;M$10, M$10-K46, 0),J47)</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="4">
+        <f>J47-L47</f>
+        <v>80</v>
+      </c>
+      <c r="N47" s="5">
+        <f>SUM(M$45:M47)</f>
+        <v>161</v>
+      </c>
+      <c r="O47" s="4">
+        <f t="shared" ref="O47:O49" si="4">IF(N47&gt;=P$10, IF(N46&lt;P$10, P$10-N46, 0),M47)</f>
+        <v>0</v>
+      </c>
+      <c r="P47" s="4">
+        <f>M47-O47</f>
+        <v>80</v>
+      </c>
+      <c r="Q47" s="5">
+        <f>SUM(P$45:P47)</f>
+        <v>122</v>
+      </c>
+      <c r="R47" s="4">
+        <f t="shared" ref="R47:R49" si="5">IF(Q47&gt;=S$10, IF(Q46&lt;S$10, S$10-Q46, 0),P47)</f>
+        <v>63</v>
+      </c>
+      <c r="S47" s="4">
+        <f>P47-R47</f>
+        <v>17</v>
+      </c>
+      <c r="AB47" s="5"/>
+    </row>
+    <row r="48" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B48" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="5">
+        <f>SUM(D$45:D48)</f>
+        <v>85</v>
+      </c>
+      <c r="F48" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0</v>
+      </c>
+      <c r="H48" s="5">
+        <f>SUM(G$45:G48)</f>
+        <v>165</v>
+      </c>
+      <c r="I48" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="4">
+        <f>J11</f>
+        <v>92</v>
+      </c>
+      <c r="K48" s="5">
+        <f>SUM(J$45:J48)</f>
+        <v>257</v>
+      </c>
+      <c r="L48" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="4">
+        <f>J48-L48</f>
+        <v>92</v>
+      </c>
+      <c r="N48" s="5">
+        <f>SUM(M$45:M48)</f>
+        <v>253</v>
+      </c>
+      <c r="O48" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P48" s="4">
+        <f>M48-O48</f>
+        <v>92</v>
+      </c>
+      <c r="Q48" s="5">
+        <f>SUM(P$45:P48)</f>
+        <v>214</v>
+      </c>
+      <c r="R48" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S48" s="4">
+        <f>P48-R48</f>
+        <v>92</v>
+      </c>
+      <c r="AB48" s="5"/>
+    </row>
+    <row r="49" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B49" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="5">
+        <f>SUM(D$45:D49)</f>
+        <v>85</v>
+      </c>
+      <c r="F49" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0</v>
+      </c>
+      <c r="H49" s="5">
+        <f>SUM(G$45:G49)</f>
+        <v>165</v>
+      </c>
+      <c r="I49" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="4">
+        <v>0</v>
+      </c>
+      <c r="K49" s="5">
+        <f>SUM(J$45:J49)</f>
+        <v>257</v>
+      </c>
+      <c r="L49" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="4">
+        <f>M11</f>
+        <v>43</v>
+      </c>
+      <c r="N49" s="5">
+        <f>SUM(M$45:M49)</f>
+        <v>296</v>
+      </c>
+      <c r="O49" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P49" s="4">
+        <f>M49-O49</f>
+        <v>43</v>
+      </c>
+      <c r="Q49" s="5">
+        <f>SUM(P$45:P49)</f>
+        <v>257</v>
+      </c>
+      <c r="R49" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S49" s="4">
+        <f>P49-R49</f>
+        <v>43</v>
+      </c>
+      <c r="AB49" s="5"/>
+    </row>
+    <row r="50" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B50" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB50" s="5"/>
+    </row>
+    <row r="51" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B51" s="14"/>
+      <c r="AB51" s="5"/>
+    </row>
+    <row r="52" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B52" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="4">
+        <f>D46*V6</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="4">
+        <f>G46*V7</f>
+        <v>0.85</v>
+      </c>
+      <c r="J52" s="4">
+        <f>J46*V8</f>
+        <v>5.1000000000000005</v>
+      </c>
+      <c r="M52" s="4">
+        <f>M46*V9</f>
+        <v>14.58</v>
+      </c>
+      <c r="P52" s="4">
+        <f>P46*V10</f>
+        <v>15.96</v>
+      </c>
+      <c r="S52" s="4">
+        <f>S46*V11</f>
+        <v>0</v>
+      </c>
+      <c r="AB52" s="5"/>
+    </row>
+    <row r="53" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B53" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="G53" s="4">
+        <f>G47*V6</f>
+        <v>0</v>
+      </c>
+      <c r="J53" s="4">
+        <f>J47*V7</f>
+        <v>0.8</v>
+      </c>
+      <c r="M53" s="4">
+        <f>M47*V8</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="P53" s="4">
+        <f>P47*V9</f>
+        <v>14.399999999999999</v>
+      </c>
+      <c r="S53" s="4">
+        <f>S47*V10</f>
+        <v>6.46</v>
+      </c>
+      <c r="AB53" s="5"/>
+    </row>
+    <row r="54" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B54" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J54" s="4">
+        <f>J48*V6</f>
+        <v>0</v>
+      </c>
+      <c r="M54" s="4">
+        <f>M48*V7</f>
+        <v>0.92</v>
+      </c>
+      <c r="P54" s="4">
+        <f>P48*V8</f>
+        <v>5.5200000000000005</v>
+      </c>
+      <c r="S54" s="4">
+        <f>S48*V9</f>
+        <v>16.559999999999999</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB54" s="5"/>
+    </row>
+    <row r="55" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B55" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="M55" s="4">
+        <f>M49*V6</f>
+        <v>0</v>
+      </c>
+      <c r="P55" s="4">
+        <f>P49*V7</f>
+        <v>0.43</v>
+      </c>
+      <c r="S55" s="4">
+        <f>S49*V8</f>
+        <v>2.58</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB55" s="5"/>
+    </row>
+    <row r="56" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B56" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="W56" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB56" s="5"/>
+    </row>
+    <row r="57" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B57" s="14"/>
+      <c r="W57" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB57" s="5"/>
+    </row>
+    <row r="58" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B58" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB58" s="5"/>
+    </row>
+    <row r="59" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B59" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB59" s="5"/>
+    </row>
+    <row r="60" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B60" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB60" s="5"/>
+    </row>
+    <row r="61" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B61" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB61" s="5"/>
+    </row>
+    <row r="62" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B62" s="14"/>
+      <c r="AB62" s="5"/>
+    </row>
+    <row r="63" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B63" s="14"/>
+      <c r="AB63" s="5"/>
+    </row>
+    <row r="64" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B64" s="14"/>
+      <c r="AB64" s="5"/>
+    </row>
+    <row r="65" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B65" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="AB65" s="5"/>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B66" s="14"/>
+      <c r="AB66" s="5"/>
+    </row>
+    <row r="67" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B67" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D67" s="4">
+        <f>MAX(D$23-(D$7-D$9), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G67" s="4">
+        <f>MAX(G$23-(G$7-G$9), 0)</f>
+        <v>210</v>
+      </c>
+      <c r="J67" s="4">
+        <f>MAX(J$23-(J$7-J$9), 0)</f>
+        <v>304</v>
+      </c>
+      <c r="M67" s="4">
+        <f>MAX(M$23-(M$7-M$9), 0)</f>
+        <v>249804</v>
+      </c>
+      <c r="P67" s="4">
+        <f>MAX(P$23-(P$7-P$9), 0)</f>
+        <v>49039</v>
+      </c>
+      <c r="S67" s="4">
+        <f>MAX(S$23-(S$7-S$9), 0)</f>
+        <v>49605</v>
+      </c>
+      <c r="AB67" s="5"/>
+    </row>
+    <row r="68" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B68" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0</v>
+      </c>
+      <c r="G68" s="4">
+        <v>0</v>
+      </c>
+      <c r="J68" s="4">
+        <v>0</v>
+      </c>
+      <c r="M68" s="4">
+        <v>0</v>
+      </c>
+      <c r="P68" s="4">
+        <v>0</v>
+      </c>
+      <c r="S68" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB68" s="5"/>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B69" s="14"/>
+      <c r="AB69" s="5"/>
+    </row>
+    <row r="70" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B70" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D70" s="4">
+        <f>U6</f>
+        <v>0</v>
+      </c>
+      <c r="G70" s="4">
+        <f>U7</f>
+        <v>0.01</v>
+      </c>
+      <c r="J70" s="4">
+        <f>U8</f>
+        <v>0.05</v>
+      </c>
+      <c r="M70" s="4">
+        <f>U9</f>
+        <v>0.12</v>
+      </c>
+      <c r="P70" s="4">
+        <f>U10</f>
+        <v>0.2</v>
+      </c>
+      <c r="S70" s="4">
+        <f>U11</f>
+        <v>0.36</v>
+      </c>
+      <c r="AB70" s="5"/>
+    </row>
+    <row r="71" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B71" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D71" s="4">
+        <v>0</v>
+      </c>
+      <c r="G71" s="4">
+        <v>0</v>
+      </c>
+      <c r="J71" s="4">
+        <f>U7</f>
+        <v>0.01</v>
+      </c>
+      <c r="M71" s="4">
+        <f>U8</f>
+        <v>0.05</v>
+      </c>
+      <c r="P71" s="4">
+        <f>U9</f>
+        <v>0.12</v>
+      </c>
+      <c r="S71" s="4">
+        <f>U10</f>
+        <v>0.2</v>
+      </c>
+      <c r="AB71" s="5"/>
+    </row>
+    <row r="72" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B72" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D72" s="4">
+        <v>0</v>
+      </c>
+      <c r="G72" s="4">
+        <v>0</v>
+      </c>
+      <c r="J72" s="4">
+        <v>0</v>
+      </c>
+      <c r="M72" s="4">
+        <f>U7</f>
+        <v>0.01</v>
+      </c>
+      <c r="P72" s="4">
+        <f>U8</f>
+        <v>0.05</v>
+      </c>
+      <c r="S72" s="4">
+        <f>U9</f>
+        <v>0.12</v>
+      </c>
+      <c r="AB72" s="5"/>
+    </row>
+    <row r="73" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B73" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D73" s="4">
+        <v>0</v>
+      </c>
+      <c r="G73" s="4">
+        <v>0</v>
+      </c>
+      <c r="J73" s="4">
+        <v>0</v>
+      </c>
+      <c r="M73" s="4">
+        <v>0</v>
+      </c>
+      <c r="P73" s="4">
+        <f>U7</f>
+        <v>0.01</v>
+      </c>
+      <c r="S73" s="4">
+        <f>U8</f>
+        <v>0.05</v>
+      </c>
+      <c r="AB73" s="5"/>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B74" s="14"/>
+      <c r="AB74" s="5"/>
+    </row>
+    <row r="75" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>0</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D75" s="4">
+        <f>D70</f>
+        <v>0</v>
+      </c>
+      <c r="G75" s="4">
+        <f>INT(F$4-$W$6 &gt; $A75)*G52</f>
+        <v>0</v>
+      </c>
+      <c r="J75" s="4">
+        <f>INT(I$4-$W$6 &gt; $A75)*J52</f>
+        <v>0</v>
+      </c>
+      <c r="M75" s="4">
+        <f>INT(L$4-$W$6 &gt; $A75)*M52</f>
+        <v>14.58</v>
+      </c>
+      <c r="P75" s="4">
+        <f>INT(O$4-$W$6 &gt; $A75)*P52</f>
+        <v>15.96</v>
+      </c>
+      <c r="S75" s="4">
+        <f>INT(R$4-$W$6 &gt; $A75)*S52</f>
+        <v>0</v>
+      </c>
+      <c r="AB75" s="5"/>
+    </row>
+    <row r="76" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
         <v>1</v>
       </c>
-      <c r="D27" s="4">
-        <f>D15</f>
+      <c r="B76" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D76" s="4">
+        <f t="shared" ref="D76:D78" si="6">D71</f>
+        <v>0</v>
+      </c>
+      <c r="G76" s="4">
+        <f>INT(F$4-$W$6 &gt; $A76)*G53</f>
+        <v>0</v>
+      </c>
+      <c r="J76" s="4">
+        <f>INT(I$4-$W$6 &gt; $A76)*J53</f>
+        <v>0</v>
+      </c>
+      <c r="M76" s="4">
+        <f>INT(L$4-$W$6 &gt; $A76)*M53</f>
+        <v>0</v>
+      </c>
+      <c r="P76" s="4">
+        <f>INT(O$4-$W$6 &gt; $A76)*P53</f>
+        <v>14.399999999999999</v>
+      </c>
+      <c r="S76" s="4">
+        <f>INT(R$4-$W$6 &gt; $A76)*S53</f>
+        <v>6.46</v>
+      </c>
+      <c r="AB76" s="5"/>
+    </row>
+    <row r="77" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="3">
+        <v>2</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D77" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G77" s="4">
+        <f>INT(F$4-$W$6 &gt; $A77)*G54</f>
+        <v>0</v>
+      </c>
+      <c r="J77" s="4">
+        <f>INT(I$4-$W$6 &gt; $A77)*J54</f>
+        <v>0</v>
+      </c>
+      <c r="M77" s="4">
+        <f>INT(L$4-$W$6 &gt; $A77)*M54</f>
+        <v>0</v>
+      </c>
+      <c r="P77" s="4">
+        <f>INT(O$4-$W$6 &gt; $A77)*P54</f>
+        <v>0</v>
+      </c>
+      <c r="S77" s="4">
+        <f>INT(R$4-$W$6 &gt; $A77)*S54</f>
+        <v>16.559999999999999</v>
+      </c>
+      <c r="AB77" s="5"/>
+    </row>
+    <row r="78" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="3">
         <v>3</v>
       </c>
-      <c r="T27" s="5"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B28" s="20"/>
-      <c r="T28" s="5"/>
-    </row>
-    <row r="29" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="T29" s="5"/>
-    </row>
-    <row r="30" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B30" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="4">
-        <f>D9</f>
-        <v>85</v>
-      </c>
-      <c r="G30" s="4">
-        <f>D9</f>
-        <v>85</v>
-      </c>
-      <c r="J30" s="4">
-        <f>D9</f>
-        <v>85</v>
-      </c>
-      <c r="T30" s="5"/>
-    </row>
-    <row r="31" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B31" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0</v>
-      </c>
-      <c r="G31" s="4">
-        <f>G9</f>
-        <v>80</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="J31" s="4">
-        <f>G9</f>
-        <v>80</v>
-      </c>
-      <c r="T31" s="5"/>
-    </row>
-    <row r="32" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B32" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0</v>
-      </c>
-      <c r="G32" s="4">
-        <v>0</v>
-      </c>
-      <c r="J32" s="4">
-        <f>J9</f>
-        <v>92</v>
-      </c>
-      <c r="T32" s="5"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B33" s="20"/>
-      <c r="T33" s="5"/>
-    </row>
-    <row r="34" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B34" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" s="4">
-        <f>D30*N6</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="4">
-        <f>G30*N7</f>
-        <v>0.85</v>
-      </c>
-      <c r="J34" s="4">
-        <f>J30*N8</f>
-        <v>5.1000000000000005</v>
-      </c>
-      <c r="T34" s="5"/>
-    </row>
-    <row r="35" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B35" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="4">
-        <f>G31*N6</f>
-        <v>0</v>
-      </c>
-      <c r="J35" s="4">
-        <f>J31*N7</f>
-        <v>0.8</v>
-      </c>
-      <c r="T35" s="5"/>
-    </row>
-    <row r="36" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B36" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="J36" s="4">
-        <f>J32*N6</f>
-        <v>0</v>
-      </c>
-      <c r="T36" s="5"/>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B37" s="19"/>
-      <c r="T37" s="5"/>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B38" s="19"/>
-      <c r="T38" s="5"/>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B39" s="19"/>
-      <c r="T39" s="5"/>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B40" s="19"/>
-      <c r="T40" s="5"/>
-    </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B41" s="19"/>
-      <c r="T41" s="5"/>
-    </row>
-    <row r="42" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B42" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="T42" s="5"/>
-    </row>
-    <row r="43" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B43" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="4">
-        <f>C8*C12*$C$10</f>
-        <v>5250</v>
-      </c>
-      <c r="D43" s="4">
-        <f>D8*D12*$C$10</f>
-        <v>7000</v>
-      </c>
-      <c r="M43">
+      <c r="B78" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D78" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G78" s="4">
+        <f>INT(F$4-$W$6 &gt; $A78)*G55</f>
+        <v>0</v>
+      </c>
+      <c r="J78" s="4">
+        <f>INT(I$4-$W$6 &gt; $A78)*J55</f>
+        <v>0</v>
+      </c>
+      <c r="M78" s="4">
+        <f>INT(L$4-$W$6 &gt; $A78)*M55</f>
+        <v>0</v>
+      </c>
+      <c r="P78" s="4">
+        <f>INT(O$4-$W$6 &gt; $A78)*P55</f>
+        <v>0</v>
+      </c>
+      <c r="S78" s="4">
+        <f>INT(R$4-$W$6 &gt; $A78)*S55</f>
+        <v>0</v>
+      </c>
+      <c r="AB78" s="5"/>
+    </row>
+    <row r="79" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B79" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB79" s="5"/>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B80" s="14"/>
+      <c r="AB80" s="5"/>
+    </row>
+    <row r="81" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B81" s="13"/>
+      <c r="AB81" s="5"/>
+    </row>
+    <row r="82" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B82" s="13"/>
+      <c r="AB82" s="5"/>
+    </row>
+    <row r="83" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B83" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="12"/>
+      <c r="L83" s="12"/>
+      <c r="M83" s="12"/>
+      <c r="O83" s="12"/>
+      <c r="P83" s="12"/>
+      <c r="R83" s="12"/>
+      <c r="S83" s="12"/>
+      <c r="AB83" s="5"/>
+    </row>
+    <row r="84" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B84" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C84" s="4">
+        <f>C19*C7</f>
+        <v>1500000</v>
+      </c>
+      <c r="D84" s="4">
+        <f>D19*D7</f>
+        <v>25000000</v>
+      </c>
+      <c r="U84">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N43">
-        <f>SUM(M$6:M43)</f>
-        <v>81.059999999999988</v>
-      </c>
-      <c r="O43">
+      <c r="V84">
+        <f>SUM(U$6:U84)</f>
+        <v>81.539999999999992</v>
+      </c>
+      <c r="W84">
         <v>20</v>
       </c>
-      <c r="T43" s="5">
+      <c r="AB84" s="5">
         <v>5495710</v>
       </c>
-      <c r="U43">
+      <c r="AC84">
         <f t="shared" si="0"/>
         <v>1373928</v>
       </c>
     </row>
-    <row r="44" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B44" s="16" t="s">
+    <row r="85" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B85" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D85" s="4">
+        <f>SUM(D104:D107)</f>
+        <v>0</v>
+      </c>
+      <c r="AB85" s="5"/>
+    </row>
+    <row r="86" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B86" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C86" s="4">
+        <f>C84+C85</f>
+        <v>1500000</v>
+      </c>
+      <c r="D86" s="4">
+        <f>D84+D85</f>
+        <v>25000000</v>
+      </c>
+      <c r="AB86" s="5"/>
+    </row>
+    <row r="87" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AB87" s="5"/>
+    </row>
+    <row r="88" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B88" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C88" s="4">
+        <f>C9*C19*$C$13</f>
+        <v>5250</v>
+      </c>
+      <c r="D88" s="4">
+        <f>D9*D19*$C$13</f>
+        <v>7000</v>
+      </c>
+      <c r="AB88" s="5"/>
+    </row>
+    <row r="89" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B89" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C89" s="4">
+        <f>C23*C19</f>
+        <v>750000</v>
+      </c>
+      <c r="D89" s="4">
+        <f>D23*D19</f>
+        <v>5000000</v>
+      </c>
+      <c r="AB89" s="5"/>
+    </row>
+    <row r="90" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B90" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C90" s="4">
+        <f>$C20*MAX(C7-C9-C23,0)</f>
+        <v>222750</v>
+      </c>
+      <c r="D90" s="4">
+        <f>$D20*MAX(D7-D9-D23,0)</f>
+        <v>5997000</v>
+      </c>
+      <c r="AB90" s="5"/>
+    </row>
+    <row r="91" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AB91" s="5"/>
+    </row>
+    <row r="92" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B92" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C92" s="4">
+        <f>MAX(C7-C9-C23, 0)*C95</f>
+        <v>519750</v>
+      </c>
+      <c r="D92" s="4">
+        <f>MAX(D7-D9-D23, 0)*D95</f>
+        <v>13993000</v>
+      </c>
+      <c r="AB92" s="5"/>
+    </row>
+    <row r="93" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AB93" s="5"/>
+    </row>
+    <row r="94" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B94" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="AB94" s="5"/>
+    </row>
+    <row r="95" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B95" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C95" s="4">
+        <f>MAX(C84/C7-C20,0)</f>
+        <v>105</v>
+      </c>
+      <c r="D95" s="4">
+        <f>MAX(D84/D7-D20,0)</f>
+        <v>70</v>
+      </c>
+      <c r="AB95" s="5"/>
+    </row>
+    <row r="96" spans="2:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="B96" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C96" s="4">
+        <f>C95/$C$21</f>
+        <v>1</v>
+      </c>
+      <c r="D96" s="4">
+        <f>D95/$D$21</f>
+        <v>1</v>
+      </c>
+      <c r="AB96" s="5"/>
+    </row>
+    <row r="97" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B97" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C97" s="4">
+        <f>MAX(MIN((C96-C14)/$C$15, 1), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D97" s="4">
+        <f>MAX(MIN((D96-$C$14)/$C$15, 1), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB97" s="5"/>
+    </row>
+    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB98" s="5"/>
+    </row>
+    <row r="99" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B99" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C99" s="4">
+        <f>C92*C97</f>
+        <v>519750</v>
+      </c>
+      <c r="D99" s="4">
+        <f>D92*D97</f>
+        <v>13993000</v>
+      </c>
+      <c r="AB99" s="5"/>
+    </row>
+    <row r="100" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B100" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C100" s="4">
+        <f>C99+D99</f>
+        <v>14512750</v>
+      </c>
+      <c r="AB100" s="5"/>
+    </row>
+    <row r="101" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B101" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C101" s="4">
+        <f>C99/$C100</f>
+        <v>3.5813336548896658E-2</v>
+      </c>
+      <c r="D101" s="4">
+        <f>D99/$C100</f>
+        <v>0.96418666345110338</v>
+      </c>
+      <c r="AB101" s="5"/>
+    </row>
+    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB102" s="5"/>
+    </row>
+    <row r="103" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B103" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="AB103" s="5"/>
+    </row>
+    <row r="104" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B104" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D104" s="4">
+        <f>D46*D75</f>
+        <v>0</v>
+      </c>
+      <c r="G104" s="4">
+        <f>D104 - D116 + G70*G46</f>
+        <v>0.85</v>
+      </c>
+      <c r="J104" s="4">
+        <f>G104 - G116 + J70*J46</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M104" s="4">
+        <f>J104 - J116 + M70*M46</f>
+        <v>14.819999999999999</v>
+      </c>
+      <c r="P104" s="4">
+        <f>M104 - M116 + P70*P46</f>
+        <v>22.22</v>
+      </c>
+      <c r="S104" s="4">
+        <f>P104 - P116 + S70*S46</f>
+        <v>22.22</v>
+      </c>
+      <c r="AB104" s="5"/>
+    </row>
+    <row r="105" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B105" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D105" s="4">
+        <v>0</v>
+      </c>
+      <c r="G105" s="4">
+        <f>D105 - D117 + G71*G47</f>
+        <v>0</v>
+      </c>
+      <c r="J105" s="4">
+        <f>G105 - G117 + J71*J47</f>
+        <v>0.8</v>
+      </c>
+      <c r="M105" s="4">
+        <f>J105 - J117 + M71*M47</f>
+        <v>4.8</v>
+      </c>
+      <c r="P105" s="4">
+        <f>M105 - M117 + P71*P47</f>
+        <v>14.399999999999999</v>
+      </c>
+      <c r="S105" s="4">
+        <f>P105 - P117 + S71*S47</f>
+        <v>17.799999999999997</v>
+      </c>
+      <c r="AB105" s="5"/>
+    </row>
+    <row r="106" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B106" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D106" s="4">
+        <v>0</v>
+      </c>
+      <c r="G106" s="4">
+        <f>D106 - D118 + G72*G48</f>
+        <v>0</v>
+      </c>
+      <c r="J106" s="4">
+        <f>G106 - G118 + J72*J48</f>
+        <v>0</v>
+      </c>
+      <c r="M106" s="4">
+        <f>J106 - J118 + M72*M48</f>
+        <v>0.92</v>
+      </c>
+      <c r="P106" s="4">
+        <f>M106 - M118 + P72*P48</f>
+        <v>5.5200000000000005</v>
+      </c>
+      <c r="S106" s="4">
+        <f>P106 - P118 + S72*S48</f>
+        <v>16.559999999999999</v>
+      </c>
+      <c r="Y106" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB106" s="5"/>
+    </row>
+    <row r="107" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B107" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D107" s="4">
+        <v>0</v>
+      </c>
+      <c r="G107" s="4">
+        <f>D107 - D119 + G73*G49</f>
+        <v>0</v>
+      </c>
+      <c r="J107" s="4">
+        <f>G107 - G119 + J73*J49</f>
+        <v>0</v>
+      </c>
+      <c r="M107" s="4">
+        <f>J107 - J119 + M73*M49</f>
+        <v>0</v>
+      </c>
+      <c r="P107" s="4">
+        <f>M107 - M119 + P73*P49</f>
+        <v>0.43</v>
+      </c>
+      <c r="S107" s="4">
+        <f>P107 - P119 + S73*S49</f>
+        <v>2.58</v>
+      </c>
+      <c r="Y107" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB107" s="5"/>
+    </row>
+    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B108" s="14"/>
+      <c r="AB108" s="5"/>
+    </row>
+    <row r="109" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>0</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D109" s="4">
+        <f>INT(C$4-$W$6&gt;$A109)*D104</f>
+        <v>0</v>
+      </c>
+      <c r="G109" s="4">
+        <f>INT(F$4-$W$6&gt;$A109)*G104</f>
+        <v>0</v>
+      </c>
+      <c r="J109" s="4">
+        <f>INT(I$4-$W$6&gt;$A109)*J104</f>
+        <v>0</v>
+      </c>
+      <c r="M109" s="4">
+        <f>INT(L$4-$W$6&gt;$A109)*M104</f>
+        <v>14.819999999999999</v>
+      </c>
+      <c r="P109" s="4">
+        <f>INT(O$4-$W$6&gt;$A109)*P104</f>
+        <v>22.22</v>
+      </c>
+      <c r="S109" s="4">
+        <f>INT(R$4-$W$6&gt;$A109)*S104</f>
+        <v>22.22</v>
+      </c>
+      <c r="AB109" s="5"/>
+    </row>
+    <row r="110" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
+        <v>1</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D110" s="4">
+        <f t="shared" ref="D110:D112" si="7">INT(C$4-$W$6&gt;$A110)*D105</f>
+        <v>0</v>
+      </c>
+      <c r="G110" s="4">
+        <f t="shared" ref="G110:G112" si="8">INT(F$4-$W$6&gt;$A110)*G105</f>
+        <v>0</v>
+      </c>
+      <c r="J110" s="4">
+        <f t="shared" ref="J110:J112" si="9">INT(I$4-$W$6&gt;$A110)*J105</f>
+        <v>0</v>
+      </c>
+      <c r="M110" s="4">
+        <f t="shared" ref="M110:M112" si="10">INT(L$4-$W$6&gt;$A110)*M105</f>
+        <v>0</v>
+      </c>
+      <c r="P110" s="4">
+        <f t="shared" ref="P110:P112" si="11">INT(O$4-$W$6&gt;$A110)*P105</f>
+        <v>14.399999999999999</v>
+      </c>
+      <c r="S110" s="4">
+        <f t="shared" ref="S110:S112" si="12">INT(R$4-$W$6&gt;$A110)*S105</f>
+        <v>17.799999999999997</v>
+      </c>
+      <c r="AB110" s="5"/>
+    </row>
+    <row r="111" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>2</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D111" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G111" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J111" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M111" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P111" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="S111" s="4">
+        <f t="shared" si="12"/>
+        <v>16.559999999999999</v>
+      </c>
+      <c r="AB111" s="5"/>
+    </row>
+    <row r="112" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>3</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D112" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G112" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J112" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M112" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P112" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="S112" s="4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AB112" s="5"/>
+    </row>
+    <row r="113" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B113" s="14"/>
+      <c r="AB113" s="5"/>
+    </row>
+    <row r="114" spans="2:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="X114" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB114" s="5"/>
+    </row>
+    <row r="115" spans="2:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B115" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB115" s="5"/>
+    </row>
+    <row r="116" spans="2:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B116" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D116" s="4">
+        <v>0</v>
+      </c>
+      <c r="G116" s="4">
+        <f>INT(F4-$W$6 &gt; 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J116" s="4">
+        <f>INT(I4-$W$6 &gt; 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M116" s="4">
+        <f>INT(L4-$W$6 &gt; 0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB116" s="5"/>
+    </row>
+    <row r="117" spans="2:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B117" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D117" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB117" s="5"/>
+    </row>
+    <row r="118" spans="2:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B118" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D118" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB118" s="5"/>
+    </row>
+    <row r="119" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B119" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D119" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB119" s="5"/>
+    </row>
+    <row r="120" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AB120" s="5"/>
+    </row>
+    <row r="121" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B121" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="4">
-        <f>C13*C12</f>
-        <v>750000</v>
-      </c>
-      <c r="D44" s="4">
-        <f>D13*D12</f>
-        <v>5000000</v>
-      </c>
-      <c r="T44" s="5"/>
-    </row>
-    <row r="45" spans="2:21" ht="34" x14ac:dyDescent="0.2">
-      <c r="B45" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="4">
-        <f>MAX(C12 - $C$12*$C$11, 0)</f>
-        <v>105</v>
-      </c>
-      <c r="D45" s="4">
-        <f>MAX(D12 - $D$12*$C$11, 0)</f>
-        <v>70</v>
-      </c>
-      <c r="T45" s="5"/>
-    </row>
-    <row r="46" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B46" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" s="4">
-        <f>MAX(C7-C8 - C13, 0)*C45</f>
-        <v>519750</v>
-      </c>
-      <c r="D46" s="4">
-        <f>MAX(D7-D8 - D13, 0)*D45</f>
-        <v>13993000</v>
-      </c>
-      <c r="T46" s="5"/>
-    </row>
-    <row r="47" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B47" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="T47" s="5"/>
-    </row>
-    <row r="48" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B48" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="4">
-        <v>0</v>
-      </c>
-      <c r="T48" s="5"/>
-    </row>
-    <row r="49" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B49" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="4">
-        <f>C46+C43+D46+D43+D48</f>
-        <v>14525000</v>
-      </c>
-      <c r="M49">
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="AB121" s="5"/>
+    </row>
+    <row r="122" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B122" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C122" s="4">
+        <f>MIN(C100,C29)</f>
+        <v>200000</v>
+      </c>
+      <c r="U122">
         <v>0.5</v>
       </c>
-      <c r="N49">
-        <f>SUM(M$6:M49)</f>
-        <v>81.559999999999988</v>
-      </c>
-      <c r="O49">
+      <c r="V122">
+        <f>SUM(U$6:U122)</f>
+        <v>82.039999999999992</v>
+      </c>
+      <c r="W122">
         <v>20</v>
       </c>
-      <c r="T49" s="5">
+      <c r="AB122" s="5">
         <v>5605620</v>
       </c>
-      <c r="U49">
+      <c r="AC122">
         <f t="shared" si="0"/>
         <v>1401405</v>
       </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M50">
+    <row r="123" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B123" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C123" s="4">
+        <f>C29-C122</f>
+        <v>0</v>
+      </c>
+      <c r="U123">
         <v>0.3</v>
       </c>
-      <c r="N50">
-        <f>SUM(M$6:M50)</f>
-        <v>81.859999999999985</v>
-      </c>
-      <c r="O50">
+      <c r="V123">
+        <f>SUM(U$6:U123)</f>
+        <v>82.339999999999989</v>
+      </c>
+      <c r="W123">
         <v>20</v>
       </c>
-      <c r="T50" s="5">
+      <c r="AB123" s="5">
         <v>5717730</v>
       </c>
-      <c r="U50">
+      <c r="AC123">
         <f t="shared" si="0"/>
         <v>1429433</v>
       </c>
     </row>
-    <row r="51" spans="2:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" s="4">
-        <f>MIN(C19,C49)</f>
-        <v>1000000</v>
-      </c>
-      <c r="M51">
+    <row r="124" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B124" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C124" s="4">
+        <f>MIN(C29,C122)</f>
+        <v>200000</v>
+      </c>
+      <c r="U124">
         <v>0.2</v>
       </c>
-      <c r="N51">
-        <f>SUM(M$6:M51)</f>
-        <v>82.059999999999988</v>
-      </c>
-      <c r="O51">
+      <c r="V124">
+        <f>SUM(U$6:U124)</f>
+        <v>82.539999999999992</v>
+      </c>
+      <c r="W124">
         <v>20</v>
       </c>
-      <c r="T51" s="5">
+      <c r="AB124" s="5">
         <v>5832080</v>
       </c>
-      <c r="U51">
+      <c r="AC124">
         <f t="shared" si="0"/>
         <v>1458020</v>
       </c>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M52">
+    <row r="125" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="U125">
         <v>0.18</v>
       </c>
-      <c r="N52">
-        <f>SUM(M$6:M52)</f>
-        <v>82.24</v>
-      </c>
-      <c r="O52">
+      <c r="V125">
+        <f>SUM(U$6:U125)</f>
+        <v>82.72</v>
+      </c>
+      <c r="W125">
         <v>20</v>
       </c>
-      <c r="T52" s="5">
+      <c r="AB125" s="5">
         <v>5948720</v>
       </c>
-      <c r="U52">
+      <c r="AC125">
         <f t="shared" si="0"/>
         <v>1487180</v>
       </c>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M53">
+    <row r="126" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="U126">
         <v>0.17</v>
       </c>
-      <c r="N53">
-        <f>SUM(M$6:M53)</f>
-        <v>82.41</v>
-      </c>
-      <c r="O53">
+      <c r="V126">
+        <f>SUM(U$6:U126)</f>
+        <v>82.89</v>
+      </c>
+      <c r="W126">
         <v>20</v>
       </c>
-      <c r="T53" s="5">
+      <c r="AB126" s="5">
         <v>6067690</v>
       </c>
-      <c r="U53">
+      <c r="AC126">
         <f t="shared" si="0"/>
         <v>1516923</v>
       </c>
     </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M54">
+    <row r="127" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="U127">
         <v>0.16</v>
       </c>
-      <c r="N54">
-        <f>SUM(M$6:M54)</f>
-        <v>82.57</v>
-      </c>
-      <c r="O54">
+      <c r="V127">
+        <f>SUM(U$6:U127)</f>
+        <v>83.05</v>
+      </c>
+      <c r="W127">
         <v>20</v>
       </c>
-      <c r="T54" s="5">
+      <c r="AB127" s="5">
         <v>6189040</v>
       </c>
-      <c r="U54">
+      <c r="AC127">
         <f t="shared" si="0"/>
         <v>1547260</v>
       </c>
     </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M55">
+    <row r="128" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="U128">
         <v>0.15</v>
       </c>
-      <c r="N55">
-        <f>SUM(M$6:M55)</f>
-        <v>82.72</v>
-      </c>
-      <c r="O55">
+      <c r="V128">
+        <f>SUM(U$6:U128)</f>
+        <v>83.2</v>
+      </c>
+      <c r="W128">
         <v>20</v>
       </c>
-      <c r="T55" s="5">
+      <c r="AB128" s="5">
         <v>6312820</v>
       </c>
-      <c r="U55">
+      <c r="AC128">
         <f t="shared" si="0"/>
         <v>1578205</v>
       </c>
     </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M56">
+    <row r="129" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="U129">
         <v>0.14000000000000001</v>
       </c>
-      <c r="N56">
-        <f>SUM(M$6:M56)</f>
-        <v>82.86</v>
-      </c>
-      <c r="O56">
+      <c r="V129">
+        <f>SUM(U$6:U129)</f>
+        <v>83.34</v>
+      </c>
+      <c r="W129">
         <v>20</v>
       </c>
-      <c r="T56" s="5">
+      <c r="AB129" s="5">
         <v>6439080</v>
       </c>
-      <c r="U56">
+      <c r="AC129">
         <f t="shared" si="0"/>
         <v>1609770</v>
       </c>
     </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M57">
+    <row r="130" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="U130">
         <v>0.13</v>
       </c>
-      <c r="N57">
-        <f>SUM(M$6:M57)</f>
-        <v>82.99</v>
-      </c>
-      <c r="O57">
+      <c r="V130">
+        <f>SUM(U$6:U130)</f>
+        <v>83.47</v>
+      </c>
+      <c r="W130">
         <v>20</v>
       </c>
-      <c r="T57" s="5">
+      <c r="AB130" s="5">
         <v>6567860</v>
       </c>
-      <c r="U57">
+      <c r="AC130">
         <f t="shared" si="0"/>
         <v>1641965</v>
       </c>
     </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M58">
+    <row r="131" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="B131" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C131" s="4">
+        <f>C25*(C7-C9)</f>
+        <v>9154</v>
+      </c>
+      <c r="D131" s="4">
+        <f>D25*(D7-D9)</f>
+        <v>74970</v>
+      </c>
+      <c r="U131">
         <v>0.125</v>
       </c>
-      <c r="N58">
-        <f>SUM(M$6:M58)</f>
-        <v>83.114999999999995</v>
-      </c>
-      <c r="O58">
+      <c r="V131">
+        <f>SUM(U$6:U131)</f>
+        <v>83.594999999999999</v>
+      </c>
+      <c r="W131">
         <v>20</v>
       </c>
-      <c r="T58" s="5">
+      <c r="AB131" s="5">
         <v>6699220</v>
       </c>
-      <c r="U58">
+      <c r="AC131">
         <f t="shared" si="0"/>
         <v>1674805</v>
       </c>
     </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M59">
+    <row r="132" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="U132">
         <v>0.1225</v>
       </c>
-      <c r="N59">
-        <f>SUM(M$6:M59)</f>
-        <v>83.237499999999997</v>
-      </c>
-      <c r="O59">
+      <c r="V132">
+        <f>SUM(U$6:U132)</f>
+        <v>83.717500000000001</v>
+      </c>
+      <c r="W132">
         <v>20</v>
       </c>
-      <c r="T59" s="5">
+      <c r="AB132" s="5">
         <v>6833200</v>
       </c>
-      <c r="U59">
+      <c r="AC132">
         <f t="shared" si="0"/>
         <v>1708300</v>
       </c>
     </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M60">
+    <row r="133" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="U133">
         <v>0.12239999999999999</v>
       </c>
-      <c r="N60">
-        <f>SUM(M$6:M60)</f>
-        <v>83.359899999999996</v>
-      </c>
-      <c r="O60">
+      <c r="V133">
+        <f>SUM(U$6:U133)</f>
+        <v>83.8399</v>
+      </c>
+      <c r="W133">
         <v>20</v>
       </c>
-      <c r="T60" s="5">
+      <c r="AB133" s="5">
         <v>6969860</v>
       </c>
-      <c r="U60">
+      <c r="AC133">
         <f t="shared" si="0"/>
         <v>1742465</v>
       </c>
     </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M61">
+    <row r="134" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="U134">
         <v>0.12230000000000001</v>
       </c>
-      <c r="N61">
-        <f>SUM(M$6:M61)</f>
-        <v>83.482199999999992</v>
-      </c>
-      <c r="O61">
+      <c r="V134">
+        <f>SUM(U$6:U134)</f>
+        <v>83.962199999999996</v>
+      </c>
+      <c r="W134">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="U4:W4"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated carbon ledger with adjustment calculation in new forest sequestration factor
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7571DA-52A7-8645-AA69-9CA167440341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984A3765-5932-754A-B648-01A41D8B7BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33680" windowHeight="19880" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="179">
   <si>
     <t>forest_primary_c_ha</t>
   </si>
@@ -472,24 +472,15 @@
     <t>buffer</t>
   </si>
   <si>
-    <t>dead storage (minimum fraction of original stock that must remain on the land to allow it to remain that land use type)</t>
-  </si>
-  <si>
     <t>buffer zone (fraction of stock above dead storage which contributes to slowing removals)</t>
   </si>
   <si>
     <t>some reservoir terms</t>
   </si>
   <si>
-    <t>(percentage of forest stock available out of full stock  ) carbon_stock_factor</t>
-  </si>
-  <si>
     <t>healthy storage available</t>
   </si>
   <si>
-    <t>frac_removals_satisficable</t>
-  </si>
-  <si>
     <t>removals allocation</t>
   </si>
   <si>
@@ -563,6 +554,27 @@
   </si>
   <si>
     <t>t = 6</t>
+  </si>
+  <si>
+    <t>adjustment factor</t>
+  </si>
+  <si>
+    <t>calculate how much is available for removals when considering dead storage</t>
+  </si>
+  <si>
+    <t>(percentage of forest stock available out of full stock not in dead storage ) carbon_stock_factor</t>
+  </si>
+  <si>
+    <t>frac_removables_satisficable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is the fraciton of total wood removal deamands from forest that can be taken </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dead storage (minimum fraction of original stock that must remain on the land to allow it to remain that land use type). Note that sequestration factors dcline linearly below the </t>
+  </si>
+  <si>
+    <t>sequestration adjustment threshold--below this carbon stock depletion level, sequestration factors will start to decline</t>
   </si>
 </sst>
 </file>
@@ -709,14 +721,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -724,22 +741,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1286,60 +1298,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="19" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="22" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="21" t="s">
+      <c r="M1" s="25"/>
+      <c r="N1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="22" t="s">
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="23" t="s">
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="23"/>
+      <c r="V1" s="26"/>
       <c r="W1" s="4" t="s">
         <v>46</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AC1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
       <c r="AI1" s="7" t="s">
         <v>37</v>
       </c>
@@ -5876,16 +5888,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="N1:Q1"/>
     <mergeCell ref="AC1:AH1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="R1:T1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5895,14 +5907,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40F0562-A765-A442-B9DB-CF71D123E451}">
   <dimension ref="A1:AL150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" zoomScale="108" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="V75" sqref="V75"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="125" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="34.5" style="10" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" style="10" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.5" style="5" customWidth="1"/>
@@ -5926,7 +5938,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5"/>
+      <c r="A1" s="22"/>
       <c r="B1" s="10"/>
       <c r="C1" s="5" t="s">
         <v>60</v>
@@ -5956,7 +5968,7 @@
       <c r="V1" s="5"/>
     </row>
     <row r="2" spans="1:31" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="10"/>
       <c r="C2" s="5" t="s">
         <v>61</v>
@@ -5964,10 +5976,10 @@
       <c r="D2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="27">
         <v>150</v>
       </c>
-      <c r="F2" s="21"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -5988,16 +6000,16 @@
       <c r="V2" s="5"/>
     </row>
     <row r="3" spans="1:31" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="10"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="27">
         <v>30</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -6021,85 +6033,85 @@
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="16"/>
-      <c r="F4" s="26">
+      <c r="F4" s="20">
         <v>1</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="18"/>
-      <c r="I4" s="26">
+      <c r="I4" s="20">
         <v>2</v>
       </c>
-      <c r="J4" s="26"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="18"/>
-      <c r="L4" s="26">
+      <c r="L4" s="20">
         <v>3</v>
       </c>
-      <c r="M4" s="26"/>
+      <c r="M4" s="20"/>
       <c r="N4" s="18"/>
-      <c r="O4" s="26">
+      <c r="O4" s="20">
         <v>4</v>
       </c>
-      <c r="P4" s="26"/>
+      <c r="P4" s="20"/>
       <c r="Q4" s="18"/>
-      <c r="R4" s="26">
+      <c r="R4" s="20">
         <v>5</v>
       </c>
-      <c r="S4" s="26"/>
+      <c r="S4" s="20"/>
       <c r="T4" s="18"/>
-      <c r="U4" s="26">
+      <c r="U4" s="20">
         <v>6</v>
       </c>
-      <c r="V4" s="26"/>
-      <c r="Z4" s="28" t="s">
+      <c r="V4" s="20"/>
+      <c r="Z4" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
       <c r="AE4" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="17"/>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="I5" s="25" t="s">
+      <c r="G5" s="29"/>
+      <c r="I5" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="L5" s="25" t="s">
+      <c r="J5" s="29"/>
+      <c r="L5" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="M5" s="25"/>
-      <c r="O5" s="25" t="s">
+      <c r="M5" s="29"/>
+      <c r="O5" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="P5" s="25"/>
-      <c r="R5" s="25" t="s">
+      <c r="P5" s="29"/>
+      <c r="R5" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="S5" s="25"/>
-      <c r="U5" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="V5" s="25"/>
-      <c r="Z5" s="27" t="s">
+      <c r="S5" s="29"/>
+      <c r="U5" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="V5" s="29"/>
+      <c r="Z5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="AA5" s="27" t="s">
+      <c r="AA5" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="AB5" s="27" t="s">
+      <c r="AB5" s="21" t="s">
         <v>41</v>
       </c>
       <c r="AE5" t="s">
@@ -6107,7 +6119,7 @@
       </c>
     </row>
     <row r="6" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -6155,14 +6167,14 @@
       <c r="V6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Z6" s="24">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="24">
+      <c r="Z6" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="19">
         <f>SUM(Z$6:Z6)</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="24">
+      <c r="AB6" s="19">
         <v>2</v>
       </c>
     </row>
@@ -6224,14 +6236,14 @@
         <f>MAX(S7-S9,0)</f>
         <v>249360</v>
       </c>
-      <c r="Z7" s="24">
+      <c r="Z7" s="19">
         <v>0.01</v>
       </c>
-      <c r="AA7" s="24">
+      <c r="AA7" s="19">
         <f>SUM(Z$6:Z7)</f>
         <v>0.01</v>
       </c>
-      <c r="AB7" s="24">
+      <c r="AB7" s="19">
         <v>2</v>
       </c>
       <c r="AD7" s="5">
@@ -6302,14 +6314,14 @@
         <f>S8-S9+S11</f>
         <v>249795</v>
       </c>
-      <c r="Z8" s="24">
+      <c r="Z8" s="19">
         <v>0.05</v>
       </c>
-      <c r="AA8" s="24">
+      <c r="AA8" s="19">
         <f>SUM(Z$6:Z8)</f>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="AB8" s="24">
+      <c r="AB8" s="19">
         <v>2</v>
       </c>
       <c r="AD8" s="5"/>
@@ -6360,14 +6372,14 @@
       <c r="V9" s="4">
         <v>105</v>
       </c>
-      <c r="Z9" s="24">
+      <c r="Z9" s="19">
         <v>0.12</v>
       </c>
-      <c r="AA9" s="24">
+      <c r="AA9" s="19">
         <f>SUM(Z$6:Z9)</f>
         <v>0.18</v>
       </c>
-      <c r="AB9" s="24">
+      <c r="AB9" s="19">
         <v>2</v>
       </c>
       <c r="AD9" s="5">
@@ -6378,7 +6390,7 @@
         <v>1025000</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
         <v>134</v>
       </c>
@@ -6410,14 +6422,14 @@
         <f>-MIN(V7-V9,0)</f>
         <v>0</v>
       </c>
-      <c r="Z10" s="24">
+      <c r="Z10" s="19">
         <v>0.2</v>
       </c>
-      <c r="AA10" s="24">
+      <c r="AA10" s="19">
         <f>SUM(Z$6:Z10)</f>
         <v>0.38</v>
       </c>
-      <c r="AB10" s="24">
+      <c r="AB10" s="19">
         <v>20</v>
       </c>
       <c r="AD10" s="5"/>
@@ -6447,27 +6459,27 @@
       <c r="V11" s="4">
         <v>43</v>
       </c>
-      <c r="Z11" s="24">
+      <c r="Z11" s="19">
         <v>0.36</v>
       </c>
-      <c r="AA11" s="24">
+      <c r="AA11" s="19">
         <f>SUM(Z$6:Z11)</f>
         <v>0.74</v>
       </c>
-      <c r="AB11" s="24">
+      <c r="AB11" s="19">
         <v>20</v>
       </c>
       <c r="AD11" s="5"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="Z12" s="24">
+      <c r="Z12" s="19">
         <v>0.6</v>
       </c>
-      <c r="AA12" s="24">
+      <c r="AA12" s="19">
         <f>SUM(Z$6:Z12)</f>
         <v>1.3399999999999999</v>
       </c>
-      <c r="AB12" s="24">
+      <c r="AB12" s="19">
         <v>20</v>
       </c>
       <c r="AD12" s="5"/>
@@ -6497,14 +6509,14 @@
       <c r="U13" s="4">
         <v>0.7</v>
       </c>
-      <c r="Z13" s="24">
+      <c r="Z13" s="19">
         <v>1.8</v>
       </c>
-      <c r="AA13" s="24">
+      <c r="AA13" s="19">
         <f>SUM(Z$6:Z13)</f>
         <v>3.1399999999999997</v>
       </c>
-      <c r="AB13" s="24">
+      <c r="AB13" s="19">
         <v>20</v>
       </c>
       <c r="AD13" s="5">
@@ -6515,12 +6527,12 @@
         <v>1062500</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="68" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
-        <v>146</v>
+    <row r="14" spans="1:31" ht="85" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
+        <v>145</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
       <c r="C14" s="4">
         <v>1E-3</v>
@@ -6543,81 +6555,84 @@
       <c r="U14" s="4">
         <v>0.3</v>
       </c>
-      <c r="Z14" s="24">
+      <c r="Z14" s="19">
         <v>3</v>
       </c>
-      <c r="AA14" s="24">
+      <c r="AA14" s="19">
         <f>SUM(Z$6:Z14)</f>
         <v>6.14</v>
       </c>
-      <c r="AB14" s="24">
+      <c r="AB14" s="19">
         <v>20</v>
       </c>
       <c r="AD14" s="5"/>
     </row>
     <row r="15" spans="1:31" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C15" s="4">
         <v>0.2</v>
       </c>
-      <c r="Z15" s="24">
+      <c r="Z15" s="19">
         <v>6</v>
       </c>
-      <c r="AA15" s="24">
+      <c r="AA15" s="19">
         <f>SUM(Z$6:Z15)</f>
         <v>12.14</v>
       </c>
-      <c r="AB15" s="24">
+      <c r="AB15" s="19">
         <v>20</v>
       </c>
       <c r="AD15" s="5"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
-      <c r="Z16" s="24">
+    <row r="16" spans="1:31" ht="51" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="Z16" s="19">
         <v>10</v>
       </c>
-      <c r="AA16" s="24">
+      <c r="AA16" s="19">
         <f>SUM(Z$6:Z16)</f>
         <v>22.14</v>
       </c>
-      <c r="AB16" s="24">
+      <c r="AB16" s="19">
         <v>20</v>
       </c>
       <c r="AD16" s="5"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="Z17" s="24">
+    <row r="17" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="Z17" s="19">
         <v>12</v>
       </c>
-      <c r="AA17" s="24">
+      <c r="AA17" s="19">
         <f>SUM(Z$6:Z17)</f>
         <v>34.14</v>
       </c>
-      <c r="AB17" s="24">
+      <c r="AB17" s="19">
         <v>20</v>
       </c>
       <c r="AD17" s="5"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="Z18" s="24">
+    <row r="18" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="Z18" s="19">
         <v>13.5</v>
       </c>
-      <c r="AA18" s="24">
+      <c r="AA18" s="19">
         <f>SUM(Z$6:Z18)</f>
         <v>47.64</v>
       </c>
-      <c r="AB18" s="24">
+      <c r="AB18" s="19">
         <v>20</v>
       </c>
       <c r="AD18" s="5"/>
     </row>
-    <row r="19" spans="1:38" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:38" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>141</v>
       </c>
@@ -6627,14 +6642,14 @@
       <c r="D19" s="4">
         <v>100</v>
       </c>
-      <c r="Z19" s="24">
+      <c r="Z19" s="19">
         <v>12</v>
       </c>
-      <c r="AA19" s="24">
+      <c r="AA19" s="19">
         <f>SUM(Z$6:Z19)</f>
         <v>59.64</v>
       </c>
-      <c r="AB19" s="24">
+      <c r="AB19" s="19">
         <v>20</v>
       </c>
       <c r="AD19" s="5">
@@ -6645,7 +6660,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:38" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>140</v>
       </c>
@@ -6657,21 +6672,21 @@
         <f>D$19*$C$14</f>
         <v>0.1</v>
       </c>
-      <c r="Z20" s="24">
+      <c r="Z20" s="19">
         <v>10</v>
       </c>
-      <c r="AA20" s="24">
+      <c r="AA20" s="19">
         <f>SUM(Z$6:Z20)</f>
         <v>69.64</v>
       </c>
-      <c r="AB20" s="24">
+      <c r="AB20" s="19">
         <v>20</v>
       </c>
       <c r="AD20" s="5"/>
     </row>
-    <row r="21" spans="1:38" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:38" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C21" s="4">
         <f>C19-C20</f>
@@ -6681,32 +6696,32 @@
         <f>D19-D20</f>
         <v>99.9</v>
       </c>
-      <c r="Z21" s="24">
+      <c r="Z21" s="19">
         <v>6</v>
       </c>
-      <c r="AA21" s="24">
+      <c r="AA21" s="19">
         <f>SUM(Z$6:Z21)</f>
         <v>75.64</v>
       </c>
-      <c r="AB21" s="24">
+      <c r="AB21" s="19">
         <v>20</v>
       </c>
       <c r="AD21" s="5"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="Z22" s="24">
+    <row r="22" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="Z22" s="19">
         <v>3</v>
       </c>
-      <c r="AA22" s="24">
+      <c r="AA22" s="19">
         <f>SUM(Z$6:Z22)</f>
         <v>78.64</v>
       </c>
-      <c r="AB22" s="24">
+      <c r="AB22" s="19">
         <v>20</v>
       </c>
       <c r="AD22" s="5"/>
     </row>
-    <row r="23" spans="1:38" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:38" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
         <v>52</v>
       </c>
@@ -6752,14 +6767,14 @@
       <c r="V23" s="4">
         <v>49500</v>
       </c>
-      <c r="Z23" s="24">
+      <c r="Z23" s="19">
         <v>1.8</v>
       </c>
-      <c r="AA23" s="24">
+      <c r="AA23" s="19">
         <f>SUM(Z$6:Z23)</f>
         <v>80.44</v>
       </c>
-      <c r="AB23" s="24">
+      <c r="AB23" s="19">
         <v>20</v>
       </c>
       <c r="AD23" s="5">
@@ -6773,7 +6788,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:38" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="15" t="s">
         <v>59</v>
       </c>
@@ -6799,7 +6814,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:38" ht="34" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
         <v>71</v>
       </c>
@@ -6823,7 +6838,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:38" x14ac:dyDescent="0.2">
       <c r="AD26" s="5"/>
       <c r="AI26" t="s">
         <v>102</v>
@@ -6838,7 +6853,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:38" x14ac:dyDescent="0.2">
       <c r="AD27" s="5">
         <v>4508400</v>
       </c>
@@ -6859,7 +6874,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:38" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:38" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="15" t="s">
         <v>56</v>
       </c>
@@ -6897,7 +6912,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:38" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
         <v>53</v>
       </c>
@@ -6942,7 +6957,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:38" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" s="10" t="s">
         <v>143</v>
       </c>
@@ -6966,7 +6981,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:38" x14ac:dyDescent="0.2">
       <c r="AD31" s="5">
         <v>4880040</v>
       </c>
@@ -6975,7 +6990,7 @@
         <v>1220010</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:38" x14ac:dyDescent="0.2">
       <c r="AD32" s="5">
         <v>4977640</v>
       </c>
@@ -7081,20 +7096,20 @@
         <v>72</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D44" s="8"/>
       <c r="F44" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AD44" s="5"/>
     </row>
@@ -7494,8 +7509,8 @@
       <c r="AD51" s="5"/>
     </row>
     <row r="52" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="29" t="s">
-        <v>163</v>
+      <c r="A52" s="28" t="s">
+        <v>160</v>
       </c>
       <c r="B52" s="14" t="s">
         <v>98</v>
@@ -7531,7 +7546,7 @@
       <c r="AD52" s="5"/>
     </row>
     <row r="53" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="29"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="14" t="s">
         <v>99</v>
       </c>
@@ -7564,7 +7579,7 @@
       <c r="AD53" s="5"/>
     </row>
     <row r="54" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="29"/>
+      <c r="A54" s="28"/>
       <c r="B54" s="14" t="s">
         <v>100</v>
       </c>
@@ -7596,7 +7611,7 @@
       <c r="AD54" s="5"/>
     </row>
     <row r="55" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="29"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="14" t="s">
         <v>101</v>
       </c>
@@ -7637,8 +7652,8 @@
       <c r="AD57" s="5"/>
     </row>
     <row r="58" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="29" t="s">
-        <v>164</v>
+      <c r="A58" s="28" t="s">
+        <v>161</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>130</v>
@@ -7674,7 +7689,7 @@
       <c r="AD58" s="5"/>
     </row>
     <row r="59" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="29"/>
+      <c r="A59" s="28"/>
       <c r="B59" s="14" t="s">
         <v>131</v>
       </c>
@@ -7705,7 +7720,7 @@
       <c r="AD59" s="5"/>
     </row>
     <row r="60" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="29"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="14" t="s">
         <v>132</v>
       </c>
@@ -7735,7 +7750,7 @@
       <c r="AD60" s="5"/>
     </row>
     <row r="61" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="29"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="14" t="s">
         <v>133</v>
       </c>
@@ -7781,11 +7796,11 @@
       <c r="AD63" s="5"/>
     </row>
     <row r="64" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="5">
+      <c r="A64" s="22">
         <v>0</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D64" s="4">
         <f>D31</f>
@@ -7818,11 +7833,11 @@
       <c r="AD64" s="5"/>
     </row>
     <row r="65" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="5">
+      <c r="A65" s="22">
         <v>1</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D65" s="4">
         <f>D32</f>
@@ -7855,11 +7870,11 @@
       <c r="AD65" s="5"/>
     </row>
     <row r="66" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="5">
+      <c r="A66" s="22">
         <v>2</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D66" s="4">
         <f>D33</f>
@@ -7892,11 +7907,11 @@
       <c r="AD66" s="5"/>
     </row>
     <row r="67" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="5">
+      <c r="A67" s="22">
         <v>3</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D67" s="4">
         <f>D34</f>
@@ -7930,21 +7945,28 @@
     </row>
     <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B68" s="14"/>
+      <c r="F68" s="4" t="s">
+        <v>172</v>
+      </c>
       <c r="AD68" s="5"/>
     </row>
     <row r="69" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="29" t="s">
-        <v>169</v>
+      <c r="A69" s="28" t="s">
+        <v>166</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D69" s="4">
         <f>D52</f>
         <v>0</v>
       </c>
+      <c r="F69" s="4">
+        <f>IF(D74=0,1,MIN(MAX((D74/D58-$C$14)/($C$16-$C$14), 0), 1))</f>
+        <v>1</v>
+      </c>
       <c r="G69" s="4">
-        <f>G52</f>
+        <f>G52*F69</f>
         <v>0.01</v>
       </c>
       <c r="J69" s="4">
@@ -7970,9 +7992,9 @@
       <c r="AD69" s="5"/>
     </row>
     <row r="70" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="29"/>
+      <c r="A70" s="28"/>
       <c r="B70" s="14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D70" s="4">
         <f t="shared" ref="D70:D72" si="10">D53</f>
@@ -8005,9 +8027,9 @@
       <c r="AD70" s="5"/>
     </row>
     <row r="71" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="29"/>
+      <c r="A71" s="28"/>
       <c r="B71" s="14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D71" s="4">
         <f>D54</f>
@@ -8040,9 +8062,9 @@
       <c r="AD71" s="5"/>
     </row>
     <row r="72" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="29"/>
+      <c r="A72" s="28"/>
       <c r="B72" s="14" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D72" s="4">
         <f t="shared" si="10"/>
@@ -8308,7 +8330,7 @@
       <c r="AD90" s="5"/>
     </row>
     <row r="91" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="5">
+      <c r="A91" s="22">
         <v>0</v>
       </c>
       <c r="B91" s="14" t="s">
@@ -8345,7 +8367,7 @@
       <c r="AD91" s="5"/>
     </row>
     <row r="92" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="5">
+      <c r="A92" s="22">
         <v>1</v>
       </c>
       <c r="B92" s="14" t="s">
@@ -8382,7 +8404,7 @@
       <c r="AD92" s="5"/>
     </row>
     <row r="93" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="5">
+      <c r="A93" s="22">
         <v>2</v>
       </c>
       <c r="B93" s="14" t="s">
@@ -8419,7 +8441,7 @@
       <c r="AD93" s="5"/>
     </row>
     <row r="94" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="5">
+      <c r="A94" s="22">
         <v>3</v>
       </c>
       <c r="B94" s="14" t="s">
@@ -8465,15 +8487,15 @@
       <c r="B96" s="14"/>
       <c r="AD96" s="5"/>
     </row>
-    <row r="97" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B97" s="13"/>
       <c r="AD97" s="5"/>
     </row>
-    <row r="98" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B98" s="13"/>
       <c r="AD98" s="5"/>
     </row>
-    <row r="99" spans="2:31" ht="17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B99" s="11" t="s">
         <v>58</v>
       </c>
@@ -8493,9 +8515,9 @@
       <c r="V99" s="12"/>
       <c r="AD99" s="5"/>
     </row>
-    <row r="100" spans="2:31" ht="17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B100" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C100" s="4">
         <f>C19*C7</f>
@@ -8523,9 +8545,9 @@
         <v>1373928</v>
       </c>
     </row>
-    <row r="101" spans="2:31" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B101" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D101" s="4">
         <f>SUM(D120:D123)</f>
@@ -8533,9 +8555,9 @@
       </c>
       <c r="AD101" s="5"/>
     </row>
-    <row r="102" spans="2:31" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B102" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C102" s="4">
         <f>C100+C101</f>
@@ -8547,12 +8569,12 @@
       </c>
       <c r="AD102" s="5"/>
     </row>
-    <row r="103" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.2">
       <c r="AD103" s="5"/>
     </row>
-    <row r="104" spans="2:31" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B104" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C104" s="4">
         <f>C9*C19*$C$13</f>
@@ -8564,7 +8586,7 @@
       </c>
       <c r="AD104" s="5"/>
     </row>
-    <row r="105" spans="2:31" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B105" s="10" t="s">
         <v>70</v>
       </c>
@@ -8578,9 +8600,9 @@
       </c>
       <c r="AD105" s="5"/>
     </row>
-    <row r="106" spans="2:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B106" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C106" s="4">
         <f>$C20*MAX(C7-C9-C23,0)</f>
@@ -8592,12 +8614,12 @@
       </c>
       <c r="AD106" s="5"/>
     </row>
-    <row r="107" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.2">
       <c r="AD107" s="5"/>
     </row>
-    <row r="108" spans="2:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="B108" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C108" s="4">
         <f>MAX(C7-C9-C23, 0)*C111</f>
@@ -8609,10 +8631,10 @@
       </c>
       <c r="AD108" s="5"/>
     </row>
-    <row r="109" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.2">
       <c r="AD109" s="5"/>
     </row>
-    <row r="110" spans="2:31" ht="17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B110" s="15" t="s">
         <v>79</v>
       </c>
@@ -8620,7 +8642,10 @@
       <c r="D110" s="8"/>
       <c r="AD110" s="5"/>
     </row>
-    <row r="111" spans="2:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:31" ht="68" x14ac:dyDescent="0.2">
+      <c r="A111" s="22" t="s">
+        <v>173</v>
+      </c>
       <c r="B111" s="10" t="s">
         <v>80</v>
       </c>
@@ -8634,9 +8659,9 @@
       </c>
       <c r="AD111" s="5"/>
     </row>
-    <row r="112" spans="2:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="B112" s="10" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="C112" s="4">
         <f>C111/$C$21</f>
@@ -8648,12 +8673,15 @@
       </c>
       <c r="AD112" s="5"/>
     </row>
-    <row r="113" spans="1:30" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:30" ht="51" x14ac:dyDescent="0.2">
+      <c r="A113" s="22" t="s">
+        <v>176</v>
+      </c>
       <c r="B113" s="10" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="C113" s="4">
-        <f>MAX(MIN((C112-C14)/$C$15, 1), 0)</f>
+        <f>MAX(MIN(C112/$C$15, 1), 0)</f>
         <v>1</v>
       </c>
       <c r="D113" s="4">
@@ -8681,7 +8709,7 @@
     </row>
     <row r="116" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="B116" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C116" s="4">
         <f>C115+D115</f>
@@ -8691,7 +8719,7 @@
     </row>
     <row r="117" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="B117" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C117" s="4">
         <f>C115/$C116</f>
@@ -8858,7 +8886,7 @@
       <c r="AD124" s="5"/>
     </row>
     <row r="125" spans="1:30" ht="34" x14ac:dyDescent="0.2">
-      <c r="A125" s="5">
+      <c r="A125" s="22">
         <v>0</v>
       </c>
       <c r="B125" s="14" t="s">
@@ -8895,7 +8923,7 @@
       <c r="AD125" s="5"/>
     </row>
     <row r="126" spans="1:30" ht="34" x14ac:dyDescent="0.2">
-      <c r="A126" s="5">
+      <c r="A126" s="22">
         <v>1</v>
       </c>
       <c r="B126" s="14" t="s">
@@ -8932,7 +8960,7 @@
       <c r="AD126" s="5"/>
     </row>
     <row r="127" spans="1:30" ht="34" x14ac:dyDescent="0.2">
-      <c r="A127" s="5">
+      <c r="A127" s="22">
         <v>2</v>
       </c>
       <c r="B127" s="14" t="s">
@@ -8969,7 +8997,7 @@
       <c r="AD127" s="5"/>
     </row>
     <row r="128" spans="1:30" ht="34" x14ac:dyDescent="0.2">
-      <c r="A128" s="5">
+      <c r="A128" s="22">
         <v>3</v>
       </c>
       <c r="B128" s="14" t="s">
@@ -9085,7 +9113,7 @@
     </row>
     <row r="138" spans="2:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B138" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C138" s="4">
         <f>MIN(C116,C29)</f>
@@ -9111,7 +9139,7 @@
     </row>
     <row r="139" spans="2:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B139" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C139" s="4">
         <f>C29-C138</f>
@@ -9137,7 +9165,7 @@
     </row>
     <row r="140" spans="2:31" ht="17" x14ac:dyDescent="0.2">
       <c r="B140" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C140" s="4">
         <f>MIN(C29,C138)</f>
@@ -9357,6 +9385,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="A58:A61"/>
@@ -9366,11 +9399,6 @@
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="R5:S5"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
updated carbon ledger and notebook to reflect progress
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F102C4-5E23-194D-A289-C3FA26E1E7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBE7CB3-3C87-4D48-8A0E-87CF406EF9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="760" windowWidth="33680" windowHeight="19880" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="33680" windowHeight="19400" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="264">
   <si>
     <t>forest_primary_c_ha</t>
   </si>
@@ -522,12 +522,6 @@
     <t>arr_area_remaining_from_orig_after_conversion_away</t>
   </si>
   <si>
-    <t>arr_biomass_factor_min_reqd</t>
-  </si>
-  <si>
-    <t>arr_biomass_factor_healthy_available</t>
-  </si>
-  <si>
     <t>arr_area_protected_total</t>
   </si>
   <si>
@@ -564,9 +558,6 @@
     <t>bg c lost from conversion</t>
   </si>
   <si>
-    <t>arr_annual_sf_nominal</t>
-  </si>
-  <si>
     <t>vec_total_removals_demanded</t>
   </si>
   <si>
@@ -597,25 +588,16 @@
     <t>healthy storage available per ha</t>
   </si>
   <si>
-    <t>arr_frac_biomass_ag_decomposition</t>
-  </si>
-  <si>
     <t>arr_biomass_c_ag_lost_conversion</t>
   </si>
   <si>
     <t>arr_biomass_c_bg_lost_conversion</t>
   </si>
   <si>
-    <t>arr_young_stock_if_untouched (T x T)</t>
-  </si>
-  <si>
     <t>arr_young_sf_base_by_tp_planted (T x T)</t>
   </si>
   <si>
     <t>T = number of time periods</t>
-  </si>
-  <si>
-    <t>arr_young_c_available_for_removals_mask (T x T)</t>
   </si>
   <si>
     <t>arr_young_area_by_tp_planted (T x T)   [e.g., col J]
@@ -623,10 +605,6 @@
 arr_young_area_by_tp_planted_drops (T x T)   [e.g., col I]</t>
   </si>
   <si>
-    <t>arr_young_c_stock_removal_allocation (T x T)   [e.g., col G]
-arr_young_c_stock_removal_allocation_aux (T x T)   [e.g., col F]</t>
-  </si>
-  <si>
     <t>arr_biomass_c_converted_away</t>
   </si>
   <si>
@@ -691,9 +669,6 @@
     <t>arr_orig_allocation_removals</t>
   </si>
   <si>
-    <t>vec_young_c_available_for_removals_total</t>
-  </si>
-  <si>
     <t>arr_young_biomass_c_ag_converted_by_tp_planted (T x T)</t>
   </si>
   <si>
@@ -826,10 +801,41 @@
     <t xml:space="preserve">dead storage (minimum fraction of original stock that must remain on the land to allow it to remain that land use type). </t>
   </si>
   <si>
-    <t>arr_biomass_c_ag_factor_stst_storage</t>
-  </si>
-  <si>
-    <t>arr_biomass_c_bg_to_ag_ratio</t>
+    <t>arr_biomass_c_min_reqd_per_area</t>
+  </si>
+  <si>
+    <t>vec_biomass_c_ag_init_stst_storage</t>
+  </si>
+  <si>
+    <t>vec_biomass_c_ag_init_healthy_available</t>
+  </si>
+  <si>
+    <t>vec_biomass_c_bg_to_ag_ratio</t>
+  </si>
+  <si>
+    <t>vec_annual_sf_nominal</t>
+  </si>
+  <si>
+    <t>vec_frac_biomass_ag_decomposition</t>
+  </si>
+  <si>
+    <t>vec_young_sf_curve</t>
+  </si>
+  <si>
+    <t>arr_young_biomass_c_available_for_removals_mask (T x T)</t>
+  </si>
+  <si>
+    <t>vec_young_biomass_c_available_for_removals_total</t>
+  </si>
+  <si>
+    <t>arr_young_biomass_c_stock_removal_allocation (T x T)   [e.g., col G]
+arr_young_biomass_c_stock_removal_allocation_aux (T x T)   [e.g., col F]</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>arr_young_biomass_c_ag_stock_if_untouched (T x T)</t>
   </si>
 </sst>
 </file>
@@ -977,7 +983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1086,10 +1092,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1112,6 +1115,13 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6266,14 +6276,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40F0562-A765-A442-B9DB-CF71D123E451}">
   <dimension ref="A1:AM150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D17"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77:A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" style="33" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" style="36" customWidth="1"/>
+    <col min="1" max="1" width="62.1640625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="14" style="36" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" style="32" customWidth="1"/>
     <col min="4" max="4" width="27" style="22" customWidth="1"/>
     <col min="5" max="5" width="44" style="10" customWidth="1"/>
@@ -6456,7 +6466,7 @@
         <v>156</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>154</v>
@@ -6493,6 +6503,9 @@
         <v>136</v>
       </c>
       <c r="Y5" s="29"/>
+      <c r="AB5" s="49" t="s">
+        <v>258</v>
+      </c>
       <c r="AC5" s="21" t="s">
         <v>33</v>
       </c>
@@ -6515,9 +6528,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="B6" s="36" t="s">
-        <v>167</v>
+    <row r="6" spans="1:39" ht="51" x14ac:dyDescent="0.2">
+      <c r="B6" s="39" t="s">
+        <v>165</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>24</v>
@@ -6585,11 +6598,11 @@
       </c>
     </row>
     <row r="7" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="B7" s="41" t="s">
-        <v>183</v>
+      <c r="B7" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>67</v>
@@ -6672,11 +6685,11 @@
       </c>
     </row>
     <row r="8" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="B8" s="42" t="s">
-        <v>166</v>
+      <c r="B8" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>114</v>
@@ -6761,11 +6774,11 @@
       </c>
     </row>
     <row r="9" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>166</v>
+      <c r="A9" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>55</v>
@@ -6836,11 +6849,11 @@
       </c>
     </row>
     <row r="10" spans="1:39" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>183</v>
+      <c r="A10" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>146</v>
@@ -6885,11 +6898,11 @@
       </c>
     </row>
     <row r="11" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>183</v>
+      <c r="A11" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>113</v>
@@ -6934,11 +6947,11 @@
       </c>
     </row>
     <row r="12" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="B12" s="42" t="s">
-        <v>166</v>
+      <c r="A12" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>66</v>
@@ -6976,11 +6989,11 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>183</v>
+      <c r="B13" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>144</v>
@@ -7046,11 +7059,11 @@
       <c r="AE13" s="19"/>
     </row>
     <row r="14" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="B14" s="42" t="s">
-        <v>166</v>
+      <c r="A14" s="46" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>54</v>
@@ -7088,14 +7101,14 @@
       </c>
     </row>
     <row r="15" spans="1:39" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="B15" s="42" t="s">
-        <v>166</v>
+      <c r="A15" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="F15" s="4">
         <v>1E-3</v>
@@ -7130,11 +7143,11 @@
       </c>
     </row>
     <row r="16" spans="1:39" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
-        <v>257</v>
-      </c>
-      <c r="B16" s="42" t="s">
-        <v>166</v>
+      <c r="A16" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>118</v>
@@ -7157,11 +7170,11 @@
       </c>
     </row>
     <row r="17" spans="1:31" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="47" t="s">
-        <v>258</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>166</v>
+      <c r="A17" s="46" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="10" t="s">
@@ -7182,11 +7195,11 @@
       </c>
     </row>
     <row r="18" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="33" t="s">
-        <v>260</v>
-      </c>
-      <c r="B18" s="42" t="s">
-        <v>166</v>
+      <c r="A18" s="46" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>116</v>
@@ -7209,14 +7222,14 @@
       </c>
     </row>
     <row r="19" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>166</v>
+      <c r="A19" s="46" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F19" s="4">
         <v>0.3</v>
@@ -7229,11 +7242,11 @@
       <c r="AE19" s="19"/>
     </row>
     <row r="20" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>183</v>
+      <c r="A20" s="46" t="s">
+        <v>252</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>180</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>115</v>
@@ -7258,14 +7271,14 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>183</v>
+      <c r="A21" s="46" t="s">
+        <v>254</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>180</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F21" s="4">
         <f>F18-F20</f>
@@ -7299,11 +7312,11 @@
       </c>
     </row>
     <row r="23" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>166</v>
+      <c r="A23" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>52</v>
@@ -7362,11 +7375,11 @@
       </c>
     </row>
     <row r="24" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="B24" s="44" t="s">
-        <v>168</v>
+      <c r="A24" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>108</v>
@@ -7411,11 +7424,11 @@
       </c>
     </row>
     <row r="25" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>168</v>
+      <c r="A25" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>145</v>
@@ -7489,7 +7502,7 @@
     </row>
     <row r="26" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="E26" s="15" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
@@ -7517,14 +7530,14 @@
       </c>
     </row>
     <row r="27" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="46" t="s">
+        <v>256</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="28" t="s">
         <v>174</v>
-      </c>
-      <c r="B27" s="42" t="s">
-        <v>166</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>177</v>
       </c>
       <c r="E27" s="34" t="s">
         <v>68</v>
@@ -7537,15 +7550,15 @@
       </c>
     </row>
     <row r="28" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="B28" s="43" t="s">
-        <v>183</v>
+      <c r="A28" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>180</v>
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F28" s="4">
         <f>F27/F18</f>
@@ -7579,11 +7592,11 @@
       <c r="Y30" s="8"/>
     </row>
     <row r="31" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="B31" s="42" t="s">
-        <v>166</v>
+      <c r="A31" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>164</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>53</v>
@@ -7652,7 +7665,7 @@
     </row>
     <row r="35" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>88</v>
@@ -7704,11 +7717,11 @@
       </c>
     </row>
     <row r="36" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="38" t="s">
-        <v>192</v>
+      <c r="A36" s="47" t="s">
+        <v>186</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>87</v>
@@ -7794,7 +7807,7 @@
       </c>
     </row>
     <row r="37" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="39"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="37"/>
       <c r="E37" s="14" t="s">
         <v>69</v>
@@ -7879,7 +7892,7 @@
       </c>
     </row>
     <row r="38" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="39"/>
+      <c r="A38" s="48"/>
       <c r="B38" s="37"/>
       <c r="E38" s="14" t="s">
         <v>79</v>
@@ -7895,7 +7908,7 @@
         <v>85</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" ref="I38:I39" si="5">IF(H38&gt;=J$11, IF(H37&lt;J$11, J$11-H37, 0),G38)</f>
+        <f>IF(H38&gt;=J$11, IF(H37&lt;J$11, J$11-H37, 0),G38)</f>
         <v>0</v>
       </c>
       <c r="J38" s="4">
@@ -7963,7 +7976,7 @@
       </c>
     </row>
     <row r="39" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="39"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="37"/>
       <c r="E39" s="14" t="s">
         <v>80</v>
@@ -7979,7 +7992,7 @@
         <v>85</v>
       </c>
       <c r="I39" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="I38:I39" si="5">IF(H39&gt;=J$11, IF(H38&lt;J$11, J$11-H38, 0),G39)</f>
         <v>0</v>
       </c>
       <c r="J39" s="4">
@@ -8054,14 +8067,14 @@
       </c>
     </row>
     <row r="41" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="39" t="s">
-        <v>216</v>
+      <c r="A41" s="48" t="s">
+        <v>208</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="G41" s="4">
         <v>0</v>
@@ -8092,10 +8105,10 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="39"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="37"/>
       <c r="E42" s="14" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="G42" s="4">
         <v>0</v>
@@ -8126,10 +8139,10 @@
       </c>
     </row>
     <row r="43" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="39"/>
+      <c r="A43" s="48"/>
       <c r="B43" s="37"/>
       <c r="E43" s="14" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="G43" s="4">
         <v>0</v>
@@ -8160,10 +8173,10 @@
       </c>
     </row>
     <row r="44" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="39"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="37"/>
       <c r="E44" s="14" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="G44" s="4">
         <v>0</v>
@@ -8194,11 +8207,11 @@
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="B45" s="41" t="s">
-        <v>183</v>
+      <c r="A45" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E45" s="14"/>
       <c r="G45" s="4">
@@ -8234,14 +8247,14 @@
       <c r="E46" s="14"/>
     </row>
     <row r="47" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="39" t="s">
-        <v>218</v>
+      <c r="A47" s="48" t="s">
+        <v>210</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="G47" s="4">
         <f>G41*$G$19</f>
@@ -8273,10 +8286,10 @@
       </c>
     </row>
     <row r="48" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
+      <c r="A48" s="48"/>
       <c r="B48" s="37"/>
       <c r="E48" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="G48" s="4">
         <f t="shared" ref="G48:G50" si="6">G42*$G$19</f>
@@ -8308,10 +8321,10 @@
       </c>
     </row>
     <row r="49" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="37"/>
       <c r="E49" s="14" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="G49" s="4">
         <f t="shared" si="6"/>
@@ -8343,10 +8356,10 @@
       </c>
     </row>
     <row r="50" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
+      <c r="A50" s="48"/>
       <c r="B50" s="37"/>
       <c r="E50" s="14" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="G50" s="4">
         <f t="shared" si="6"/>
@@ -8378,11 +8391,11 @@
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A51" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="B51" s="41" t="s">
-        <v>183</v>
+      <c r="A51" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="B51" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E51" s="14"/>
       <c r="G51" s="4">
@@ -8418,11 +8431,11 @@
       <c r="E52" s="14"/>
     </row>
     <row r="53" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="39" t="s">
-        <v>189</v>
+      <c r="A53" s="48" t="s">
+        <v>184</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E53" s="14" t="s">
         <v>90</v>
@@ -8457,7 +8470,7 @@
       </c>
     </row>
     <row r="54" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="39"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="37"/>
       <c r="E54" s="14" t="s">
         <v>91</v>
@@ -8490,7 +8503,7 @@
       </c>
     </row>
     <row r="55" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="39"/>
+      <c r="A55" s="48"/>
       <c r="B55" s="37"/>
       <c r="E55" s="14" t="s">
         <v>92</v>
@@ -8522,7 +8535,7 @@
       </c>
     </row>
     <row r="56" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="39"/>
+      <c r="A56" s="48"/>
       <c r="B56" s="37"/>
       <c r="E56" s="14" t="s">
         <v>93</v>
@@ -8561,11 +8574,11 @@
       <c r="E58" s="14"/>
     </row>
     <row r="59" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="39" t="s">
-        <v>188</v>
+      <c r="A59" s="48" t="s">
+        <v>263</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E59" s="14" t="s">
         <v>109</v>
@@ -8600,7 +8613,7 @@
       </c>
     </row>
     <row r="60" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="39"/>
+      <c r="A60" s="48"/>
       <c r="B60" s="37"/>
       <c r="E60" s="14" t="s">
         <v>110</v>
@@ -8631,7 +8644,7 @@
       </c>
     </row>
     <row r="61" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="39"/>
+      <c r="A61" s="48"/>
       <c r="B61" s="37"/>
       <c r="D61" s="28"/>
       <c r="E61" s="14" t="s">
@@ -8659,7 +8672,7 @@
       </c>
     </row>
     <row r="62" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="39"/>
+      <c r="A62" s="48"/>
       <c r="B62" s="37"/>
       <c r="D62" s="28"/>
       <c r="E62" s="14" t="s">
@@ -8691,11 +8704,11 @@
       <c r="E63" s="14"/>
     </row>
     <row r="64" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="39" t="s">
-        <v>191</v>
+      <c r="A64" s="48" t="s">
+        <v>259</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E64" s="14" t="s">
         <v>128</v>
@@ -8729,7 +8742,7 @@
       </c>
     </row>
     <row r="65" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="39"/>
+      <c r="A65" s="48"/>
       <c r="B65" s="37"/>
       <c r="E65" s="14" t="s">
         <v>129</v>
@@ -8763,7 +8776,7 @@
       </c>
     </row>
     <row r="66" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="39"/>
+      <c r="A66" s="48"/>
       <c r="B66" s="37"/>
       <c r="D66" s="28" t="s">
         <v>153</v>
@@ -8800,7 +8813,7 @@
       </c>
     </row>
     <row r="67" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="39"/>
+      <c r="A67" s="48"/>
       <c r="B67" s="37"/>
       <c r="D67" s="28"/>
       <c r="E67" s="14" t="s">
@@ -8835,11 +8848,11 @@
       </c>
     </row>
     <row r="68" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="B68" s="41" t="s">
-        <v>183</v>
+      <c r="A68" s="46" t="s">
+        <v>260</v>
+      </c>
+      <c r="B68" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="D68" s="28"/>
       <c r="E68" s="14" t="s">
@@ -8887,11 +8900,11 @@
       </c>
     </row>
     <row r="70" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="38" t="s">
-        <v>193</v>
+      <c r="A70" s="47" t="s">
+        <v>261</v>
       </c>
       <c r="B70" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>88</v>
@@ -8922,7 +8935,7 @@
       </c>
     </row>
     <row r="71" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="38"/>
+      <c r="A71" s="47"/>
       <c r="B71" s="37"/>
       <c r="E71" s="14" t="s">
         <v>149</v>
@@ -8985,7 +8998,7 @@
       </c>
     </row>
     <row r="72" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="38"/>
+      <c r="A72" s="47"/>
       <c r="B72" s="37"/>
       <c r="D72" s="22">
         <v>0</v>
@@ -9051,7 +9064,7 @@
       </c>
     </row>
     <row r="73" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="38"/>
+      <c r="A73" s="47"/>
       <c r="B73" s="37"/>
       <c r="D73" s="22">
         <v>1</v>
@@ -9180,9 +9193,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="D75" s="22">
-        <v>3</v>
+    <row r="75" spans="1:30" ht="17" x14ac:dyDescent="0.2">
+      <c r="D75" s="22" t="s">
+        <v>262</v>
       </c>
       <c r="E75" s="14"/>
     </row>
@@ -9208,11 +9221,11 @@
       </c>
     </row>
     <row r="77" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="38" t="s">
-        <v>195</v>
+      <c r="A77" s="47" t="s">
+        <v>188</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E77" s="14" t="s">
         <v>132</v>
@@ -9271,7 +9284,7 @@
       </c>
     </row>
     <row r="78" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="38"/>
+      <c r="A78" s="47"/>
       <c r="B78" s="37"/>
       <c r="E78" s="14" t="s">
         <v>133</v>
@@ -9330,7 +9343,7 @@
       </c>
     </row>
     <row r="79" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="38"/>
+      <c r="A79" s="47"/>
       <c r="B79" s="37"/>
       <c r="E79" s="14" t="s">
         <v>134</v>
@@ -9389,7 +9402,7 @@
       </c>
     </row>
     <row r="80" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="38"/>
+      <c r="A80" s="47"/>
       <c r="B80" s="37"/>
       <c r="E80" s="14" t="s">
         <v>135</v>
@@ -9451,14 +9464,14 @@
       <c r="E81" s="14"/>
     </row>
     <row r="82" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="38" t="s">
-        <v>229</v>
+      <c r="A82" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="B82" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E82" s="14" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="G82" s="4">
         <f>G48*G31</f>
@@ -9490,10 +9503,10 @@
       </c>
     </row>
     <row r="83" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="38"/>
+      <c r="A83" s="47"/>
       <c r="B83" s="37"/>
       <c r="E83" s="14" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="G83" s="4">
         <f>G49*G32</f>
@@ -9525,10 +9538,10 @@
       </c>
     </row>
     <row r="84" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="38"/>
+      <c r="A84" s="47"/>
       <c r="B84" s="37"/>
       <c r="E84" s="14" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G84" s="4">
         <f>G50*G33</f>
@@ -9560,10 +9573,10 @@
       </c>
     </row>
     <row r="85" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="38"/>
+      <c r="A85" s="47"/>
       <c r="B85" s="37"/>
       <c r="E85" s="14" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G85" s="4">
         <f>G51*G34</f>
@@ -9598,11 +9611,11 @@
       <c r="E86" s="14"/>
     </row>
     <row r="87" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="38" t="s">
-        <v>234</v>
+      <c r="A87" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="B87" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E87" s="14" t="s">
         <v>70</v>
@@ -9637,7 +9650,7 @@
       </c>
     </row>
     <row r="88" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="38"/>
+      <c r="A88" s="47"/>
       <c r="B88" s="37"/>
       <c r="E88" s="14" t="s">
         <v>71</v>
@@ -9672,7 +9685,7 @@
       </c>
     </row>
     <row r="89" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="38"/>
+      <c r="A89" s="47"/>
       <c r="B89" s="37"/>
       <c r="E89" s="14" t="s">
         <v>72</v>
@@ -9707,7 +9720,7 @@
       </c>
     </row>
     <row r="90" spans="1:25" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="38"/>
+      <c r="A90" s="47"/>
       <c r="B90" s="37"/>
       <c r="E90" s="14" t="s">
         <v>81</v>
@@ -9746,15 +9759,15 @@
       <c r="E91" s="14"/>
     </row>
     <row r="92" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="38" t="s">
-        <v>235</v>
+      <c r="A92" s="47" t="s">
+        <v>227</v>
       </c>
       <c r="B92" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D92" s="35"/>
       <c r="E92" s="14" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="G92" s="4">
         <f>G58*G41</f>
@@ -9786,11 +9799,11 @@
       </c>
     </row>
     <row r="93" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="38"/>
+      <c r="A93" s="47"/>
       <c r="B93" s="37"/>
       <c r="D93" s="35"/>
       <c r="E93" s="14" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="G93" s="4">
         <f>G59*G42</f>
@@ -9822,11 +9835,11 @@
       </c>
     </row>
     <row r="94" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="38"/>
+      <c r="A94" s="47"/>
       <c r="B94" s="37"/>
       <c r="D94" s="35"/>
       <c r="E94" s="14" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="G94" s="4">
         <f>G60*G43</f>
@@ -9858,11 +9871,11 @@
       </c>
     </row>
     <row r="95" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="38"/>
+      <c r="A95" s="47"/>
       <c r="B95" s="37"/>
       <c r="D95" s="35"/>
       <c r="E95" s="14" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G95" s="4">
         <f>G61*G44</f>
@@ -9894,8 +9907,8 @@
       </c>
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A96" s="40"/>
-      <c r="B96" s="46"/>
+      <c r="A96" s="38"/>
+      <c r="B96" s="45"/>
       <c r="D96" s="35"/>
       <c r="E96" s="14"/>
     </row>
@@ -9911,10 +9924,10 @@
     </row>
     <row r="98" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="33" t="s">
-        <v>199</v>
-      </c>
-      <c r="B98" s="45" t="s">
-        <v>196</v>
+        <v>192</v>
+      </c>
+      <c r="B98" s="44" t="s">
+        <v>189</v>
       </c>
       <c r="D98" s="35"/>
       <c r="E98" s="14" t="s">
@@ -9979,10 +9992,10 @@
     </row>
     <row r="99" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="B99" s="41" t="s">
-        <v>183</v>
+        <v>191</v>
+      </c>
+      <c r="B99" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E99" s="14" t="s">
         <v>142</v>
@@ -10046,13 +10059,13 @@
     </row>
     <row r="100" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="B100" s="41" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="B100" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F100" s="4">
         <v>1</v>
@@ -10111,10 +10124,10 @@
     </row>
     <row r="101" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="B101" s="44" t="s">
-        <v>168</v>
+        <v>193</v>
+      </c>
+      <c r="B101" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E101" s="14" t="s">
         <v>132</v>
@@ -10178,13 +10191,13 @@
     </row>
     <row r="102" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="B102" s="44" t="s">
-        <v>168</v>
+        <v>194</v>
+      </c>
+      <c r="B102" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E102" s="14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F102" s="4">
         <f>F7*F18</f>
@@ -10245,10 +10258,10 @@
     </row>
     <row r="103" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="B103" s="44" t="s">
-        <v>168</v>
+        <v>195</v>
+      </c>
+      <c r="B103" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E103" s="14" t="s">
         <v>143</v>
@@ -10334,13 +10347,13 @@
     </row>
     <row r="106" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="B106" s="45" t="s">
-        <v>196</v>
+        <v>194</v>
+      </c>
+      <c r="B106" s="44" t="s">
+        <v>189</v>
       </c>
       <c r="E106" s="10" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F106" s="4">
         <f>F103*F7</f>
@@ -10401,13 +10414,13 @@
     </row>
     <row r="107" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="B107" s="44" t="s">
-        <v>168</v>
+        <v>196</v>
+      </c>
+      <c r="B107" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="G107" s="4">
         <f>SUM(G87:G90)</f>
@@ -10440,13 +10453,13 @@
     </row>
     <row r="108" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="33" t="s">
-        <v>204</v>
-      </c>
-      <c r="B108" s="44" t="s">
-        <v>168</v>
+        <v>197</v>
+      </c>
+      <c r="B108" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="F108" s="4">
         <f>F106+F107</f>
@@ -10507,13 +10520,13 @@
     </row>
     <row r="109" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="B109" s="44" t="s">
-        <v>168</v>
+        <v>238</v>
+      </c>
+      <c r="B109" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="F109" s="4">
         <f>F102*$F$19</f>
@@ -10574,13 +10587,13 @@
     </row>
     <row r="110" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="B110" s="41" t="s">
-        <v>183</v>
+        <v>187</v>
+      </c>
+      <c r="B110" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E110" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F110" s="4">
         <f>F9*F103</f>
@@ -10641,10 +10654,10 @@
     </row>
     <row r="111" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="B111" s="44" t="s">
-        <v>168</v>
+        <v>179</v>
+      </c>
+      <c r="B111" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E111" s="10" t="s">
         <v>126</v>
@@ -10708,13 +10721,13 @@
     </row>
     <row r="112" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="B112" s="44" t="s">
-        <v>168</v>
+        <v>182</v>
+      </c>
+      <c r="B112" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F112" s="4">
         <f>F110*(1-$F$14)</f>
@@ -10775,13 +10788,13 @@
     </row>
     <row r="113" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="B113" s="44" t="s">
-        <v>168</v>
+        <v>183</v>
+      </c>
+      <c r="B113" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E113" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F113" s="4">
         <f>F110*$F19</f>
@@ -10806,10 +10819,10 @@
     </row>
     <row r="115" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="33" t="s">
-        <v>205</v>
-      </c>
-      <c r="B115" s="41" t="s">
-        <v>183</v>
+        <v>198</v>
+      </c>
+      <c r="B115" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E115" s="10" t="s">
         <v>121</v>
@@ -10892,10 +10905,10 @@
     </row>
     <row r="118" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="B118" s="41" t="s">
-        <v>183</v>
+        <v>199</v>
+      </c>
+      <c r="B118" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E118" s="10" t="s">
         <v>120</v>
@@ -10931,10 +10944,10 @@
     </row>
     <row r="119" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="33" t="s">
-        <v>207</v>
-      </c>
-      <c r="B119" s="41" t="s">
-        <v>183</v>
+        <v>200</v>
+      </c>
+      <c r="B119" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E119" s="10" t="s">
         <v>123</v>
@@ -10970,13 +10983,13 @@
     </row>
     <row r="120" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="B120" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="B120" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="E120" s="10" t="s">
         <v>168</v>
-      </c>
-      <c r="E120" s="10" t="s">
-        <v>170</v>
       </c>
       <c r="F120" s="4">
         <f>MIN(F31,F118)</f>
@@ -11009,10 +11022,10 @@
     </row>
     <row r="121" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="33" t="s">
-        <v>245</v>
-      </c>
-      <c r="B121" s="44" t="s">
-        <v>168</v>
+        <v>237</v>
+      </c>
+      <c r="B121" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E121" s="10" t="s">
         <v>147</v>
@@ -11048,13 +11061,13 @@
     </row>
     <row r="122" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B122" s="44" t="s">
-        <v>168</v>
+        <v>236</v>
+      </c>
+      <c r="B122" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E122" s="10" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F122" s="4">
         <f>F131*F120</f>
@@ -11114,7 +11127,7 @@
       </c>
     </row>
     <row r="123" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B123" s="46"/>
+      <c r="B123" s="45"/>
     </row>
     <row r="124" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="E124" s="15" t="s">
@@ -11137,10 +11150,10 @@
     </row>
     <row r="125" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="B125" s="41" t="s">
-        <v>183</v>
+        <v>195</v>
+      </c>
+      <c r="B125" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E125" s="10" t="s">
         <v>75</v>
@@ -11204,10 +11217,10 @@
     </row>
     <row r="126" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="B126" s="41" t="s">
-        <v>183</v>
+        <v>202</v>
+      </c>
+      <c r="B126" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E126" s="10" t="s">
         <v>138</v>
@@ -11281,13 +11294,13 @@
     </row>
     <row r="127" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="B127" s="41" t="s">
-        <v>183</v>
+        <v>203</v>
+      </c>
+      <c r="B127" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E127" s="10" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F127" s="4">
         <f>MAX(MIN(F126/$F$16, 1), 0)</f>
@@ -11370,10 +11383,10 @@
     </row>
     <row r="129" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="B129" s="41" t="s">
-        <v>183</v>
+        <v>205</v>
+      </c>
+      <c r="B129" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E129" s="10" t="s">
         <v>76</v>
@@ -11447,10 +11460,10 @@
     </row>
     <row r="130" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="B130" s="41" t="s">
-        <v>183</v>
+        <v>206</v>
+      </c>
+      <c r="B130" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E130" s="10" t="s">
         <v>122</v>
@@ -11514,10 +11527,10 @@
     </row>
     <row r="131" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="B131" s="41" t="s">
-        <v>183</v>
+        <v>207</v>
+      </c>
+      <c r="B131" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E131" s="10" t="s">
         <v>119</v>
@@ -11581,20 +11594,20 @@
     </row>
     <row r="133" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="E133" s="15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F133" s="8"/>
       <c r="G133" s="8"/>
     </row>
     <row r="134" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="33" t="s">
-        <v>241</v>
-      </c>
-      <c r="B134" s="44" t="s">
-        <v>168</v>
+        <v>233</v>
+      </c>
+      <c r="B134" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E134" s="10" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F134" s="4">
         <f>(F102 - F122 - F110)*$F$28</f>
@@ -11655,13 +11668,13 @@
     </row>
     <row r="135" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="33" t="s">
-        <v>242</v>
-      </c>
-      <c r="B135" s="44" t="s">
-        <v>168</v>
+        <v>234</v>
+      </c>
+      <c r="B135" s="43" t="s">
+        <v>166</v>
       </c>
       <c r="E135" s="14" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F135" s="4">
         <f>F122*$F19</f>

</xml_diff>

<commit_message>
completed variable transfer and init in carbon ledger.
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0D3A5A-4BFA-A141-BA66-D7C1EA47B56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD0B891-E9E5-5146-80A9-5D06FF780813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6820" yWindow="760" windowWidth="26440" windowHeight="19880" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="284">
   <si>
     <t>forest_primary_c_ha</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>removals allocation</t>
+  </si>
+  <si>
+    <t>removals from original</t>
   </si>
   <si>
     <t>stock to allocate from original pool excluding conversion</t>
@@ -609,9 +612,6 @@
     <t>arr_orig_biomass_c_allocation_excluding_conversion</t>
   </si>
   <si>
-    <t>arr_biomass_c_removed_from_original_unmet</t>
-  </si>
-  <si>
     <t>arr_orig_frac_stock available</t>
   </si>
   <si>
@@ -709,9 +709,6 @@
   </si>
   <si>
     <t>arr_biomass_c_bg_loss_removals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">removals </t>
   </si>
   <si>
     <t>vec_biomass_c_removed_from_young</t>
@@ -883,9 +880,6 @@
     <t>arr_orig_biomass_c_removed_from_forests</t>
   </si>
   <si>
-    <t>vec_total_removals_fulfilled</t>
-  </si>
-  <si>
     <t>total removals met</t>
   </si>
   <si>
@@ -896,6 +890,12 @@
   </si>
   <si>
     <t>allocation of removals</t>
+  </si>
+  <si>
+    <t>vec_biomass_c_removed_from_original_unmet</t>
+  </si>
+  <si>
+    <t>arr_biomass_c_removed_from_forests_excluding_conversion</t>
   </si>
 </sst>
 </file>
@@ -6339,8 +6339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40F0562-A765-A442-B9DB-CF71D123E451}">
   <dimension ref="A1:AM158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6526,16 +6526,16 @@
     </row>
     <row r="5" spans="1:39" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>154</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>153</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>51</v>
@@ -6563,11 +6563,11 @@
       </c>
       <c r="V5" s="29"/>
       <c r="X5" s="29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y5" s="29"/>
       <c r="AB5" s="49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AC5" s="21" t="s">
         <v>33</v>
@@ -6593,7 +6593,7 @@
     </row>
     <row r="6" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="39" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>24</v>
@@ -6662,10 +6662,10 @@
     </row>
     <row r="7" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="46" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>67</v>
@@ -6749,10 +6749,10 @@
     </row>
     <row r="8" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="46" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>114</v>
@@ -6838,10 +6838,10 @@
     </row>
     <row r="9" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>55</v>
@@ -6913,13 +6913,13 @@
     </row>
     <row r="10" spans="1:39" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G10" s="4">
         <f>-MIN(G7-G9,0)</f>
@@ -6962,10 +6962,10 @@
     </row>
     <row r="11" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>113</v>
@@ -7011,10 +7011,10 @@
     </row>
     <row r="12" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>66</v>
@@ -7053,13 +7053,13 @@
     </row>
     <row r="13" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F13" s="4">
         <f>MAX(F7-F9,0)</f>
@@ -7123,10 +7123,10 @@
     </row>
     <row r="14" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>54</v>
@@ -7165,16 +7165,16 @@
     </row>
     <row r="15" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F15" s="4">
         <v>5</v>
@@ -7224,13 +7224,13 @@
     </row>
     <row r="16" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F16" s="4">
         <v>1E-3</v>
@@ -7266,10 +7266,10 @@
     </row>
     <row r="17" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>118</v>
@@ -7293,14 +7293,14 @@
     </row>
     <row r="18" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F18" s="4">
         <v>0.67</v>
@@ -7318,10 +7318,10 @@
     </row>
     <row r="19" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="46" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>116</v>
@@ -7345,13 +7345,13 @@
     </row>
     <row r="20" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F20" s="4">
         <v>0.3</v>
@@ -7365,10 +7365,10 @@
     </row>
     <row r="21" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>115</v>
@@ -7394,13 +7394,13 @@
     </row>
     <row r="22" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="46" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F22" s="4">
         <f>F19-F21</f>
@@ -7435,10 +7435,10 @@
     </row>
     <row r="24" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="46" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>52</v>
@@ -7498,10 +7498,10 @@
     </row>
     <row r="25" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>108</v>
@@ -7547,13 +7547,13 @@
     </row>
     <row r="26" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="46" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F26" s="4">
         <f>MIN(F13,F24)</f>
@@ -7624,7 +7624,7 @@
     </row>
     <row r="27" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="E27" s="15" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -7653,13 +7653,13 @@
     </row>
     <row r="28" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>68</v>
@@ -7673,14 +7673,14 @@
     </row>
     <row r="29" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F29" s="4">
         <f>F28/F19</f>
@@ -7715,10 +7715,10 @@
     </row>
     <row r="32" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="46" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>53</v>
@@ -7766,28 +7766,28 @@
     </row>
     <row r="35" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="E35" s="15" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G35" s="8"/>
       <c r="I35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="N35" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="L35" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="O35" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>88</v>
@@ -7840,10 +7840,10 @@
     </row>
     <row r="37" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="47" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>87</v>
@@ -8193,7 +8193,7 @@
         <v>195</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>199</v>
@@ -8333,7 +8333,7 @@
         <v>196</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E46" s="14"/>
       <c r="G46" s="4">
@@ -8375,16 +8375,16 @@
     </row>
     <row r="48" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G48" s="4">
         <f>MIN(G42,G$15*F37)</f>
@@ -8420,7 +8420,7 @@
       <c r="B49" s="37"/>
       <c r="D49" s="28"/>
       <c r="E49" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G49" s="4">
         <f t="shared" ref="G49" si="6">MIN(G43,G$15*F38)</f>
@@ -8456,7 +8456,7 @@
       <c r="B50" s="37"/>
       <c r="D50" s="28"/>
       <c r="E50" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G50" s="4">
         <f>MIN(G44,G$15*F39)</f>
@@ -8492,7 +8492,7 @@
       <c r="B51" s="37"/>
       <c r="D51" s="28"/>
       <c r="E51" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G51" s="4">
         <f>MIN(G45,G$15*F40)</f>
@@ -8525,10 +8525,10 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" s="46" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E52" s="14"/>
       <c r="G52" s="4">
@@ -8568,7 +8568,7 @@
         <v>197</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E54" s="14" t="s">
         <v>203</v>
@@ -8712,7 +8712,7 @@
         <v>198</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E58" s="14"/>
       <c r="G58" s="4">
@@ -8749,10 +8749,10 @@
     </row>
     <row r="60" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="48" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E60" s="14" t="s">
         <v>90</v>
@@ -8892,10 +8892,10 @@
     </row>
     <row r="66" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E66" s="14" t="s">
         <v>109</v>
@@ -9022,13 +9022,13 @@
     </row>
     <row r="71" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="48" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B71" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G71" s="4">
         <v>0</v>
@@ -9062,7 +9062,7 @@
       <c r="A72" s="48"/>
       <c r="B72" s="37"/>
       <c r="E72" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G72" s="4">
         <v>0</v>
@@ -9096,10 +9096,10 @@
       <c r="A73" s="48"/>
       <c r="B73" s="37"/>
       <c r="D73" s="28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G73" s="4">
         <v>0</v>
@@ -9134,7 +9134,7 @@
       <c r="B74" s="37"/>
       <c r="D74" s="28"/>
       <c r="E74" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G74" s="4">
         <v>0</v>
@@ -9166,14 +9166,14 @@
     </row>
     <row r="75" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D75" s="28"/>
       <c r="E75" s="14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G75" s="4">
         <v>0</v>
@@ -9218,10 +9218,10 @@
     </row>
     <row r="77" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E77" s="14" t="s">
         <v>88</v>
@@ -9255,7 +9255,7 @@
       <c r="A78" s="50"/>
       <c r="B78" s="37"/>
       <c r="E78" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F78" s="4">
         <f>SUM(G$71:G71)</f>
@@ -9321,7 +9321,7 @@
         <v>0</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F79" s="4">
         <f>SUM(G$71:G72)</f>
@@ -9387,7 +9387,7 @@
         <v>1</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F80" s="4">
         <f>SUM(G$71:G73)</f>
@@ -9453,7 +9453,7 @@
         <v>2</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F81" s="4">
         <f>SUM(G$71:G74)</f>
@@ -9521,33 +9521,33 @@
     <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="E83" s="14"/>
       <c r="I83" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L83" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O83" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="R83" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="U83" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="X83" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="47" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B84" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G84" s="4">
         <f>G60</f>
@@ -9606,7 +9606,7 @@
       <c r="A85" s="47"/>
       <c r="B85" s="37"/>
       <c r="E85" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G85" s="4">
         <f>G61</f>
@@ -9665,7 +9665,7 @@
       <c r="A86" s="47"/>
       <c r="B86" s="37"/>
       <c r="E86" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G86" s="4">
         <f>G62</f>
@@ -9724,7 +9724,7 @@
       <c r="A87" s="47"/>
       <c r="B87" s="37"/>
       <c r="E87" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G87" s="4">
         <f>G63</f>
@@ -9787,7 +9787,7 @@
         <v>208</v>
       </c>
       <c r="B89" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E89" s="14" t="s">
         <v>209</v>
@@ -9934,7 +9934,7 @@
         <v>213</v>
       </c>
       <c r="B94" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E94" s="14" t="s">
         <v>70</v>
@@ -10082,7 +10082,7 @@
         <v>214</v>
       </c>
       <c r="B99" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D99" s="35"/>
       <c r="E99" s="14" t="s">
@@ -10240,19 +10240,19 @@
     <row r="105" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="D105" s="35"/>
       <c r="E105" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G105" s="8"/>
     </row>
     <row r="106" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B106" s="44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D106" s="35"/>
       <c r="E106" s="14" t="s">
@@ -10317,13 +10317,13 @@
     </row>
     <row r="107" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B107" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E107" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F107" s="4">
         <f>F7*$F$19</f>
@@ -10384,13 +10384,13 @@
     </row>
     <row r="108" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="46" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E108" s="14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F108" s="4">
         <v>1</v>
@@ -10449,13 +10449,13 @@
     </row>
     <row r="109" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="46" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B109" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E109" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F109" s="4">
         <f>F106</f>
@@ -10516,13 +10516,13 @@
     </row>
     <row r="110" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B110" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E110" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F110" s="4">
         <f>F7*F19</f>
@@ -10583,13 +10583,13 @@
     </row>
     <row r="111" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="46" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B111" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E111" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F111" s="4">
         <f>F110/F7</f>
@@ -10672,13 +10672,13 @@
     </row>
     <row r="114" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B114" s="44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F114" s="4">
         <f>F111*F7</f>
@@ -10739,13 +10739,13 @@
     </row>
     <row r="115" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B115" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E115" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G115" s="4">
         <f>SUM(G94:G97)</f>
@@ -10778,13 +10778,13 @@
     </row>
     <row r="116" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="46" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B116" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E116" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F116" s="4">
         <f>F114+F115</f>
@@ -10845,13 +10845,13 @@
     </row>
     <row r="117" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="46" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B117" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E117" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F117" s="4">
         <f>F110*$F$20</f>
@@ -10912,13 +10912,13 @@
     </row>
     <row r="118" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="46" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B118" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F118" s="4">
         <f>F9*F111</f>
@@ -10979,13 +10979,13 @@
     </row>
     <row r="119" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B119" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E119" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F119" s="4">
         <f>MIN(F118,F9*F15)</f>
@@ -11046,13 +11046,13 @@
     </row>
     <row r="120" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E120" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F120" s="4">
         <f>(F118-F119)*$F$14</f>
@@ -11113,13 +11113,13 @@
     </row>
     <row r="121" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B121" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E121" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F121" s="4">
         <f>MIN(F120+G120, F32)</f>
@@ -11152,13 +11152,13 @@
     </row>
     <row r="122" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B122" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E122" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F122" s="4">
         <f>F120/(F120+G120)</f>
@@ -11219,13 +11219,13 @@
     </row>
     <row r="123" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="46" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E123" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F123" s="4">
         <f>MAX(F13-F26, 0)*F133</f>
@@ -11304,14 +11304,14 @@
       <c r="Y125" s="8"/>
     </row>
     <row r="126" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A126" s="33" t="s">
-        <v>270</v>
+      <c r="A126" s="46" t="s">
+        <v>269</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E126" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F126" s="4">
         <f>MAX(F32-F121,0)</f>
@@ -11343,14 +11343,14 @@
       </c>
     </row>
     <row r="127" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" s="33" t="s">
-        <v>271</v>
+      <c r="A127" s="46" t="s">
+        <v>270</v>
       </c>
       <c r="B127" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E127" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F127" s="4">
         <f>MIN(F138,F126)</f>
@@ -11382,14 +11382,14 @@
       </c>
     </row>
     <row r="128" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="33" t="s">
-        <v>188</v>
+      <c r="A128" s="46" t="s">
+        <v>282</v>
       </c>
       <c r="B128" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E128" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F128" s="4">
         <f>F126-F127</f>
@@ -11421,14 +11421,14 @@
       </c>
     </row>
     <row r="129" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="33" t="s">
-        <v>223</v>
-      </c>
-      <c r="B129" s="43" t="s">
-        <v>164</v>
+      <c r="A129" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="B129" s="40" t="s">
+        <v>176</v>
       </c>
       <c r="E129" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F129" s="4">
         <f>MIN(F128,G75)</f>
@@ -11460,14 +11460,14 @@
       </c>
     </row>
     <row r="130" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="B130" s="43" t="s">
-        <v>164</v>
+      <c r="A130" s="46" t="s">
+        <v>277</v>
+      </c>
+      <c r="B130" s="40" t="s">
+        <v>176</v>
       </c>
       <c r="E130" s="10" t="s">
-        <v>222</v>
+        <v>120</v>
       </c>
       <c r="F130" s="4">
         <f>F139*F127</f>
@@ -11526,12 +11526,71 @@
         <v>1595357.4202249863</v>
       </c>
     </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A131" s="33" t="s">
-        <v>279</v>
+    <row r="131" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="46" t="s">
+        <v>283</v>
       </c>
       <c r="B131" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
+      </c>
+      <c r="E131" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F131" s="4">
+        <f>F130</f>
+        <v>71219.296394549616</v>
+      </c>
+      <c r="G131" s="4">
+        <f>G130+F129</f>
+        <v>1917405.7036054505</v>
+      </c>
+      <c r="I131" s="4">
+        <f>I130</f>
+        <v>73756.795864359185</v>
+      </c>
+      <c r="J131" s="4">
+        <f>J130+I129</f>
+        <v>1963853.343497976</v>
+      </c>
+      <c r="L131" s="4">
+        <f>L130</f>
+        <v>69369.234990881247</v>
+      </c>
+      <c r="M131" s="4">
+        <f>M130+L129</f>
+        <v>2030332.8804317201</v>
+      </c>
+      <c r="O131" s="4">
+        <f>O130</f>
+        <v>65578.525427093409</v>
+      </c>
+      <c r="P131" s="4">
+        <f>P130+O129</f>
+        <v>2129128.4940902959</v>
+      </c>
+      <c r="R131" s="4">
+        <f>R130</f>
+        <v>78897.979298843828</v>
+      </c>
+      <c r="S131" s="4">
+        <f>S130+R129</f>
+        <v>2911285.5647014757</v>
+      </c>
+      <c r="U131" s="4">
+        <f>U130</f>
+        <v>268100.68087206065</v>
+      </c>
+      <c r="V131" s="4">
+        <f>V130+U129</f>
+        <v>11963929.090238368</v>
+      </c>
+      <c r="X131" s="4">
+        <f>X130</f>
+        <v>193790.29082328439</v>
+      </c>
+      <c r="Y131" s="4">
+        <f>Y130+X129</f>
+        <v>1595411.3343486662</v>
       </c>
     </row>
     <row r="132" spans="1:28" ht="17" x14ac:dyDescent="0.2">
@@ -11555,10 +11614,10 @@
     </row>
     <row r="133" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" s="33" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B133" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E133" s="10" t="s">
         <v>75</v>
@@ -11625,10 +11684,10 @@
         <v>189</v>
       </c>
       <c r="B134" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E134" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F134" s="4">
         <f>F133/$F$22</f>
@@ -11702,7 +11761,7 @@
         <v>190</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E135" s="10" t="s">
         <v>191</v>
@@ -11791,7 +11850,7 @@
         <v>192</v>
       </c>
       <c r="B137" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E137" s="10" t="s">
         <v>76</v>
@@ -11868,10 +11927,10 @@
         <v>193</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E138" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F138" s="4">
         <f>F137+G137</f>
@@ -11935,7 +11994,7 @@
         <v>194</v>
       </c>
       <c r="B139" s="40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E139" s="10" t="s">
         <v>119</v>
@@ -11999,7 +12058,7 @@
     </row>
     <row r="141" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="E141" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
@@ -12021,7 +12080,7 @@
         <v>220</v>
       </c>
       <c r="B142" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E142" s="10" t="s">
         <v>207</v>
@@ -12088,7 +12147,7 @@
         <v>221</v>
       </c>
       <c r="B143" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E143" s="14" t="s">
         <v>219</v>
@@ -12152,13 +12211,13 @@
     </row>
     <row r="144" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="46" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B144" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E144" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F144" s="4">
         <f>F118-F121*F122-F119</f>
@@ -12219,13 +12278,13 @@
     </row>
     <row r="145" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B145" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E145" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F145" s="4">
         <f>F118*$F20</f>
@@ -12286,7 +12345,7 @@
     </row>
     <row r="148" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A148" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F148" s="4">
         <f>F144+F119</f>
@@ -12347,10 +12406,10 @@
     </row>
     <row r="150" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A150" s="33" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F150" s="4">
-        <f>F121+F130+G130</f>
+        <f>F121+F130+G130+F129</f>
         <v>2000000</v>
       </c>
       <c r="I150" s="4">

</xml_diff>

<commit_message>
working on update function in ledger
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD0B891-E9E5-5146-80A9-5D06FF780813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871C3B71-9414-D04A-8BCB-63E748650B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="760" windowWidth="26440" windowHeight="19880" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
+    <workbookView xWindow="10020" yWindow="500" windowWidth="33680" windowHeight="19400" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="284">
   <si>
     <t>forest_primary_c_ha</t>
   </si>
@@ -606,15 +606,9 @@
     <t>arr_orig_sf_adjusted</t>
   </si>
   <si>
-    <t>arr_orig_biomass_average_per_area</t>
-  </si>
-  <si>
     <t>arr_orig_biomass_c_allocation_excluding_conversion</t>
   </si>
   <si>
-    <t>arr_orig_frac_stock available</t>
-  </si>
-  <si>
     <t>arr_orig_frac_removables_satisfiable</t>
   </si>
   <si>
@@ -705,12 +699,6 @@
     <t>bg biomass loss from stock removals</t>
   </si>
   <si>
-    <t>arr_biomass_c_ag_loss_decomposition</t>
-  </si>
-  <si>
-    <t>arr_biomass_c_bg_loss_removals</t>
-  </si>
-  <si>
     <t>vec_biomass_c_removed_from_young</t>
   </si>
   <si>
@@ -760,9 +748,6 @@
   </si>
   <si>
     <t>vec_biomass_c_bg_to_ag_ratio</t>
-  </si>
-  <si>
-    <t>vec_annual_sf_nominal</t>
   </si>
   <si>
     <t>vec_frac_biomass_ag_decomposition</t>
@@ -880,9 +865,6 @@
     <t>arr_orig_biomass_c_removed_from_forests</t>
   </si>
   <si>
-    <t>total removals met</t>
-  </si>
-  <si>
     <t>orig c converted</t>
   </si>
   <si>
@@ -896,6 +878,24 @@
   </si>
   <si>
     <t>arr_biomass_c_removed_from_forests_excluding_conversion</t>
+  </si>
+  <si>
+    <t>arr_biomass_c_ag_lost_decomposition</t>
+  </si>
+  <si>
+    <t>arr_biomass_c_bg_lost_removals</t>
+  </si>
+  <si>
+    <t>arr_orig_frac_stock_available</t>
+  </si>
+  <si>
+    <t>arr_orig_biomass_c_average_per_area_no_ds</t>
+  </si>
+  <si>
+    <t>vec_total_removals_met</t>
+  </si>
+  <si>
+    <t>vec_sf_nominal_initial</t>
   </si>
 </sst>
 </file>
@@ -6339,8 +6339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40F0562-A765-A442-B9DB-CF71D123E451}">
   <dimension ref="A1:AM158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6567,7 +6567,7 @@
       </c>
       <c r="Y5" s="29"/>
       <c r="AB5" s="49" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="AC5" s="21" t="s">
         <v>33</v>
@@ -6838,7 +6838,7 @@
     </row>
     <row r="9" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B9" s="41" t="s">
         <v>163</v>
@@ -6913,7 +6913,7 @@
     </row>
     <row r="10" spans="1:39" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B10" s="40" t="s">
         <v>176</v>
@@ -6962,7 +6962,7 @@
     </row>
     <row r="11" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="46" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>176</v>
@@ -7011,7 +7011,7 @@
     </row>
     <row r="12" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B12" s="41" t="s">
         <v>163</v>
@@ -7123,7 +7123,7 @@
     </row>
     <row r="14" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="46" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B14" s="41" t="s">
         <v>163</v>
@@ -7165,16 +7165,16 @@
     </row>
     <row r="15" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="46" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B15" s="41" t="s">
         <v>163</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F15" s="4">
         <v>5</v>
@@ -7224,13 +7224,13 @@
     </row>
     <row r="16" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="46" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B16" s="41" t="s">
         <v>163</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F16" s="4">
         <v>1E-3</v>
@@ -7266,7 +7266,7 @@
     </row>
     <row r="17" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="46" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B17" s="41" t="s">
         <v>163</v>
@@ -7293,7 +7293,7 @@
     </row>
     <row r="18" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="46" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B18" s="41" t="s">
         <v>163</v>
@@ -7318,7 +7318,7 @@
     </row>
     <row r="19" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="46" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B19" s="41" t="s">
         <v>163</v>
@@ -7345,7 +7345,7 @@
     </row>
     <row r="20" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="46" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B20" s="41" t="s">
         <v>163</v>
@@ -7365,7 +7365,7 @@
     </row>
     <row r="21" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="46" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B21" s="42" t="s">
         <v>176</v>
@@ -7394,7 +7394,7 @@
     </row>
     <row r="22" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="46" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>176</v>
@@ -7653,7 +7653,7 @@
     </row>
     <row r="28" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="46" t="s">
-        <v>239</v>
+        <v>283</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>163</v>
@@ -7673,7 +7673,7 @@
     </row>
     <row r="29" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="46" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B29" s="42" t="s">
         <v>176</v>
@@ -8190,13 +8190,13 @@
     </row>
     <row r="42" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B42" s="37" t="s">
         <v>176</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G42" s="4">
         <v>0</v>
@@ -8230,7 +8230,7 @@
       <c r="A43" s="48"/>
       <c r="B43" s="37"/>
       <c r="E43" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G43" s="4">
         <v>0</v>
@@ -8264,7 +8264,7 @@
       <c r="A44" s="48"/>
       <c r="B44" s="37"/>
       <c r="E44" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G44" s="4">
         <v>0</v>
@@ -8298,7 +8298,7 @@
       <c r="A45" s="48"/>
       <c r="B45" s="37"/>
       <c r="E45" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G45" s="4">
         <v>0</v>
@@ -8330,7 +8330,7 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B46" s="40" t="s">
         <v>176</v>
@@ -8375,16 +8375,16 @@
     </row>
     <row r="48" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="48" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B48" s="37" t="s">
         <v>176</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="G48" s="4">
         <f>MIN(G42,G$15*F37)</f>
@@ -8420,7 +8420,7 @@
       <c r="B49" s="37"/>
       <c r="D49" s="28"/>
       <c r="E49" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="G49" s="4">
         <f t="shared" ref="G49" si="6">MIN(G43,G$15*F38)</f>
@@ -8456,7 +8456,7 @@
       <c r="B50" s="37"/>
       <c r="D50" s="28"/>
       <c r="E50" s="14" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G50" s="4">
         <f>MIN(G44,G$15*F39)</f>
@@ -8492,7 +8492,7 @@
       <c r="B51" s="37"/>
       <c r="D51" s="28"/>
       <c r="E51" s="14" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="G51" s="4">
         <f>MIN(G45,G$15*F40)</f>
@@ -8525,7 +8525,7 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" s="46" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>176</v>
@@ -8565,13 +8565,13 @@
     </row>
     <row r="54" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="48" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B54" s="37" t="s">
         <v>176</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G54" s="4">
         <f>G42*$G$20</f>
@@ -8606,7 +8606,7 @@
       <c r="A55" s="48"/>
       <c r="B55" s="37"/>
       <c r="E55" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G55" s="4">
         <f t="shared" ref="G55:G57" si="13">G43*$G$20</f>
@@ -8641,7 +8641,7 @@
       <c r="A56" s="48"/>
       <c r="B56" s="37"/>
       <c r="E56" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G56" s="4">
         <f t="shared" si="13"/>
@@ -8676,7 +8676,7 @@
       <c r="A57" s="48"/>
       <c r="B57" s="37"/>
       <c r="E57" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G57" s="4">
         <f t="shared" si="13"/>
@@ -8709,7 +8709,7 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" s="46" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B58" s="40" t="s">
         <v>176</v>
@@ -8892,7 +8892,7 @@
     </row>
     <row r="66" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="48" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B66" s="37" t="s">
         <v>176</v>
@@ -9022,7 +9022,7 @@
     </row>
     <row r="71" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="48" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B71" s="37" t="s">
         <v>176</v>
@@ -9166,7 +9166,7 @@
     </row>
     <row r="75" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="46" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B75" s="40" t="s">
         <v>176</v>
@@ -9218,7 +9218,7 @@
     </row>
     <row r="77" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="50" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B77" s="37" t="s">
         <v>176</v>
@@ -9784,13 +9784,13 @@
     </row>
     <row r="89" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="47" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B89" s="37" t="s">
         <v>176</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G89" s="4">
         <f>G55*G32</f>
@@ -9825,7 +9825,7 @@
       <c r="A90" s="47"/>
       <c r="B90" s="37"/>
       <c r="E90" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G90" s="4">
         <f>G56*G33</f>
@@ -9860,7 +9860,7 @@
       <c r="A91" s="47"/>
       <c r="B91" s="37"/>
       <c r="E91" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G91" s="4">
         <f>G57*G34</f>
@@ -9895,7 +9895,7 @@
       <c r="A92" s="47"/>
       <c r="B92" s="37"/>
       <c r="E92" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G92" s="4">
         <f>G58*G35</f>
@@ -9931,7 +9931,7 @@
     </row>
     <row r="94" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B94" s="37" t="s">
         <v>176</v>
@@ -10079,14 +10079,14 @@
     </row>
     <row r="99" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B99" s="37" t="s">
         <v>176</v>
       </c>
       <c r="D99" s="35"/>
       <c r="E99" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G99" s="4">
         <f>G94*$G$20</f>
@@ -10122,7 +10122,7 @@
       <c r="B100" s="37"/>
       <c r="D100" s="35"/>
       <c r="E100" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G100" s="4">
         <f t="shared" ref="G100:G102" si="26">G95*$G$20</f>
@@ -10158,7 +10158,7 @@
       <c r="B101" s="37"/>
       <c r="D101" s="35"/>
       <c r="E101" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G101" s="4">
         <f>G96*$G$20</f>
@@ -10194,7 +10194,7 @@
       <c r="B102" s="37"/>
       <c r="D102" s="35"/>
       <c r="E102" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G102" s="4">
         <f t="shared" si="26"/>
@@ -10249,7 +10249,7 @@
     </row>
     <row r="106" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="46" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B106" s="44" t="s">
         <v>184</v>
@@ -10317,7 +10317,7 @@
     </row>
     <row r="107" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="46" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B107" s="40" t="s">
         <v>176</v>
@@ -10516,7 +10516,7 @@
     </row>
     <row r="110" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="46" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B110" s="43" t="s">
         <v>165</v>
@@ -10583,7 +10583,7 @@
     </row>
     <row r="111" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="46" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B111" s="43" t="s">
         <v>165</v>
@@ -10672,13 +10672,13 @@
     </row>
     <row r="114" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="46" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B114" s="44" t="s">
         <v>184</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F114" s="4">
         <f>F111*F7</f>
@@ -10739,13 +10739,13 @@
     </row>
     <row r="115" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="46" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B115" s="43" t="s">
         <v>165</v>
       </c>
       <c r="E115" s="10" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G115" s="4">
         <f>SUM(G94:G97)</f>
@@ -10778,13 +10778,13 @@
     </row>
     <row r="116" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="46" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B116" s="43" t="s">
         <v>165</v>
       </c>
       <c r="E116" s="10" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F116" s="4">
         <f>F114+F115</f>
@@ -10845,13 +10845,13 @@
     </row>
     <row r="117" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="46" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B117" s="43" t="s">
         <v>165</v>
       </c>
       <c r="E117" s="10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F117" s="4">
         <f>F110*$F$20</f>
@@ -10912,13 +10912,13 @@
     </row>
     <row r="118" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="46" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B118" s="40" t="s">
         <v>176</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F118" s="4">
         <f>F9*F111</f>
@@ -10979,13 +10979,13 @@
     </row>
     <row r="119" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="46" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B119" s="40" t="s">
         <v>176</v>
       </c>
       <c r="E119" s="10" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F119" s="4">
         <f>MIN(F118,F9*F15)</f>
@@ -11046,13 +11046,13 @@
     </row>
     <row r="120" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="46" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B120" s="40" t="s">
         <v>176</v>
       </c>
       <c r="E120" s="10" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F120" s="4">
         <f>(F118-F119)*$F$14</f>
@@ -11113,13 +11113,13 @@
     </row>
     <row r="121" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="46" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B121" s="43" t="s">
         <v>165</v>
       </c>
       <c r="E121" s="14" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="F121" s="4">
         <f>MIN(F120+G120, F32)</f>
@@ -11152,13 +11152,13 @@
     </row>
     <row r="122" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="46" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B122" s="40" t="s">
         <v>176</v>
       </c>
       <c r="E122" s="14" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F122" s="4">
         <f>F120/(F120+G120)</f>
@@ -11219,7 +11219,7 @@
     </row>
     <row r="123" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="46" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B123" s="40" t="s">
         <v>176</v>
@@ -11305,13 +11305,13 @@
     </row>
     <row r="126" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="46" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B126" s="40" t="s">
         <v>176</v>
       </c>
       <c r="E126" s="14" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F126" s="4">
         <f>MAX(F32-F121,0)</f>
@@ -11344,7 +11344,7 @@
     </row>
     <row r="127" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="46" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B127" s="40" t="s">
         <v>176</v>
@@ -11383,7 +11383,7 @@
     </row>
     <row r="128" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="46" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B128" s="40" t="s">
         <v>176</v>
@@ -11422,7 +11422,7 @@
     </row>
     <row r="129" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="46" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B129" s="40" t="s">
         <v>176</v>
@@ -11461,7 +11461,7 @@
     </row>
     <row r="130" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="46" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B130" s="40" t="s">
         <v>176</v>
@@ -11528,7 +11528,7 @@
     </row>
     <row r="131" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="46" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B131" s="43" t="s">
         <v>165</v>
@@ -11613,8 +11613,8 @@
       <c r="Y132" s="8"/>
     </row>
     <row r="133" spans="1:28" ht="34" x14ac:dyDescent="0.2">
-      <c r="A133" s="33" t="s">
-        <v>187</v>
+      <c r="A133" s="46" t="s">
+        <v>281</v>
       </c>
       <c r="B133" s="40" t="s">
         <v>176</v>
@@ -11680,8 +11680,8 @@
       </c>
     </row>
     <row r="134" spans="1:28" ht="34" x14ac:dyDescent="0.2">
-      <c r="A134" s="33" t="s">
-        <v>189</v>
+      <c r="A134" s="46" t="s">
+        <v>280</v>
       </c>
       <c r="B134" s="40" t="s">
         <v>176</v>
@@ -11757,14 +11757,14 @@
       </c>
     </row>
     <row r="135" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A135" s="33" t="s">
-        <v>190</v>
+      <c r="A135" s="46" t="s">
+        <v>188</v>
       </c>
       <c r="B135" s="40" t="s">
         <v>176</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F135" s="4">
         <f>MAX(MIN(F134/$F$17, 1), 0)</f>
@@ -11834,6 +11834,7 @@
       </c>
     </row>
     <row r="136" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A136" s="46"/>
       <c r="Z136">
         <v>0.2</v>
       </c>
@@ -11846,8 +11847,8 @@
       </c>
     </row>
     <row r="137" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="33" t="s">
-        <v>192</v>
+      <c r="A137" s="46" t="s">
+        <v>190</v>
       </c>
       <c r="B137" s="40" t="s">
         <v>176</v>
@@ -11923,8 +11924,8 @@
       </c>
     </row>
     <row r="138" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A138" s="33" t="s">
-        <v>193</v>
+      <c r="A138" s="46" t="s">
+        <v>191</v>
       </c>
       <c r="B138" s="40" t="s">
         <v>176</v>
@@ -11990,8 +11991,8 @@
       </c>
     </row>
     <row r="139" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A139" s="33" t="s">
-        <v>194</v>
+      <c r="A139" s="46" t="s">
+        <v>192</v>
       </c>
       <c r="B139" s="40" t="s">
         <v>176</v>
@@ -12058,7 +12059,7 @@
     </row>
     <row r="141" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="E141" s="15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
@@ -12076,14 +12077,14 @@
       <c r="Y141" s="8"/>
     </row>
     <row r="142" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" s="33" t="s">
-        <v>220</v>
+      <c r="A142" s="46" t="s">
+        <v>278</v>
       </c>
       <c r="B142" s="43" t="s">
         <v>165</v>
       </c>
       <c r="E142" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F142" s="4">
         <f>(F110 - F130 - F118)*$F$29</f>
@@ -12143,14 +12144,14 @@
       </c>
     </row>
     <row r="143" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" s="33" t="s">
-        <v>221</v>
+      <c r="A143" s="46" t="s">
+        <v>279</v>
       </c>
       <c r="B143" s="43" t="s">
         <v>165</v>
       </c>
       <c r="E143" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F143" s="4">
         <f>F130*$F20</f>
@@ -12345,7 +12346,7 @@
     </row>
     <row r="148" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A148" s="33" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F148" s="4">
         <f>F144+F119</f>
@@ -12405,8 +12406,11 @@
       </c>
     </row>
     <row r="150" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A150" s="33" t="s">
-        <v>278</v>
+      <c r="A150" s="46" t="s">
+        <v>282</v>
+      </c>
+      <c r="B150" s="43" t="s">
+        <v>165</v>
       </c>
       <c r="F150" s="4">
         <f>F121+F130+G130+F129</f>

</xml_diff>

<commit_message>
updated carbon ledger, intermediate update
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871C3B71-9414-D04A-8BCB-63E748650B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE6D6BB-3EDE-CB43-8A49-46D25A5A8C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="500" windowWidth="33680" windowHeight="19400" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
+    <workbookView xWindow="7100" yWindow="760" windowWidth="26440" windowHeight="19880" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,9 +522,6 @@
     <t>arr_area_protected_total</t>
   </si>
   <si>
-    <t>arr_area_protected_young</t>
-  </si>
-  <si>
     <t>arr_area_protected_original</t>
   </si>
   <si>
@@ -796,9 +793,6 @@
     <t>arr_biomass_c_ag_converted_away</t>
   </si>
   <si>
-    <t>arr_biomass_c_ag_min_reqd_per_area</t>
-  </si>
-  <si>
     <t>average stock in target land use classes</t>
   </si>
   <si>
@@ -896,6 +890,12 @@
   </si>
   <si>
     <t>vec_sf_nominal_initial</t>
+  </si>
+  <si>
+    <t>vec_area_protected_young</t>
+  </si>
+  <si>
+    <t>vec_biomass_c_ag_min_reqd_per_area</t>
   </si>
 </sst>
 </file>
@@ -6339,8 +6339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40F0562-A765-A442-B9DB-CF71D123E451}">
   <dimension ref="A1:AM158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6529,7 +6529,7 @@
         <v>155</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>153</v>
@@ -6567,7 +6567,7 @@
       </c>
       <c r="Y5" s="29"/>
       <c r="AB5" s="49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AC5" s="21" t="s">
         <v>33</v>
@@ -6593,7 +6593,7 @@
     </row>
     <row r="6" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>24</v>
@@ -6665,7 +6665,7 @@
         <v>156</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>67</v>
@@ -6752,7 +6752,7 @@
         <v>157</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>114</v>
@@ -6838,10 +6838,10 @@
     </row>
     <row r="9" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>55</v>
@@ -6913,10 +6913,10 @@
     </row>
     <row r="10" spans="1:39" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>145</v>
@@ -6962,10 +6962,10 @@
     </row>
     <row r="11" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>113</v>
@@ -7011,10 +7011,10 @@
     </row>
     <row r="12" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>66</v>
@@ -7056,7 +7056,7 @@
         <v>158</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>143</v>
@@ -7123,10 +7123,10 @@
     </row>
     <row r="14" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>54</v>
@@ -7165,16 +7165,16 @@
     </row>
     <row r="15" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="46" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F15" s="4">
         <v>5</v>
@@ -7224,13 +7224,13 @@
     </row>
     <row r="16" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F16" s="4">
         <v>1E-3</v>
@@ -7266,10 +7266,10 @@
     </row>
     <row r="17" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>118</v>
@@ -7293,10 +7293,10 @@
     </row>
     <row r="18" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="10" t="s">
@@ -7318,10 +7318,10 @@
     </row>
     <row r="19" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>116</v>
@@ -7345,13 +7345,13 @@
     </row>
     <row r="20" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F20" s="4">
         <v>0.3</v>
@@ -7365,10 +7365,10 @@
     </row>
     <row r="21" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="46" t="s">
-        <v>250</v>
+        <v>283</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>115</v>
@@ -7394,13 +7394,13 @@
     </row>
     <row r="22" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B22" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>177</v>
       </c>
       <c r="F22" s="4">
         <f>F19-F21</f>
@@ -7438,7 +7438,7 @@
         <v>159</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>52</v>
@@ -7498,10 +7498,10 @@
     </row>
     <row r="25" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="46" t="s">
-        <v>160</v>
+        <v>282</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>108</v>
@@ -7547,10 +7547,10 @@
     </row>
     <row r="26" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>144</v>
@@ -7560,7 +7560,7 @@
         <v>5000</v>
       </c>
       <c r="G26" s="4">
-        <f>MIN(G13,G24)-G25</f>
+        <f>MIN(G13,G24)</f>
         <v>50000</v>
       </c>
       <c r="I26" s="4">
@@ -7568,7 +7568,7 @@
         <v>5000</v>
       </c>
       <c r="J26" s="4">
-        <f>MIN(J13,J24)-J25</f>
+        <f>MIN(J13,J24)</f>
         <v>50000</v>
       </c>
       <c r="L26" s="4">
@@ -7576,7 +7576,7 @@
         <v>5500</v>
       </c>
       <c r="M26" s="4">
-        <f>MIN(M13,M24)-M25</f>
+        <f>MIN(M13,M24)</f>
         <v>50000</v>
       </c>
       <c r="O26" s="4">
@@ -7584,7 +7584,7 @@
         <v>6000</v>
       </c>
       <c r="P26" s="4">
-        <f>MIN(P13,P24)-P25</f>
+        <f>MIN(P13,P24)</f>
         <v>50000</v>
       </c>
       <c r="R26" s="4">
@@ -7592,7 +7592,7 @@
         <v>6500</v>
       </c>
       <c r="S26" s="4">
-        <f>MIN(S13,S24)-S25</f>
+        <f>MIN(S13,S24)</f>
         <v>49000</v>
       </c>
       <c r="U26" s="4">
@@ -7600,7 +7600,7 @@
         <v>7200</v>
       </c>
       <c r="V26" s="4">
-        <f>MIN(V13,V24)-V25</f>
+        <f>MIN(V13,V24)</f>
         <v>49500</v>
       </c>
       <c r="X26" s="4">
@@ -7608,7 +7608,7 @@
         <v>7200</v>
       </c>
       <c r="Y26" s="4">
-        <f>MIN(Y13,Y24)-Y25</f>
+        <f>MIN(Y13,Y24)</f>
         <v>49500</v>
       </c>
       <c r="AC26" s="19">
@@ -7624,7 +7624,7 @@
     </row>
     <row r="27" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="E27" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -7653,13 +7653,13 @@
     </row>
     <row r="28" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="46" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>68</v>
@@ -7673,14 +7673,14 @@
     </row>
     <row r="29" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F29" s="4">
         <f>F28/F19</f>
@@ -7715,10 +7715,10 @@
     </row>
     <row r="32" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>53</v>
@@ -7787,7 +7787,7 @@
     </row>
     <row r="36" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>88</v>
@@ -7840,10 +7840,10 @@
     </row>
     <row r="37" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>87</v>
@@ -7957,7 +7957,7 @@
         <v>165</v>
       </c>
       <c r="L38" s="4">
-        <f t="shared" ref="L38:L40" si="0">IF(K38&gt;=M$11, IF(K37&lt;M$11, M$11-K37, 0),J38)</f>
+        <f>IF(K38&gt;=M$11, IF(K37&lt;M$11, M$11-K37, 0),J38)</f>
         <v>0</v>
       </c>
       <c r="M38" s="4">
@@ -7969,7 +7969,7 @@
         <v>165</v>
       </c>
       <c r="O38" s="4">
-        <f t="shared" ref="O38:O40" si="1">IF(N38&gt;=P$11, IF(N37&lt;P$11, P$11-N37, 0),M38)</f>
+        <f t="shared" ref="O38:O40" si="0">IF(N38&gt;=P$11, IF(N37&lt;P$11, P$11-N37, 0),M38)</f>
         <v>0</v>
       </c>
       <c r="P38" s="4">
@@ -7981,7 +7981,7 @@
         <v>165</v>
       </c>
       <c r="R38" s="4">
-        <f t="shared" ref="R38:R40" si="2">IF(Q38&gt;=S$11, IF(Q37&lt;S$11, S$11-Q37, 0),P38)</f>
+        <f t="shared" ref="R38:R40" si="1">IF(Q38&gt;=S$11, IF(Q37&lt;S$11, S$11-Q37, 0),P38)</f>
         <v>0</v>
       </c>
       <c r="S38" s="4">
@@ -7993,7 +7993,7 @@
         <v>165</v>
       </c>
       <c r="U38" s="4">
-        <f t="shared" ref="U38:U40" si="3">IF(T38&gt;=V$11, IF(T37&lt;V$11, V$11-T37, 0),S38)</f>
+        <f t="shared" ref="U38:U40" si="2">IF(T38&gt;=V$11, IF(T37&lt;V$11, V$11-T37, 0),S38)</f>
         <v>0</v>
       </c>
       <c r="V38" s="4">
@@ -8005,7 +8005,7 @@
         <v>165</v>
       </c>
       <c r="X38" s="4">
-        <f t="shared" ref="X38:X40" si="4">IF(W38&gt;=Y$11, IF(W37&lt;Y$11, Y$11-W37, 0),V38)</f>
+        <f t="shared" ref="X38:X40" si="3">IF(W38&gt;=Y$11, IF(W37&lt;Y$11, Y$11-W37, 0),V38)</f>
         <v>0</v>
       </c>
       <c r="Y38" s="4">
@@ -8041,7 +8041,7 @@
         <v>165</v>
       </c>
       <c r="L39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L38:L40" si="4">IF(K39&gt;=M$11, IF(K38&lt;M$11, M$11-K38, 0),J39)</f>
         <v>0</v>
       </c>
       <c r="M39" s="4">
@@ -8053,7 +8053,7 @@
         <v>257</v>
       </c>
       <c r="O39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P39" s="4">
@@ -8065,7 +8065,7 @@
         <v>257</v>
       </c>
       <c r="R39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S39" s="4">
@@ -8077,7 +8077,7 @@
         <v>257</v>
       </c>
       <c r="U39" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V39" s="4">
@@ -8089,7 +8089,7 @@
         <v>257</v>
       </c>
       <c r="X39" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y39" s="4">
@@ -8114,7 +8114,7 @@
         <v>85</v>
       </c>
       <c r="I40" s="4">
-        <f t="shared" ref="I40" si="5">IF(H40&gt;=J$11, IF(H39&lt;J$11, J$11-H39, 0),G40)</f>
+        <f>IF(H40&gt;=J$11, IF(H39&lt;J$11, J$11-H39, 0),G40)</f>
         <v>0</v>
       </c>
       <c r="J40" s="4">
@@ -8125,7 +8125,7 @@
         <v>165</v>
       </c>
       <c r="L40" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M40" s="4">
@@ -8136,7 +8136,7 @@
         <v>257</v>
       </c>
       <c r="O40" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P40" s="4">
@@ -8148,7 +8148,7 @@
         <v>300</v>
       </c>
       <c r="R40" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S40" s="4">
@@ -8160,7 +8160,7 @@
         <v>300</v>
       </c>
       <c r="U40" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V40" s="4">
@@ -8172,7 +8172,7 @@
         <v>300</v>
       </c>
       <c r="X40" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y40" s="4">
@@ -8190,13 +8190,13 @@
     </row>
     <row r="42" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G42" s="4">
         <v>0</v>
@@ -8230,7 +8230,7 @@
       <c r="A43" s="48"/>
       <c r="B43" s="37"/>
       <c r="E43" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G43" s="4">
         <v>0</v>
@@ -8264,7 +8264,7 @@
       <c r="A44" s="48"/>
       <c r="B44" s="37"/>
       <c r="E44" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G44" s="4">
         <v>0</v>
@@ -8298,7 +8298,7 @@
       <c r="A45" s="48"/>
       <c r="B45" s="37"/>
       <c r="E45" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G45" s="4">
         <v>0</v>
@@ -8330,10 +8330,10 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E46" s="14"/>
       <c r="G46" s="4">
@@ -8375,16 +8375,16 @@
     </row>
     <row r="48" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="48" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G48" s="4">
         <f>MIN(G42,G$15*F37)</f>
@@ -8420,34 +8420,34 @@
       <c r="B49" s="37"/>
       <c r="D49" s="28"/>
       <c r="E49" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G49" s="4">
-        <f t="shared" ref="G49" si="6">MIN(G43,G$15*F38)</f>
+        <f t="shared" ref="G49" si="5">MIN(G43,G$15*F38)</f>
         <v>0</v>
       </c>
       <c r="J49" s="4">
-        <f t="shared" ref="J49" si="7">MIN(J43,J$15*I38)</f>
+        <f>MIN(J43,J$15*I38)</f>
         <v>0</v>
       </c>
       <c r="M49" s="4">
-        <f t="shared" ref="M49" si="8">MIN(M43,M$15*L38)</f>
+        <f t="shared" ref="M49" si="6">MIN(M43,M$15*L38)</f>
         <v>0</v>
       </c>
       <c r="P49" s="4">
-        <f t="shared" ref="P49" si="9">MIN(P43,P$15*O38)</f>
+        <f t="shared" ref="P49" si="7">MIN(P43,P$15*O38)</f>
         <v>0</v>
       </c>
       <c r="S49" s="4">
-        <f t="shared" ref="S49" si="10">MIN(S43,S$15*R38)</f>
+        <f t="shared" ref="S49" si="8">MIN(S43,S$15*R38)</f>
         <v>0</v>
       </c>
       <c r="V49" s="4">
-        <f t="shared" ref="V49" si="11">MIN(V43,V$15*U38)</f>
+        <f t="shared" ref="V49" si="9">MIN(V43,V$15*U38)</f>
         <v>0</v>
       </c>
       <c r="Y49" s="4">
-        <f t="shared" ref="Y49" si="12">MIN(Y43,Y$15*X38)</f>
+        <f t="shared" ref="Y49" si="10">MIN(Y43,Y$15*X38)</f>
         <v>0</v>
       </c>
     </row>
@@ -8456,7 +8456,7 @@
       <c r="B50" s="37"/>
       <c r="D50" s="28"/>
       <c r="E50" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G50" s="4">
         <f>MIN(G44,G$15*F39)</f>
@@ -8492,7 +8492,7 @@
       <c r="B51" s="37"/>
       <c r="D51" s="28"/>
       <c r="E51" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G51" s="4">
         <f>MIN(G45,G$15*F40)</f>
@@ -8525,10 +8525,10 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" s="46" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E52" s="14"/>
       <c r="G52" s="4">
@@ -8565,13 +8565,13 @@
     </row>
     <row r="54" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="48" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G54" s="4">
         <f>G42*$G$20</f>
@@ -8606,34 +8606,34 @@
       <c r="A55" s="48"/>
       <c r="B55" s="37"/>
       <c r="E55" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G55" s="4">
-        <f t="shared" ref="G55:G57" si="13">G43*$G$20</f>
+        <f t="shared" ref="G55:G57" si="11">G43*$G$20</f>
         <v>0</v>
       </c>
       <c r="J55" s="4">
-        <f t="shared" ref="J55:J57" si="14">J43*$G$20</f>
+        <f t="shared" ref="J55:J57" si="12">J43*$G$20</f>
         <v>0</v>
       </c>
       <c r="M55" s="4">
-        <f t="shared" ref="M55:M57" si="15">M43*$G$20</f>
+        <f t="shared" ref="M55:M57" si="13">M43*$G$20</f>
         <v>0</v>
       </c>
       <c r="P55" s="4">
-        <f t="shared" ref="P55:P57" si="16">P43*$G$20</f>
+        <f t="shared" ref="P55:P57" si="14">P43*$G$20</f>
         <v>0</v>
       </c>
       <c r="S55" s="4">
-        <f t="shared" ref="S55:S57" si="17">S43*$G$20</f>
+        <f t="shared" ref="S55:S57" si="15">S43*$G$20</f>
         <v>0</v>
       </c>
       <c r="V55" s="4">
-        <f t="shared" ref="V55:V57" si="18">V43*$G$20</f>
+        <f t="shared" ref="V55:V57" si="16">V43*$G$20</f>
         <v>0</v>
       </c>
       <c r="Y55" s="4">
-        <f t="shared" ref="Y55:Y57" si="19">Y43*$G$20</f>
+        <f t="shared" ref="Y55:Y57" si="17">Y43*$G$20</f>
         <v>0</v>
       </c>
     </row>
@@ -8641,34 +8641,34 @@
       <c r="A56" s="48"/>
       <c r="B56" s="37"/>
       <c r="E56" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G56" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="4">
+        <f>J44*$G$20</f>
+        <v>0</v>
+      </c>
+      <c r="M56" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="J56" s="4">
+      <c r="P56" s="4">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M56" s="4">
+      <c r="S56" s="4">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="P56" s="4">
+      <c r="V56" s="4">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="S56" s="4">
+      <c r="Y56" s="4">
         <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="V56" s="4">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Y56" s="4">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -8676,43 +8676,43 @@
       <c r="A57" s="48"/>
       <c r="B57" s="37"/>
       <c r="E57" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G57" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M57" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="J57" s="4">
+      <c r="P57" s="4">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M57" s="4">
+      <c r="S57" s="4">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="P57" s="4">
+      <c r="V57" s="4">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="S57" s="4">
+      <c r="Y57" s="4">
         <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="V57" s="4">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Y57" s="4">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" s="46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E58" s="14"/>
       <c r="G58" s="4">
@@ -8749,10 +8749,10 @@
     </row>
     <row r="60" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E60" s="14" t="s">
         <v>90</v>
@@ -8892,10 +8892,10 @@
     </row>
     <row r="66" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E66" s="14" t="s">
         <v>109</v>
@@ -9022,10 +9022,10 @@
     </row>
     <row r="71" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B71" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E71" s="14" t="s">
         <v>127</v>
@@ -9166,10 +9166,10 @@
     </row>
     <row r="75" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="46" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D75" s="28"/>
       <c r="E75" s="14" t="s">
@@ -9218,10 +9218,10 @@
     </row>
     <row r="77" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E77" s="14" t="s">
         <v>88</v>
@@ -9541,10 +9541,10 @@
     </row>
     <row r="84" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B84" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E84" s="14" t="s">
         <v>131</v>
@@ -9784,13 +9784,13 @@
     </row>
     <row r="89" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="B89" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="E89" s="14" t="s">
         <v>206</v>
-      </c>
-      <c r="B89" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="E89" s="14" t="s">
-        <v>207</v>
       </c>
       <c r="G89" s="4">
         <f>G55*G32</f>
@@ -9825,34 +9825,34 @@
       <c r="A90" s="47"/>
       <c r="B90" s="37"/>
       <c r="E90" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G90" s="4">
         <f>G56*G33</f>
         <v>0</v>
       </c>
       <c r="J90" s="4">
-        <f t="shared" ref="J90:J92" si="20">(G95-J79)*$F$29</f>
+        <f>(G95-J79)*$F$29</f>
         <v>0</v>
       </c>
       <c r="M90" s="4">
-        <f t="shared" ref="M90:M92" si="21">(J95-M79)*$F$29</f>
+        <f t="shared" ref="M90:M92" si="18">(J95-M79)*$F$29</f>
         <v>0</v>
       </c>
       <c r="P90" s="4">
-        <f t="shared" ref="P90:P92" si="22">(M95-P79)*$F$29</f>
+        <f t="shared" ref="P90:P92" si="19">(M95-P79)*$F$29</f>
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="S90" s="4">
-        <f t="shared" ref="S90:S92" si="23">(P95-S79)*$F$29</f>
+        <f t="shared" ref="S90:S92" si="20">(P95-S79)*$F$29</f>
         <v>9.5968000000000008E-3</v>
       </c>
       <c r="V90" s="4">
-        <f t="shared" ref="V90:V92" si="24">(S95-V79)*$F$29</f>
+        <f t="shared" ref="V90:V92" si="21">(S95-V79)*$F$29</f>
         <v>1.6000000000000004E-2</v>
       </c>
       <c r="Y90" s="4">
-        <f t="shared" ref="Y90:Y92" si="25">(V95-Y79)*$F$29</f>
+        <f t="shared" ref="Y90:Y92" si="22">(V95-Y79)*$F$29</f>
         <v>1.6E-2</v>
       </c>
     </row>
@@ -9860,34 +9860,34 @@
       <c r="A91" s="47"/>
       <c r="B91" s="37"/>
       <c r="E91" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G91" s="4">
         <f>G57*G34</f>
         <v>0</v>
       </c>
       <c r="J91" s="4">
+        <f t="shared" ref="J90:J92" si="23">(G96-J80)*$F$29</f>
+        <v>0</v>
+      </c>
+      <c r="M91" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="P91" s="4">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S91" s="4">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="M91" s="4">
+        <v>1.8400000000000001E-3</v>
+      </c>
+      <c r="V91" s="4">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="P91" s="4">
+        <v>1.1036320000000002E-2</v>
+      </c>
+      <c r="Y91" s="4">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="S91" s="4">
-        <f t="shared" si="23"/>
-        <v>1.8400000000000001E-3</v>
-      </c>
-      <c r="V91" s="4">
-        <f t="shared" si="24"/>
-        <v>1.1036320000000002E-2</v>
-      </c>
-      <c r="Y91" s="4">
-        <f t="shared" si="25"/>
         <v>1.8400000000000007E-2</v>
       </c>
     </row>
@@ -9895,34 +9895,34 @@
       <c r="A92" s="47"/>
       <c r="B92" s="37"/>
       <c r="E92" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G92" s="4">
         <f>G58*G35</f>
         <v>0</v>
       </c>
       <c r="J92" s="4">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="M92" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="P92" s="4">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S92" s="4">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="M92" s="4">
+      <c r="V92" s="4">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="P92" s="4">
+        <v>8.5999999999999998E-4</v>
+      </c>
+      <c r="Y92" s="4">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="S92" s="4">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="V92" s="4">
-        <f t="shared" si="24"/>
-        <v>8.5999999999999998E-4</v>
-      </c>
-      <c r="Y92" s="4">
-        <f t="shared" si="25"/>
         <v>5.1582799999999995E-3</v>
       </c>
     </row>
@@ -9931,10 +9931,10 @@
     </row>
     <row r="94" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B94" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E94" s="14" t="s">
         <v>70</v>
@@ -10079,14 +10079,14 @@
     </row>
     <row r="99" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="47" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B99" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D99" s="35"/>
       <c r="E99" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G99" s="4">
         <f>G94*$G$20</f>
@@ -10122,34 +10122,34 @@
       <c r="B100" s="37"/>
       <c r="D100" s="35"/>
       <c r="E100" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G100" s="4">
-        <f t="shared" ref="G100:G102" si="26">G95*$G$20</f>
+        <f t="shared" ref="G100:G102" si="24">G95*$G$20</f>
         <v>0</v>
       </c>
       <c r="J100" s="4">
-        <f t="shared" ref="J100:J102" si="27">J95*$G$20</f>
+        <f t="shared" ref="J100:J102" si="25">J95*$G$20</f>
         <v>0</v>
       </c>
       <c r="M100" s="4">
-        <f t="shared" ref="M100:M102" si="28">M95*$G$20</f>
+        <f t="shared" ref="M100:M102" si="26">M95*$G$20</f>
         <v>0.2</v>
       </c>
       <c r="P100" s="4">
-        <f t="shared" ref="P100:P102" si="29">P95*$G$20</f>
+        <f t="shared" ref="P100:P102" si="27">P95*$G$20</f>
         <v>1.1996</v>
       </c>
       <c r="S100" s="4">
-        <f t="shared" ref="S100:S102" si="30">S95*$G$20</f>
+        <f t="shared" ref="S100:S102" si="28">S95*$G$20</f>
         <v>3.5972008</v>
       </c>
       <c r="V100" s="4">
-        <f t="shared" ref="V100:V102" si="31">V95*$G$20</f>
+        <f t="shared" ref="V100:V102" si="29">V95*$G$20</f>
         <v>5.9960000000000004</v>
       </c>
       <c r="Y100" s="4">
-        <f t="shared" ref="Y100:Y102" si="32">Y95*$G$20</f>
+        <f t="shared" ref="Y100:Y102" si="30">Y95*$G$20</f>
         <v>9.1959999999999997</v>
       </c>
     </row>
@@ -10158,7 +10158,7 @@
       <c r="B101" s="37"/>
       <c r="D101" s="35"/>
       <c r="E101" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G101" s="4">
         <f>G96*$G$20</f>
@@ -10194,34 +10194,34 @@
       <c r="B102" s="37"/>
       <c r="D102" s="35"/>
       <c r="E102" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G102" s="4">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="J102" s="4">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="M102" s="4">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="J102" s="4">
+      <c r="P102" s="4">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="M102" s="4">
+      <c r="S102" s="4">
         <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="P102" s="4">
+        <v>0.1075</v>
+      </c>
+      <c r="V102" s="4">
         <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="S102" s="4">
+        <v>0.64478499999999994</v>
+      </c>
+      <c r="Y102" s="4">
         <f t="shared" si="30"/>
-        <v>0.1075</v>
-      </c>
-      <c r="V102" s="4">
-        <f t="shared" si="31"/>
-        <v>0.64478499999999994</v>
-      </c>
-      <c r="Y102" s="4">
-        <f t="shared" si="32"/>
         <v>1.93349543</v>
       </c>
     </row>
@@ -10249,10 +10249,10 @@
     </row>
     <row r="106" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B106" s="44" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D106" s="35"/>
       <c r="E106" s="14" t="s">
@@ -10317,10 +10317,10 @@
     </row>
     <row r="107" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B107" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E107" s="14" t="s">
         <v>141</v>
@@ -10384,13 +10384,13 @@
     </row>
     <row r="108" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E108" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F108" s="4">
         <v>1</v>
@@ -10449,10 +10449,10 @@
     </row>
     <row r="109" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B109" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E109" s="14" t="s">
         <v>131</v>
@@ -10516,13 +10516,13 @@
     </row>
     <row r="110" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B110" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E110" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F110" s="4">
         <f>F7*F19</f>
@@ -10583,10 +10583,10 @@
     </row>
     <row r="111" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B111" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E111" s="14" t="s">
         <v>142</v>
@@ -10672,13 +10672,13 @@
     </row>
     <row r="114" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B114" s="44" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E114" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F114" s="4">
         <f>F111*F7</f>
@@ -10739,13 +10739,13 @@
     </row>
     <row r="115" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B115" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E115" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G115" s="4">
         <f>SUM(G94:G97)</f>
@@ -10778,13 +10778,13 @@
     </row>
     <row r="116" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B116" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E116" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F116" s="4">
         <f>F114+F115</f>
@@ -10845,13 +10845,13 @@
     </row>
     <row r="117" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B117" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E117" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F117" s="4">
         <f>F110*$F$20</f>
@@ -10912,13 +10912,13 @@
     </row>
     <row r="118" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B118" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F118" s="4">
         <f>F9*F111</f>
@@ -10979,13 +10979,13 @@
     </row>
     <row r="119" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="46" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B119" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E119" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F119" s="4">
         <f>MIN(F118,F9*F15)</f>
@@ -11046,13 +11046,13 @@
     </row>
     <row r="120" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="46" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E120" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F120" s="4">
         <f>(F118-F119)*$F$14</f>
@@ -11113,13 +11113,13 @@
     </row>
     <row r="121" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="46" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B121" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E121" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F121" s="4">
         <f>MIN(F120+G120, F32)</f>
@@ -11152,13 +11152,13 @@
     </row>
     <row r="122" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="46" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B122" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E122" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F122" s="4">
         <f>F120/(F120+G120)</f>
@@ -11219,10 +11219,10 @@
     </row>
     <row r="123" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E123" s="10" t="s">
         <v>121</v>
@@ -11305,13 +11305,13 @@
     </row>
     <row r="126" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="B126" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E126" s="14" t="s">
         <v>264</v>
-      </c>
-      <c r="B126" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="E126" s="14" t="s">
-        <v>266</v>
       </c>
       <c r="F126" s="4">
         <f>MAX(F32-F121,0)</f>
@@ -11344,13 +11344,13 @@
     </row>
     <row r="127" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="46" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B127" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E127" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F127" s="4">
         <f>MIN(F138,F126)</f>
@@ -11383,10 +11383,10 @@
     </row>
     <row r="128" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="46" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B128" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E128" s="10" t="s">
         <v>123</v>
@@ -11422,10 +11422,10 @@
     </row>
     <row r="129" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E129" s="10" t="s">
         <v>146</v>
@@ -11461,10 +11461,10 @@
     </row>
     <row r="130" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="46" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B130" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E130" s="10" t="s">
         <v>120</v>
@@ -11528,13 +11528,13 @@
     </row>
     <row r="131" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="46" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B131" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E131" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F131" s="4">
         <f>F130</f>
@@ -11614,10 +11614,10 @@
     </row>
     <row r="133" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" s="46" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B133" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E133" s="10" t="s">
         <v>75</v>
@@ -11681,10 +11681,10 @@
     </row>
     <row r="134" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B134" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E134" s="10" t="s">
         <v>137</v>
@@ -11758,13 +11758,13 @@
     </row>
     <row r="135" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="B135" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E135" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="B135" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="E135" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="F135" s="4">
         <f>MAX(MIN(F134/$F$17, 1), 0)</f>
@@ -11848,10 +11848,10 @@
     </row>
     <row r="137" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="46" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B137" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E137" s="10" t="s">
         <v>76</v>
@@ -11925,10 +11925,10 @@
     </row>
     <row r="138" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E138" s="10" t="s">
         <v>122</v>
@@ -11992,10 +11992,10 @@
     </row>
     <row r="139" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B139" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E139" s="10" t="s">
         <v>119</v>
@@ -12059,7 +12059,7 @@
     </row>
     <row r="141" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="E141" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
@@ -12078,13 +12078,13 @@
     </row>
     <row r="142" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="46" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B142" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E142" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F142" s="4">
         <f>(F110 - F130 - F118)*$F$29</f>
@@ -12145,13 +12145,13 @@
     </row>
     <row r="143" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="46" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B143" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E143" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F143" s="4">
         <f>F130*$F20</f>
@@ -12212,13 +12212,13 @@
     </row>
     <row r="144" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B144" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E144" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F144" s="4">
         <f>F118-F121*F122-F119</f>
@@ -12279,13 +12279,13 @@
     </row>
     <row r="145" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B145" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E145" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F145" s="4">
         <f>F118*$F20</f>
@@ -12346,7 +12346,7 @@
     </row>
     <row r="148" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A148" s="33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F148" s="4">
         <f>F144+F119</f>
@@ -12407,10 +12407,10 @@
     </row>
     <row r="150" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A150" s="46" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B150" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F150" s="4">
         <f>F121+F130+G130+F129</f>

</xml_diff>

<commit_message>
updated carbon ledger, neared completion of young forest arrays in BCL.
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE6D6BB-3EDE-CB43-8A49-46D25A5A8C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC78003-B42E-B647-9794-4D0FE38B4C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="760" windowWidth="26440" windowHeight="19880" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
+    <workbookView xWindow="12440" yWindow="560" windowWidth="33680" windowHeight="19400" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -951,7 +951,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1030,6 +1030,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1043,7 +1049,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1178,11 +1184,17 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6339,8 +6351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40F0562-A765-A442-B9DB-CF71D123E451}">
   <dimension ref="A1:AM158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6348,8 +6360,8 @@
     <col min="1" max="1" width="62.1640625" style="33" customWidth="1"/>
     <col min="2" max="2" width="14" style="36" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="27" style="22" customWidth="1"/>
-    <col min="5" max="5" width="44" style="10" customWidth="1"/>
+    <col min="4" max="4" width="27" style="22" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="44" style="10" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" style="4" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="5" customWidth="1"/>
@@ -6566,7 +6578,7 @@
         <v>135</v>
       </c>
       <c r="Y5" s="29"/>
-      <c r="AB5" s="49" t="s">
+      <c r="AB5" s="48" t="s">
         <v>235</v>
       </c>
       <c r="AC5" s="21" t="s">
@@ -6661,7 +6673,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="51" t="s">
         <v>156</v>
       </c>
       <c r="B7" s="40" t="s">
@@ -6748,7 +6760,7 @@
       </c>
     </row>
     <row r="8" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="51" t="s">
         <v>157</v>
       </c>
       <c r="B8" s="41" t="s">
@@ -6837,7 +6849,7 @@
       </c>
     </row>
     <row r="9" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="51" t="s">
         <v>225</v>
       </c>
       <c r="B9" s="41" t="s">
@@ -6912,7 +6924,7 @@
       </c>
     </row>
     <row r="10" spans="1:39" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="51" t="s">
         <v>224</v>
       </c>
       <c r="B10" s="40" t="s">
@@ -6961,7 +6973,7 @@
       </c>
     </row>
     <row r="11" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="51" t="s">
         <v>222</v>
       </c>
       <c r="B11" s="40" t="s">
@@ -7010,7 +7022,7 @@
       </c>
     </row>
     <row r="12" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="51" t="s">
         <v>223</v>
       </c>
       <c r="B12" s="41" t="s">
@@ -7052,7 +7064,7 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="51" t="s">
         <v>158</v>
       </c>
       <c r="B13" s="40" t="s">
@@ -7122,7 +7134,7 @@
       <c r="AE13" s="19"/>
     </row>
     <row r="14" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="51" t="s">
         <v>226</v>
       </c>
       <c r="B14" s="41" t="s">
@@ -7164,7 +7176,7 @@
       </c>
     </row>
     <row r="15" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="51" t="s">
         <v>251</v>
       </c>
       <c r="B15" s="41" t="s">
@@ -7223,7 +7235,7 @@
       <c r="AE15" s="19"/>
     </row>
     <row r="16" spans="1:39" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="51" t="s">
         <v>227</v>
       </c>
       <c r="B16" s="41" t="s">
@@ -7265,7 +7277,7 @@
       </c>
     </row>
     <row r="17" spans="1:31" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="51" t="s">
         <v>228</v>
       </c>
       <c r="B17" s="41" t="s">
@@ -7292,7 +7304,7 @@
       </c>
     </row>
     <row r="18" spans="1:31" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="51" t="s">
         <v>229</v>
       </c>
       <c r="B18" s="41" t="s">
@@ -7317,7 +7329,7 @@
       </c>
     </row>
     <row r="19" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="51" t="s">
         <v>231</v>
       </c>
       <c r="B19" s="41" t="s">
@@ -7344,7 +7356,7 @@
       </c>
     </row>
     <row r="20" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="51" t="s">
         <v>233</v>
       </c>
       <c r="B20" s="41" t="s">
@@ -7364,7 +7376,7 @@
       <c r="AE20" s="19"/>
     </row>
     <row r="21" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="51" t="s">
         <v>283</v>
       </c>
       <c r="B21" s="42" t="s">
@@ -7393,7 +7405,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="51" t="s">
         <v>232</v>
       </c>
       <c r="B22" s="42" t="s">
@@ -7434,7 +7446,7 @@
       </c>
     </row>
     <row r="24" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="51" t="s">
         <v>159</v>
       </c>
       <c r="B24" s="41" t="s">
@@ -7497,7 +7509,7 @@
       </c>
     </row>
     <row r="25" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="51" t="s">
         <v>282</v>
       </c>
       <c r="B25" s="43" t="s">
@@ -7546,7 +7558,7 @@
       </c>
     </row>
     <row r="26" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="51" t="s">
         <v>160</v>
       </c>
       <c r="B26" s="43" t="s">
@@ -7652,7 +7664,7 @@
       </c>
     </row>
     <row r="28" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="51" t="s">
         <v>281</v>
       </c>
       <c r="B28" s="41" t="s">
@@ -7672,7 +7684,7 @@
       </c>
     </row>
     <row r="29" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>234</v>
       </c>
       <c r="B29" s="42" t="s">
@@ -7714,7 +7726,7 @@
       <c r="Y31" s="8"/>
     </row>
     <row r="32" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="51" t="s">
         <v>169</v>
       </c>
       <c r="B32" s="41" t="s">
@@ -7839,7 +7851,7 @@
       </c>
     </row>
     <row r="37" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="47" t="s">
+      <c r="A37" s="49" t="s">
         <v>181</v>
       </c>
       <c r="B37" s="37" t="s">
@@ -7929,7 +7941,7 @@
       </c>
     </row>
     <row r="38" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="48"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="37"/>
       <c r="E38" s="14" t="s">
         <v>69</v>
@@ -8014,7 +8026,7 @@
       </c>
     </row>
     <row r="39" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="48"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="37"/>
       <c r="E39" s="14" t="s">
         <v>79</v>
@@ -8098,7 +8110,7 @@
       </c>
     </row>
     <row r="40" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="48"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="37"/>
       <c r="E40" s="14" t="s">
         <v>80</v>
@@ -8189,7 +8201,7 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="50" t="s">
         <v>192</v>
       </c>
       <c r="B42" s="37" t="s">
@@ -8227,7 +8239,7 @@
       </c>
     </row>
     <row r="43" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="48"/>
+      <c r="A43" s="50"/>
       <c r="B43" s="37"/>
       <c r="E43" s="14" t="s">
         <v>197</v>
@@ -8261,7 +8273,7 @@
       </c>
     </row>
     <row r="44" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="48"/>
+      <c r="A44" s="50"/>
       <c r="B44" s="37"/>
       <c r="E44" s="14" t="s">
         <v>198</v>
@@ -8295,7 +8307,7 @@
       </c>
     </row>
     <row r="45" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="48"/>
+      <c r="A45" s="50"/>
       <c r="B45" s="37"/>
       <c r="E45" s="14" t="s">
         <v>199</v>
@@ -8329,7 +8341,7 @@
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="46" t="s">
+      <c r="A46" s="51" t="s">
         <v>193</v>
       </c>
       <c r="B46" s="40" t="s">
@@ -8374,7 +8386,7 @@
       </c>
     </row>
     <row r="48" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="48" t="s">
+      <c r="A48" s="50" t="s">
         <v>265</v>
       </c>
       <c r="B48" s="37" t="s">
@@ -8416,14 +8428,14 @@
       </c>
     </row>
     <row r="49" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="48"/>
+      <c r="A49" s="50"/>
       <c r="B49" s="37"/>
       <c r="D49" s="28"/>
       <c r="E49" s="14" t="s">
         <v>254</v>
       </c>
       <c r="G49" s="4">
-        <f t="shared" ref="G49" si="5">MIN(G43,G$15*F38)</f>
+        <f>MIN(G43,G$15*F38)</f>
         <v>0</v>
       </c>
       <c r="J49" s="4">
@@ -8431,28 +8443,28 @@
         <v>0</v>
       </c>
       <c r="M49" s="4">
-        <f t="shared" ref="M49" si="6">MIN(M43,M$15*L38)</f>
+        <f>MIN(M43,M$15*L38)</f>
         <v>0</v>
       </c>
       <c r="P49" s="4">
-        <f t="shared" ref="P49" si="7">MIN(P43,P$15*O38)</f>
+        <f t="shared" ref="P49" si="5">MIN(P43,P$15*O38)</f>
         <v>0</v>
       </c>
       <c r="S49" s="4">
-        <f t="shared" ref="S49" si="8">MIN(S43,S$15*R38)</f>
+        <f t="shared" ref="S49" si="6">MIN(S43,S$15*R38)</f>
         <v>0</v>
       </c>
       <c r="V49" s="4">
-        <f t="shared" ref="V49" si="9">MIN(V43,V$15*U38)</f>
+        <f t="shared" ref="V49" si="7">MIN(V43,V$15*U38)</f>
         <v>0</v>
       </c>
       <c r="Y49" s="4">
-        <f t="shared" ref="Y49" si="10">MIN(Y43,Y$15*X38)</f>
+        <f t="shared" ref="Y49" si="8">MIN(Y43,Y$15*X38)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="48"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="37"/>
       <c r="D50" s="28"/>
       <c r="E50" s="14" t="s">
@@ -8488,7 +8500,7 @@
       </c>
     </row>
     <row r="51" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="48"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="37"/>
       <c r="D51" s="28"/>
       <c r="E51" s="14" t="s">
@@ -8524,7 +8536,7 @@
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A52" s="46" t="s">
+      <c r="A52" s="51" t="s">
         <v>266</v>
       </c>
       <c r="B52" s="40" t="s">
@@ -8564,7 +8576,7 @@
       <c r="E53" s="14"/>
     </row>
     <row r="54" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="48" t="s">
+      <c r="A54" s="50" t="s">
         <v>194</v>
       </c>
       <c r="B54" s="37" t="s">
@@ -8603,48 +8615,48 @@
       </c>
     </row>
     <row r="55" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="48"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="37"/>
       <c r="E55" s="14" t="s">
         <v>201</v>
       </c>
       <c r="G55" s="4">
-        <f t="shared" ref="G55:G57" si="11">G43*$G$20</f>
+        <f>G43*$G$20</f>
         <v>0</v>
       </c>
       <c r="J55" s="4">
-        <f t="shared" ref="J55:J57" si="12">J43*$G$20</f>
+        <f>J43*$G$20</f>
         <v>0</v>
       </c>
       <c r="M55" s="4">
-        <f t="shared" ref="M55:M57" si="13">M43*$G$20</f>
+        <f>M43*$G$20</f>
         <v>0</v>
       </c>
       <c r="P55" s="4">
-        <f t="shared" ref="P55:P57" si="14">P43*$G$20</f>
+        <f t="shared" ref="P55:P57" si="9">P43*$G$20</f>
         <v>0</v>
       </c>
       <c r="S55" s="4">
-        <f t="shared" ref="S55:S57" si="15">S43*$G$20</f>
+        <f t="shared" ref="S55:S57" si="10">S43*$G$20</f>
         <v>0</v>
       </c>
       <c r="V55" s="4">
-        <f t="shared" ref="V55:V57" si="16">V43*$G$20</f>
+        <f t="shared" ref="V55:V57" si="11">V43*$G$20</f>
         <v>0</v>
       </c>
       <c r="Y55" s="4">
-        <f t="shared" ref="Y55:Y57" si="17">Y43*$G$20</f>
+        <f t="shared" ref="Y55:Y57" si="12">Y43*$G$20</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="48"/>
+      <c r="A56" s="50"/>
       <c r="B56" s="37"/>
       <c r="E56" s="14" t="s">
         <v>202</v>
       </c>
       <c r="G56" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="G55:G57" si="13">G44*$G$20</f>
         <v>0</v>
       </c>
       <c r="J56" s="4">
@@ -8652,63 +8664,63 @@
         <v>0</v>
       </c>
       <c r="M56" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="M55:M57" si="14">M44*$G$20</f>
         <v>0</v>
       </c>
       <c r="P56" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S56" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V56" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Y56" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="48"/>
+      <c r="A57" s="50"/>
       <c r="B57" s="37"/>
       <c r="E57" s="14" t="s">
         <v>203</v>
       </c>
       <c r="G57" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="4">
+        <f t="shared" ref="J55:J57" si="15">J45*$G$20</f>
+        <v>0</v>
+      </c>
+      <c r="M57" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="P57" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S57" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V57" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J57" s="4">
+      <c r="Y57" s="4">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M57" s="4">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="P57" s="4">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="S57" s="4">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="V57" s="4">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="Y57" s="4">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A58" s="46" t="s">
+      <c r="A58" s="51" t="s">
         <v>195</v>
       </c>
       <c r="B58" s="40" t="s">
@@ -8748,7 +8760,7 @@
       <c r="E59" s="14"/>
     </row>
     <row r="60" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="48" t="s">
+      <c r="A60" s="50" t="s">
         <v>179</v>
       </c>
       <c r="B60" s="37" t="s">
@@ -8787,7 +8799,7 @@
       </c>
     </row>
     <row r="61" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="48"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="37"/>
       <c r="E61" s="14" t="s">
         <v>91</v>
@@ -8820,7 +8832,7 @@
       </c>
     </row>
     <row r="62" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="48"/>
+      <c r="A62" s="50"/>
       <c r="B62" s="37"/>
       <c r="E62" s="14" t="s">
         <v>92</v>
@@ -8852,7 +8864,7 @@
       </c>
     </row>
     <row r="63" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="48"/>
+      <c r="A63" s="50"/>
       <c r="B63" s="37"/>
       <c r="E63" s="14" t="s">
         <v>93</v>
@@ -8891,7 +8903,7 @@
       <c r="E65" s="14"/>
     </row>
     <row r="66" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="48" t="s">
+      <c r="A66" s="50" t="s">
         <v>239</v>
       </c>
       <c r="B66" s="37" t="s">
@@ -8909,28 +8921,28 @@
         <v>0.85</v>
       </c>
       <c r="M66" s="4">
-        <f>J66+M37*M60</f>
-        <v>5.0999999999999996</v>
+        <f>J66*(1- $F$29)+M37*M60</f>
+        <v>5.0983000000000001</v>
       </c>
       <c r="P66" s="4">
-        <f>M66+P37*P60</f>
-        <v>15.299999999999999</v>
+        <f>M66*(1- $F$29)+P37*P60</f>
+        <v>15.288103399999999</v>
       </c>
       <c r="S66" s="4">
-        <f>P66+S37*S60</f>
-        <v>32.299999999999997</v>
+        <f>P66*(1- $F$29)+S37*S60</f>
+        <v>32.257527193199998</v>
       </c>
       <c r="V66" s="4">
-        <f>S66+V37*V60</f>
-        <v>62.899999999999991</v>
+        <f>S66*(1- $F$29)+V37*V60</f>
+        <v>62.793012138813594</v>
       </c>
       <c r="Y66" s="4">
-        <f>V66+Y37*Y60</f>
-        <v>113.89999999999999</v>
+        <f>V66*(1- $F$29)+Y37*Y60</f>
+        <v>113.66742611453597</v>
       </c>
     </row>
     <row r="67" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="48"/>
+      <c r="A67" s="50"/>
       <c r="B67" s="37"/>
       <c r="E67" s="14" t="s">
         <v>110</v>
@@ -8940,80 +8952,80 @@
         <v>0</v>
       </c>
       <c r="M67" s="4">
-        <f>J67+M38*M61</f>
+        <f>J67*(1- $F$29)+M38*M61</f>
         <v>0.8</v>
       </c>
       <c r="P67" s="4">
-        <f>M67+P38*P61</f>
-        <v>4.8</v>
+        <f>M67*(1- $F$29)+P38*P61</f>
+        <v>4.7984</v>
       </c>
       <c r="S67" s="4">
-        <f>P67+S38*S61</f>
-        <v>14.399999999999999</v>
+        <f>P67*(1- $F$29)+S38*S61</f>
+        <v>14.3888032</v>
       </c>
       <c r="V67" s="4">
-        <f>S67+V38*V61</f>
-        <v>30.4</v>
+        <f>S67*(1- $F$29)+V38*V61</f>
+        <v>30.3600255936</v>
       </c>
       <c r="Y67" s="4">
-        <f>V67+Y38*Y61</f>
-        <v>59.199999999999996</v>
+        <f>V67*(1- $F$29)+Y38*Y61</f>
+        <v>59.099305542412793</v>
       </c>
     </row>
     <row r="68" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="48"/>
+      <c r="A68" s="50"/>
       <c r="B68" s="37"/>
       <c r="D68" s="28"/>
       <c r="E68" s="14" t="s">
         <v>111</v>
       </c>
       <c r="M68" s="4">
-        <f>J68+M39*M62</f>
+        <f>J68*(1- $F$29)+M39*M62</f>
         <v>0</v>
       </c>
       <c r="P68" s="4">
-        <f>M68+P39*P62</f>
+        <f>M68*(1- $F$29)+P39*P62</f>
         <v>0.92</v>
       </c>
       <c r="S68" s="4">
-        <f>P68+S39*S62</f>
-        <v>5.5200000000000005</v>
+        <f>P68*(1- $F$29)+S39*S62</f>
+        <v>5.5181600000000008</v>
       </c>
       <c r="V68" s="4">
-        <f>S68+V39*V62</f>
-        <v>16.559999999999999</v>
+        <f>S68*(1- $F$29)+V39*V62</f>
+        <v>16.547123679999999</v>
       </c>
       <c r="Y68" s="4">
-        <f>V68+Y39*Y62</f>
-        <v>34.96</v>
+        <f>V68*(1- $F$29)+Y39*Y62</f>
+        <v>34.91402943264</v>
       </c>
     </row>
     <row r="69" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="48"/>
+      <c r="A69" s="50"/>
       <c r="B69" s="37"/>
       <c r="D69" s="28"/>
       <c r="E69" s="14" t="s">
         <v>112</v>
       </c>
       <c r="M69" s="4">
-        <f>J69+M40*M63</f>
+        <f>J69*(1- $F$29)+M40*M63</f>
         <v>0</v>
       </c>
       <c r="P69" s="4">
-        <f>M69+P40*P63</f>
+        <f>M69*(1- $F$29)+P40*P63</f>
         <v>0</v>
       </c>
       <c r="S69" s="4">
-        <f>P69+S40*S63</f>
+        <f>P69*(1- $F$29)+S40*S63</f>
         <v>0.43</v>
       </c>
       <c r="V69" s="4">
-        <f>S69+V40*V63</f>
-        <v>2.58</v>
+        <f>S69*(1- $F$29)+V40*V63</f>
+        <v>2.5791399999999998</v>
       </c>
       <c r="Y69" s="4">
-        <f>V69+Y40*Y63</f>
-        <v>7.74</v>
+        <f>V69*(1- $F$29)+Y40*Y63</f>
+        <v>7.7339817200000001</v>
       </c>
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.2">
@@ -9021,7 +9033,7 @@
       <c r="E70" s="14"/>
     </row>
     <row r="71" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="48" t="s">
+      <c r="A71" s="50" t="s">
         <v>236</v>
       </c>
       <c r="B71" s="37" t="s">
@@ -9059,7 +9071,7 @@
       </c>
     </row>
     <row r="72" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="48"/>
+      <c r="A72" s="50"/>
       <c r="B72" s="37"/>
       <c r="E72" s="14" t="s">
         <v>128</v>
@@ -9093,7 +9105,7 @@
       </c>
     </row>
     <row r="73" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="48"/>
+      <c r="A73" s="50"/>
       <c r="B73" s="37"/>
       <c r="D73" s="28" t="s">
         <v>152</v>
@@ -9130,7 +9142,7 @@
       </c>
     </row>
     <row r="74" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="48"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="37"/>
       <c r="D74" s="28"/>
       <c r="E74" s="14" t="s">
@@ -9165,7 +9177,7 @@
       </c>
     </row>
     <row r="75" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="46" t="s">
+      <c r="A75" s="51" t="s">
         <v>237</v>
       </c>
       <c r="B75" s="40" t="s">
@@ -9217,7 +9229,7 @@
       </c>
     </row>
     <row r="77" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="50" t="s">
+      <c r="A77" s="52" t="s">
         <v>238</v>
       </c>
       <c r="B77" s="37" t="s">
@@ -9252,7 +9264,7 @@
       </c>
     </row>
     <row r="78" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="50"/>
+      <c r="A78" s="52"/>
       <c r="B78" s="37"/>
       <c r="E78" s="14" t="s">
         <v>148</v>
@@ -9315,7 +9327,7 @@
       </c>
     </row>
     <row r="79" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="50"/>
+      <c r="A79" s="52"/>
       <c r="B79" s="37"/>
       <c r="D79" s="22">
         <v>0</v>
@@ -9381,7 +9393,7 @@
       </c>
     </row>
     <row r="80" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="50"/>
+      <c r="A80" s="52"/>
       <c r="B80" s="37"/>
       <c r="D80" s="22">
         <v>1</v>
@@ -9447,7 +9459,7 @@
       </c>
     </row>
     <row r="81" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="50"/>
+      <c r="A81" s="52"/>
       <c r="B81" s="37"/>
       <c r="D81" s="22">
         <v>2</v>
@@ -9540,7 +9552,7 @@
       </c>
     </row>
     <row r="84" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="47" t="s">
+      <c r="A84" s="49" t="s">
         <v>182</v>
       </c>
       <c r="B84" s="37" t="s">
@@ -9595,15 +9607,15 @@
       </c>
       <c r="X84" s="4">
         <f>IF(V94=0,1,MIN(MAX((V94/V66-$F$16)/($F$18-$F$16), 0), 1))</f>
-        <v>0.92728154163131749</v>
+        <v>0.92886400737928387</v>
       </c>
       <c r="Y84" s="4">
         <f>Y60*X84</f>
-        <v>0.55636892497879042</v>
+        <v>0.5573184044275703</v>
       </c>
     </row>
     <row r="85" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="47"/>
+      <c r="A85" s="49"/>
       <c r="B85" s="37"/>
       <c r="E85" s="14" t="s">
         <v>132</v>
@@ -9662,7 +9674,7 @@
       </c>
     </row>
     <row r="86" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="47"/>
+      <c r="A86" s="49"/>
       <c r="B86" s="37"/>
       <c r="E86" s="14" t="s">
         <v>133</v>
@@ -9721,7 +9733,7 @@
       </c>
     </row>
     <row r="87" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="47"/>
+      <c r="A87" s="49"/>
       <c r="B87" s="37"/>
       <c r="E87" s="14" t="s">
         <v>134</v>
@@ -9783,7 +9795,7 @@
       <c r="E88" s="14"/>
     </row>
     <row r="89" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="47" t="s">
+      <c r="A89" s="49" t="s">
         <v>205</v>
       </c>
       <c r="B89" s="37" t="s">
@@ -9822,7 +9834,7 @@
       </c>
     </row>
     <row r="90" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="47"/>
+      <c r="A90" s="49"/>
       <c r="B90" s="37"/>
       <c r="E90" s="14" t="s">
         <v>207</v>
@@ -9836,28 +9848,28 @@
         <v>0</v>
       </c>
       <c r="M90" s="4">
-        <f t="shared" ref="M90:M92" si="18">(J95-M79)*$F$29</f>
+        <f t="shared" ref="M90:M92" si="16">(J95-M79)*$F$29</f>
         <v>0</v>
       </c>
       <c r="P90" s="4">
-        <f t="shared" ref="P90:P92" si="19">(M95-P79)*$F$29</f>
+        <f t="shared" ref="P90:P92" si="17">(M95-P79)*$F$29</f>
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="S90" s="4">
-        <f t="shared" ref="S90:S92" si="20">(P95-S79)*$F$29</f>
+        <f t="shared" ref="S90:S92" si="18">(P95-S79)*$F$29</f>
         <v>9.5968000000000008E-3</v>
       </c>
       <c r="V90" s="4">
-        <f t="shared" ref="V90:V92" si="21">(S95-V79)*$F$29</f>
+        <f t="shared" ref="V90:V92" si="19">(S95-V79)*$F$29</f>
         <v>1.6000000000000004E-2</v>
       </c>
       <c r="Y90" s="4">
-        <f t="shared" ref="Y90:Y92" si="22">(V95-Y79)*$F$29</f>
+        <f t="shared" ref="Y90:Y92" si="20">(V95-Y79)*$F$29</f>
         <v>1.6E-2</v>
       </c>
     </row>
     <row r="91" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="47"/>
+      <c r="A91" s="49"/>
       <c r="B91" s="37"/>
       <c r="E91" s="14" t="s">
         <v>208</v>
@@ -9867,32 +9879,32 @@
         <v>0</v>
       </c>
       <c r="J91" s="4">
-        <f t="shared" ref="J90:J92" si="23">(G96-J80)*$F$29</f>
+        <f t="shared" ref="J90:J92" si="21">(G96-J80)*$F$29</f>
         <v>0</v>
       </c>
       <c r="M91" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="P91" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="S91" s="4">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="P91" s="4">
+        <v>1.8400000000000001E-3</v>
+      </c>
+      <c r="V91" s="4">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="S91" s="4">
+        <v>1.1036320000000002E-2</v>
+      </c>
+      <c r="Y91" s="4">
         <f t="shared" si="20"/>
-        <v>1.8400000000000001E-3</v>
-      </c>
-      <c r="V91" s="4">
-        <f t="shared" si="21"/>
-        <v>1.1036320000000002E-2</v>
-      </c>
-      <c r="Y91" s="4">
-        <f t="shared" si="22"/>
         <v>1.8400000000000007E-2</v>
       </c>
     </row>
     <row r="92" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="47"/>
+      <c r="A92" s="49"/>
       <c r="B92" s="37"/>
       <c r="E92" s="14" t="s">
         <v>209</v>
@@ -9902,27 +9914,27 @@
         <v>0</v>
       </c>
       <c r="J92" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M92" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="P92" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="S92" s="4">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="P92" s="4">
+      <c r="V92" s="4">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="S92" s="4">
+        <v>8.5999999999999998E-4</v>
+      </c>
+      <c r="Y92" s="4">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="V92" s="4">
-        <f t="shared" si="21"/>
-        <v>8.5999999999999998E-4</v>
-      </c>
-      <c r="Y92" s="4">
-        <f t="shared" si="22"/>
         <v>5.1582799999999995E-3</v>
       </c>
     </row>
@@ -9944,28 +9956,28 @@
         <v>0</v>
       </c>
       <c r="J94" s="4">
-        <f>G94 - J78 - J89 + J37*J84</f>
+        <f>G94 - J78 - J89 - J42 + J37*J84</f>
         <v>0.85</v>
       </c>
       <c r="M94" s="4">
-        <f>J94 - M78 - M89 + M37*M84</f>
+        <f>J94 - M78 - M89 - M42 + M37*M84</f>
         <v>5.0983000000000001</v>
       </c>
       <c r="P94" s="4">
-        <f>M94 - P78 - P89 + P37*P84</f>
+        <f>M94 - P78 - P89 - P42 + P37*P84</f>
         <v>15.288103399999999</v>
       </c>
       <c r="S94" s="4">
-        <f>P94 - S78 - S89 + S37*S84</f>
+        <f>P94 - S78 - S89 - S42 + S37*S84</f>
         <v>32.257527193199998</v>
       </c>
       <c r="V94" s="4">
-        <f>S94 - V78 - V89 + V37*V84</f>
+        <f>S94 - V78 - V89 - V42 + V37*V84</f>
         <v>39.082999999999998</v>
       </c>
       <c r="Y94" s="4">
-        <f>V94 - Y78 - Y89 + Y37*Y84</f>
-        <v>55.774358623197188</v>
+        <f>V94 - Y78 - Y89 - Y42 + Y37*Y84</f>
+        <v>55.855064376343478</v>
       </c>
     </row>
     <row r="95" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -9979,27 +9991,27 @@
         <v>0</v>
       </c>
       <c r="J95" s="4">
-        <f>G95 - J79 - J90 + J38*J85</f>
+        <f t="shared" ref="J95:J97" si="22">G95 - J79 - J90 - J43 + J38*J85</f>
         <v>0</v>
       </c>
       <c r="M95" s="4">
-        <f>J95 - M79 - M90 + M38*M85</f>
+        <f t="shared" ref="M95:M97" si="23">J95 - M79 - M90 - M43 + M38*M85</f>
         <v>0.8</v>
       </c>
       <c r="P95" s="4">
-        <f>M95 - P79 - P90 + P38*P85</f>
+        <f t="shared" ref="P95:P97" si="24">M95 - P79 - P90 - P43 + P38*P85</f>
         <v>4.7984</v>
       </c>
       <c r="S95" s="4">
-        <f>P95 - S79 - S90 + S38*S85</f>
+        <f t="shared" ref="S95:S97" si="25">P95 - S79 - S90 - S43 + S38*S85</f>
         <v>14.3888032</v>
       </c>
       <c r="V95" s="4">
-        <f>S95 - V79 - V90 + V38*V85</f>
+        <f t="shared" ref="V95:V97" si="26">S95 - V79 - V90 - V43 + V38*V85</f>
         <v>23.984000000000002</v>
       </c>
       <c r="Y95" s="4">
-        <f>V95 - Y79 - Y90 + Y38*Y85</f>
+        <f t="shared" ref="Y95:Y97" si="27">V95 - Y79 - Y90 - Y43 + Y38*Y85</f>
         <v>36.783999999999999</v>
       </c>
     </row>
@@ -10014,27 +10026,27 @@
         <v>0</v>
       </c>
       <c r="J96" s="4">
-        <f>G96 - J80 - J91 + J39*J86</f>
+        <f>G96 - J80 - J91 - J44 + J39*J86</f>
         <v>0</v>
       </c>
       <c r="M96" s="4">
-        <f>J96 - M80 - M91 + M39*M86</f>
+        <f>J96 - M80 - M91 - M44 + M39*M86</f>
         <v>0</v>
       </c>
       <c r="P96" s="4">
-        <f>M96 - P80 - P91 + P39*P86</f>
+        <f>M96 - P80 - P91 - P44 + P39*P86</f>
         <v>0.92</v>
       </c>
       <c r="S96" s="4">
-        <f>P96 - S80 - S91 + S39*S86</f>
+        <f>P96 - S80 - S91 - S44 + S39*S86</f>
         <v>5.5181600000000008</v>
       </c>
       <c r="V96" s="4">
-        <f>S96 - V80 - V91 + V39*V86</f>
+        <f>S96 - V80 - V91 - V44 + V39*V86</f>
         <v>16.547123679999999</v>
       </c>
       <c r="Y96" s="4">
-        <f>V96 - Y80 - Y91 + Y39*Y86</f>
+        <f>V96 - Y80 - Y91 - Y44 + Y39*Y86</f>
         <v>27.581600000000005</v>
       </c>
     </row>
@@ -10049,27 +10061,27 @@
         <v>0</v>
       </c>
       <c r="J97" s="4">
-        <f>G97 - J81 - J92 + J40*J87</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M97" s="4">
-        <f>J97 - M81 - M92 + M40*M87</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="P97" s="4">
-        <f>M97 - P81 - P92 + P40*P87</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="S97" s="4">
-        <f>P97 - S81 - S92 + S40*S87</f>
+        <f t="shared" si="25"/>
         <v>0.43</v>
       </c>
       <c r="V97" s="4">
-        <f>S97 - V81 - V92 + V40*V87</f>
+        <f t="shared" si="26"/>
         <v>2.5791399999999998</v>
       </c>
       <c r="Y97" s="4">
-        <f>V97 - Y81 - Y92 + Y40*Y87</f>
+        <f t="shared" si="27"/>
         <v>7.7339817200000001</v>
       </c>
     </row>
@@ -10114,7 +10126,7 @@
       </c>
       <c r="Y99" s="4">
         <f>Y94*$G$20</f>
-        <v>13.943589655799297</v>
+        <v>13.963766094085869</v>
       </c>
     </row>
     <row r="100" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -10125,31 +10137,31 @@
         <v>213</v>
       </c>
       <c r="G100" s="4">
-        <f t="shared" ref="G100:G102" si="24">G95*$G$20</f>
+        <f t="shared" ref="G100:G102" si="28">G95*$G$20</f>
         <v>0</v>
       </c>
       <c r="J100" s="4">
-        <f t="shared" ref="J100:J102" si="25">J95*$G$20</f>
+        <f t="shared" ref="J100:J102" si="29">J95*$G$20</f>
         <v>0</v>
       </c>
       <c r="M100" s="4">
-        <f t="shared" ref="M100:M102" si="26">M95*$G$20</f>
+        <f t="shared" ref="M100:M102" si="30">M95*$G$20</f>
         <v>0.2</v>
       </c>
       <c r="P100" s="4">
-        <f t="shared" ref="P100:P102" si="27">P95*$G$20</f>
+        <f t="shared" ref="P100:P102" si="31">P95*$G$20</f>
         <v>1.1996</v>
       </c>
       <c r="S100" s="4">
-        <f t="shared" ref="S100:S102" si="28">S95*$G$20</f>
+        <f t="shared" ref="S100:S102" si="32">S95*$G$20</f>
         <v>3.5972008</v>
       </c>
       <c r="V100" s="4">
-        <f t="shared" ref="V100:V102" si="29">V95*$G$20</f>
+        <f t="shared" ref="V100:V102" si="33">V95*$G$20</f>
         <v>5.9960000000000004</v>
       </c>
       <c r="Y100" s="4">
-        <f t="shared" ref="Y100:Y102" si="30">Y95*$G$20</f>
+        <f t="shared" ref="Y100:Y102" si="34">Y95*$G$20</f>
         <v>9.1959999999999997</v>
       </c>
     </row>
@@ -10197,31 +10209,31 @@
         <v>215</v>
       </c>
       <c r="G102" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="J102" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M102" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="P102" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="S102" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.1075</v>
       </c>
       <c r="V102" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.64478499999999994</v>
       </c>
       <c r="Y102" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>1.93349543</v>
       </c>
     </row>
@@ -10773,7 +10785,7 @@
       </c>
       <c r="Y115" s="4">
         <f>SUM(Y94:Y97)</f>
-        <v>127.87394034319721</v>
+        <v>127.95464609634348</v>
       </c>
     </row>
     <row r="116" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -10840,7 +10852,7 @@
       </c>
       <c r="Y116" s="4">
         <f>Y114+Y115</f>
-        <v>3187501.5744820591</v>
+        <v>3187501.6551878126</v>
       </c>
     </row>
     <row r="117" spans="1:25" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
neared completion of python version. Working to add a fix for missing loss from conversion in young forests
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC78003-B42E-B647-9794-4D0FE38B4C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08D78AE-190A-D342-B014-DBE3E572ADE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12440" yWindow="560" windowWidth="33680" windowHeight="19400" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
+    <workbookView xWindow="6180" yWindow="760" windowWidth="31100" windowHeight="19860" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -790,9 +790,6 @@
     <t>n/af ref to arr_orig_biomass_c_ag_starting</t>
   </si>
   <si>
-    <t>arr_biomass_c_ag_converted_away</t>
-  </si>
-  <si>
     <t>average stock in target land use classes</t>
   </si>
   <si>
@@ -883,9 +880,6 @@
     <t>arr_orig_frac_stock_available</t>
   </si>
   <si>
-    <t>arr_orig_biomass_c_average_per_area_no_ds</t>
-  </si>
-  <si>
     <t>vec_total_removals_met</t>
   </si>
   <si>
@@ -896,6 +890,12 @@
   </si>
   <si>
     <t>vec_biomass_c_ag_min_reqd_per_area</t>
+  </si>
+  <si>
+    <t>arr_orig_biomass_c_ag_converted_away</t>
+  </si>
+  <si>
+    <t>arr_orig_biomass_c_ag_average_per_area_no_ds</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1049,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1180,9 +1180,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6351,8 +6348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40F0562-A765-A442-B9DB-CF71D123E451}">
   <dimension ref="A1:AM158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="J72" sqref="J72"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6578,7 +6575,7 @@
         <v>135</v>
       </c>
       <c r="Y5" s="29"/>
-      <c r="AB5" s="48" t="s">
+      <c r="AB5" s="47" t="s">
         <v>235</v>
       </c>
       <c r="AC5" s="21" t="s">
@@ -6673,7 +6670,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="50" t="s">
         <v>156</v>
       </c>
       <c r="B7" s="40" t="s">
@@ -6760,7 +6757,7 @@
       </c>
     </row>
     <row r="8" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="50" t="s">
         <v>157</v>
       </c>
       <c r="B8" s="41" t="s">
@@ -6849,7 +6846,7 @@
       </c>
     </row>
     <row r="9" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="50" t="s">
         <v>225</v>
       </c>
       <c r="B9" s="41" t="s">
@@ -6924,7 +6921,7 @@
       </c>
     </row>
     <row r="10" spans="1:39" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>224</v>
       </c>
       <c r="B10" s="40" t="s">
@@ -6973,7 +6970,7 @@
       </c>
     </row>
     <row r="11" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="50" t="s">
         <v>222</v>
       </c>
       <c r="B11" s="40" t="s">
@@ -7022,7 +7019,7 @@
       </c>
     </row>
     <row r="12" spans="1:39" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="50" t="s">
         <v>223</v>
       </c>
       <c r="B12" s="41" t="s">
@@ -7064,7 +7061,7 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="50" t="s">
         <v>158</v>
       </c>
       <c r="B13" s="40" t="s">
@@ -7134,7 +7131,7 @@
       <c r="AE13" s="19"/>
     </row>
     <row r="14" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="50" t="s">
         <v>226</v>
       </c>
       <c r="B14" s="41" t="s">
@@ -7176,17 +7173,17 @@
       </c>
     </row>
     <row r="15" spans="1:39" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="51" t="s">
-        <v>251</v>
+      <c r="A15" s="50" t="s">
+        <v>250</v>
       </c>
       <c r="B15" s="41" t="s">
         <v>162</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F15" s="4">
         <v>5</v>
@@ -7235,7 +7232,7 @@
       <c r="AE15" s="19"/>
     </row>
     <row r="16" spans="1:39" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="50" t="s">
         <v>227</v>
       </c>
       <c r="B16" s="41" t="s">
@@ -7277,7 +7274,7 @@
       </c>
     </row>
     <row r="17" spans="1:31" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="50" t="s">
         <v>228</v>
       </c>
       <c r="B17" s="41" t="s">
@@ -7304,7 +7301,7 @@
       </c>
     </row>
     <row r="18" spans="1:31" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="50" t="s">
         <v>229</v>
       </c>
       <c r="B18" s="41" t="s">
@@ -7329,7 +7326,7 @@
       </c>
     </row>
     <row r="19" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="50" t="s">
         <v>231</v>
       </c>
       <c r="B19" s="41" t="s">
@@ -7356,7 +7353,7 @@
       </c>
     </row>
     <row r="20" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="50" t="s">
         <v>233</v>
       </c>
       <c r="B20" s="41" t="s">
@@ -7376,8 +7373,8 @@
       <c r="AE20" s="19"/>
     </row>
     <row r="21" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="51" t="s">
-        <v>283</v>
+      <c r="A21" s="50" t="s">
+        <v>281</v>
       </c>
       <c r="B21" s="42" t="s">
         <v>175</v>
@@ -7405,7 +7402,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="50" t="s">
         <v>232</v>
       </c>
       <c r="B22" s="42" t="s">
@@ -7446,7 +7443,7 @@
       </c>
     </row>
     <row r="24" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="50" t="s">
         <v>159</v>
       </c>
       <c r="B24" s="41" t="s">
@@ -7509,8 +7506,8 @@
       </c>
     </row>
     <row r="25" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="51" t="s">
-        <v>282</v>
+      <c r="A25" s="50" t="s">
+        <v>280</v>
       </c>
       <c r="B25" s="43" t="s">
         <v>164</v>
@@ -7558,7 +7555,7 @@
       </c>
     </row>
     <row r="26" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="50" t="s">
         <v>160</v>
       </c>
       <c r="B26" s="43" t="s">
@@ -7664,8 +7661,8 @@
       </c>
     </row>
     <row r="28" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="51" t="s">
-        <v>281</v>
+      <c r="A28" s="50" t="s">
+        <v>279</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>162</v>
@@ -7684,7 +7681,7 @@
       </c>
     </row>
     <row r="29" spans="1:31" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="50" t="s">
         <v>234</v>
       </c>
       <c r="B29" s="42" t="s">
@@ -7726,7 +7723,7 @@
       <c r="Y31" s="8"/>
     </row>
     <row r="32" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="50" t="s">
         <v>169</v>
       </c>
       <c r="B32" s="41" t="s">
@@ -7851,7 +7848,7 @@
       </c>
     </row>
     <row r="37" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="48" t="s">
         <v>181</v>
       </c>
       <c r="B37" s="37" t="s">
@@ -7941,7 +7938,7 @@
       </c>
     </row>
     <row r="38" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="50"/>
+      <c r="A38" s="49"/>
       <c r="B38" s="37"/>
       <c r="E38" s="14" t="s">
         <v>69</v>
@@ -8026,7 +8023,7 @@
       </c>
     </row>
     <row r="39" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="50"/>
+      <c r="A39" s="49"/>
       <c r="B39" s="37"/>
       <c r="E39" s="14" t="s">
         <v>79</v>
@@ -8110,7 +8107,7 @@
       </c>
     </row>
     <row r="40" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
+      <c r="A40" s="49"/>
       <c r="B40" s="37"/>
       <c r="E40" s="14" t="s">
         <v>80</v>
@@ -8201,7 +8198,7 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="49" t="s">
         <v>192</v>
       </c>
       <c r="B42" s="37" t="s">
@@ -8239,7 +8236,7 @@
       </c>
     </row>
     <row r="43" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="50"/>
+      <c r="A43" s="49"/>
       <c r="B43" s="37"/>
       <c r="E43" s="14" t="s">
         <v>197</v>
@@ -8273,7 +8270,7 @@
       </c>
     </row>
     <row r="44" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="50"/>
+      <c r="A44" s="49"/>
       <c r="B44" s="37"/>
       <c r="E44" s="14" t="s">
         <v>198</v>
@@ -8307,7 +8304,7 @@
       </c>
     </row>
     <row r="45" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="50"/>
+      <c r="A45" s="49"/>
       <c r="B45" s="37"/>
       <c r="E45" s="14" t="s">
         <v>199</v>
@@ -8341,7 +8338,7 @@
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="50" t="s">
         <v>193</v>
       </c>
       <c r="B46" s="40" t="s">
@@ -8386,17 +8383,17 @@
       </c>
     </row>
     <row r="48" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="50" t="s">
-        <v>265</v>
+      <c r="A48" s="49" t="s">
+        <v>264</v>
       </c>
       <c r="B48" s="37" t="s">
         <v>175</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G48" s="4">
         <f>MIN(G42,G$15*F37)</f>
@@ -8428,11 +8425,11 @@
       </c>
     </row>
     <row r="49" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="50"/>
+      <c r="A49" s="49"/>
       <c r="B49" s="37"/>
       <c r="D49" s="28"/>
       <c r="E49" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G49" s="4">
         <f>MIN(G43,G$15*F38)</f>
@@ -8464,11 +8461,11 @@
       </c>
     </row>
     <row r="50" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="50"/>
+      <c r="A50" s="49"/>
       <c r="B50" s="37"/>
       <c r="D50" s="28"/>
       <c r="E50" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G50" s="4">
         <f>MIN(G44,G$15*F39)</f>
@@ -8500,11 +8497,11 @@
       </c>
     </row>
     <row r="51" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="50"/>
+      <c r="A51" s="49"/>
       <c r="B51" s="37"/>
       <c r="D51" s="28"/>
       <c r="E51" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G51" s="4">
         <f>MIN(G45,G$15*F40)</f>
@@ -8536,8 +8533,8 @@
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A52" s="51" t="s">
-        <v>266</v>
+      <c r="A52" s="50" t="s">
+        <v>265</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>175</v>
@@ -8576,7 +8573,7 @@
       <c r="E53" s="14"/>
     </row>
     <row r="54" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="50" t="s">
+      <c r="A54" s="49" t="s">
         <v>194</v>
       </c>
       <c r="B54" s="37" t="s">
@@ -8615,7 +8612,7 @@
       </c>
     </row>
     <row r="55" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="50"/>
+      <c r="A55" s="49"/>
       <c r="B55" s="37"/>
       <c r="E55" s="14" t="s">
         <v>201</v>
@@ -8650,7 +8647,7 @@
       </c>
     </row>
     <row r="56" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="50"/>
+      <c r="A56" s="49"/>
       <c r="B56" s="37"/>
       <c r="E56" s="14" t="s">
         <v>202</v>
@@ -8685,7 +8682,7 @@
       </c>
     </row>
     <row r="57" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="50"/>
+      <c r="A57" s="49"/>
       <c r="B57" s="37"/>
       <c r="E57" s="14" t="s">
         <v>203</v>
@@ -8720,7 +8717,7 @@
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A58" s="51" t="s">
+      <c r="A58" s="50" t="s">
         <v>195</v>
       </c>
       <c r="B58" s="40" t="s">
@@ -8760,7 +8757,7 @@
       <c r="E59" s="14"/>
     </row>
     <row r="60" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="50" t="s">
+      <c r="A60" s="49" t="s">
         <v>179</v>
       </c>
       <c r="B60" s="37" t="s">
@@ -8799,7 +8796,7 @@
       </c>
     </row>
     <row r="61" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="50"/>
+      <c r="A61" s="49"/>
       <c r="B61" s="37"/>
       <c r="E61" s="14" t="s">
         <v>91</v>
@@ -8832,7 +8829,7 @@
       </c>
     </row>
     <row r="62" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="50"/>
+      <c r="A62" s="49"/>
       <c r="B62" s="37"/>
       <c r="E62" s="14" t="s">
         <v>92</v>
@@ -8864,7 +8861,7 @@
       </c>
     </row>
     <row r="63" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="50"/>
+      <c r="A63" s="49"/>
       <c r="B63" s="37"/>
       <c r="E63" s="14" t="s">
         <v>93</v>
@@ -8903,7 +8900,7 @@
       <c r="E65" s="14"/>
     </row>
     <row r="66" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="50" t="s">
+      <c r="A66" s="49" t="s">
         <v>239</v>
       </c>
       <c r="B66" s="37" t="s">
@@ -8942,7 +8939,7 @@
       </c>
     </row>
     <row r="67" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="50"/>
+      <c r="A67" s="49"/>
       <c r="B67" s="37"/>
       <c r="E67" s="14" t="s">
         <v>110</v>
@@ -8973,7 +8970,7 @@
       </c>
     </row>
     <row r="68" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="50"/>
+      <c r="A68" s="49"/>
       <c r="B68" s="37"/>
       <c r="D68" s="28"/>
       <c r="E68" s="14" t="s">
@@ -9001,7 +8998,7 @@
       </c>
     </row>
     <row r="69" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="50"/>
+      <c r="A69" s="49"/>
       <c r="B69" s="37"/>
       <c r="D69" s="28"/>
       <c r="E69" s="14" t="s">
@@ -9033,7 +9030,7 @@
       <c r="E70" s="14"/>
     </row>
     <row r="71" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="50" t="s">
+      <c r="A71" s="49" t="s">
         <v>236</v>
       </c>
       <c r="B71" s="37" t="s">
@@ -9071,7 +9068,7 @@
       </c>
     </row>
     <row r="72" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="50"/>
+      <c r="A72" s="49"/>
       <c r="B72" s="37"/>
       <c r="E72" s="14" t="s">
         <v>128</v>
@@ -9105,7 +9102,7 @@
       </c>
     </row>
     <row r="73" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="50"/>
+      <c r="A73" s="49"/>
       <c r="B73" s="37"/>
       <c r="D73" s="28" t="s">
         <v>152</v>
@@ -9142,7 +9139,7 @@
       </c>
     </row>
     <row r="74" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="50"/>
+      <c r="A74" s="49"/>
       <c r="B74" s="37"/>
       <c r="D74" s="28"/>
       <c r="E74" s="14" t="s">
@@ -9177,7 +9174,7 @@
       </c>
     </row>
     <row r="75" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="51" t="s">
+      <c r="A75" s="50" t="s">
         <v>237</v>
       </c>
       <c r="B75" s="40" t="s">
@@ -9229,7 +9226,7 @@
       </c>
     </row>
     <row r="77" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="52" t="s">
+      <c r="A77" s="51" t="s">
         <v>238</v>
       </c>
       <c r="B77" s="37" t="s">
@@ -9264,7 +9261,7 @@
       </c>
     </row>
     <row r="78" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="52"/>
+      <c r="A78" s="51"/>
       <c r="B78" s="37"/>
       <c r="E78" s="14" t="s">
         <v>148</v>
@@ -9274,7 +9271,7 @@
         <v>0</v>
       </c>
       <c r="G78" s="4">
-        <f>IF(F78&gt;=F$129, IF(F77&lt;F$129, F$129-F77, 0),G71)</f>
+        <f>IF(F78&gt;=F$130, IF(F77&lt;F$130, F$130-F77, 0),G71)</f>
         <v>0</v>
       </c>
       <c r="I78" s="4">
@@ -9282,7 +9279,7 @@
         <v>0</v>
       </c>
       <c r="J78" s="4">
-        <f>IF(I78&gt;=I$129, IF(I77&lt;I$129, I$129-I77, 0),J71)</f>
+        <f>IF(I78&gt;=I$130, IF(I77&lt;I$130, I$130-I77, 0),J71)</f>
         <v>0</v>
       </c>
       <c r="L78" s="4">
@@ -9290,7 +9287,7 @@
         <v>0</v>
       </c>
       <c r="M78" s="4">
-        <f>IF(L78&gt;=L$129, IF(L77&lt;L$129, L$129-L77, 0),M71)</f>
+        <f>IF(L78&gt;=L$130, IF(L77&lt;L$130, L$130-L77, 0),M71)</f>
         <v>0</v>
       </c>
       <c r="O78" s="4">
@@ -9298,7 +9295,7 @@
         <v>0</v>
       </c>
       <c r="P78" s="4">
-        <f>IF(O78&gt;=O$129, IF(O77&lt;O$129, O$129-O77, 0),P71)</f>
+        <f>IF(O78&gt;=O$130, IF(O77&lt;O$130, O$130-O77, 0),P71)</f>
         <v>0</v>
       </c>
       <c r="R78" s="4">
@@ -9306,7 +9303,7 @@
         <v>6.7881033999999989</v>
       </c>
       <c r="S78" s="4">
-        <f>IF(R78&gt;=R$129, IF(R77&lt;R$129, R$129-R77, 0),S71)</f>
+        <f>IF(R78&gt;=R$130, IF(R77&lt;R$130, R$130-R77, 0),S71)</f>
         <v>0</v>
       </c>
       <c r="U78" s="4">
@@ -9314,7 +9311,7 @@
         <v>23.757527193199998</v>
       </c>
       <c r="V78" s="4">
-        <f>IF(U78&gt;=U$129, IF(U77&lt;U$129, U$129-U77, 0),V71)</f>
+        <f>IF(U78&gt;=U$130, IF(U77&lt;U$130, U$130-U77, 0),V71)</f>
         <v>23.757527193199998</v>
       </c>
       <c r="X78" s="4">
@@ -9322,12 +9319,12 @@
         <v>30.582999999999998</v>
       </c>
       <c r="Y78" s="4">
-        <f>IF(X78&gt;=X$129, IF(X77&lt;X$129, X$129-X77, 0),Y71)</f>
+        <f>IF(X78&gt;=X$130, IF(X77&lt;X$130, X$130-X77, 0),Y71)</f>
         <v>30.582999999999998</v>
       </c>
     </row>
     <row r="79" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="52"/>
+      <c r="A79" s="51"/>
       <c r="B79" s="37"/>
       <c r="D79" s="22">
         <v>0</v>
@@ -9340,7 +9337,7 @@
         <v>0</v>
       </c>
       <c r="G79" s="4">
-        <f>IF(F79&gt;=F$129, IF(F78&lt;F$129, F$129-F78, 0),G72)</f>
+        <f>IF(F79&gt;=F$130, IF(F78&lt;F$130, F$130-F78, 0),G72)</f>
         <v>0</v>
       </c>
       <c r="I79" s="4">
@@ -9348,7 +9345,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="4">
-        <f>IF(I79&gt;=I$129, IF(I78&lt;I$129, I$129-I78, 0),J72)</f>
+        <f>IF(I79&gt;=I$130, IF(I78&lt;I$130, I$130-I78, 0),J72)</f>
         <v>0</v>
       </c>
       <c r="L79" s="4">
@@ -9356,7 +9353,7 @@
         <v>0</v>
       </c>
       <c r="M79" s="4">
-        <f>IF(L79&gt;=L$129, IF(L78&lt;L$129, L$129-L78, 0),M72)</f>
+        <f>IF(L79&gt;=L$130, IF(L78&lt;L$130, L$130-L78, 0),M72)</f>
         <v>0</v>
       </c>
       <c r="O79" s="4">
@@ -9364,7 +9361,7 @@
         <v>0</v>
       </c>
       <c r="P79" s="4">
-        <f>IF(O79&gt;=O$129, IF(O78&lt;O$129, O$129-O78, 0),P72)</f>
+        <f>IF(O79&gt;=O$130, IF(O78&lt;O$130, O$130-O78, 0),P72)</f>
         <v>0</v>
       </c>
       <c r="R79" s="4">
@@ -9372,7 +9369,7 @@
         <v>6.7881033999999989</v>
       </c>
       <c r="S79" s="4">
-        <f>IF(R79&gt;=R$129, IF(R78&lt;R$129, R$129-R78, 0),S72)</f>
+        <f>IF(R79&gt;=R$130, IF(R78&lt;R$130, R$130-R78, 0),S72)</f>
         <v>0</v>
       </c>
       <c r="U79" s="4">
@@ -9380,7 +9377,7 @@
         <v>30.146330393199996</v>
       </c>
       <c r="V79" s="4">
-        <f>IF(U79&gt;=U$129, IF(U78&lt;U$129, U$129-U78, 0),V72)</f>
+        <f>IF(U79&gt;=U$130, IF(U78&lt;U$130, U$130-U78, 0),V72)</f>
         <v>6.3888031999999981</v>
       </c>
       <c r="X79" s="4">
@@ -9388,12 +9385,12 @@
         <v>46.567</v>
       </c>
       <c r="Y79" s="4">
-        <f>IF(X79&gt;=X$129, IF(X78&lt;X$129, X$129-X78, 0),Y72)</f>
+        <f>IF(X79&gt;=X$130, IF(X78&lt;X$130, X$130-X78, 0),Y72)</f>
         <v>15.984000000000002</v>
       </c>
     </row>
     <row r="80" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="52"/>
+      <c r="A80" s="51"/>
       <c r="B80" s="37"/>
       <c r="D80" s="22">
         <v>1</v>
@@ -9406,7 +9403,7 @@
         <v>0</v>
       </c>
       <c r="G80" s="4">
-        <f>IF(F80&gt;=F$129, IF(F79&lt;F$129, F$129-F79, 0),G73)</f>
+        <f>IF(F80&gt;=F$130, IF(F79&lt;F$130, F$130-F79, 0),G73)</f>
         <v>0</v>
       </c>
       <c r="I80" s="4">
@@ -9414,7 +9411,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="4">
-        <f>IF(I80&gt;=I$129, IF(I79&lt;I$129, I$129-I79, 0),J73)</f>
+        <f>IF(I80&gt;=I$130, IF(I79&lt;I$130, I$130-I79, 0),J73)</f>
         <v>0</v>
       </c>
       <c r="L80" s="4">
@@ -9422,7 +9419,7 @@
         <v>0</v>
       </c>
       <c r="M80" s="4">
-        <f>IF(L80&gt;=L$129, IF(L79&lt;L$129, L$129-L79, 0),M73)</f>
+        <f>IF(L80&gt;=L$130, IF(L79&lt;L$130, L$130-L79, 0),M73)</f>
         <v>0</v>
       </c>
       <c r="O80" s="4">
@@ -9430,7 +9427,7 @@
         <v>0</v>
       </c>
       <c r="P80" s="4">
-        <f>IF(O80&gt;=O$129, IF(O79&lt;O$129, O$129-O79, 0),P73)</f>
+        <f>IF(O80&gt;=O$130, IF(O79&lt;O$130, O$130-O79, 0),P73)</f>
         <v>0</v>
       </c>
       <c r="R80" s="4">
@@ -9438,7 +9435,7 @@
         <v>6.7881033999999989</v>
       </c>
       <c r="S80" s="4">
-        <f>IF(R80&gt;=R$129, IF(R79&lt;R$129, R$129-R79, 0),S73)</f>
+        <f>IF(R80&gt;=R$130, IF(R79&lt;R$130, R$130-R79, 0),S73)</f>
         <v>0</v>
       </c>
       <c r="U80" s="4">
@@ -9446,7 +9443,7 @@
         <v>30.146330393199996</v>
       </c>
       <c r="V80" s="4">
-        <f>IF(U80&gt;=U$129, IF(U79&lt;U$129, U$129-U79, 0),V73)</f>
+        <f>IF(U80&gt;=U$130, IF(U79&lt;U$130, U$130-U79, 0),V73)</f>
         <v>0</v>
       </c>
       <c r="X80" s="4">
@@ -9454,12 +9451,12 @@
         <v>53.914123679999996</v>
       </c>
       <c r="Y80" s="4">
-        <f>IF(X80&gt;=X$129, IF(X79&lt;X$129, X$129-X79, 0),Y73)</f>
+        <f>IF(X80&gt;=X$130, IF(X79&lt;X$130, X$130-X79, 0),Y73)</f>
         <v>7.3471236799999957</v>
       </c>
     </row>
     <row r="81" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="52"/>
+      <c r="A81" s="51"/>
       <c r="B81" s="37"/>
       <c r="D81" s="22">
         <v>2</v>
@@ -9472,7 +9469,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="4">
-        <f>IF(F81&gt;=F$129, IF(F80&lt;F$129, F$129-F80, 0),G74)</f>
+        <f>IF(F81&gt;=F$130, IF(F80&lt;F$130, F$130-F80, 0),G74)</f>
         <v>0</v>
       </c>
       <c r="I81" s="4">
@@ -9480,7 +9477,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4">
-        <f>IF(I81&gt;=I$129, IF(I80&lt;I$129, I$129-I80, 0),J74)</f>
+        <f>IF(I81&gt;=I$130, IF(I80&lt;I$130, I$130-I80, 0),J74)</f>
         <v>0</v>
       </c>
       <c r="L81" s="4">
@@ -9488,7 +9485,7 @@
         <v>0</v>
       </c>
       <c r="M81" s="4">
-        <f>IF(L81&gt;=L$129, IF(L80&lt;L$129, L$129-L80, 0),M74)</f>
+        <f>IF(L81&gt;=L$130, IF(L80&lt;L$130, L$130-L80, 0),M74)</f>
         <v>0</v>
       </c>
       <c r="O81" s="4">
@@ -9496,7 +9493,7 @@
         <v>0</v>
       </c>
       <c r="P81" s="4">
-        <f>IF(O81&gt;=O$129, IF(O80&lt;O$129, O$129-O80, 0),P74)</f>
+        <f>IF(O81&gt;=O$130, IF(O80&lt;O$130, O$130-O80, 0),P74)</f>
         <v>0</v>
       </c>
       <c r="R81" s="4">
@@ -9504,7 +9501,7 @@
         <v>6.7881033999999989</v>
       </c>
       <c r="S81" s="4">
-        <f>IF(R81&gt;=R$129, IF(R80&lt;R$129, R$129-R80, 0),S74)</f>
+        <f>IF(R81&gt;=R$130, IF(R80&lt;R$130, R$130-R80, 0),S74)</f>
         <v>0</v>
       </c>
       <c r="U81" s="4">
@@ -9512,7 +9509,7 @@
         <v>30.146330393199996</v>
       </c>
       <c r="V81" s="4">
-        <f>IF(U81&gt;=U$129, IF(U80&lt;U$129, U$129-U80, 0),V74)</f>
+        <f>IF(U81&gt;=U$130, IF(U80&lt;U$130, U$130-U80, 0),V74)</f>
         <v>0</v>
       </c>
       <c r="X81" s="4">
@@ -9520,7 +9517,7 @@
         <v>53.914123679999996</v>
       </c>
       <c r="Y81" s="4">
-        <f>IF(X81&gt;=X$129, IF(X80&lt;X$129, X$129-X80, 0),Y74)</f>
+        <f>IF(X81&gt;=X$130, IF(X80&lt;X$130, X$130-X80, 0),Y74)</f>
         <v>0</v>
       </c>
     </row>
@@ -9552,7 +9549,7 @@
       </c>
     </row>
     <row r="84" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="49" t="s">
+      <c r="A84" s="48" t="s">
         <v>182</v>
       </c>
       <c r="B84" s="37" t="s">
@@ -9615,7 +9612,7 @@
       </c>
     </row>
     <row r="85" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="49"/>
+      <c r="A85" s="48"/>
       <c r="B85" s="37"/>
       <c r="E85" s="14" t="s">
         <v>132</v>
@@ -9674,7 +9671,7 @@
       </c>
     </row>
     <row r="86" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="49"/>
+      <c r="A86" s="48"/>
       <c r="B86" s="37"/>
       <c r="E86" s="14" t="s">
         <v>133</v>
@@ -9733,7 +9730,7 @@
       </c>
     </row>
     <row r="87" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="49"/>
+      <c r="A87" s="48"/>
       <c r="B87" s="37"/>
       <c r="E87" s="14" t="s">
         <v>134</v>
@@ -9795,7 +9792,7 @@
       <c r="E88" s="14"/>
     </row>
     <row r="89" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="49" t="s">
+      <c r="A89" s="48" t="s">
         <v>205</v>
       </c>
       <c r="B89" s="37" t="s">
@@ -9809,32 +9806,32 @@
         <v>0</v>
       </c>
       <c r="J89" s="4">
-        <f>(G94-J78)*$F$29</f>
+        <f>(G94-J78-J42)*$F$29</f>
         <v>0</v>
       </c>
       <c r="M89" s="4">
-        <f>(J94-M78)*$F$29</f>
+        <f>(J94-M78-M42)*$F$29</f>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="P89" s="4">
-        <f>(M94-P78)*$F$29</f>
+        <f>(M94-P78-P42)*$F$29</f>
         <v>1.01966E-2</v>
       </c>
       <c r="S89" s="4">
-        <f>(P94-S78)*$F$29</f>
+        <f>(P94-S78-S42)*$F$29</f>
         <v>3.0576206799999998E-2</v>
       </c>
       <c r="V89" s="4">
-        <f>(S94-V78)*$F$29</f>
+        <f>(S94-V78-V42)*$F$29</f>
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="Y89" s="4">
-        <f>(V94-Y78)*$F$29</f>
+        <f>(V94-Y78-Y42)*$F$29</f>
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="90" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="49"/>
+      <c r="A90" s="48"/>
       <c r="B90" s="37"/>
       <c r="E90" s="14" t="s">
         <v>207</v>
@@ -9844,32 +9841,32 @@
         <v>0</v>
       </c>
       <c r="J90" s="4">
-        <f>(G95-J79)*$F$29</f>
+        <f t="shared" ref="J90:J92" si="16">(G95-J79-J43)*$F$29</f>
         <v>0</v>
       </c>
       <c r="M90" s="4">
-        <f t="shared" ref="M90:M92" si="16">(J95-M79)*$F$29</f>
+        <f t="shared" ref="M90:M92" si="17">(J95-M79-M43)*$F$29</f>
         <v>0</v>
       </c>
       <c r="P90" s="4">
-        <f t="shared" ref="P90:P92" si="17">(M95-P79)*$F$29</f>
+        <f t="shared" ref="P90:P92" si="18">(M95-P79-P43)*$F$29</f>
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="S90" s="4">
-        <f t="shared" ref="S90:S92" si="18">(P95-S79)*$F$29</f>
+        <f t="shared" ref="S90:S92" si="19">(P95-S79-S43)*$F$29</f>
         <v>9.5968000000000008E-3</v>
       </c>
       <c r="V90" s="4">
-        <f t="shared" ref="V90:V92" si="19">(S95-V79)*$F$29</f>
+        <f t="shared" ref="V90:V92" si="20">(S95-V79-V43)*$F$29</f>
         <v>1.6000000000000004E-2</v>
       </c>
       <c r="Y90" s="4">
-        <f t="shared" ref="Y90:Y92" si="20">(V95-Y79)*$F$29</f>
+        <f t="shared" ref="Y90:Y92" si="21">(V95-Y79-Y43)*$F$29</f>
         <v>1.6E-2</v>
       </c>
     </row>
     <row r="91" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="49"/>
+      <c r="A91" s="48"/>
       <c r="B91" s="37"/>
       <c r="E91" s="14" t="s">
         <v>208</v>
@@ -9879,32 +9876,32 @@
         <v>0</v>
       </c>
       <c r="J91" s="4">
-        <f t="shared" ref="J90:J92" si="21">(G96-J80)*$F$29</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M91" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="P91" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="S91" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.8400000000000001E-3</v>
       </c>
       <c r="V91" s="4">
-        <f t="shared" si="19"/>
+        <f>(S96-V80-V44)*$F$29</f>
         <v>1.1036320000000002E-2</v>
       </c>
       <c r="Y91" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.8400000000000007E-2</v>
       </c>
     </row>
     <row r="92" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="49"/>
+      <c r="A92" s="48"/>
       <c r="B92" s="37"/>
       <c r="E92" s="14" t="s">
         <v>209</v>
@@ -9914,27 +9911,27 @@
         <v>0</v>
       </c>
       <c r="J92" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M92" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P92" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S92" s="4">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V92" s="4">
+        <f t="shared" si="20"/>
+        <v>8.5999999999999998E-4</v>
+      </c>
+      <c r="Y92" s="4">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="M92" s="4">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P92" s="4">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="S92" s="4">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="V92" s="4">
-        <f t="shared" si="19"/>
-        <v>8.5999999999999998E-4</v>
-      </c>
-      <c r="Y92" s="4">
-        <f t="shared" si="20"/>
         <v>5.1582799999999995E-3</v>
       </c>
     </row>
@@ -9942,7 +9939,7 @@
       <c r="E93" s="14"/>
     </row>
     <row r="94" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="47" t="s">
+      <c r="A94" s="48" t="s">
         <v>210</v>
       </c>
       <c r="B94" s="37" t="s">
@@ -9981,7 +9978,7 @@
       </c>
     </row>
     <row r="95" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="47"/>
+      <c r="A95" s="48"/>
       <c r="B95" s="37"/>
       <c r="E95" s="14" t="s">
         <v>71</v>
@@ -10016,7 +10013,7 @@
       </c>
     </row>
     <row r="96" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="47"/>
+      <c r="A96" s="48"/>
       <c r="B96" s="37"/>
       <c r="E96" s="14" t="s">
         <v>72</v>
@@ -10051,7 +10048,7 @@
       </c>
     </row>
     <row r="97" spans="1:25" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="47"/>
+      <c r="A97" s="48"/>
       <c r="B97" s="37"/>
       <c r="E97" s="14" t="s">
         <v>81</v>
@@ -10090,7 +10087,7 @@
       <c r="E98" s="14"/>
     </row>
     <row r="99" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="47" t="s">
+      <c r="A99" s="48" t="s">
         <v>211</v>
       </c>
       <c r="B99" s="37" t="s">
@@ -10130,7 +10127,7 @@
       </c>
     </row>
     <row r="100" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="47"/>
+      <c r="A100" s="48"/>
       <c r="B100" s="37"/>
       <c r="D100" s="35"/>
       <c r="E100" s="14" t="s">
@@ -10166,7 +10163,7 @@
       </c>
     </row>
     <row r="101" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="47"/>
+      <c r="A101" s="48"/>
       <c r="B101" s="37"/>
       <c r="D101" s="35"/>
       <c r="E101" s="14" t="s">
@@ -10202,7 +10199,7 @@
       </c>
     </row>
     <row r="102" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="47"/>
+      <c r="A102" s="48"/>
       <c r="B102" s="37"/>
       <c r="D102" s="35"/>
       <c r="E102" s="14" t="s">
@@ -10260,7 +10257,7 @@
       <c r="G105" s="8"/>
     </row>
     <row r="106" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="46" t="s">
+      <c r="A106" s="50" t="s">
         <v>240</v>
       </c>
       <c r="B106" s="44" t="s">
@@ -10328,7 +10325,7 @@
       </c>
     </row>
     <row r="107" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="46" t="s">
+      <c r="A107" s="50" t="s">
         <v>241</v>
       </c>
       <c r="B107" s="40" t="s">
@@ -10395,7 +10392,7 @@
       </c>
     </row>
     <row r="108" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="46" t="s">
+      <c r="A108" s="50" t="s">
         <v>184</v>
       </c>
       <c r="B108" s="40" t="s">
@@ -10460,7 +10457,7 @@
       </c>
     </row>
     <row r="109" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="46" t="s">
+      <c r="A109" s="50" t="s">
         <v>185</v>
       </c>
       <c r="B109" s="43" t="s">
@@ -10527,7 +10524,7 @@
       </c>
     </row>
     <row r="110" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="46" t="s">
+      <c r="A110" s="50" t="s">
         <v>242</v>
       </c>
       <c r="B110" s="43" t="s">
@@ -10545,56 +10542,56 @@
         <v>25000000</v>
       </c>
       <c r="I110" s="4">
-        <f>F110 - F130 - F118 - F142+I109*I7</f>
+        <f>F110 - F131 - F119 - F142+I109*I7</f>
         <v>1421423.1421982395</v>
       </c>
       <c r="J110" s="4">
-        <f>G110 - G130 - G118 - G142 + J109*J7</f>
+        <f>G110 - G131 - G119 - G142 + J109*J7</f>
         <v>23256357.107801761</v>
       </c>
       <c r="L110" s="4">
-        <f>I110 - I130 - I118 - I142+L109*L7</f>
+        <f>I110 - I131 - I119 - I142+L109*L7</f>
         <v>1339098.0188325029</v>
       </c>
       <c r="M110" s="4">
-        <f>J110 - J130 - J118 - J142 + M109*M7</f>
+        <f>J110 - J131 - J119 - J142 + M109*M7</f>
         <v>21469509.138674762</v>
       </c>
       <c r="O110" s="4">
-        <f>L110 - L130 - L118 - L142+O109*O7</f>
+        <f>L110 - L131 - L119 - L142+O109*O7</f>
         <v>1262299.2941418488</v>
       </c>
       <c r="P110" s="4">
-        <f>M110 - M130 - M118 - M142 + P109*P7</f>
+        <f>M110 - M131 - M119 - M142 + P109*P7</f>
         <v>19621955.062304016</v>
       </c>
       <c r="R110" s="4">
-        <f>O110 - O130 - O118 - O142+R109*R7</f>
+        <f>O110 - O131 - O119 - O142+R109*R7</f>
         <v>1188284.3985212983</v>
       </c>
       <c r="S110" s="4">
-        <f>P110 - P130 - P118 - P142 + S109*S7</f>
+        <f>P110 - P131 - P119 - P142 + S109*S7</f>
         <v>17672326.76258811</v>
       </c>
       <c r="U110" s="4">
-        <f>R110 - R130 - R118 - R142+U109*U7</f>
+        <f>R110 - R131 - R119 - R142+U109*U7</f>
         <v>1097914.9514073269</v>
       </c>
       <c r="V110" s="4">
-        <f>S110 - S130 - S118 - S142 + V109*V7</f>
+        <f>S110 - S131 - S119 - S142 + V109*V7</f>
         <v>14958270.076713715</v>
       </c>
       <c r="X110" s="4">
-        <f>U110 - U130 - U118 - U142+X109*X7</f>
+        <f>U110 - U131 - U119 - U142+X109*X7</f>
         <v>819907.25090646883</v>
       </c>
       <c r="Y110" s="4">
-        <f>V110 - V130 - V118 - V142 + Y109*Y7</f>
+        <f>V110 - V131 - V119 - V142 + Y109*Y7</f>
         <v>3187373.7005417161</v>
       </c>
     </row>
     <row r="111" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="46" t="s">
+      <c r="A111" s="50" t="s">
         <v>245</v>
       </c>
       <c r="B111" s="43" t="s">
@@ -10660,1040 +10657,1040 @@
         <v>12.782217278399568</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="E112" s="13"/>
-    </row>
-    <row r="113" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="E113" s="11" t="s">
+    <row r="112" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="A112" s="50" t="s">
+        <v>283</v>
+      </c>
+      <c r="B112" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E112" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F112" s="4">
+        <f>MAX(F111-$F21,0)</f>
+        <v>149.85</v>
+      </c>
+      <c r="G112" s="4">
+        <f>MAX(G111-$G21,0)</f>
+        <v>99.9</v>
+      </c>
+      <c r="I112" s="4">
+        <f>MAX(I111-$F21,0)</f>
+        <v>142.7065972058532</v>
+      </c>
+      <c r="J112" s="4">
+        <f>MAX(J111-$G21,0)</f>
+        <v>92.96265349260409</v>
+      </c>
+      <c r="L112" s="4">
+        <f>MAX(L111-$F21,0)</f>
+        <v>135.27657957448451</v>
+      </c>
+      <c r="M112" s="4">
+        <f>MAX(M111-$G21,0)</f>
+        <v>85.850234751890639</v>
+      </c>
+      <c r="O112" s="4">
+        <f>MAX(O111-$F21,0)</f>
+        <v>128.2629495566479</v>
+      </c>
+      <c r="P112" s="4">
+        <f>MAX(P111-$G21,0)</f>
+        <v>78.483377636421963</v>
+      </c>
+      <c r="R112" s="4">
+        <f>MAX(R111-$F21,0)</f>
+        <v>121.60045066816581</v>
+      </c>
+      <c r="S112" s="4">
+        <f>MAX(S111-$G21,0)</f>
+        <v>70.729833439897206</v>
+      </c>
+      <c r="U112" s="4">
+        <f>MAX(U111-$F21,0)</f>
+        <v>113.50579207115184</v>
+      </c>
+      <c r="V112" s="4">
+        <f>MAX(V111-$G21,0)</f>
+        <v>59.861397697928425</v>
+      </c>
+      <c r="X112" s="4">
+        <f>MAX(X111-$F21,0)</f>
+        <v>85.596418208164479</v>
+      </c>
+      <c r="Y112" s="4">
+        <f>MAX(Y111-$G21,0)</f>
+        <v>12.682217278399568</v>
+      </c>
+    </row>
+    <row r="113" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="E113" s="13"/>
+    </row>
+    <row r="114" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="E114" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F113" s="12"/>
-      <c r="G113" s="12"/>
-      <c r="I113" s="12"/>
-      <c r="J113" s="12"/>
-      <c r="L113" s="12"/>
-      <c r="M113" s="12"/>
-      <c r="O113" s="12"/>
-      <c r="P113" s="12"/>
-      <c r="R113" s="12"/>
-      <c r="S113" s="12"/>
-      <c r="U113" s="12"/>
-      <c r="V113" s="12"/>
-      <c r="X113" s="12"/>
-      <c r="Y113" s="12"/>
-    </row>
-    <row r="114" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="46" t="s">
+      <c r="F114" s="12"/>
+      <c r="G114" s="12"/>
+      <c r="I114" s="12"/>
+      <c r="J114" s="12"/>
+      <c r="L114" s="12"/>
+      <c r="M114" s="12"/>
+      <c r="O114" s="12"/>
+      <c r="P114" s="12"/>
+      <c r="R114" s="12"/>
+      <c r="S114" s="12"/>
+      <c r="U114" s="12"/>
+      <c r="V114" s="12"/>
+      <c r="X114" s="12"/>
+      <c r="Y114" s="12"/>
+    </row>
+    <row r="115" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="46" t="s">
         <v>247</v>
       </c>
-      <c r="B114" s="44" t="s">
+      <c r="B115" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="E114" s="10" t="s">
+      <c r="E115" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="F114" s="4">
+      <c r="F115" s="4">
         <f>F111*F7</f>
         <v>1500000</v>
       </c>
-      <c r="G114" s="4">
+      <c r="G115" s="4">
         <f>G111*G7</f>
         <v>25000000</v>
       </c>
-      <c r="I114" s="4">
+      <c r="I115" s="4">
         <f>I111*I7</f>
         <v>1421423.1421982395</v>
       </c>
-      <c r="J114" s="4">
+      <c r="J115" s="4">
         <f>J111*J7</f>
         <v>23256357.107801761</v>
       </c>
-      <c r="L114" s="4">
+      <c r="L115" s="4">
         <f>L111*L7</f>
         <v>1339098.0188325029</v>
       </c>
-      <c r="M114" s="4">
+      <c r="M115" s="4">
         <f>M111*M7</f>
         <v>21469509.138674762</v>
       </c>
-      <c r="O114" s="4">
+      <c r="O115" s="4">
         <f>O111*O7</f>
         <v>1262299.2941418488</v>
       </c>
-      <c r="P114" s="4">
+      <c r="P115" s="4">
         <f>P111*P7</f>
         <v>19621955.062304016</v>
       </c>
-      <c r="R114" s="4">
+      <c r="R115" s="4">
         <f>R111*R7</f>
         <v>1188284.3985212983</v>
       </c>
-      <c r="S114" s="4">
+      <c r="S115" s="4">
         <f>S111*S7</f>
         <v>17672326.76258811</v>
       </c>
-      <c r="U114" s="4">
+      <c r="U115" s="4">
         <f>U111*U7</f>
         <v>1097914.9514073269</v>
       </c>
-      <c r="V114" s="4">
+      <c r="V115" s="4">
         <f>V111*V7</f>
         <v>14958270.076713715</v>
       </c>
-      <c r="X114" s="4">
+      <c r="X115" s="4">
         <f>X111*X7</f>
         <v>819907.25090646883</v>
       </c>
-      <c r="Y114" s="4">
+      <c r="Y115" s="4">
         <f>Y111*Y7</f>
         <v>3187373.7005417161</v>
       </c>
     </row>
-    <row r="115" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A115" s="46" t="s">
+    <row r="116" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="50" t="s">
         <v>246</v>
       </c>
-      <c r="B115" s="43" t="s">
+      <c r="B116" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="E115" s="10" t="s">
+      <c r="E116" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="G115" s="4">
+      <c r="G116" s="4">
         <f>SUM(G94:G97)</f>
         <v>0</v>
       </c>
-      <c r="J115" s="4">
+      <c r="J116" s="4">
         <f>SUM(J94:J97)</f>
         <v>0.85</v>
       </c>
-      <c r="M115" s="4">
+      <c r="M116" s="4">
         <f>SUM(M94:M97)</f>
         <v>5.8982999999999999</v>
       </c>
-      <c r="P115" s="4">
+      <c r="P116" s="4">
         <f>SUM(P94:P97)</f>
         <v>21.0065034</v>
       </c>
-      <c r="S115" s="4">
+      <c r="S116" s="4">
         <f>SUM(S94:S97)</f>
         <v>52.594490393199997</v>
       </c>
-      <c r="V115" s="4">
+      <c r="V116" s="4">
         <f>SUM(V94:V97)</f>
         <v>82.193263680000001</v>
       </c>
-      <c r="Y115" s="4">
+      <c r="Y116" s="4">
         <f>SUM(Y94:Y97)</f>
         <v>127.95464609634348</v>
       </c>
     </row>
-    <row r="116" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="46" t="s">
+    <row r="117" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="50" t="s">
         <v>243</v>
-      </c>
-      <c r="B116" s="43" t="s">
-        <v>164</v>
-      </c>
-      <c r="E116" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="F116" s="4">
-        <f>F114+F115</f>
-        <v>1500000</v>
-      </c>
-      <c r="G116" s="4">
-        <f>G114+G115</f>
-        <v>25000000</v>
-      </c>
-      <c r="I116" s="4">
-        <f>I114+I115</f>
-        <v>1421423.1421982395</v>
-      </c>
-      <c r="J116" s="4">
-        <f>J114+J115</f>
-        <v>23256357.957801763</v>
-      </c>
-      <c r="L116" s="4">
-        <f>L114+L115</f>
-        <v>1339098.0188325029</v>
-      </c>
-      <c r="M116" s="4">
-        <f>M114+M115</f>
-        <v>21469515.036974762</v>
-      </c>
-      <c r="O116" s="4">
-        <f>O114+O115</f>
-        <v>1262299.2941418488</v>
-      </c>
-      <c r="P116" s="4">
-        <f>P114+P115</f>
-        <v>19621976.068807416</v>
-      </c>
-      <c r="R116" s="4">
-        <f>R114+R115</f>
-        <v>1188284.3985212983</v>
-      </c>
-      <c r="S116" s="4">
-        <f>S114+S115</f>
-        <v>17672379.357078504</v>
-      </c>
-      <c r="U116" s="4">
-        <f>U114+U115</f>
-        <v>1097914.9514073269</v>
-      </c>
-      <c r="V116" s="4">
-        <f>V114+V115</f>
-        <v>14958352.269977394</v>
-      </c>
-      <c r="X116" s="4">
-        <f>X114+X115</f>
-        <v>819907.25090646883</v>
-      </c>
-      <c r="Y116" s="4">
-        <f>Y114+Y115</f>
-        <v>3187501.6551878126</v>
-      </c>
-    </row>
-    <row r="117" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" s="46" t="s">
-        <v>244</v>
       </c>
       <c r="B117" s="43" t="s">
         <v>164</v>
       </c>
       <c r="E117" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F117" s="4">
+        <f>F115+F116</f>
+        <v>1500000</v>
+      </c>
+      <c r="G117" s="4">
+        <f>G115+G116</f>
+        <v>25000000</v>
+      </c>
+      <c r="I117" s="4">
+        <f>I115+I116</f>
+        <v>1421423.1421982395</v>
+      </c>
+      <c r="J117" s="4">
+        <f>J115+J116</f>
+        <v>23256357.957801763</v>
+      </c>
+      <c r="L117" s="4">
+        <f>L115+L116</f>
+        <v>1339098.0188325029</v>
+      </c>
+      <c r="M117" s="4">
+        <f>M115+M116</f>
+        <v>21469515.036974762</v>
+      </c>
+      <c r="O117" s="4">
+        <f>O115+O116</f>
+        <v>1262299.2941418488</v>
+      </c>
+      <c r="P117" s="4">
+        <f>P115+P116</f>
+        <v>19621976.068807416</v>
+      </c>
+      <c r="R117" s="4">
+        <f>R115+R116</f>
+        <v>1188284.3985212983</v>
+      </c>
+      <c r="S117" s="4">
+        <f>S115+S116</f>
+        <v>17672379.357078504</v>
+      </c>
+      <c r="U117" s="4">
+        <f>U115+U116</f>
+        <v>1097914.9514073269</v>
+      </c>
+      <c r="V117" s="4">
+        <f>V115+V116</f>
+        <v>14958352.269977394</v>
+      </c>
+      <c r="X117" s="4">
+        <f>X115+X116</f>
+        <v>819907.25090646883</v>
+      </c>
+      <c r="Y117" s="4">
+        <f>Y115+Y116</f>
+        <v>3187501.6551878126</v>
+      </c>
+    </row>
+    <row r="118" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="B118" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="E118" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="F117" s="4">
+      <c r="F118" s="4">
         <f>F110*$F$20</f>
         <v>450000</v>
       </c>
-      <c r="G117" s="4">
+      <c r="G118" s="4">
         <f>G110*$G$20</f>
         <v>6250000</v>
       </c>
-      <c r="I117" s="4">
+      <c r="I118" s="4">
         <f>I110*$F$20</f>
         <v>426426.94265947182</v>
       </c>
-      <c r="J117" s="4">
+      <c r="J118" s="4">
         <f>J110*$G$20</f>
         <v>5814089.2769504404</v>
       </c>
-      <c r="L117" s="4">
+      <c r="L118" s="4">
         <f>L110*$F$20</f>
         <v>401729.40564975084</v>
       </c>
-      <c r="M117" s="4">
+      <c r="M118" s="4">
         <f>M110*$G$20</f>
         <v>5367377.2846686905</v>
       </c>
-      <c r="O117" s="4">
+      <c r="O118" s="4">
         <f>O110*$F$20</f>
         <v>378689.78824255464</v>
       </c>
-      <c r="P117" s="4">
+      <c r="P118" s="4">
         <f>P110*$G$20</f>
         <v>4905488.7655760041</v>
       </c>
-      <c r="R117" s="4">
+      <c r="R118" s="4">
         <f>R110*$F$20</f>
         <v>356485.31955638947</v>
       </c>
-      <c r="S117" s="4">
+      <c r="S118" s="4">
         <f>S110*$G$20</f>
         <v>4418081.6906470275</v>
       </c>
-      <c r="U117" s="4">
+      <c r="U118" s="4">
         <f>U110*$F$20</f>
         <v>329374.48542219802</v>
       </c>
-      <c r="V117" s="4">
+      <c r="V118" s="4">
         <f>V110*$G$20</f>
         <v>3739567.5191784287</v>
       </c>
-      <c r="X117" s="4">
+      <c r="X118" s="4">
         <f>X110*$F$20</f>
         <v>245972.17527194065</v>
       </c>
-      <c r="Y117" s="4">
+      <c r="Y118" s="4">
         <f>Y110*$G$20</f>
         <v>796843.42513542902</v>
       </c>
     </row>
-    <row r="118" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="46" t="s">
-        <v>248</v>
-      </c>
-      <c r="B118" s="40" t="s">
+    <row r="119" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="50" t="s">
+        <v>282</v>
+      </c>
+      <c r="B119" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="E118" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="F118" s="4">
+      <c r="E119" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="F119" s="4">
         <f>F9*F111</f>
         <v>7500</v>
       </c>
-      <c r="G118" s="4">
+      <c r="G119" s="4">
         <f>G9*G111</f>
         <v>10000</v>
       </c>
-      <c r="I118" s="4">
+      <c r="I119" s="4">
         <f>I9*I111</f>
         <v>8857.1090267628988</v>
       </c>
-      <c r="J118" s="4">
+      <c r="J119" s="4">
         <f>J9*J111</f>
         <v>10236.891884186449</v>
       </c>
-      <c r="L118" s="4">
+      <c r="L119" s="4">
         <f>L9*L111</f>
         <v>7854.741615320102</v>
       </c>
-      <c r="M118" s="4">
+      <c r="M119" s="4">
         <f>M9*M111</f>
         <v>8079.3220666777197</v>
       </c>
-      <c r="O118" s="4">
+      <c r="O119" s="4">
         <f>O9*O111</f>
         <v>8988.9064689653533</v>
       </c>
-      <c r="P118" s="4">
+      <c r="P119" s="4">
         <f>P9*P111</f>
         <v>15088.008506193015</v>
       </c>
-      <c r="R118" s="4">
+      <c r="R119" s="4">
         <f>R9*R111</f>
         <v>12175.045066816581</v>
       </c>
-      <c r="S118" s="4">
+      <c r="S119" s="4">
         <f>S9*S111</f>
         <v>2762.363504155991</v>
       </c>
-      <c r="U118" s="4">
+      <c r="U119" s="4">
         <f>U9*U111</f>
         <v>11138.267622972882</v>
       </c>
-      <c r="V118" s="4">
+      <c r="V119" s="4">
         <f>V9*V111</f>
         <v>6295.9467582824846</v>
       </c>
-      <c r="X118" s="4">
+      <c r="X119" s="4">
         <f>X9*X111</f>
         <v>8403.1489844001189</v>
       </c>
-      <c r="Y118" s="4">
+      <c r="Y119" s="4">
         <f>Y9*Y111</f>
         <v>1342.1328142319546</v>
       </c>
     </row>
-    <row r="119" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="46" t="s">
-        <v>267</v>
-      </c>
-      <c r="B119" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="E119" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="F119" s="4">
-        <f>MIN(F118,F9*F15)</f>
-        <v>250</v>
-      </c>
-      <c r="G119" s="4">
-        <f>MIN(G118,G9*G15)</f>
-        <v>1000</v>
-      </c>
-      <c r="I119" s="4">
-        <f>MIN(I118,I9*I15)</f>
-        <v>316.2</v>
-      </c>
-      <c r="J119" s="4">
-        <f>MIN(J118,J9*J15)</f>
-        <v>1078</v>
-      </c>
-      <c r="L119" s="4">
-        <f>MIN(L118,L9*L15)</f>
-        <v>301.60000000000002</v>
-      </c>
-      <c r="M119" s="4">
-        <f>MIN(M118,M9*M15)</f>
-        <v>921.2</v>
-      </c>
-      <c r="O119" s="4">
-        <f>MIN(O118,O9*O15)</f>
-        <v>329</v>
-      </c>
-      <c r="P119" s="4">
-        <f>MIN(P118,P9*P15)</f>
-        <v>1900.8000000000002</v>
-      </c>
-      <c r="R119" s="4">
-        <f>MIN(R118,R9*R15)</f>
-        <v>520</v>
-      </c>
-      <c r="S119" s="4">
-        <f>MIN(S118,S9*S15)</f>
-        <v>393.9</v>
-      </c>
-      <c r="U119" s="4">
-        <f>MIN(U118,U9*U15)</f>
-        <v>401.79999999999995</v>
-      </c>
-      <c r="V119" s="4">
-        <f>MIN(V118,V9*V15)</f>
-        <v>1155</v>
-      </c>
-      <c r="X119" s="4">
-        <f>MIN(X118,X9*X15)</f>
-        <v>499.79999999999995</v>
-      </c>
-      <c r="Y119" s="4">
-        <f>MIN(Y118,Y9*Y15)</f>
-        <v>945</v>
-      </c>
-    </row>
     <row r="120" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="46" t="s">
-        <v>268</v>
+      <c r="A120" s="50" t="s">
+        <v>266</v>
       </c>
       <c r="B120" s="40" t="s">
         <v>175</v>
       </c>
       <c r="E120" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="F120" s="4">
+        <f>MIN(F119,F9*F15)</f>
+        <v>250</v>
+      </c>
+      <c r="G120" s="4">
+        <f>MIN(G119,G9*G15)</f>
+        <v>1000</v>
+      </c>
+      <c r="I120" s="4">
+        <f>MIN(I119,I9*I15)</f>
+        <v>316.2</v>
+      </c>
+      <c r="J120" s="4">
+        <f>MIN(J119,J9*J15)</f>
+        <v>1078</v>
+      </c>
+      <c r="L120" s="4">
+        <f>MIN(L119,L9*L15)</f>
+        <v>301.60000000000002</v>
+      </c>
+      <c r="M120" s="4">
+        <f>MIN(M119,M9*M15)</f>
+        <v>921.2</v>
+      </c>
+      <c r="O120" s="4">
+        <f>MIN(O119,O9*O15)</f>
+        <v>329</v>
+      </c>
+      <c r="P120" s="4">
+        <f>MIN(P119,P9*P15)</f>
+        <v>1900.8000000000002</v>
+      </c>
+      <c r="R120" s="4">
+        <f>MIN(R119,R9*R15)</f>
+        <v>520</v>
+      </c>
+      <c r="S120" s="4">
+        <f>MIN(S119,S9*S15)</f>
+        <v>393.9</v>
+      </c>
+      <c r="U120" s="4">
+        <f>MIN(U119,U9*U15)</f>
+        <v>401.79999999999995</v>
+      </c>
+      <c r="V120" s="4">
+        <f>MIN(V119,V9*V15)</f>
+        <v>1155</v>
+      </c>
+      <c r="X120" s="4">
+        <f>MIN(X119,X9*X15)</f>
+        <v>499.79999999999995</v>
+      </c>
+      <c r="Y120" s="4">
+        <f>MIN(Y119,Y9*Y15)</f>
+        <v>945</v>
+      </c>
+    </row>
+    <row r="121" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="B121" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E121" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="F121" s="4">
+        <f>(F119-F120)*$F$14</f>
+        <v>5075</v>
+      </c>
+      <c r="G121" s="4">
+        <f>(G119-G120+G46-G52)*$F$14</f>
+        <v>6300</v>
+      </c>
+      <c r="I121" s="4">
+        <f>(I119-I120)*$F$14</f>
+        <v>5978.6363187340285</v>
+      </c>
+      <c r="J121" s="4">
+        <f>(J119-J120+J46-J52)*$F$14</f>
+        <v>6411.2243189305136</v>
+      </c>
+      <c r="L121" s="4">
+        <f>(L119-L120)*$F$14</f>
+        <v>5287.1991307240705</v>
+      </c>
+      <c r="M121" s="4">
+        <f>(M119-M120+M46-M52)*$F$14</f>
+        <v>5010.6854466744035</v>
+      </c>
+      <c r="O121" s="4">
+        <f>(O119-O120)*$F$14</f>
+        <v>6061.9345282757467</v>
+      </c>
+      <c r="P121" s="4">
+        <f>(P119-P120+P46-P52)*$F$14</f>
+        <v>9231.0459543351099</v>
+      </c>
+      <c r="R121" s="4">
+        <f>(R119-R120)*$F$14</f>
+        <v>8158.5315467716064</v>
+      </c>
+      <c r="S121" s="4">
+        <f>(S119-S120+S46-S52)*$F$14</f>
+        <v>1657.9244529091936</v>
+      </c>
+      <c r="U121" s="4">
+        <f>(U119-U120)*$F$14</f>
+        <v>7515.5273360810179</v>
+      </c>
+      <c r="V121" s="4">
+        <f>(V119-V120+V46-V52)*$F$14</f>
+        <v>3598.6627307977387</v>
+      </c>
+      <c r="X121" s="4">
+        <f>(X119-X120)*$F$14</f>
+        <v>5532.3442890800825</v>
+      </c>
+      <c r="Y121" s="4">
+        <f>(Y119-Y120+Y46-Y52)*$F$14</f>
+        <v>277.99296996236819</v>
+      </c>
+    </row>
+    <row r="122" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="50" t="s">
         <v>259</v>
       </c>
-      <c r="F120" s="4">
-        <f>(F118-F119)*$F$14</f>
-        <v>5075</v>
-      </c>
-      <c r="G120" s="4">
-        <f>(G118-G119+G46-G52)*$F$14</f>
-        <v>6300</v>
-      </c>
-      <c r="I120" s="4">
-        <f>(I118-I119)*$F$14</f>
-        <v>5978.6363187340285</v>
-      </c>
-      <c r="J120" s="4">
-        <f>(J118-J119+J46-J52)*$F$14</f>
-        <v>6411.2243189305136</v>
-      </c>
-      <c r="L120" s="4">
-        <f>(L118-L119)*$F$14</f>
-        <v>5287.1991307240705</v>
-      </c>
-      <c r="M120" s="4">
-        <f>(M118-M119+M46-M52)*$F$14</f>
-        <v>5010.6854466744035</v>
-      </c>
-      <c r="O120" s="4">
-        <f>(O118-O119)*$F$14</f>
-        <v>6061.9345282757467</v>
-      </c>
-      <c r="P120" s="4">
-        <f>(P118-P119+P46-P52)*$F$14</f>
-        <v>9231.0459543351099</v>
-      </c>
-      <c r="R120" s="4">
-        <f>(R118-R119)*$F$14</f>
-        <v>8158.5315467716064</v>
-      </c>
-      <c r="S120" s="4">
-        <f>(S118-S119+S46-S52)*$F$14</f>
-        <v>1657.9244529091936</v>
-      </c>
-      <c r="U120" s="4">
-        <f>(U118-U119)*$F$14</f>
-        <v>7515.5273360810179</v>
-      </c>
-      <c r="V120" s="4">
-        <f>(V118-V119+V46-V52)*$F$14</f>
-        <v>3598.6627307977387</v>
-      </c>
-      <c r="X120" s="4">
-        <f>(X118-X119)*$F$14</f>
-        <v>5532.3442890800825</v>
-      </c>
-      <c r="Y120" s="4">
-        <f>(Y118-Y119+Y46-Y52)*$F$14</f>
-        <v>277.99296996236819</v>
-      </c>
-    </row>
-    <row r="121" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="46" t="s">
+      <c r="B122" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="E122" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="F122" s="4">
+        <f>MIN(F121+G121, F32)</f>
+        <v>11375</v>
+      </c>
+      <c r="I122" s="4">
+        <f>MIN(I121+J121, I32)</f>
+        <v>12389.860637664542</v>
+      </c>
+      <c r="L122" s="4">
+        <f>MIN(L121+M121, L32)</f>
+        <v>10297.884577398474</v>
+      </c>
+      <c r="O122" s="4">
+        <f>MIN(O121+P121, O32)</f>
+        <v>15292.980482610856</v>
+      </c>
+      <c r="R122" s="4">
+        <f>MIN(R121+S121, R32)</f>
+        <v>9816.4559996808002</v>
+      </c>
+      <c r="U122" s="4">
+        <f>MIN(U121+V121, U32)</f>
+        <v>11114.190066878757</v>
+      </c>
+      <c r="X122" s="4">
+        <f>MIN(X121+Y121, X32)</f>
+        <v>5810.3372590424506</v>
+      </c>
+    </row>
+    <row r="123" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="50" t="s">
         <v>260</v>
-      </c>
-      <c r="B121" s="43" t="s">
-        <v>164</v>
-      </c>
-      <c r="E121" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="F121" s="4">
-        <f>MIN(F120+G120, F32)</f>
-        <v>11375</v>
-      </c>
-      <c r="I121" s="4">
-        <f>MIN(I120+J120, I32)</f>
-        <v>12389.860637664542</v>
-      </c>
-      <c r="L121" s="4">
-        <f>MIN(L120+M120, L32)</f>
-        <v>10297.884577398474</v>
-      </c>
-      <c r="O121" s="4">
-        <f>MIN(O120+P120, O32)</f>
-        <v>15292.980482610856</v>
-      </c>
-      <c r="R121" s="4">
-        <f>MIN(R120+S120, R32)</f>
-        <v>9816.4559996808002</v>
-      </c>
-      <c r="U121" s="4">
-        <f>MIN(U120+V120, U32)</f>
-        <v>11114.190066878757</v>
-      </c>
-      <c r="X121" s="4">
-        <f>MIN(X120+Y120, X32)</f>
-        <v>5810.3372590424506</v>
-      </c>
-    </row>
-    <row r="122" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="46" t="s">
-        <v>261</v>
-      </c>
-      <c r="B122" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="E122" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="F122" s="4">
-        <f>F120/(F120+G120)</f>
-        <v>0.44615384615384618</v>
-      </c>
-      <c r="G122" s="4">
-        <f>G120/(F120+G120)</f>
-        <v>0.55384615384615388</v>
-      </c>
-      <c r="I122" s="4">
-        <f>I120/(I120+J120)</f>
-        <v>0.48254266077531816</v>
-      </c>
-      <c r="J122" s="4">
-        <f>J120/(I120+J120)</f>
-        <v>0.51745733922468184</v>
-      </c>
-      <c r="L122" s="4">
-        <f>L120/(L120+M120)</f>
-        <v>0.51342575176345207</v>
-      </c>
-      <c r="M122" s="4">
-        <f>M120/(L120+M120)</f>
-        <v>0.48657424823654793</v>
-      </c>
-      <c r="O122" s="4">
-        <f>O120/(O120+P120)</f>
-        <v>0.39638673018438575</v>
-      </c>
-      <c r="P122" s="4">
-        <f>P120/(O120+P120)</f>
-        <v>0.60361326981561425</v>
-      </c>
-      <c r="R122" s="4">
-        <f>R120/(R120+S120)</f>
-        <v>0.83110763671093679</v>
-      </c>
-      <c r="S122" s="4">
-        <f>S120/(R120+S120)</f>
-        <v>0.16889236328906318</v>
-      </c>
-      <c r="U122" s="4">
-        <f>U120/(U120+V120)</f>
-        <v>0.67621007836440883</v>
-      </c>
-      <c r="V122" s="4">
-        <f>V120/(U120+V120)</f>
-        <v>0.32378992163559123</v>
-      </c>
-      <c r="X122" s="4">
-        <f>X120/(X120+Y120)</f>
-        <v>0.95215545026586257</v>
-      </c>
-      <c r="Y122" s="4">
-        <f>Y120/(X120+Y120)</f>
-        <v>4.7844549734137418E-2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:25" ht="34" x14ac:dyDescent="0.2">
-      <c r="A123" s="46" t="s">
-        <v>186</v>
       </c>
       <c r="B123" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="E123" s="10" t="s">
+      <c r="E123" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="F123" s="4">
+        <f>F121/(F121+G121)</f>
+        <v>0.44615384615384618</v>
+      </c>
+      <c r="G123" s="4">
+        <f>G121/(F121+G121)</f>
+        <v>0.55384615384615388</v>
+      </c>
+      <c r="I123" s="4">
+        <f>I121/(I121+J121)</f>
+        <v>0.48254266077531816</v>
+      </c>
+      <c r="J123" s="4">
+        <f>J121/(I121+J121)</f>
+        <v>0.51745733922468184</v>
+      </c>
+      <c r="L123" s="4">
+        <f>L121/(L121+M121)</f>
+        <v>0.51342575176345207</v>
+      </c>
+      <c r="M123" s="4">
+        <f>M121/(L121+M121)</f>
+        <v>0.48657424823654793</v>
+      </c>
+      <c r="O123" s="4">
+        <f>O121/(O121+P121)</f>
+        <v>0.39638673018438575</v>
+      </c>
+      <c r="P123" s="4">
+        <f>P121/(O121+P121)</f>
+        <v>0.60361326981561425</v>
+      </c>
+      <c r="R123" s="4">
+        <f>R121/(R121+S121)</f>
+        <v>0.83110763671093679</v>
+      </c>
+      <c r="S123" s="4">
+        <f>S121/(R121+S121)</f>
+        <v>0.16889236328906318</v>
+      </c>
+      <c r="U123" s="4">
+        <f>U121/(U121+V121)</f>
+        <v>0.67621007836440883</v>
+      </c>
+      <c r="V123" s="4">
+        <f>V121/(U121+V121)</f>
+        <v>0.32378992163559123</v>
+      </c>
+      <c r="X123" s="4">
+        <f>X121/(X121+Y121)</f>
+        <v>0.95215545026586257</v>
+      </c>
+      <c r="Y123" s="4">
+        <f>Y121/(X121+Y121)</f>
+        <v>4.7844549734137418E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="A124" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="B124" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E124" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F123" s="4">
-        <f>MAX(F13-F26, 0)*F133</f>
+      <c r="F124" s="4">
+        <f>MAX(F13-F26, 0)*F112</f>
         <v>741757.5</v>
       </c>
-      <c r="G123" s="4">
-        <f>MAX(G13-G26, 0)*G133</f>
+      <c r="G124" s="4">
+        <f>MAX(G13-G26, 0)*G112</f>
         <v>19970010</v>
       </c>
-      <c r="I123" s="4">
-        <f>MAX(I13-I26, 0)*I133</f>
+      <c r="I124" s="4">
+        <f>MAX(I13-I26, 0)*I112</f>
         <v>697549.84714221046</v>
       </c>
-      <c r="J123" s="4">
-        <f>MAX(J13-J26, 0)*J133</f>
+      <c r="J124" s="4">
+        <f>MAX(J13-J26, 0)*J112</f>
         <v>18573008.54128737</v>
       </c>
-      <c r="L123" s="4">
-        <f>MAX(L13-L26, 0)*L133</f>
+      <c r="L124" s="4">
+        <f>MAX(L13-L26, 0)*L112</f>
         <v>585747.5895575179</v>
       </c>
-      <c r="M123" s="4">
-        <f>MAX(M13-M26, 0)*M133</f>
+      <c r="M124" s="4">
+        <f>MAX(M13-M26, 0)*M112</f>
         <v>17143948.479013555</v>
       </c>
-      <c r="O123" s="4">
-        <f>MAX(O13-O26, 0)*O133</f>
+      <c r="O124" s="4">
+        <f>MAX(O13-O26, 0)*O112</f>
         <v>482268.69033299608</v>
       </c>
-      <c r="P123" s="4">
-        <f>MAX(P13-P26, 0)*P133</f>
+      <c r="P124" s="4">
+        <f>MAX(P13-P26, 0)*P112</f>
         <v>15657747.771976728</v>
       </c>
-      <c r="R123" s="4">
-        <f>MAX(R13-R26, 0)*R133</f>
+      <c r="R124" s="4">
+        <f>MAX(R13-R26, 0)*R112</f>
         <v>384257.42411140393</v>
       </c>
-      <c r="S123" s="4">
-        <f>MAX(S13-S26, 0)*S133</f>
+      <c r="S124" s="4">
+        <f>MAX(S13-S26, 0)*S112</f>
         <v>14178856.060528994</v>
       </c>
-      <c r="U123" s="4">
-        <f>MAX(U13-U26, 0)*U133</f>
+      <c r="U124" s="4">
+        <f>MAX(U13-U26, 0)*U112</f>
         <v>268100.68087206065</v>
       </c>
-      <c r="V123" s="4">
-        <f>MAX(V13-V26, 0)*V133</f>
+      <c r="V124" s="4">
+        <f>MAX(V13-V26, 0)*V112</f>
         <v>11963898.943907974</v>
       </c>
-      <c r="X123" s="4">
-        <f>MAX(X13-X26, 0)*X133</f>
+      <c r="X124" s="4">
+        <f>MAX(X13-X26, 0)*X112</f>
         <v>193790.29082328439</v>
       </c>
-      <c r="Y123" s="4">
-        <f>MAX(Y13-Y26, 0)*Y133</f>
+      <c r="Y124" s="4">
+        <f>MAX(Y13-Y26, 0)*Y112</f>
         <v>2533336.3124467055</v>
       </c>
     </row>
-    <row r="125" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="E125" s="15" t="s">
+    <row r="126" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="E126" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F125" s="8"/>
-      <c r="G125" s="8"/>
-      <c r="I125" s="8"/>
-      <c r="J125" s="8"/>
-      <c r="L125" s="8"/>
-      <c r="M125" s="8"/>
-      <c r="O125" s="8"/>
-      <c r="P125" s="8"/>
-      <c r="R125" s="8"/>
-      <c r="S125" s="8"/>
-      <c r="U125" s="8"/>
-      <c r="V125" s="8"/>
-      <c r="X125" s="8"/>
-      <c r="Y125" s="8"/>
-    </row>
-    <row r="126" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A126" s="46" t="s">
-        <v>262</v>
-      </c>
-      <c r="B126" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="E126" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="F126" s="4">
-        <f>MAX(F32-F121,0)</f>
-        <v>1988625</v>
-      </c>
-      <c r="I126" s="4">
-        <f>MAX(I32-I121,0)</f>
-        <v>2037610.1393623354</v>
-      </c>
-      <c r="L126" s="4">
-        <f>MAX(L32-L121,0)</f>
-        <v>2099702.1154226013</v>
-      </c>
-      <c r="O126" s="4">
-        <f>MAX(O32-O121,0)</f>
-        <v>2194707.0195173891</v>
-      </c>
-      <c r="R126" s="4">
-        <f>MAX(R32-R121,0)</f>
-        <v>2990183.5440003192</v>
-      </c>
-      <c r="U126" s="4">
-        <f>MAX(U32-U121,0)</f>
-        <v>24988885.809933122</v>
-      </c>
-      <c r="X126" s="4">
-        <f>MAX(X32-X121,0)</f>
-        <v>2514189.6627409575</v>
-      </c>
+      <c r="F126" s="8"/>
+      <c r="G126" s="8"/>
+      <c r="I126" s="8"/>
+      <c r="J126" s="8"/>
+      <c r="L126" s="8"/>
+      <c r="M126" s="8"/>
+      <c r="O126" s="8"/>
+      <c r="P126" s="8"/>
+      <c r="R126" s="8"/>
+      <c r="S126" s="8"/>
+      <c r="U126" s="8"/>
+      <c r="V126" s="8"/>
+      <c r="X126" s="8"/>
+      <c r="Y126" s="8"/>
     </row>
     <row r="127" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" s="46" t="s">
-        <v>263</v>
+      <c r="A127" s="50" t="s">
+        <v>261</v>
       </c>
       <c r="B127" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="E127" s="10" t="s">
-        <v>166</v>
+      <c r="E127" s="14" t="s">
+        <v>263</v>
       </c>
       <c r="F127" s="4">
-        <f>MIN(F138,F126)</f>
+        <f>MAX(F32-F122,0)</f>
         <v>1988625</v>
       </c>
       <c r="I127" s="4">
-        <f>MIN(I138,I126)</f>
+        <f>MAX(I32-I122,0)</f>
         <v>2037610.1393623354</v>
       </c>
       <c r="L127" s="4">
-        <f>MIN(L138,L126)</f>
+        <f>MAX(L32-L122,0)</f>
         <v>2099702.1154226013</v>
       </c>
       <c r="O127" s="4">
-        <f>MIN(O138,O126)</f>
+        <f>MAX(O32-O122,0)</f>
         <v>2194707.0195173891</v>
       </c>
       <c r="R127" s="4">
-        <f>MIN(R138,R126)</f>
+        <f>MAX(R32-R122,0)</f>
         <v>2990183.5440003192</v>
       </c>
       <c r="U127" s="4">
-        <f>MIN(U138,U126)</f>
-        <v>12231999.624780035</v>
+        <f>MAX(U32-U122,0)</f>
+        <v>24988885.809933122</v>
       </c>
       <c r="X127" s="4">
-        <f>MIN(X138,X126)</f>
-        <v>1789147.7110482706</v>
+        <f>MAX(X32-X122,0)</f>
+        <v>2514189.6627409575</v>
       </c>
     </row>
     <row r="128" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="46" t="s">
-        <v>274</v>
+      <c r="A128" s="50" t="s">
+        <v>262</v>
       </c>
       <c r="B128" s="40" t="s">
         <v>175</v>
       </c>
       <c r="E128" s="10" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="F128" s="4">
-        <f>F126-F127</f>
-        <v>0</v>
+        <f>MIN(F138,F127)</f>
+        <v>1988625</v>
       </c>
       <c r="I128" s="4">
-        <f>I126-I127</f>
-        <v>0</v>
+        <f>MIN(I138,I127)</f>
+        <v>2037610.1393623354</v>
       </c>
       <c r="L128" s="4">
-        <f>L126-L127</f>
-        <v>0</v>
+        <f>MIN(L138,L127)</f>
+        <v>2099702.1154226013</v>
       </c>
       <c r="O128" s="4">
-        <f>O126-O127</f>
-        <v>0</v>
+        <f>MIN(O138,O127)</f>
+        <v>2194707.0195173891</v>
       </c>
       <c r="R128" s="4">
-        <f>R126-R127</f>
-        <v>0</v>
+        <f>MIN(R138,R127)</f>
+        <v>2990183.5440003192</v>
       </c>
       <c r="U128" s="4">
-        <f>U126-U127</f>
-        <v>12756886.185153088</v>
+        <f>MIN(U138,U127)</f>
+        <v>12231999.624780035</v>
       </c>
       <c r="X128" s="4">
-        <f>X126-X127</f>
-        <v>725041.95169268688</v>
+        <f>MIN(X138,X127)</f>
+        <v>1789147.7110482706</v>
       </c>
     </row>
     <row r="129" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="46" t="s">
-        <v>217</v>
+      <c r="A129" s="50" t="s">
+        <v>273</v>
       </c>
       <c r="B129" s="40" t="s">
         <v>175</v>
       </c>
       <c r="E129" s="10" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="F129" s="4">
-        <f>MIN(F128,G75)</f>
+        <f>F127-F128</f>
         <v>0</v>
       </c>
       <c r="I129" s="4">
-        <f>MIN(I128,J75)</f>
+        <f>I127-I128</f>
         <v>0</v>
       </c>
       <c r="L129" s="4">
-        <f>MIN(L128,M75)</f>
+        <f>L127-L128</f>
         <v>0</v>
       </c>
       <c r="O129" s="4">
-        <f>MIN(O128,P75)</f>
+        <f>O127-O128</f>
         <v>0</v>
       </c>
       <c r="R129" s="4">
-        <f>MIN(R128,S75)</f>
+        <f>R127-R128</f>
         <v>0</v>
       </c>
       <c r="U129" s="4">
-        <f>MIN(U128,V75)</f>
-        <v>30.146330393199996</v>
+        <f>U127-U128</f>
+        <v>12756886.185153088</v>
       </c>
       <c r="X129" s="4">
-        <f>MIN(X128,Y75)</f>
-        <v>53.914123679999996</v>
+        <f>X127-X128</f>
+        <v>725041.95169268688</v>
       </c>
     </row>
     <row r="130" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="46" t="s">
-        <v>270</v>
+      <c r="A130" s="50" t="s">
+        <v>217</v>
       </c>
       <c r="B130" s="40" t="s">
         <v>175</v>
       </c>
       <c r="E130" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F130" s="4">
+        <f>MIN(F129,G75)</f>
+        <v>0</v>
+      </c>
+      <c r="I130" s="4">
+        <f>MIN(I129,J75)</f>
+        <v>0</v>
+      </c>
+      <c r="L130" s="4">
+        <f>MIN(L129,M75)</f>
+        <v>0</v>
+      </c>
+      <c r="O130" s="4">
+        <f>MIN(O129,P75)</f>
+        <v>0</v>
+      </c>
+      <c r="R130" s="4">
+        <f>MIN(R129,S75)</f>
+        <v>0</v>
+      </c>
+      <c r="U130" s="4">
+        <f>MIN(U129,V75)</f>
+        <v>30.146330393199996</v>
+      </c>
+      <c r="X130" s="4">
+        <f>MIN(X129,Y75)</f>
+        <v>53.914123679999996</v>
+      </c>
+    </row>
+    <row r="131" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="B131" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E131" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F130" s="4">
-        <f>F139*F127</f>
+      <c r="F131" s="4">
+        <f>F139*F128</f>
         <v>71219.296394549616</v>
       </c>
-      <c r="G130" s="4">
-        <f>G139*F127</f>
+      <c r="G131" s="4">
+        <f>G139*F128</f>
         <v>1917405.7036054505</v>
       </c>
-      <c r="I130" s="4">
-        <f>I139*I127</f>
+      <c r="I131" s="4">
+        <f>I139*I128</f>
         <v>73756.795864359185</v>
       </c>
-      <c r="J130" s="4">
-        <f>J139*I127</f>
+      <c r="J131" s="4">
+        <f>J139*I128</f>
         <v>1963853.343497976</v>
       </c>
-      <c r="L130" s="4">
-        <f>L139*L127</f>
+      <c r="L131" s="4">
+        <f>L139*L128</f>
         <v>69369.234990881247</v>
       </c>
-      <c r="M130" s="4">
-        <f>M139*L127</f>
+      <c r="M131" s="4">
+        <f>M139*L128</f>
         <v>2030332.8804317201</v>
       </c>
-      <c r="O130" s="4">
-        <f>O139*O127</f>
+      <c r="O131" s="4">
+        <f>O139*O128</f>
         <v>65578.525427093409</v>
       </c>
-      <c r="P130" s="4">
-        <f>P139*O127</f>
+      <c r="P131" s="4">
+        <f>P139*O128</f>
         <v>2129128.4940902959</v>
       </c>
-      <c r="R130" s="4">
-        <f>R139*R127</f>
+      <c r="R131" s="4">
+        <f>R139*R128</f>
         <v>78897.979298843828</v>
       </c>
-      <c r="S130" s="4">
-        <f>S139*R127</f>
+      <c r="S131" s="4">
+        <f>S139*R128</f>
         <v>2911285.5647014757</v>
       </c>
-      <c r="U130" s="4">
-        <f>U139*U127</f>
+      <c r="U131" s="4">
+        <f>U139*U128</f>
         <v>268100.68087206065</v>
       </c>
-      <c r="V130" s="4">
-        <f>V139*U127</f>
+      <c r="V131" s="4">
+        <f>V139*U128</f>
         <v>11963898.943907974</v>
       </c>
-      <c r="X130" s="4">
-        <f>X139*X127</f>
+      <c r="X131" s="4">
+        <f>X139*X128</f>
         <v>193790.29082328439</v>
       </c>
-      <c r="Y130" s="4">
-        <f>Y139*X127</f>
+      <c r="Y131" s="4">
+        <f>Y139*X128</f>
         <v>1595357.4202249863</v>
       </c>
     </row>
-    <row r="131" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="46" t="s">
-        <v>275</v>
-      </c>
-      <c r="B131" s="43" t="s">
+    <row r="132" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="50" t="s">
+        <v>274</v>
+      </c>
+      <c r="B132" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="E131" s="10" t="s">
+      <c r="E132" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="F131" s="4">
-        <f>F130</f>
+      <c r="F132" s="4">
+        <f>F131</f>
         <v>71219.296394549616</v>
       </c>
-      <c r="G131" s="4">
-        <f>G130+F129</f>
+      <c r="G132" s="4">
+        <f>G131+F130</f>
         <v>1917405.7036054505</v>
       </c>
-      <c r="I131" s="4">
-        <f>I130</f>
+      <c r="I132" s="4">
+        <f>I131</f>
         <v>73756.795864359185</v>
       </c>
-      <c r="J131" s="4">
-        <f>J130+I129</f>
+      <c r="J132" s="4">
+        <f>J131+I130</f>
         <v>1963853.343497976</v>
       </c>
-      <c r="L131" s="4">
-        <f>L130</f>
+      <c r="L132" s="4">
+        <f>L131</f>
         <v>69369.234990881247</v>
       </c>
-      <c r="M131" s="4">
-        <f>M130+L129</f>
+      <c r="M132" s="4">
+        <f>M131+L130</f>
         <v>2030332.8804317201</v>
       </c>
-      <c r="O131" s="4">
-        <f>O130</f>
+      <c r="O132" s="4">
+        <f>O131</f>
         <v>65578.525427093409</v>
       </c>
-      <c r="P131" s="4">
-        <f>P130+O129</f>
+      <c r="P132" s="4">
+        <f>P131+O130</f>
         <v>2129128.4940902959</v>
       </c>
-      <c r="R131" s="4">
-        <f>R130</f>
+      <c r="R132" s="4">
+        <f>R131</f>
         <v>78897.979298843828</v>
       </c>
-      <c r="S131" s="4">
-        <f>S130+R129</f>
+      <c r="S132" s="4">
+        <f>S131+R130</f>
         <v>2911285.5647014757</v>
       </c>
-      <c r="U131" s="4">
-        <f>U130</f>
+      <c r="U132" s="4">
+        <f>U131</f>
         <v>268100.68087206065</v>
       </c>
-      <c r="V131" s="4">
-        <f>V130+U129</f>
+      <c r="V132" s="4">
+        <f>V131+U130</f>
         <v>11963929.090238368</v>
       </c>
-      <c r="X131" s="4">
-        <f>X130</f>
+      <c r="X132" s="4">
+        <f>X131</f>
         <v>193790.29082328439</v>
       </c>
-      <c r="Y131" s="4">
-        <f>Y130+X129</f>
+      <c r="Y132" s="4">
+        <f>Y131+X130</f>
         <v>1595411.3343486662</v>
       </c>
     </row>
-    <row r="132" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="E132" s="15" t="s">
+    <row r="133" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="E133" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F132" s="8"/>
-      <c r="G132" s="8"/>
-      <c r="I132" s="8"/>
-      <c r="J132" s="8"/>
-      <c r="L132" s="8"/>
-      <c r="M132" s="8"/>
-      <c r="O132" s="8"/>
-      <c r="P132" s="8"/>
-      <c r="R132" s="8"/>
-      <c r="S132" s="8"/>
-      <c r="U132" s="8"/>
-      <c r="V132" s="8"/>
-      <c r="X132" s="8"/>
-      <c r="Y132" s="8"/>
-    </row>
-    <row r="133" spans="1:28" ht="34" x14ac:dyDescent="0.2">
-      <c r="A133" s="46" t="s">
-        <v>279</v>
-      </c>
-      <c r="B133" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="E133" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F133" s="4">
-        <f>MAX(F111-$F21,0)</f>
-        <v>149.85</v>
-      </c>
-      <c r="G133" s="4">
-        <f>MAX(G111-$G21,0)</f>
-        <v>99.9</v>
-      </c>
-      <c r="I133" s="4">
-        <f>MAX(I111-$F21,0)</f>
-        <v>142.7065972058532</v>
-      </c>
-      <c r="J133" s="4">
-        <f>MAX(J111-$G21,0)</f>
-        <v>92.96265349260409</v>
-      </c>
-      <c r="L133" s="4">
-        <f>MAX(L111-$F21,0)</f>
-        <v>135.27657957448451</v>
-      </c>
-      <c r="M133" s="4">
-        <f>MAX(M111-$G21,0)</f>
-        <v>85.850234751890639</v>
-      </c>
-      <c r="O133" s="4">
-        <f>MAX(O111-$F21,0)</f>
-        <v>128.2629495566479</v>
-      </c>
-      <c r="P133" s="4">
-        <f>MAX(P111-$G21,0)</f>
-        <v>78.483377636421963</v>
-      </c>
-      <c r="R133" s="4">
-        <f>MAX(R111-$F21,0)</f>
-        <v>121.60045066816581</v>
-      </c>
-      <c r="S133" s="4">
-        <f>MAX(S111-$G21,0)</f>
-        <v>70.729833439897206</v>
-      </c>
-      <c r="U133" s="4">
-        <f>MAX(U111-$F21,0)</f>
-        <v>113.50579207115184</v>
-      </c>
-      <c r="V133" s="4">
-        <f>MAX(V111-$G21,0)</f>
-        <v>59.861397697928425</v>
-      </c>
-      <c r="X133" s="4">
-        <f>MAX(X111-$F21,0)</f>
-        <v>85.596418208164479</v>
-      </c>
-      <c r="Y133" s="4">
-        <f>MAX(Y111-$G21,0)</f>
-        <v>12.682217278399568</v>
-      </c>
+      <c r="F133" s="8"/>
+      <c r="G133" s="8"/>
+      <c r="I133" s="8"/>
+      <c r="J133" s="8"/>
+      <c r="L133" s="8"/>
+      <c r="M133" s="8"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="8"/>
+      <c r="R133" s="8"/>
+      <c r="S133" s="8"/>
+      <c r="U133" s="8"/>
+      <c r="V133" s="8"/>
+      <c r="X133" s="8"/>
+      <c r="Y133" s="8"/>
     </row>
     <row r="134" spans="1:28" ht="34" x14ac:dyDescent="0.2">
-      <c r="A134" s="46" t="s">
-        <v>278</v>
+      <c r="A134" s="50" t="s">
+        <v>277</v>
       </c>
       <c r="B134" s="40" t="s">
         <v>175</v>
@@ -11702,59 +11699,59 @@
         <v>137</v>
       </c>
       <c r="F134" s="4">
-        <f>F133/$F$22</f>
+        <f>F112/$F$22</f>
         <v>1</v>
       </c>
       <c r="G134" s="4">
-        <f>G133/$G$22</f>
+        <f>G112/$G$22</f>
         <v>1</v>
       </c>
       <c r="I134" s="4">
-        <f>I133/$F$22</f>
+        <f>I112/$F$22</f>
         <v>0.95232964435003808</v>
       </c>
       <c r="J134" s="4">
-        <f>J133/$G$22</f>
+        <f>J112/$G$22</f>
         <v>0.93055709201805892</v>
       </c>
       <c r="L134" s="4">
-        <f>L133/$F$22</f>
+        <f>L112/$F$22</f>
         <v>0.9027466104403371</v>
       </c>
       <c r="M134" s="4">
-        <f>M133/$G$22</f>
+        <f>M112/$G$22</f>
         <v>0.85936170922813448</v>
       </c>
       <c r="O134" s="4">
-        <f>O133/$F$22</f>
+        <f>O112/$F$22</f>
         <v>0.85594227265030298</v>
       </c>
       <c r="P134" s="4">
-        <f>P133/$G$22</f>
+        <f>P112/$G$22</f>
         <v>0.78561939575997952</v>
       </c>
       <c r="R134" s="4">
-        <f>R133/$F$22</f>
+        <f>R112/$F$22</f>
         <v>0.8114811522733788</v>
       </c>
       <c r="S134" s="4">
-        <f>S133/$G$22</f>
+        <f>S112/$G$22</f>
         <v>0.70800634073971169</v>
       </c>
       <c r="U134" s="4">
-        <f>U133/$F$22</f>
+        <f>U112/$F$22</f>
         <v>0.75746274321756324</v>
       </c>
       <c r="V134" s="4">
-        <f>V133/$G$22</f>
+        <f>V112/$G$22</f>
         <v>0.59921319016945362</v>
       </c>
       <c r="X134" s="4">
-        <f>X133/$F$22</f>
+        <f>X112/$F$22</f>
         <v>0.57121400205648643</v>
       </c>
       <c r="Y134" s="4">
-        <f>Y133/$G$22</f>
+        <f>Y112/$G$22</f>
         <v>0.12694912190590157</v>
       </c>
       <c r="Z134">
@@ -11769,7 +11766,7 @@
       </c>
     </row>
     <row r="135" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A135" s="46" t="s">
+      <c r="A135" s="50" t="s">
         <v>187</v>
       </c>
       <c r="B135" s="40" t="s">
@@ -11779,7 +11776,7 @@
         <v>188</v>
       </c>
       <c r="F135" s="4">
-        <f>MAX(MIN(F134/$F$17, 1), 0)</f>
+        <f>MAX(MIN((F134-$F$16)/$F$17, 1), 0)</f>
         <v>1</v>
       </c>
       <c r="G135" s="4">
@@ -11787,7 +11784,7 @@
         <v>1</v>
       </c>
       <c r="I135" s="4">
-        <f>MAX(MIN(I134/$F$17, 1), 0)</f>
+        <f>MAX(MIN((I134-$F$16)/$F$17, 1), 0)</f>
         <v>1</v>
       </c>
       <c r="J135" s="4">
@@ -11795,7 +11792,7 @@
         <v>1</v>
       </c>
       <c r="L135" s="4">
-        <f>MAX(MIN(L134/$F$17, 1), 0)</f>
+        <f>MAX(MIN((L134-$F$16)/$F$17, 1), 0)</f>
         <v>1</v>
       </c>
       <c r="M135" s="4">
@@ -11803,7 +11800,7 @@
         <v>1</v>
       </c>
       <c r="O135" s="4">
-        <f>MAX(MIN(O134/$F$17, 1), 0)</f>
+        <f>MAX(MIN((O134-$F$16)/$F$17, 1), 0)</f>
         <v>1</v>
       </c>
       <c r="P135" s="4">
@@ -11811,7 +11808,7 @@
         <v>1</v>
       </c>
       <c r="R135" s="4">
-        <f>MAX(MIN(R134/$F$17, 1), 0)</f>
+        <f>MAX(MIN((R134-$F$16)/$F$17, 1), 0)</f>
         <v>1</v>
       </c>
       <c r="S135" s="4">
@@ -11819,7 +11816,7 @@
         <v>1</v>
       </c>
       <c r="U135" s="4">
-        <f>MAX(MIN(U134/$F$17, 1), 0)</f>
+        <f>MAX(MIN((U134-$F$16)/$F$17, 1), 0)</f>
         <v>1</v>
       </c>
       <c r="V135" s="4">
@@ -11827,7 +11824,7 @@
         <v>1</v>
       </c>
       <c r="X135" s="4">
-        <f>MAX(MIN(X134/$F$17, 1), 0)</f>
+        <f>MAX(MIN((X134-$F$16)/$F$17, 1), 0)</f>
         <v>1</v>
       </c>
       <c r="Y135" s="4">
@@ -11846,7 +11843,7 @@
       </c>
     </row>
     <row r="136" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A136" s="46"/>
+      <c r="A136" s="50"/>
       <c r="Z136">
         <v>0.2</v>
       </c>
@@ -11859,7 +11856,7 @@
       </c>
     </row>
     <row r="137" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="46" t="s">
+      <c r="A137" s="50" t="s">
         <v>189</v>
       </c>
       <c r="B137" s="40" t="s">
@@ -11869,59 +11866,59 @@
         <v>76</v>
       </c>
       <c r="F137" s="4">
-        <f>F123*F135</f>
+        <f>F124*F135</f>
         <v>741757.5</v>
       </c>
       <c r="G137" s="4">
-        <f>G123*G135</f>
+        <f>G124*G135</f>
         <v>19970010</v>
       </c>
       <c r="I137" s="4">
-        <f>I123*I135</f>
+        <f>I124*I135</f>
         <v>697549.84714221046</v>
       </c>
       <c r="J137" s="4">
-        <f>J123*J135</f>
+        <f>J124*J135</f>
         <v>18573008.54128737</v>
       </c>
       <c r="L137" s="4">
-        <f>L123*L135</f>
+        <f>L124*L135</f>
         <v>585747.5895575179</v>
       </c>
       <c r="M137" s="4">
-        <f>M123*M135</f>
+        <f>M124*M135</f>
         <v>17143948.479013555</v>
       </c>
       <c r="O137" s="4">
-        <f>O123*O135</f>
+        <f>O124*O135</f>
         <v>482268.69033299608</v>
       </c>
       <c r="P137" s="4">
-        <f>P123*P135</f>
+        <f>P124*P135</f>
         <v>15657747.771976728</v>
       </c>
       <c r="R137" s="4">
-        <f>R123*R135</f>
+        <f>R124*R135</f>
         <v>384257.42411140393</v>
       </c>
       <c r="S137" s="4">
-        <f>S123*S135</f>
+        <f>S124*S135</f>
         <v>14178856.060528994</v>
       </c>
       <c r="U137" s="4">
-        <f>U123*U135</f>
+        <f>U124*U135</f>
         <v>268100.68087206065</v>
       </c>
       <c r="V137" s="4">
-        <f>V123*V135</f>
+        <f>V124*V135</f>
         <v>11963898.943907974</v>
       </c>
       <c r="X137" s="4">
-        <f>X123*X135</f>
+        <f>X124*X135</f>
         <v>193790.29082328439</v>
       </c>
       <c r="Y137" s="4">
-        <f>Y123*Y135</f>
+        <f>Y124*Y135</f>
         <v>1595357.4202249863</v>
       </c>
       <c r="Z137">
@@ -11936,7 +11933,7 @@
       </c>
     </row>
     <row r="138" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A138" s="46" t="s">
+      <c r="A138" s="50" t="s">
         <v>190</v>
       </c>
       <c r="B138" s="40" t="s">
@@ -12003,7 +12000,7 @@
       </c>
     </row>
     <row r="139" spans="1:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="A139" s="46" t="s">
+      <c r="A139" s="50" t="s">
         <v>191</v>
       </c>
       <c r="B139" s="40" t="s">
@@ -12071,7 +12068,7 @@
     </row>
     <row r="141" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="E141" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
@@ -12090,7 +12087,7 @@
     </row>
     <row r="142" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B142" s="43" t="s">
         <v>164</v>
@@ -12099,65 +12096,65 @@
         <v>204</v>
       </c>
       <c r="F142" s="4">
-        <f>(F110 - F130 - F118)*$F$29</f>
+        <f>(F110 - F131 - F119)*$F$29</f>
         <v>2842.5614072109011</v>
       </c>
       <c r="G142" s="4">
-        <f>(G110 - G130 - G118)*$G$29</f>
+        <f>(G110 - G131 - G119)*$G$29</f>
         <v>46145.188592789098</v>
       </c>
       <c r="I142" s="4">
-        <f>(I110 - I130 - I118)*$F$29</f>
+        <f>(I110 - I131 - I119)*$F$29</f>
         <v>2677.6184746142349</v>
       </c>
       <c r="J142" s="4">
-        <f>(J110 - J130 - J118)*$G$29</f>
+        <f>(J110 - J131 - J119)*$G$29</f>
         <v>42564.533744839202</v>
       </c>
       <c r="L142" s="4">
-        <f>(L110 - L130 - L118)*$F$29</f>
+        <f>(L110 - L131 - L119)*$F$29</f>
         <v>2523.7480844526031</v>
       </c>
       <c r="M142" s="4">
-        <f>(M110 - M130 - M118)*$G$29</f>
+        <f>(M110 - M131 - M119)*$G$29</f>
         <v>38862.193872352735</v>
       </c>
       <c r="O142" s="4">
-        <f>(O110 - O130 - O118)*$F$29</f>
+        <f>(O110 - O131 - O119)*$F$29</f>
         <v>2375.4637244915798</v>
       </c>
       <c r="P142" s="4">
-        <f>(P110 - P130 - P118)*$G$29</f>
+        <f>(P110 - P131 - P119)*$G$29</f>
         <v>34955.477119415053</v>
       </c>
       <c r="R142" s="4">
-        <f>(R110 - R130 - R118)*$F$29</f>
+        <f>(R110 - R131 - R119)*$F$29</f>
         <v>2194.4227483112763</v>
       </c>
       <c r="S142" s="4">
-        <f>(S110 - S130 - S118)*$G$29</f>
+        <f>(S110 - S131 - S119)*$G$29</f>
         <v>29516.557668764955</v>
       </c>
       <c r="U142" s="4">
-        <f>(U110 - U130 - U118)*$F$29</f>
+        <f>(U110 - U131 - U119)*$F$29</f>
         <v>1637.352005824587</v>
       </c>
       <c r="V142" s="4">
-        <f>(V110 - V130 - V118)*$G$29</f>
+        <f>(V110 - V131 - V119)*$G$29</f>
         <v>5976.1503720949167</v>
       </c>
       <c r="X142" s="4">
-        <f>(X110 - X130 - X118)*$F$29</f>
+        <f>(X110 - X131 - X119)*$F$29</f>
         <v>1235.4276221975688</v>
       </c>
       <c r="Y142" s="4">
-        <f>(Y110 - Y130 - Y118)*$G$29</f>
+        <f>(Y110 - Y131 - Y119)*$G$29</f>
         <v>3181.3482950049956</v>
       </c>
     </row>
     <row r="143" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="46" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B143" s="43" t="s">
         <v>164</v>
@@ -12166,59 +12163,59 @@
         <v>216</v>
       </c>
       <c r="F143" s="4">
-        <f>F130*$F20</f>
+        <f>F131*$F20</f>
         <v>21365.788918364884</v>
       </c>
       <c r="G143" s="4">
-        <f>(G130+F129)*$G20</f>
+        <f>(G131+F130)*$G20</f>
         <v>479351.42590136261</v>
       </c>
       <c r="I143" s="4">
-        <f>I130*$F20</f>
+        <f>I131*$F20</f>
         <v>22127.038759307754</v>
       </c>
       <c r="J143" s="4">
-        <f>(J130+I129)*$G20</f>
+        <f>(J131+I130)*$G20</f>
         <v>490963.33587449399</v>
       </c>
       <c r="L143" s="4">
-        <f>L130*$F20</f>
+        <f>L131*$F20</f>
         <v>20810.770497264373</v>
       </c>
       <c r="M143" s="4">
-        <f>(M130+L129)*$G20</f>
+        <f>(M131+L130)*$G20</f>
         <v>507583.22010793001</v>
       </c>
       <c r="O143" s="4">
-        <f>O130*$F20</f>
+        <f>O131*$F20</f>
         <v>19673.557628128023</v>
       </c>
       <c r="P143" s="4">
-        <f>(P130+O129)*$G20</f>
+        <f>(P131+O130)*$G20</f>
         <v>532282.12352257397</v>
       </c>
       <c r="R143" s="4">
-        <f>R130*$F20</f>
+        <f>R131*$F20</f>
         <v>23669.393789653146</v>
       </c>
       <c r="S143" s="4">
-        <f>(S130+R129)*$G20</f>
+        <f>(S131+R130)*$G20</f>
         <v>727821.39117536892</v>
       </c>
       <c r="U143" s="4">
-        <f>U130*$F20</f>
+        <f>U131*$F20</f>
         <v>80430.204261618186</v>
       </c>
       <c r="V143" s="4">
-        <f>(V130+U129)*$G20</f>
+        <f>(V131+U130)*$G20</f>
         <v>2990982.272559592</v>
       </c>
       <c r="X143" s="4">
-        <f>X130*$F20</f>
+        <f>X131*$F20</f>
         <v>58137.087246985313</v>
       </c>
       <c r="Y143" s="4">
-        <f>(Y130+X129)*$G20</f>
+        <f>(Y131+X130)*$G20</f>
         <v>398852.83358716656</v>
       </c>
     </row>
@@ -12233,59 +12230,59 @@
         <v>167</v>
       </c>
       <c r="F144" s="4">
-        <f>F118-F121*F122-F119</f>
+        <f>F119-F122*F123-F120</f>
         <v>2175</v>
       </c>
       <c r="G144" s="4">
-        <f>G118-F121*G122-G119</f>
+        <f>G119-F122*G123-G120</f>
         <v>2700</v>
       </c>
       <c r="I144" s="4">
-        <f>I118-I121*I122-I119</f>
+        <f>I119-I122*I123-I120</f>
         <v>2562.2727080288705</v>
       </c>
       <c r="J144" s="4">
-        <f>J118-I121*J122-J119</f>
+        <f>J119-I122*J123-J120</f>
         <v>2747.6675652559352</v>
       </c>
       <c r="L144" s="4">
-        <f>L118-L121*L122-L119</f>
+        <f>L119-L122*L123-L120</f>
         <v>2265.9424845960316</v>
       </c>
       <c r="M144" s="4">
-        <f>M118-L121*M122-M119</f>
+        <f>M119-L122*M123-M120</f>
         <v>2147.4366200033164</v>
       </c>
       <c r="O144" s="4">
-        <f>O118-O121*O122-O119</f>
+        <f>O119-O122*O123-O120</f>
         <v>2597.9719406896065</v>
       </c>
       <c r="P144" s="4">
-        <f>P118-O121*P122-P119</f>
+        <f>P119-O122*P123-P120</f>
         <v>3956.1625518579049</v>
       </c>
       <c r="R144" s="4">
-        <f>R118-R121*R122-R119</f>
+        <f>R119-R122*R123-R120</f>
         <v>3496.5135200449749</v>
       </c>
       <c r="S144" s="4">
-        <f>S118-R121*S122-S119</f>
+        <f>S119-R122*S123-S120</f>
         <v>710.53905124679738</v>
       </c>
       <c r="U144" s="4">
-        <f>U118-U121*U122-U119</f>
+        <f>U119-U122*U123-U120</f>
         <v>3220.9402868918642</v>
       </c>
       <c r="V144" s="4">
-        <f>V118-U121*V122-V119</f>
+        <f>V119-U122*V123-V120</f>
         <v>1542.2840274847454</v>
       </c>
       <c r="X144" s="4">
-        <f>X118-X121*X122-X119</f>
+        <f>X119-X122*X123-X120</f>
         <v>2371.0046953200363</v>
       </c>
       <c r="Y144" s="4">
-        <f>Y118-X121*Y122-Y119</f>
+        <f>Y119-X122*Y123-Y120</f>
         <v>119.13984426958632</v>
       </c>
     </row>
@@ -12300,156 +12297,156 @@
         <v>168</v>
       </c>
       <c r="F145" s="4">
-        <f>F118*$F20</f>
+        <f>F119*$F20</f>
         <v>2250</v>
       </c>
       <c r="G145" s="4">
-        <f>(G118+G46-G52)*$G20</f>
+        <f>(G119+G46-G52)*$G20</f>
         <v>2500</v>
       </c>
       <c r="I145" s="4">
-        <f>I118*$F20</f>
+        <f>I119*$F20</f>
         <v>2657.1327080288697</v>
       </c>
       <c r="J145" s="4">
-        <f>(J118+J46-J52)*$G20</f>
+        <f>(J119+J46-J52)*$G20</f>
         <v>2559.2229710466122</v>
       </c>
       <c r="L145" s="4">
-        <f>L118*$F20</f>
+        <f>L119*$F20</f>
         <v>2356.4224845960307</v>
       </c>
       <c r="M145" s="4">
-        <f>(M118+M46-M52)*$G20</f>
+        <f>(M119+M46-M52)*$G20</f>
         <v>2019.8305166694299</v>
       </c>
       <c r="O145" s="4">
-        <f>O118*$F20</f>
+        <f>O119*$F20</f>
         <v>2696.6719406896059</v>
       </c>
       <c r="P145" s="4">
-        <f>(P118+P46-P52)*$G20</f>
+        <f>(P119+P46-P52)*$G20</f>
         <v>3772.0021265482537</v>
       </c>
       <c r="R145" s="4">
-        <f>R118*$F20</f>
+        <f>R119*$F20</f>
         <v>3652.5135200449745</v>
       </c>
       <c r="S145" s="4">
-        <f>(S118+S46-S52)*$G20</f>
+        <f>(S119+S46-S52)*$G20</f>
         <v>690.59087603899775</v>
       </c>
       <c r="U145" s="4">
-        <f>U118*$F20</f>
+        <f>U119*$F20</f>
         <v>3341.4802868918646</v>
       </c>
       <c r="V145" s="4">
-        <f>(V118+V46-V52)*$G20</f>
+        <f>(V119+V46-V52)*$G20</f>
         <v>1573.9866895706211</v>
       </c>
       <c r="X145" s="4">
-        <f>X118*$F20</f>
+        <f>X119*$F20</f>
         <v>2520.9446953200354</v>
       </c>
       <c r="Y145" s="4">
-        <f>(Y118+Y46-Y52)*$G20</f>
+        <f>(Y119+Y46-Y52)*$G20</f>
         <v>335.53320355798866</v>
       </c>
     </row>
     <row r="148" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A148" s="33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F148" s="4">
-        <f>F144+F119</f>
+        <f>F144+F120</f>
         <v>2425</v>
       </c>
       <c r="G148" s="4">
-        <f>G144+G119</f>
+        <f>G144+G120</f>
         <v>3700</v>
       </c>
       <c r="I148" s="4">
-        <f>I144+I119</f>
+        <f>I144+I120</f>
         <v>2878.4727080288703</v>
       </c>
       <c r="J148" s="4">
-        <f>J144+J119</f>
+        <f>J144+J120</f>
         <v>3825.6675652559352</v>
       </c>
       <c r="L148" s="4">
-        <f>L144+L119</f>
+        <f>L144+L120</f>
         <v>2567.5424845960315</v>
       </c>
       <c r="M148" s="4">
-        <f>M144+M119</f>
+        <f>M144+M120</f>
         <v>3068.6366200033162</v>
       </c>
       <c r="O148" s="4">
-        <f>O144+O119</f>
+        <f>O144+O120</f>
         <v>2926.9719406896065</v>
       </c>
       <c r="P148" s="4">
-        <f>P144+P119</f>
+        <f>P144+P120</f>
         <v>5856.9625518579051</v>
       </c>
       <c r="R148" s="4">
-        <f>R144+R119</f>
+        <f>R144+R120</f>
         <v>4016.5135200449749</v>
       </c>
       <c r="S148" s="4">
-        <f>S144+S119</f>
+        <f>S144+S120</f>
         <v>1104.4390512467974</v>
       </c>
       <c r="U148" s="4">
-        <f>U144+U119</f>
+        <f>U144+U120</f>
         <v>3622.7402868918643</v>
       </c>
       <c r="V148" s="4">
-        <f>V144+V119</f>
+        <f>V144+V120</f>
         <v>2697.2840274847454</v>
       </c>
       <c r="X148" s="4">
-        <f>X144+X119</f>
+        <f>X144+X120</f>
         <v>2870.8046953200364</v>
       </c>
       <c r="Y148" s="4">
-        <f>Y144+Y119</f>
+        <f>Y144+Y120</f>
         <v>1064.1398442695863</v>
       </c>
     </row>
     <row r="150" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A150" s="46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B150" s="43" t="s">
         <v>164</v>
       </c>
       <c r="F150" s="4">
-        <f>F121+F130+G130+F129</f>
+        <f>F122+F131+G131+F130</f>
         <v>2000000</v>
       </c>
       <c r="I150" s="4">
-        <f>I121+I130+J130</f>
+        <f>I122+I131+J131</f>
         <v>2049999.9999999998</v>
       </c>
       <c r="L150" s="4">
-        <f>L121+L130+M130</f>
+        <f>L122+L131+M131</f>
         <v>2110000</v>
       </c>
       <c r="O150" s="4">
-        <f>O121+O130+P130</f>
+        <f>O122+O131+P131</f>
         <v>2210000</v>
       </c>
       <c r="R150" s="4">
-        <f>R121+R130+S130</f>
+        <f>R122+R131+S131</f>
         <v>3000000.0000000005</v>
       </c>
       <c r="U150" s="4">
-        <f>U121+U130+V130</f>
+        <f>U122+U131+V131</f>
         <v>12243113.814846914</v>
       </c>
       <c r="X150" s="4">
-        <f>X121+X130+Y130</f>
+        <f>X122+X131+Y131</f>
         <v>1794958.0483073131</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor update to CL
</commit_message>
<xml_diff>
--- a/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
+++ b/sisepuede/ref/validation_workbooks/carbon_ledger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/sisepuede/sisepuede/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9899F6F-C232-1241-9D48-CC7CBCB36DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6325D8A9-6329-AD4A-A219-1AE5EC10DAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="760" windowWidth="31100" windowHeight="19860" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
+    <workbookView xWindow="2680" yWindow="760" windowWidth="31100" windowHeight="19860" activeTab="2" xr2:uid="{49B92464-5B50-C04B-B571-E5276F1DC1EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="300">
   <si>
     <t>forest_primary_c_ha</t>
   </si>
@@ -922,10 +922,28 @@
     <t>A_r(t + 1)</t>
   </si>
   <si>
-    <t>\alpha_{avail}(t)</t>
-  </si>
-  <si>
-    <t>\bar{S}_{targ}</t>
+    <t>\chi_(t)</t>
+  </si>
+  <si>
+    <t>\check{\alpha}(t)</t>
+  </si>
+  <si>
+    <t>\bar{\alpha}(t)</t>
+  </si>
+  <si>
+    <t>\hat{\alpha}(t)</t>
+  </si>
+  <si>
+    <t>\bar{S}_{targ}(t)</t>
+  </si>
+  <si>
+    <t>k_0</t>
+  </si>
+  <si>
+    <t>\gamma</t>
+  </si>
+  <si>
+    <t>k_{heav}</t>
   </si>
 </sst>
 </file>
@@ -981,7 +999,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1060,6 +1078,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF12501A"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1073,7 +1097,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1220,6 +1244,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6375,8 +6402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40F0562-A765-A442-B9DB-CF71D123E451}">
   <dimension ref="A1:AN159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7232,7 +7259,7 @@
         <v>249</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C15" s="41" t="s">
         <v>162</v>
@@ -7293,7 +7320,9 @@
       <c r="A16" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="49" t="s">
+        <v>293</v>
+      </c>
       <c r="C16" s="41" t="s">
         <v>162</v>
       </c>
@@ -7336,7 +7365,9 @@
       <c r="A17" s="49" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="49"/>
+      <c r="B17" s="49" t="s">
+        <v>294</v>
+      </c>
       <c r="C17" s="41" t="s">
         <v>162</v>
       </c>
@@ -7364,7 +7395,9 @@
       <c r="A18" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="49"/>
+      <c r="B18" s="53" t="s">
+        <v>295</v>
+      </c>
       <c r="C18" s="41" t="s">
         <v>162</v>
       </c>
@@ -7390,7 +7423,9 @@
       <c r="A19" s="49" t="s">
         <v>230</v>
       </c>
-      <c r="B19" s="49"/>
+      <c r="B19" s="49" t="s">
+        <v>297</v>
+      </c>
       <c r="C19" s="41" t="s">
         <v>162</v>
       </c>
@@ -7418,7 +7453,9 @@
       <c r="A20" s="49" t="s">
         <v>232</v>
       </c>
-      <c r="B20" s="49"/>
+      <c r="B20" s="49" t="s">
+        <v>298</v>
+      </c>
       <c r="C20" s="41" t="s">
         <v>162</v>
       </c>
@@ -7469,7 +7506,9 @@
       <c r="A22" s="49" t="s">
         <v>231</v>
       </c>
-      <c r="B22" s="49"/>
+      <c r="B22" s="49" t="s">
+        <v>299</v>
+      </c>
       <c r="C22" s="42" t="s">
         <v>174</v>
       </c>

</xml_diff>